<commit_message>
Adiciona daily realizada em 22-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52471940-71F1-4810-8467-94B685763BF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB728B95-4A81-46F6-9761-1364E7D5080B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="148">
   <si>
     <t>REDES</t>
   </si>
@@ -538,6 +538,18 @@
   </si>
   <si>
     <t>Formulários para definição de personas</t>
+  </si>
+  <si>
+    <t>Entrega do diagrama de classes, entrega dos layouts login e cadastro web e ata de reunião integrando com o pessoal de redes</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do programa em linguagem C para extrair os dados solicitados</t>
+  </si>
+  <si>
+    <t>Criação do logo e continuação da estruturação do banco de dados</t>
+  </si>
+  <si>
+    <t>Análise das respostas do formulário e pesquisa mais aprofundada de sistemas semelhantes no mercado</t>
   </si>
 </sst>
 </file>
@@ -1152,18 +1164,6 @@
     <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1172,6 +1172,18 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1586,7 +1598,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1620,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="91" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -1888,7 +1900,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
@@ -1998,7 +2010,7 @@
       <c r="CR2" s="94"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
@@ -2286,10 +2298,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="92"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -2311,7 +2323,9 @@
       <c r="I4" s="86" t="s">
         <v>140</v>
       </c>
-      <c r="J4" s="86"/>
+      <c r="J4" s="86" t="s">
+        <v>144</v>
+      </c>
       <c r="K4" s="86"/>
       <c r="L4" s="86"/>
       <c r="M4" s="86"/>
@@ -2319,27 +2333,27 @@
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="93" t="s">
+      <c r="AV4" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="93" t="s">
+      <c r="AW4" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="93" t="s">
+      <c r="BT4" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="93" t="s">
+      <c r="BW4" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="93" t="s">
+      <c r="CO4" s="95" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="92"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -2361,7 +2375,9 @@
       <c r="I5" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="J5" s="86"/>
+      <c r="J5" s="86" t="s">
+        <v>145</v>
+      </c>
       <c r="K5" s="86"/>
       <c r="L5" s="86"/>
       <c r="M5" s="86"/>
@@ -2369,17 +2385,17 @@
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="93"/>
-      <c r="AW5" s="93"/>
-      <c r="BT5" s="93"/>
-      <c r="BW5" s="93"/>
-      <c r="CO5" s="93"/>
+      <c r="AV5" s="95"/>
+      <c r="AW5" s="95"/>
+      <c r="BT5" s="95"/>
+      <c r="BW5" s="95"/>
+      <c r="CO5" s="95"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -2401,7 +2417,9 @@
       <c r="I6" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="J6" s="86"/>
+      <c r="J6" s="86" t="s">
+        <v>146</v>
+      </c>
       <c r="K6" s="86"/>
       <c r="L6" s="86"/>
       <c r="M6" s="86"/>
@@ -2409,17 +2427,17 @@
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="93"/>
-      <c r="AW6" s="93"/>
-      <c r="BT6" s="93"/>
-      <c r="BW6" s="93"/>
-      <c r="CO6" s="93"/>
+      <c r="AV6" s="95"/>
+      <c r="AW6" s="95"/>
+      <c r="BT6" s="95"/>
+      <c r="BW6" s="95"/>
+      <c r="CO6" s="95"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="92"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -2441,7 +2459,9 @@
       <c r="I7" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="J7" s="86"/>
+      <c r="J7" s="86" t="s">
+        <v>147</v>
+      </c>
       <c r="K7" s="86"/>
       <c r="L7" s="86"/>
       <c r="M7" s="86"/>
@@ -2449,29 +2469,29 @@
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="93"/>
-      <c r="AW7" s="93"/>
-      <c r="BT7" s="93"/>
-      <c r="BW7" s="93"/>
-      <c r="CO7" s="93"/>
+      <c r="AV7" s="95"/>
+      <c r="AW7" s="95"/>
+      <c r="BT7" s="95"/>
+      <c r="BW7" s="95"/>
+      <c r="CO7" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 26-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB728B95-4A81-46F6-9761-1364E7D5080B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF35C1B-6D3C-49A8-9049-334EEF47C5FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="153">
   <si>
     <t>REDES</t>
   </si>
@@ -550,6 +550,22 @@
   </si>
   <si>
     <t>Análise das respostas do formulário e pesquisa mais aprofundada de sistemas semelhantes no mercado</t>
+  </si>
+  <si>
+    <t>Criação de layouts mobile e fluxograma macro da aplicação</t>
+  </si>
+  <si>
+    <t>Pesquisa de tratamento dos dados recebidos, visando performance e visualização.
+Organização de repositórios e Azure DevOps</t>
+  </si>
+  <si>
+    <t>Correção do modelo lógico e conceitual do banco de dados que continha alguns erros</t>
+  </si>
+  <si>
+    <t>Conclusão da análise das respostas e construção das personas. Análise do benchmark</t>
+  </si>
+  <si>
+    <t>Apresentação do andamento do projeto para coordenação e direção</t>
   </si>
 </sst>
 </file>
@@ -1164,6 +1180,18 @@
     <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1172,18 +1200,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1598,7 +1614,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1636,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -1900,7 +1916,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
@@ -2010,7 +2026,7 @@
       <c r="CR2" s="94"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
@@ -2298,10 +2314,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="97"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -2326,34 +2342,38 @@
       <c r="J4" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
+      <c r="K4" s="86" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" s="86" t="s">
+        <v>152</v>
+      </c>
       <c r="M4" s="86"/>
       <c r="N4" s="86"/>
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="95" t="s">
+      <c r="AV4" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="95" t="s">
+      <c r="AW4" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="95" t="s">
+      <c r="BT4" s="93" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="95" t="s">
+      <c r="BW4" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="95" t="s">
+      <c r="CO4" s="93" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="97"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -2378,24 +2398,28 @@
       <c r="J5" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
+      <c r="K5" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="L5" s="86" t="s">
+        <v>152</v>
+      </c>
       <c r="M5" s="86"/>
       <c r="N5" s="86"/>
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="95"/>
-      <c r="AW5" s="95"/>
-      <c r="BT5" s="95"/>
-      <c r="BW5" s="95"/>
-      <c r="CO5" s="95"/>
+      <c r="AV5" s="93"/>
+      <c r="AW5" s="93"/>
+      <c r="BT5" s="93"/>
+      <c r="BW5" s="93"/>
+      <c r="CO5" s="93"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="97"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -2420,24 +2444,28 @@
       <c r="J6" s="86" t="s">
         <v>146</v>
       </c>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
+      <c r="K6" s="86" t="s">
+        <v>150</v>
+      </c>
+      <c r="L6" s="86" t="s">
+        <v>152</v>
+      </c>
       <c r="M6" s="86"/>
       <c r="N6" s="86"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="95"/>
-      <c r="AW6" s="95"/>
-      <c r="BT6" s="95"/>
-      <c r="BW6" s="95"/>
-      <c r="CO6" s="95"/>
+      <c r="AV6" s="93"/>
+      <c r="AW6" s="93"/>
+      <c r="BT6" s="93"/>
+      <c r="BW6" s="93"/>
+      <c r="CO6" s="93"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="97"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -2462,36 +2490,40 @@
       <c r="J7" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
+      <c r="K7" s="86" t="s">
+        <v>151</v>
+      </c>
+      <c r="L7" s="86" t="s">
+        <v>152</v>
+      </c>
       <c r="M7" s="86"/>
       <c r="N7" s="86"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="95"/>
-      <c r="AW7" s="95"/>
-      <c r="BT7" s="95"/>
-      <c r="BW7" s="95"/>
-      <c r="CO7" s="95"/>
+      <c r="AV7" s="93"/>
+      <c r="AW7" s="93"/>
+      <c r="BT7" s="93"/>
+      <c r="BW7" s="93"/>
+      <c r="CO7" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 27-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF35C1B-6D3C-49A8-9049-334EEF47C5FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="157">
   <si>
     <t>REDES</t>
   </si>
@@ -566,12 +565,25 @@
   </si>
   <si>
     <t>Apresentação do andamento do projeto para coordenação e direção</t>
+  </si>
+  <si>
+    <t>Continuação dos layouts, estudo de arquitetura React, organização DevOps, início API e estudo Redux</t>
+  </si>
+  <si>
+    <t>Estudo das tecnologias que serão usadas no segundo projeto. Estudo de qual linguagem será utilizada</t>
+  </si>
+  <si>
+    <t>Validação de telas web, criação do script DML e diagramas</t>
+  </si>
+  <si>
+    <t>Conclusão das personas.
+Criação das users stories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1180,18 +1192,6 @@
     <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1200,6 +1200,18 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1607,14 +1619,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1636,7 +1648,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="91" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -1916,7 +1928,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
@@ -2026,7 +2038,7 @@
       <c r="CR2" s="94"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
@@ -2314,10 +2326,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="92"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -2348,32 +2360,34 @@
       <c r="L4" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="86"/>
+      <c r="M4" s="86" t="s">
+        <v>153</v>
+      </c>
       <c r="N4" s="86"/>
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="93" t="s">
+      <c r="AV4" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="93" t="s">
+      <c r="AW4" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="93" t="s">
+      <c r="BT4" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="93" t="s">
+      <c r="BW4" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="93" t="s">
+      <c r="CO4" s="95" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="92"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -2404,22 +2418,24 @@
       <c r="L5" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="M5" s="86"/>
+      <c r="M5" s="86" t="s">
+        <v>154</v>
+      </c>
       <c r="N5" s="86"/>
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="93"/>
-      <c r="AW5" s="93"/>
-      <c r="BT5" s="93"/>
-      <c r="BW5" s="93"/>
-      <c r="CO5" s="93"/>
+      <c r="AV5" s="95"/>
+      <c r="AW5" s="95"/>
+      <c r="BT5" s="95"/>
+      <c r="BW5" s="95"/>
+      <c r="CO5" s="95"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -2450,22 +2466,24 @@
       <c r="L6" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="M6" s="86"/>
+      <c r="M6" s="86" t="s">
+        <v>155</v>
+      </c>
       <c r="N6" s="86"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="93"/>
-      <c r="AW6" s="93"/>
-      <c r="BT6" s="93"/>
-      <c r="BW6" s="93"/>
-      <c r="CO6" s="93"/>
+      <c r="AV6" s="95"/>
+      <c r="AW6" s="95"/>
+      <c r="BT6" s="95"/>
+      <c r="BW6" s="95"/>
+      <c r="CO6" s="95"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="92"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -2496,34 +2514,36 @@
       <c r="L7" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="M7" s="86"/>
+      <c r="M7" s="86" t="s">
+        <v>156</v>
+      </c>
       <c r="N7" s="86"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="93"/>
-      <c r="AW7" s="93"/>
-      <c r="BT7" s="93"/>
-      <c r="BW7" s="93"/>
-      <c r="CO7" s="93"/>
+      <c r="AV7" s="95"/>
+      <c r="AW7" s="95"/>
+      <c r="BT7" s="95"/>
+      <c r="BW7" s="95"/>
+      <c r="CO7" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2532,7 +2552,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona daily realizada em 28-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB0C0A7-8F89-4F94-AC51-CD9D77F095D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="161">
   <si>
     <t>REDES</t>
   </si>
@@ -578,12 +579,24 @@
   <si>
     <t>Conclusão das personas.
 Criação das users stories</t>
+  </si>
+  <si>
+    <t>Continuação dos layouts (cadastro web), estudo Redux, continuação API e criação do banco de dados integrando com a API, integração do DevOps com a equipe de redes</t>
+  </si>
+  <si>
+    <t>Documentação do desenvolvimento do projeto I, alinhamento das ideias para o projeto II com o planejamento da sprint 2 e estudo da API Zabbix</t>
+  </si>
+  <si>
+    <t>Layout de alta fidelidade do dashboard, finalização dos scripts, finalização do wireframe web, organização do DevOps de todas as sprints</t>
+  </si>
+  <si>
+    <t>Validação das personas e user stories com o cliente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1192,6 +1205,18 @@
     <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1200,18 +1225,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1619,21 +1632,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" customWidth="1"/>
-    <col min="3" max="17" width="15.77734375" style="78" customWidth="1"/>
+    <col min="3" max="13" width="15.77734375" style="78" customWidth="1"/>
+    <col min="14" max="14" width="20.77734375" style="78" customWidth="1"/>
+    <col min="15" max="17" width="15.77734375" style="78" customWidth="1"/>
     <col min="18" max="20" width="15.77734375" customWidth="1"/>
     <col min="21" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
@@ -1648,7 +1663,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -1928,7 +1943,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
@@ -2038,7 +2053,7 @@
       <c r="CR2" s="94"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
@@ -2326,10 +2341,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="97"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -2363,31 +2378,33 @@
       <c r="M4" s="86" t="s">
         <v>153</v>
       </c>
-      <c r="N4" s="86"/>
+      <c r="N4" s="86" t="s">
+        <v>157</v>
+      </c>
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="95" t="s">
+      <c r="AV4" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="95" t="s">
+      <c r="AW4" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="95" t="s">
+      <c r="BT4" s="93" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="95" t="s">
+      <c r="BW4" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="95" t="s">
+      <c r="CO4" s="93" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="97"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -2421,21 +2438,23 @@
       <c r="M5" s="86" t="s">
         <v>154</v>
       </c>
-      <c r="N5" s="86"/>
+      <c r="N5" s="86" t="s">
+        <v>158</v>
+      </c>
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="95"/>
-      <c r="AW5" s="95"/>
-      <c r="BT5" s="95"/>
-      <c r="BW5" s="95"/>
-      <c r="CO5" s="95"/>
+      <c r="AV5" s="93"/>
+      <c r="AW5" s="93"/>
+      <c r="BT5" s="93"/>
+      <c r="BW5" s="93"/>
+      <c r="CO5" s="93"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="97"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -2469,21 +2488,23 @@
       <c r="M6" s="86" t="s">
         <v>155</v>
       </c>
-      <c r="N6" s="86"/>
+      <c r="N6" s="86" t="s">
+        <v>159</v>
+      </c>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="95"/>
-      <c r="AW6" s="95"/>
-      <c r="BT6" s="95"/>
-      <c r="BW6" s="95"/>
-      <c r="CO6" s="95"/>
+      <c r="AV6" s="93"/>
+      <c r="AW6" s="93"/>
+      <c r="BT6" s="93"/>
+      <c r="BW6" s="93"/>
+      <c r="CO6" s="93"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="97"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -2517,33 +2538,35 @@
       <c r="M7" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="N7" s="86"/>
+      <c r="N7" s="86" t="s">
+        <v>160</v>
+      </c>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="95"/>
-      <c r="AW7" s="95"/>
-      <c r="BT7" s="95"/>
-      <c r="BW7" s="95"/>
-      <c r="CO7" s="95"/>
+      <c r="AV7" s="93"/>
+      <c r="AW7" s="93"/>
+      <c r="BT7" s="93"/>
+      <c r="BW7" s="93"/>
+      <c r="CO7" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2552,14 +2575,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="T4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 29-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB0C0A7-8F89-4F94-AC51-CD9D77F095D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72240496-2119-4D52-94B3-6F6D9BF78A2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="165">
   <si>
     <t>REDES</t>
   </si>
@@ -591,6 +591,18 @@
   </si>
   <si>
     <t>Validação das personas e user stories com o cliente</t>
+  </si>
+  <si>
+    <t>Login mobile, início da estrutura de login e cadastro web, estudo e tentativa de aplicação Redux</t>
+  </si>
+  <si>
+    <t>Teste endpoints API Zabbix, interface para exibir os dados na web, estudo de implementação de um projeto básico em Python</t>
+  </si>
+  <si>
+    <t>Continuação dos layouts de alta fidelidade (faltando login), melhor organização do DevOps, finalização do Logotipo, alinhamento com o cliente reunião</t>
+  </si>
+  <si>
+    <t>Após a definição das user stories e dos critérios de aceite, foram incluídos na documentação e início da criação das jornadas dos usuários</t>
   </si>
 </sst>
 </file>
@@ -1205,18 +1217,6 @@
     <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1225,6 +1225,18 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1636,10 +1648,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1647,8 +1659,8 @@
     <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" customWidth="1"/>
     <col min="3" max="13" width="15.77734375" style="78" customWidth="1"/>
-    <col min="14" max="14" width="20.77734375" style="78" customWidth="1"/>
-    <col min="15" max="17" width="15.77734375" style="78" customWidth="1"/>
+    <col min="14" max="15" width="20.77734375" style="78" customWidth="1"/>
+    <col min="16" max="17" width="15.77734375" style="78" customWidth="1"/>
     <col min="18" max="20" width="15.77734375" customWidth="1"/>
     <col min="21" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
@@ -1663,7 +1675,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="91" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -1943,7 +1955,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
@@ -2053,7 +2065,7 @@
       <c r="CR2" s="94"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
@@ -2099,10 +2111,10 @@
       <c r="P3" s="89">
         <v>29</v>
       </c>
-      <c r="Q3" s="89">
+      <c r="Q3" s="90">
         <v>30</v>
       </c>
-      <c r="R3" s="89">
+      <c r="R3" s="90">
         <v>2</v>
       </c>
       <c r="S3" s="89">
@@ -2341,10 +2353,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="92"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -2381,30 +2393,32 @@
       <c r="N4" s="86" t="s">
         <v>157</v>
       </c>
-      <c r="O4" s="85"/>
+      <c r="O4" s="85" t="s">
+        <v>161</v>
+      </c>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="93" t="s">
+      <c r="AV4" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="93" t="s">
+      <c r="AW4" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="93" t="s">
+      <c r="BT4" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="93" t="s">
+      <c r="BW4" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="93" t="s">
+      <c r="CO4" s="95" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="92"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -2441,20 +2455,22 @@
       <c r="N5" s="86" t="s">
         <v>158</v>
       </c>
-      <c r="O5" s="85"/>
+      <c r="O5" s="85" t="s">
+        <v>162</v>
+      </c>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="93"/>
-      <c r="AW5" s="93"/>
-      <c r="BT5" s="93"/>
-      <c r="BW5" s="93"/>
-      <c r="CO5" s="93"/>
+      <c r="AV5" s="95"/>
+      <c r="AW5" s="95"/>
+      <c r="BT5" s="95"/>
+      <c r="BW5" s="95"/>
+      <c r="CO5" s="95"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -2491,20 +2507,22 @@
       <c r="N6" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="O6" s="85"/>
+      <c r="O6" s="85" t="s">
+        <v>163</v>
+      </c>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="93"/>
-      <c r="AW6" s="93"/>
-      <c r="BT6" s="93"/>
-      <c r="BW6" s="93"/>
-      <c r="CO6" s="93"/>
+      <c r="AV6" s="95"/>
+      <c r="AW6" s="95"/>
+      <c r="BT6" s="95"/>
+      <c r="BW6" s="95"/>
+      <c r="CO6" s="95"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="92"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -2541,32 +2559,34 @@
       <c r="N7" s="86" t="s">
         <v>160</v>
       </c>
-      <c r="O7" s="85"/>
+      <c r="O7" s="85" t="s">
+        <v>164</v>
+      </c>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="93"/>
-      <c r="AW7" s="93"/>
-      <c r="BT7" s="93"/>
-      <c r="BW7" s="93"/>
-      <c r="CO7" s="93"/>
+      <c r="AV7" s="95"/>
+      <c r="AW7" s="95"/>
+      <c r="BT7" s="95"/>
+      <c r="BW7" s="95"/>
+      <c r="CO7" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 03, 04 e 05-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C50D0-079A-4A83-A88E-940C5E2E6004}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415D339A-21A5-4A2B-B031-2EB2311862F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="192">
   <si>
     <t>REDES</t>
   </si>
@@ -651,6 +651,43 @@
   </si>
   <si>
     <t>Planejamento e reunião com o cliente</t>
+  </si>
+  <si>
+    <t>Organização e planejamento da Sprint. Review Sprint. Alinhamento das tarefas concluídas por e-mail com o cliente</t>
+  </si>
+  <si>
+    <t>Fluxograma da aplicação do projeto II, estudo da API Zabbix, análise do relatório e Sprint Review</t>
+  </si>
+  <si>
+    <t>Sprint Review, layouts das telas adicionais incrementadas após a reunião.
+Criação de alguns componentes para reaproveitamento</t>
+  </si>
+  <si>
+    <t>Sprint Review, fluxo de navegação de telas iniciais para new hires e definição de datas de entrega</t>
+  </si>
+  <si>
+    <t>Layout do app mobile, estudo de SPA, estudo CSS Modules e implementação do cadastro de usuários</t>
+  </si>
+  <si>
+    <t>Lista dos itens que devem compor os relatórios, teste de requisições à API Zabbix</t>
+  </si>
+  <si>
+    <t>Finalização do layout web e da modelagem do BD com alterações após a reunião, criação de componente input, estudo sobre drag and drop</t>
+  </si>
+  <si>
+    <t>Correção de user stories e fluxo de navegação de telas dos anfitriões</t>
+  </si>
+  <si>
+    <t>Testes de criação SPA, criação do HTML e CSS da página de Login Web, estilização da página de Login Mobile, Testes unitários da API</t>
+  </si>
+  <si>
+    <t>Testes de requisições à API Zabbix</t>
+  </si>
+  <si>
+    <t>Teste de requisições para mostrar o endereço buscado pelo CEP, finalização dos layouts mobile, teste de UX Web, desenho de opções de Logo</t>
+  </si>
+  <si>
+    <t>Wireframes das telas mobile, pesquisa para definição da identidade visual, requisitos funcionais e regras de negócios para o Trello</t>
   </si>
 </sst>
 </file>
@@ -1400,8 +1437,17 @@
     <xf numFmtId="0" fontId="12" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1412,17 +1458,14 @@
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1466,15 +1509,6 @@
     <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1494,6 +1528,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1889,11 +1926,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1903,7 +1940,8 @@
     <col min="3" max="13" width="15.77734375" style="78" customWidth="1"/>
     <col min="14" max="16" width="20.77734375" style="78" customWidth="1"/>
     <col min="17" max="17" width="15.77734375" style="78" customWidth="1"/>
-    <col min="18" max="27" width="15.77734375" customWidth="1"/>
+    <col min="18" max="20" width="20.77734375" customWidth="1"/>
+    <col min="21" max="27" width="15.77734375" customWidth="1"/>
     <col min="28" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -1917,7 +1955,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="98" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2197,117 +2235,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="99"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="97" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98" t="s">
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="98"/>
-      <c r="W2" s="98"/>
-      <c r="X2" s="98"/>
-      <c r="Y2" s="98"/>
-      <c r="Z2" s="98"/>
-      <c r="AA2" s="98"/>
-      <c r="AB2" s="98"/>
-      <c r="AC2" s="98"/>
-      <c r="AD2" s="98"/>
-      <c r="AE2" s="98"/>
-      <c r="AF2" s="98"/>
-      <c r="AG2" s="98"/>
-      <c r="AH2" s="98"/>
-      <c r="AI2" s="98"/>
-      <c r="AJ2" s="98"/>
-      <c r="AK2" s="98"/>
-      <c r="AL2" s="98"/>
-      <c r="AM2" s="98" t="s">
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="97"/>
+      <c r="AA2" s="97"/>
+      <c r="AB2" s="97"/>
+      <c r="AC2" s="97"/>
+      <c r="AD2" s="97"/>
+      <c r="AE2" s="97"/>
+      <c r="AF2" s="97"/>
+      <c r="AG2" s="97"/>
+      <c r="AH2" s="97"/>
+      <c r="AI2" s="97"/>
+      <c r="AJ2" s="97"/>
+      <c r="AK2" s="97"/>
+      <c r="AL2" s="97"/>
+      <c r="AM2" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="98"/>
-      <c r="AO2" s="98"/>
-      <c r="AP2" s="98"/>
-      <c r="AQ2" s="98"/>
-      <c r="AR2" s="98"/>
-      <c r="AS2" s="98"/>
-      <c r="AT2" s="98"/>
-      <c r="AU2" s="98"/>
-      <c r="AV2" s="98"/>
-      <c r="AW2" s="98"/>
-      <c r="AX2" s="98"/>
-      <c r="AY2" s="98"/>
-      <c r="AZ2" s="98"/>
-      <c r="BA2" s="98"/>
-      <c r="BB2" s="98"/>
-      <c r="BC2" s="98"/>
-      <c r="BD2" s="98"/>
-      <c r="BE2" s="98"/>
-      <c r="BF2" s="98"/>
-      <c r="BG2" s="98"/>
-      <c r="BH2" s="98"/>
-      <c r="BI2" s="98"/>
-      <c r="BJ2" s="98" t="s">
+      <c r="AN2" s="97"/>
+      <c r="AO2" s="97"/>
+      <c r="AP2" s="97"/>
+      <c r="AQ2" s="97"/>
+      <c r="AR2" s="97"/>
+      <c r="AS2" s="97"/>
+      <c r="AT2" s="97"/>
+      <c r="AU2" s="97"/>
+      <c r="AV2" s="97"/>
+      <c r="AW2" s="97"/>
+      <c r="AX2" s="97"/>
+      <c r="AY2" s="97"/>
+      <c r="AZ2" s="97"/>
+      <c r="BA2" s="97"/>
+      <c r="BB2" s="97"/>
+      <c r="BC2" s="97"/>
+      <c r="BD2" s="97"/>
+      <c r="BE2" s="97"/>
+      <c r="BF2" s="97"/>
+      <c r="BG2" s="97"/>
+      <c r="BH2" s="97"/>
+      <c r="BI2" s="97"/>
+      <c r="BJ2" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="98"/>
-      <c r="BL2" s="98"/>
-      <c r="BM2" s="98"/>
-      <c r="BN2" s="98"/>
-      <c r="BO2" s="98"/>
-      <c r="BP2" s="98"/>
-      <c r="BQ2" s="98"/>
-      <c r="BR2" s="98"/>
-      <c r="BS2" s="98"/>
-      <c r="BT2" s="98"/>
-      <c r="BU2" s="98"/>
-      <c r="BV2" s="98"/>
-      <c r="BW2" s="98"/>
-      <c r="BX2" s="98"/>
-      <c r="BY2" s="98"/>
-      <c r="BZ2" s="98"/>
-      <c r="CA2" s="98"/>
-      <c r="CB2" s="98"/>
-      <c r="CC2" s="98"/>
-      <c r="CD2" s="98"/>
-      <c r="CE2" s="98" t="s">
+      <c r="BK2" s="97"/>
+      <c r="BL2" s="97"/>
+      <c r="BM2" s="97"/>
+      <c r="BN2" s="97"/>
+      <c r="BO2" s="97"/>
+      <c r="BP2" s="97"/>
+      <c r="BQ2" s="97"/>
+      <c r="BR2" s="97"/>
+      <c r="BS2" s="97"/>
+      <c r="BT2" s="97"/>
+      <c r="BU2" s="97"/>
+      <c r="BV2" s="97"/>
+      <c r="BW2" s="97"/>
+      <c r="BX2" s="97"/>
+      <c r="BY2" s="97"/>
+      <c r="BZ2" s="97"/>
+      <c r="CA2" s="97"/>
+      <c r="CB2" s="97"/>
+      <c r="CC2" s="97"/>
+      <c r="CD2" s="97"/>
+      <c r="CE2" s="97" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="98"/>
-      <c r="CG2" s="98"/>
-      <c r="CH2" s="98"/>
-      <c r="CI2" s="98"/>
-      <c r="CJ2" s="98"/>
-      <c r="CK2" s="98"/>
-      <c r="CL2" s="98"/>
-      <c r="CM2" s="98"/>
-      <c r="CN2" s="98"/>
-      <c r="CO2" s="98"/>
-      <c r="CP2" s="98"/>
-      <c r="CQ2" s="98"/>
-      <c r="CR2" s="98"/>
+      <c r="CF2" s="97"/>
+      <c r="CG2" s="97"/>
+      <c r="CH2" s="97"/>
+      <c r="CI2" s="97"/>
+      <c r="CJ2" s="97"/>
+      <c r="CK2" s="97"/>
+      <c r="CL2" s="97"/>
+      <c r="CM2" s="97"/>
+      <c r="CN2" s="97"/>
+      <c r="CO2" s="97"/>
+      <c r="CP2" s="97"/>
+      <c r="CQ2" s="97"/>
+      <c r="CR2" s="97"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="100"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2595,10 +2633,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="94" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="95"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2644,37 +2682,43 @@
       <c r="Q4" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R4" s="94"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="94"/>
-      <c r="U4" s="94"/>
-      <c r="V4" s="94"/>
-      <c r="W4" s="94"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="94"/>
-      <c r="AV4" s="99" t="s">
+      <c r="R4" s="125" t="s">
+        <v>180</v>
+      </c>
+      <c r="S4" s="125" t="s">
+        <v>184</v>
+      </c>
+      <c r="T4" s="125" t="s">
+        <v>188</v>
+      </c>
+      <c r="U4" s="125"/>
+      <c r="V4" s="125"/>
+      <c r="W4" s="125"/>
+      <c r="X4" s="125"/>
+      <c r="Y4" s="125"/>
+      <c r="Z4" s="125"/>
+      <c r="AA4" s="125"/>
+      <c r="AV4" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="99" t="s">
+      <c r="AW4" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="99" t="s">
+      <c r="BT4" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="99" t="s">
+      <c r="BW4" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="99" t="s">
+      <c r="CO4" s="96" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2718,27 +2762,33 @@
       <c r="Q5" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R5" s="94"/>
-      <c r="S5" s="94"/>
-      <c r="T5" s="94"/>
-      <c r="U5" s="94"/>
-      <c r="V5" s="94"/>
-      <c r="W5" s="94"/>
-      <c r="X5" s="94"/>
-      <c r="Y5" s="94"/>
-      <c r="Z5" s="94"/>
-      <c r="AA5" s="94"/>
-      <c r="AV5" s="99"/>
-      <c r="AW5" s="99"/>
-      <c r="BT5" s="99"/>
-      <c r="BW5" s="99"/>
-      <c r="CO5" s="99"/>
+      <c r="R5" s="125" t="s">
+        <v>181</v>
+      </c>
+      <c r="S5" s="125" t="s">
+        <v>185</v>
+      </c>
+      <c r="T5" s="125" t="s">
+        <v>189</v>
+      </c>
+      <c r="U5" s="125"/>
+      <c r="V5" s="125"/>
+      <c r="W5" s="125"/>
+      <c r="X5" s="125"/>
+      <c r="Y5" s="125"/>
+      <c r="Z5" s="125"/>
+      <c r="AA5" s="125"/>
+      <c r="AV5" s="96"/>
+      <c r="AW5" s="96"/>
+      <c r="BT5" s="96"/>
+      <c r="BW5" s="96"/>
+      <c r="CO5" s="96"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2784,27 +2834,33 @@
       <c r="Q6" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R6" s="94"/>
-      <c r="S6" s="94"/>
-      <c r="T6" s="94"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="94"/>
-      <c r="W6" s="94"/>
-      <c r="X6" s="94"/>
-      <c r="Y6" s="94"/>
-      <c r="Z6" s="94"/>
-      <c r="AA6" s="94"/>
-      <c r="AV6" s="99"/>
-      <c r="AW6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BW6" s="99"/>
-      <c r="CO6" s="99"/>
+      <c r="R6" s="125" t="s">
+        <v>182</v>
+      </c>
+      <c r="S6" s="125" t="s">
+        <v>186</v>
+      </c>
+      <c r="T6" s="125" t="s">
+        <v>190</v>
+      </c>
+      <c r="U6" s="125"/>
+      <c r="V6" s="125"/>
+      <c r="W6" s="125"/>
+      <c r="X6" s="125"/>
+      <c r="Y6" s="125"/>
+      <c r="Z6" s="125"/>
+      <c r="AA6" s="125"/>
+      <c r="AV6" s="96"/>
+      <c r="AW6" s="96"/>
+      <c r="BT6" s="96"/>
+      <c r="BW6" s="96"/>
+      <c r="CO6" s="96"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="95"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -2850,39 +2906,45 @@
       <c r="Q7" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="94"/>
-      <c r="U7" s="94"/>
-      <c r="V7" s="94"/>
-      <c r="W7" s="94"/>
-      <c r="X7" s="94"/>
-      <c r="Y7" s="94"/>
-      <c r="Z7" s="94"/>
-      <c r="AA7" s="94"/>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="CO7" s="99"/>
+      <c r="R7" s="125" t="s">
+        <v>183</v>
+      </c>
+      <c r="S7" s="125" t="s">
+        <v>187</v>
+      </c>
+      <c r="T7" s="125" t="s">
+        <v>191</v>
+      </c>
+      <c r="U7" s="125"/>
+      <c r="V7" s="125"/>
+      <c r="W7" s="125"/>
+      <c r="X7" s="125"/>
+      <c r="Y7" s="125"/>
+      <c r="Z7" s="125"/>
+      <c r="AA7" s="125"/>
+      <c r="AV7" s="96"/>
+      <c r="AW7" s="96"/>
+      <c r="BT7" s="96"/>
+      <c r="BW7" s="96"/>
+      <c r="CO7" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2965,36 +3027,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="101" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="108"/>
+      <c r="G2" s="110"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="109" t="s">
+      <c r="I2" s="111" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="109"/>
+      <c r="J2" s="111"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="110" t="s">
+      <c r="L2" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="110"/>
+      <c r="M2" s="112"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="111" t="s">
+      <c r="O2" s="113" t="s">
         <v>170</v>
       </c>
-      <c r="P2" s="111"/>
+      <c r="P2" s="113"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="112" t="s">
+      <c r="R2" s="114" t="s">
         <v>171</v>
       </c>
-      <c r="S2" s="112"/>
+      <c r="S2" s="114"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -3028,24 +3090,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="111"/>
-      <c r="P3" s="111"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="112"/>
-      <c r="S3" s="112"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -3079,24 +3141,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="110"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="113"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -3134,20 +3196,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="110"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="112"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="111"/>
-      <c r="P5" s="111"/>
+      <c r="O5" s="113"/>
+      <c r="P5" s="113"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
+      <c r="R5" s="114"/>
+      <c r="S5" s="114"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -3181,26 +3243,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="102" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="111"/>
+      <c r="O6" s="113"/>
+      <c r="P6" s="113"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="112"/>
-      <c r="S6" s="112"/>
+      <c r="R6" s="114"/>
+      <c r="S6" s="114"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -3234,24 +3296,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="110"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="111"/>
-      <c r="P7" s="111"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="112"/>
-      <c r="S7" s="112"/>
+      <c r="R7" s="114"/>
+      <c r="S7" s="114"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -3285,24 +3347,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
+      <c r="L8" s="112"/>
+      <c r="M8" s="112"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="111"/>
-      <c r="P8" s="111"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112"/>
+      <c r="R8" s="114"/>
+      <c r="S8" s="114"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -3336,24 +3398,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="108"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="110"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="110"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="112"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="111"/>
-      <c r="P9" s="111"/>
+      <c r="O9" s="113"/>
+      <c r="P9" s="113"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="112"/>
-      <c r="S9" s="112"/>
+      <c r="R9" s="114"/>
+      <c r="S9" s="114"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -3387,24 +3449,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="118"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="108"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="109"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="110"/>
-      <c r="M10" s="110"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="111"/>
-      <c r="P10" s="111"/>
+      <c r="O10" s="113"/>
+      <c r="P10" s="113"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="112"/>
-      <c r="S10" s="112"/>
+      <c r="R10" s="114"/>
+      <c r="S10" s="114"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -3493,25 +3555,25 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="113" t="s">
+      <c r="F12" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="113"/>
+      <c r="G12" s="115"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="114" t="s">
+      <c r="I12" s="116" t="s">
         <v>173</v>
       </c>
-      <c r="J12" s="114"/>
+      <c r="J12" s="116"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="115" t="s">
+      <c r="L12" s="117" t="s">
         <v>174</v>
       </c>
-      <c r="M12" s="115"/>
+      <c r="M12" s="117"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="102" t="s">
+      <c r="O12" s="104" t="s">
         <v>175</v>
       </c>
-      <c r="P12" s="103"/>
+      <c r="P12" s="105"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -3552,17 +3614,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="114"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="105"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="107"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -3603,17 +3665,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="114"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="115"/>
+      <c r="L14" s="117"/>
+      <c r="M14" s="117"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="105"/>
+      <c r="O14" s="106"/>
+      <c r="P14" s="107"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -3654,17 +3716,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="114"/>
-      <c r="J15" s="114"/>
+      <c r="I15" s="116"/>
+      <c r="J15" s="116"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="115"/>
-      <c r="M15" s="115"/>
+      <c r="L15" s="117"/>
+      <c r="M15" s="117"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="105"/>
+      <c r="O15" s="106"/>
+      <c r="P15" s="107"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -3705,17 +3767,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="113"/>
-      <c r="G16" s="113"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="115"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="114"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="116"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="115"/>
+      <c r="L16" s="117"/>
+      <c r="M16" s="117"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="104"/>
-      <c r="P16" s="105"/>
+      <c r="O16" s="106"/>
+      <c r="P16" s="107"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -3756,17 +3818,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="113"/>
-      <c r="G17" s="113"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="115"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="114"/>
-      <c r="J17" s="114"/>
+      <c r="I17" s="116"/>
+      <c r="J17" s="116"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="117"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="104"/>
-      <c r="P17" s="105"/>
+      <c r="O17" s="106"/>
+      <c r="P17" s="107"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -3807,17 +3869,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="113"/>
+      <c r="F18" s="115"/>
+      <c r="G18" s="115"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="114"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="115"/>
+      <c r="L18" s="117"/>
+      <c r="M18" s="117"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="104"/>
-      <c r="P18" s="105"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="107"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -3858,17 +3920,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="113"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="114"/>
-      <c r="J19" s="114"/>
+      <c r="I19" s="116"/>
+      <c r="J19" s="116"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="115"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="117"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="104"/>
-      <c r="P19" s="105"/>
+      <c r="O19" s="106"/>
+      <c r="P19" s="107"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -3909,17 +3971,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="113"/>
-      <c r="G20" s="113"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="114"/>
-      <c r="J20" s="114"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="116"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
+      <c r="L20" s="117"/>
+      <c r="M20" s="117"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="106"/>
-      <c r="P20" s="107"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="109"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -16451,6 +16513,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="R2:S10"/>
+    <mergeCell ref="F12:G20"/>
+    <mergeCell ref="I12:J20"/>
+    <mergeCell ref="L12:M20"/>
     <mergeCell ref="B2:D4"/>
     <mergeCell ref="B6:D10"/>
     <mergeCell ref="O12:P20"/>
@@ -16458,10 +16524,6 @@
     <mergeCell ref="I2:J10"/>
     <mergeCell ref="L2:M10"/>
     <mergeCell ref="O2:P10"/>
-    <mergeCell ref="R2:S10"/>
-    <mergeCell ref="F12:G20"/>
-    <mergeCell ref="I12:J20"/>
-    <mergeCell ref="L12:M20"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -16473,7 +16535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -16492,7 +16554,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="120" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -16832,7 +16894,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121"/>
+      <c r="A2" s="120"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -17158,15 +17220,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="122"/>
-      <c r="DH2" s="122"/>
-      <c r="DI2" s="122"/>
-      <c r="DJ2" s="122"/>
+      <c r="DG2" s="121"/>
+      <c r="DH2" s="121"/>
+      <c r="DI2" s="121"/>
+      <c r="DJ2" s="121"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="121"/>
+      <c r="A3" s="120"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -17503,7 +17565,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="122" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -17645,7 +17707,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -17785,7 +17847,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -17925,7 +17987,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="123"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -18063,7 +18125,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="123"/>
+      <c r="B8" s="122"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -18203,7 +18265,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="123" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -18345,7 +18407,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="124"/>
+      <c r="B10" s="123"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -18485,7 +18547,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="124" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -18615,7 +18677,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="125"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -18753,7 +18815,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="125"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -18893,7 +18955,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="125"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -19029,7 +19091,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="125"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -19165,7 +19227,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="125"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -19301,7 +19363,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="125"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -19437,7 +19499,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="124"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -19577,7 +19639,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="125"/>
+      <c r="B19" s="124"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -19713,7 +19775,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="125"/>
+      <c r="B20" s="124"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -19849,7 +19911,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="118" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -19983,7 +20045,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="119"/>
+      <c r="B22" s="118"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -20119,7 +20181,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="119"/>
+      <c r="B23" s="118"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -20251,7 +20313,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="119"/>
+      <c r="B24" s="118"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -20385,7 +20447,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="119"/>
+      <c r="B25" s="118"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -20529,7 +20591,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="120" t="s">
+      <c r="B26" s="119" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -20663,7 +20725,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="120"/>
+      <c r="B27" s="119"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -20803,7 +20865,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="120"/>
+      <c r="B28" s="119"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -20935,7 +20997,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="120"/>
+      <c r="B29" s="119"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -21063,7 +21125,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="120"/>
+      <c r="B30" s="119"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -21189,7 +21251,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="120"/>
+      <c r="B31" s="119"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 06-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415D339A-21A5-4A2B-B031-2EB2311862F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9816DF11-4335-4389-B6F6-9988B9F8644B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="196">
   <si>
     <t>REDES</t>
   </si>
@@ -688,6 +688,18 @@
   </si>
   <si>
     <t>Wireframes das telas mobile, pesquisa para definição da identidade visual, requisitos funcionais e regras de negócios para o Trello</t>
+  </si>
+  <si>
+    <t>Criação do projeto SPA, finalização do Login mobile, continuação página Login web, configuração do banco de dados</t>
+  </si>
+  <si>
+    <t>Testes de requisições à API Zabbix e estrutura do relatório</t>
+  </si>
+  <si>
+    <t>Testes de UX Web e Mobile, início da API e finalização dos testes de busca de endereço pelo CEP, finalização do logo aprovado pelo cliente</t>
+  </si>
+  <si>
+    <t>Criação dos wireframes das telas de boas vindas e jornadas, definição dos requisitos funcionais, não funcionais e regras de negócio</t>
   </si>
 </sst>
 </file>
@@ -1437,17 +1449,8 @@
     <xf numFmtId="0" fontId="12" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1456,6 +1459,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1497,18 +1524,6 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1528,9 +1543,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1930,7 +1942,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1940,8 +1952,8 @@
     <col min="3" max="13" width="15.77734375" style="78" customWidth="1"/>
     <col min="14" max="16" width="20.77734375" style="78" customWidth="1"/>
     <col min="17" max="17" width="15.77734375" style="78" customWidth="1"/>
-    <col min="18" max="20" width="20.77734375" customWidth="1"/>
-    <col min="21" max="27" width="15.77734375" customWidth="1"/>
+    <col min="18" max="26" width="20.77734375" customWidth="1"/>
+    <col min="27" max="27" width="15.77734375" customWidth="1"/>
     <col min="28" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -1955,7 +1967,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2235,117 +2247,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="98" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97" t="s">
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="97"/>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="97"/>
-      <c r="AD2" s="97"/>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="97"/>
-      <c r="AG2" s="97"/>
-      <c r="AH2" s="97"/>
-      <c r="AI2" s="97"/>
-      <c r="AJ2" s="97"/>
-      <c r="AK2" s="97"/>
-      <c r="AL2" s="97"/>
-      <c r="AM2" s="97" t="s">
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="98"/>
+      <c r="AG2" s="98"/>
+      <c r="AH2" s="98"/>
+      <c r="AI2" s="98"/>
+      <c r="AJ2" s="98"/>
+      <c r="AK2" s="98"/>
+      <c r="AL2" s="98"/>
+      <c r="AM2" s="98" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="97"/>
-      <c r="AO2" s="97"/>
-      <c r="AP2" s="97"/>
-      <c r="AQ2" s="97"/>
-      <c r="AR2" s="97"/>
-      <c r="AS2" s="97"/>
-      <c r="AT2" s="97"/>
-      <c r="AU2" s="97"/>
-      <c r="AV2" s="97"/>
-      <c r="AW2" s="97"/>
-      <c r="AX2" s="97"/>
-      <c r="AY2" s="97"/>
-      <c r="AZ2" s="97"/>
-      <c r="BA2" s="97"/>
-      <c r="BB2" s="97"/>
-      <c r="BC2" s="97"/>
-      <c r="BD2" s="97"/>
-      <c r="BE2" s="97"/>
-      <c r="BF2" s="97"/>
-      <c r="BG2" s="97"/>
-      <c r="BH2" s="97"/>
-      <c r="BI2" s="97"/>
-      <c r="BJ2" s="97" t="s">
+      <c r="AN2" s="98"/>
+      <c r="AO2" s="98"/>
+      <c r="AP2" s="98"/>
+      <c r="AQ2" s="98"/>
+      <c r="AR2" s="98"/>
+      <c r="AS2" s="98"/>
+      <c r="AT2" s="98"/>
+      <c r="AU2" s="98"/>
+      <c r="AV2" s="98"/>
+      <c r="AW2" s="98"/>
+      <c r="AX2" s="98"/>
+      <c r="AY2" s="98"/>
+      <c r="AZ2" s="98"/>
+      <c r="BA2" s="98"/>
+      <c r="BB2" s="98"/>
+      <c r="BC2" s="98"/>
+      <c r="BD2" s="98"/>
+      <c r="BE2" s="98"/>
+      <c r="BF2" s="98"/>
+      <c r="BG2" s="98"/>
+      <c r="BH2" s="98"/>
+      <c r="BI2" s="98"/>
+      <c r="BJ2" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="97"/>
-      <c r="BL2" s="97"/>
-      <c r="BM2" s="97"/>
-      <c r="BN2" s="97"/>
-      <c r="BO2" s="97"/>
-      <c r="BP2" s="97"/>
-      <c r="BQ2" s="97"/>
-      <c r="BR2" s="97"/>
-      <c r="BS2" s="97"/>
-      <c r="BT2" s="97"/>
-      <c r="BU2" s="97"/>
-      <c r="BV2" s="97"/>
-      <c r="BW2" s="97"/>
-      <c r="BX2" s="97"/>
-      <c r="BY2" s="97"/>
-      <c r="BZ2" s="97"/>
-      <c r="CA2" s="97"/>
-      <c r="CB2" s="97"/>
-      <c r="CC2" s="97"/>
-      <c r="CD2" s="97"/>
-      <c r="CE2" s="97" t="s">
+      <c r="BK2" s="98"/>
+      <c r="BL2" s="98"/>
+      <c r="BM2" s="98"/>
+      <c r="BN2" s="98"/>
+      <c r="BO2" s="98"/>
+      <c r="BP2" s="98"/>
+      <c r="BQ2" s="98"/>
+      <c r="BR2" s="98"/>
+      <c r="BS2" s="98"/>
+      <c r="BT2" s="98"/>
+      <c r="BU2" s="98"/>
+      <c r="BV2" s="98"/>
+      <c r="BW2" s="98"/>
+      <c r="BX2" s="98"/>
+      <c r="BY2" s="98"/>
+      <c r="BZ2" s="98"/>
+      <c r="CA2" s="98"/>
+      <c r="CB2" s="98"/>
+      <c r="CC2" s="98"/>
+      <c r="CD2" s="98"/>
+      <c r="CE2" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="97"/>
-      <c r="CG2" s="97"/>
-      <c r="CH2" s="97"/>
-      <c r="CI2" s="97"/>
-      <c r="CJ2" s="97"/>
-      <c r="CK2" s="97"/>
-      <c r="CL2" s="97"/>
-      <c r="CM2" s="97"/>
-      <c r="CN2" s="97"/>
-      <c r="CO2" s="97"/>
-      <c r="CP2" s="97"/>
-      <c r="CQ2" s="97"/>
-      <c r="CR2" s="97"/>
+      <c r="CF2" s="98"/>
+      <c r="CG2" s="98"/>
+      <c r="CH2" s="98"/>
+      <c r="CI2" s="98"/>
+      <c r="CJ2" s="98"/>
+      <c r="CK2" s="98"/>
+      <c r="CL2" s="98"/>
+      <c r="CM2" s="98"/>
+      <c r="CN2" s="98"/>
+      <c r="CO2" s="98"/>
+      <c r="CP2" s="98"/>
+      <c r="CQ2" s="98"/>
+      <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2633,10 +2645,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2682,43 +2694,45 @@
       <c r="Q4" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R4" s="125" t="s">
+      <c r="R4" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="S4" s="125" t="s">
+      <c r="S4" s="94" t="s">
         <v>184</v>
       </c>
-      <c r="T4" s="125" t="s">
+      <c r="T4" s="94" t="s">
         <v>188</v>
       </c>
-      <c r="U4" s="125"/>
-      <c r="V4" s="125"/>
-      <c r="W4" s="125"/>
-      <c r="X4" s="125"/>
-      <c r="Y4" s="125"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="125"/>
-      <c r="AV4" s="96" t="s">
+      <c r="U4" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="V4" s="94"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AV4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="96" t="s">
+      <c r="AW4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="96" t="s">
+      <c r="BT4" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="96" t="s">
+      <c r="BW4" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="96" t="s">
+      <c r="CO4" s="99" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="95"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2762,33 +2776,35 @@
       <c r="Q5" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R5" s="125" t="s">
+      <c r="R5" s="94" t="s">
         <v>181</v>
       </c>
-      <c r="S5" s="125" t="s">
+      <c r="S5" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="T5" s="125" t="s">
+      <c r="T5" s="94" t="s">
         <v>189</v>
       </c>
-      <c r="U5" s="125"/>
-      <c r="V5" s="125"/>
-      <c r="W5" s="125"/>
-      <c r="X5" s="125"/>
-      <c r="Y5" s="125"/>
-      <c r="Z5" s="125"/>
-      <c r="AA5" s="125"/>
-      <c r="AV5" s="96"/>
-      <c r="AW5" s="96"/>
-      <c r="BT5" s="96"/>
-      <c r="BW5" s="96"/>
-      <c r="CO5" s="96"/>
+      <c r="U5" s="94" t="s">
+        <v>193</v>
+      </c>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
+      <c r="Y5" s="94"/>
+      <c r="Z5" s="94"/>
+      <c r="AA5" s="94"/>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="95"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2834,33 +2850,35 @@
       <c r="Q6" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R6" s="125" t="s">
+      <c r="R6" s="94" t="s">
         <v>182</v>
       </c>
-      <c r="S6" s="125" t="s">
+      <c r="S6" s="94" t="s">
         <v>186</v>
       </c>
-      <c r="T6" s="125" t="s">
+      <c r="T6" s="94" t="s">
         <v>190</v>
       </c>
-      <c r="U6" s="125"/>
-      <c r="V6" s="125"/>
-      <c r="W6" s="125"/>
-      <c r="X6" s="125"/>
-      <c r="Y6" s="125"/>
-      <c r="Z6" s="125"/>
-      <c r="AA6" s="125"/>
-      <c r="AV6" s="96"/>
-      <c r="AW6" s="96"/>
-      <c r="BT6" s="96"/>
-      <c r="BW6" s="96"/>
-      <c r="CO6" s="96"/>
+      <c r="U6" s="94" t="s">
+        <v>194</v>
+      </c>
+      <c r="V6" s="94"/>
+      <c r="W6" s="94"/>
+      <c r="X6" s="94"/>
+      <c r="Y6" s="94"/>
+      <c r="Z6" s="94"/>
+      <c r="AA6" s="94"/>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -2906,45 +2924,47 @@
       <c r="Q7" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="R7" s="125" t="s">
+      <c r="R7" s="94" t="s">
         <v>183</v>
       </c>
-      <c r="S7" s="125" t="s">
+      <c r="S7" s="94" t="s">
         <v>187</v>
       </c>
-      <c r="T7" s="125" t="s">
+      <c r="T7" s="94" t="s">
         <v>191</v>
       </c>
-      <c r="U7" s="125"/>
-      <c r="V7" s="125"/>
-      <c r="W7" s="125"/>
-      <c r="X7" s="125"/>
-      <c r="Y7" s="125"/>
-      <c r="Z7" s="125"/>
-      <c r="AA7" s="125"/>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="96"/>
-      <c r="BT7" s="96"/>
-      <c r="BW7" s="96"/>
-      <c r="CO7" s="96"/>
+      <c r="U7" s="94" t="s">
+        <v>195</v>
+      </c>
+      <c r="V7" s="94"/>
+      <c r="W7" s="94"/>
+      <c r="X7" s="94"/>
+      <c r="Y7" s="94"/>
+      <c r="Z7" s="94"/>
+      <c r="AA7" s="94"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3027,36 +3047,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="110" t="s">
+      <c r="F2" s="115" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="110"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="111" t="s">
+      <c r="I2" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="111"/>
+      <c r="J2" s="116"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="112" t="s">
+      <c r="L2" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="112"/>
+      <c r="M2" s="117"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="113" t="s">
+      <c r="O2" s="118" t="s">
         <v>170</v>
       </c>
-      <c r="P2" s="113"/>
+      <c r="P2" s="118"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="114" t="s">
+      <c r="R2" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="S2" s="114"/>
+      <c r="S2" s="102"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -3090,24 +3110,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="113"/>
-      <c r="P3" s="113"/>
+      <c r="O3" s="118"/>
+      <c r="P3" s="118"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -3141,24 +3161,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="113"/>
+      <c r="O4" s="118"/>
+      <c r="P4" s="118"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="114"/>
-      <c r="S4" s="114"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -3196,20 +3216,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="114"/>
-      <c r="S5" s="114"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -3243,26 +3263,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="113"/>
-      <c r="P6" s="113"/>
+      <c r="O6" s="118"/>
+      <c r="P6" s="118"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="114"/>
-      <c r="S6" s="114"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="102"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -3296,24 +3316,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="117"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="113"/>
-      <c r="P7" s="113"/>
+      <c r="O7" s="118"/>
+      <c r="P7" s="118"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="114"/>
-      <c r="S7" s="114"/>
+      <c r="R7" s="102"/>
+      <c r="S7" s="102"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -3347,24 +3367,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="110"/>
-      <c r="G8" s="110"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="115"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="112"/>
+      <c r="L8" s="117"/>
+      <c r="M8" s="117"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="113"/>
-      <c r="P8" s="113"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="118"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="114"/>
-      <c r="S8" s="114"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="102"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -3398,24 +3418,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="103"/>
-      <c r="D9" s="103"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
+      <c r="F9" s="115"/>
+      <c r="G9" s="115"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="112"/>
+      <c r="L9" s="117"/>
+      <c r="M9" s="117"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="113"/>
-      <c r="P9" s="113"/>
+      <c r="O9" s="118"/>
+      <c r="P9" s="118"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="114"/>
-      <c r="S9" s="114"/>
+      <c r="R9" s="102"/>
+      <c r="S9" s="102"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -3449,24 +3469,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="115"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
+      <c r="L10" s="117"/>
+      <c r="M10" s="117"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="113"/>
-      <c r="P10" s="113"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="118"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="114"/>
-      <c r="S10" s="114"/>
+      <c r="R10" s="102"/>
+      <c r="S10" s="102"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -3555,25 +3575,25 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="115" t="s">
+      <c r="F12" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="115"/>
+      <c r="G12" s="103"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="116" t="s">
+      <c r="I12" s="104" t="s">
         <v>173</v>
       </c>
-      <c r="J12" s="116"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="117" t="s">
+      <c r="L12" s="105" t="s">
         <v>174</v>
       </c>
-      <c r="M12" s="117"/>
+      <c r="M12" s="105"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="104" t="s">
+      <c r="O12" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="P12" s="105"/>
+      <c r="P12" s="110"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -3614,17 +3634,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="107"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="112"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -3665,17 +3685,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="115"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="116"/>
-      <c r="J14" s="116"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="105"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="106"/>
-      <c r="P14" s="107"/>
+      <c r="O14" s="111"/>
+      <c r="P14" s="112"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -3716,17 +3736,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="115"/>
-      <c r="G15" s="115"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="103"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="116"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="104"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="106"/>
-      <c r="P15" s="107"/>
+      <c r="O15" s="111"/>
+      <c r="P15" s="112"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -3767,17 +3787,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="115"/>
-      <c r="G16" s="115"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="116"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="106"/>
-      <c r="P16" s="107"/>
+      <c r="O16" s="111"/>
+      <c r="P16" s="112"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -3818,17 +3838,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="106"/>
-      <c r="P17" s="107"/>
+      <c r="O17" s="111"/>
+      <c r="P17" s="112"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -3869,17 +3889,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="115"/>
-      <c r="G18" s="115"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="105"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="106"/>
-      <c r="P18" s="107"/>
+      <c r="O18" s="111"/>
+      <c r="P18" s="112"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -3920,17 +3940,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="116"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="117"/>
-      <c r="M19" s="117"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="105"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="106"/>
-      <c r="P19" s="107"/>
+      <c r="O19" s="111"/>
+      <c r="P19" s="112"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -3971,17 +3991,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="115"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="116"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="117"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="105"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="108"/>
-      <c r="P20" s="109"/>
+      <c r="O20" s="113"/>
+      <c r="P20" s="114"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -16554,7 +16574,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -16894,7 +16914,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120"/>
+      <c r="A2" s="121"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -17220,15 +17240,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="121"/>
-      <c r="DH2" s="121"/>
-      <c r="DI2" s="121"/>
-      <c r="DJ2" s="121"/>
+      <c r="DG2" s="122"/>
+      <c r="DH2" s="122"/>
+      <c r="DI2" s="122"/>
+      <c r="DJ2" s="122"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="120"/>
+      <c r="A3" s="121"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -17565,7 +17585,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="123" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -17707,7 +17727,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -17847,7 +17867,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -17987,7 +18007,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="123"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -18125,7 +18145,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="122"/>
+      <c r="B8" s="123"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -18265,7 +18285,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="124" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -18407,7 +18427,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="123"/>
+      <c r="B10" s="124"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -18547,7 +18567,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="125" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -18677,7 +18697,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="124"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -18815,7 +18835,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="124"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -18955,7 +18975,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="124"/>
+      <c r="B14" s="125"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -19091,7 +19111,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="124"/>
+      <c r="B15" s="125"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -19227,7 +19247,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -19363,7 +19383,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -19499,7 +19519,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="124"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -19639,7 +19659,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="124"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -19775,7 +19795,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="124"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -19911,7 +19931,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="118" t="s">
+      <c r="B21" s="119" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -20045,7 +20065,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="118"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -20181,7 +20201,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="118"/>
+      <c r="B23" s="119"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -20313,7 +20333,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="118"/>
+      <c r="B24" s="119"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -20447,7 +20467,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="118"/>
+      <c r="B25" s="119"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -20591,7 +20611,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="119" t="s">
+      <c r="B26" s="120" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -20725,7 +20745,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="119"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -20865,7 +20885,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="119"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -20997,7 +21017,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="119"/>
+      <c r="B29" s="120"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -21125,7 +21145,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="119"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -21251,7 +21271,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="119"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 09-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9816DF11-4335-4389-B6F6-9988B9F8644B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B73A2-0B90-4528-9393-DDDD0C84265D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="200">
   <si>
     <t>REDES</t>
   </si>
@@ -700,6 +700,18 @@
   </si>
   <si>
     <t>Criação dos wireframes das telas de boas vindas e jornadas, definição dos requisitos funcionais, não funcionais e regras de negócio</t>
+  </si>
+  <si>
+    <t>Finalização Login web, cadastro de usuário web, cadastro de chamado web. Cadastro de usuário mobile. Estilização sidebar web</t>
+  </si>
+  <si>
+    <t>Testes de requisições à API Zabbix (eventos), finalização da estrutura do relatório</t>
+  </si>
+  <si>
+    <t>Criação de componente de lista web, alteração de layouts com o logo finalizado, importação do banco de dados para o back-end</t>
+  </si>
+  <si>
+    <t>Criação de wireframes, organização dos requisitos funcionais, não funcionais e regras de negócio</t>
   </si>
 </sst>
 </file>
@@ -1452,6 +1464,18 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1460,18 +1484,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1942,7 +1954,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1979,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2247,7 +2259,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2357,7 +2369,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2645,10 +2657,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2706,33 +2718,35 @@
       <c r="U4" s="94" t="s">
         <v>192</v>
       </c>
-      <c r="V4" s="94"/>
+      <c r="V4" s="94" t="s">
+        <v>196</v>
+      </c>
       <c r="W4" s="94"/>
       <c r="X4" s="94"/>
       <c r="Y4" s="94"/>
       <c r="Z4" s="94"/>
       <c r="AA4" s="94"/>
-      <c r="AV4" s="99" t="s">
+      <c r="AV4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="99" t="s">
+      <c r="AW4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="99" t="s">
+      <c r="BT4" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="99" t="s">
+      <c r="BW4" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="99" t="s">
+      <c r="CO4" s="97" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2788,23 +2802,25 @@
       <c r="U5" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="V5" s="94"/>
+      <c r="V5" s="94" t="s">
+        <v>197</v>
+      </c>
       <c r="W5" s="94"/>
       <c r="X5" s="94"/>
       <c r="Y5" s="94"/>
       <c r="Z5" s="94"/>
       <c r="AA5" s="94"/>
-      <c r="AV5" s="99"/>
-      <c r="AW5" s="99"/>
-      <c r="BT5" s="99"/>
-      <c r="BW5" s="99"/>
-      <c r="CO5" s="99"/>
+      <c r="AV5" s="97"/>
+      <c r="AW5" s="97"/>
+      <c r="BT5" s="97"/>
+      <c r="BW5" s="97"/>
+      <c r="CO5" s="97"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="95" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2862,23 +2878,25 @@
       <c r="U6" s="94" t="s">
         <v>194</v>
       </c>
-      <c r="V6" s="94"/>
+      <c r="V6" s="94" t="s">
+        <v>198</v>
+      </c>
       <c r="W6" s="94"/>
       <c r="X6" s="94"/>
       <c r="Y6" s="94"/>
       <c r="Z6" s="94"/>
       <c r="AA6" s="94"/>
-      <c r="AV6" s="99"/>
-      <c r="AW6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BW6" s="99"/>
-      <c r="CO6" s="99"/>
+      <c r="AV6" s="97"/>
+      <c r="AW6" s="97"/>
+      <c r="BT6" s="97"/>
+      <c r="BW6" s="97"/>
+      <c r="CO6" s="97"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -2936,35 +2954,37 @@
       <c r="U7" s="94" t="s">
         <v>195</v>
       </c>
-      <c r="V7" s="94"/>
+      <c r="V7" s="94" t="s">
+        <v>199</v>
+      </c>
       <c r="W7" s="94"/>
       <c r="X7" s="94"/>
       <c r="Y7" s="94"/>
       <c r="Z7" s="94"/>
       <c r="AA7" s="94"/>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="CO7" s="99"/>
+      <c r="AV7" s="97"/>
+      <c r="AW7" s="97"/>
+      <c r="BT7" s="97"/>
+      <c r="BW7" s="97"/>
+      <c r="CO7" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 10-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B73A2-0B90-4528-9393-DDDD0C84265D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0285EB21-F6BA-4E9B-82E3-BAD0FB3ACEA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="204">
   <si>
     <t>REDES</t>
   </si>
@@ -712,6 +712,18 @@
   </si>
   <si>
     <t>Criação de wireframes, organização dos requisitos funcionais, não funcionais e regras de negócio</t>
+  </si>
+  <si>
+    <t>Finalização cadastro de usuário web, cadastro chamados web, configuração do ícone e SplashScreen da aplicação mobile, estilização cadastro usuário mobile, estilização cadastro chamados mobile</t>
+  </si>
+  <si>
+    <t>Criação do projeto para realizar requisições e finalização dos testes à API Zabbix</t>
+  </si>
+  <si>
+    <t>Ajuste Azure DevOps, pesquisa de imagens para o banner, continuação teste de UX, finalização CRUD usuários da API, tela de Login Web, finalização do componente de lista e início componente formulário web, configuração da startup para compressão de requisições à API</t>
+  </si>
+  <si>
+    <t>Continuação dos wireframes e WorkShop Cosmos</t>
   </si>
 </sst>
 </file>
@@ -1464,18 +1476,6 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1484,6 +1484,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1954,7 +1966,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1964,7 +1976,9 @@
     <col min="3" max="13" width="15.77734375" style="78" customWidth="1"/>
     <col min="14" max="16" width="20.77734375" style="78" customWidth="1"/>
     <col min="17" max="17" width="15.77734375" style="78" customWidth="1"/>
-    <col min="18" max="26" width="20.77734375" customWidth="1"/>
+    <col min="18" max="22" width="20.77734375" customWidth="1"/>
+    <col min="23" max="23" width="35.77734375" customWidth="1"/>
+    <col min="24" max="26" width="20.77734375" customWidth="1"/>
     <col min="27" max="27" width="15.77734375" customWidth="1"/>
     <col min="28" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
@@ -1979,7 +1993,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2259,7 +2273,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2369,7 +2383,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2657,10 +2671,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2721,32 +2735,34 @@
       <c r="V4" s="94" t="s">
         <v>196</v>
       </c>
-      <c r="W4" s="94"/>
+      <c r="W4" s="94" t="s">
+        <v>200</v>
+      </c>
       <c r="X4" s="94"/>
       <c r="Y4" s="94"/>
       <c r="Z4" s="94"/>
       <c r="AA4" s="94"/>
-      <c r="AV4" s="97" t="s">
+      <c r="AV4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="97" t="s">
+      <c r="AW4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="97" t="s">
+      <c r="BT4" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="97" t="s">
+      <c r="BW4" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="97" t="s">
+      <c r="CO4" s="99" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2805,22 +2821,24 @@
       <c r="V5" s="94" t="s">
         <v>197</v>
       </c>
-      <c r="W5" s="94"/>
+      <c r="W5" s="94" t="s">
+        <v>201</v>
+      </c>
       <c r="X5" s="94"/>
       <c r="Y5" s="94"/>
       <c r="Z5" s="94"/>
       <c r="AA5" s="94"/>
-      <c r="AV5" s="97"/>
-      <c r="AW5" s="97"/>
-      <c r="BT5" s="97"/>
-      <c r="BW5" s="97"/>
-      <c r="CO5" s="97"/>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="96"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2881,22 +2899,24 @@
       <c r="V6" s="94" t="s">
         <v>198</v>
       </c>
-      <c r="W6" s="94"/>
+      <c r="W6" s="94" t="s">
+        <v>202</v>
+      </c>
       <c r="X6" s="94"/>
       <c r="Y6" s="94"/>
       <c r="Z6" s="94"/>
       <c r="AA6" s="94"/>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97"/>
-      <c r="BT6" s="97"/>
-      <c r="BW6" s="97"/>
-      <c r="CO6" s="97"/>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -2957,34 +2977,36 @@
       <c r="V7" s="94" t="s">
         <v>199</v>
       </c>
-      <c r="W7" s="94"/>
+      <c r="W7" s="94" t="s">
+        <v>203</v>
+      </c>
       <c r="X7" s="94"/>
       <c r="Y7" s="94"/>
       <c r="Z7" s="94"/>
       <c r="AA7" s="94"/>
-      <c r="AV7" s="97"/>
-      <c r="AW7" s="97"/>
-      <c r="BT7" s="97"/>
-      <c r="BW7" s="97"/>
-      <c r="CO7" s="97"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 11-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0285EB21-F6BA-4E9B-82E3-BAD0FB3ACEA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E1EDFB-79CC-420F-A673-A6EA3F78DA55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="208">
   <si>
     <t>REDES</t>
   </si>
@@ -724,6 +724,18 @@
   </si>
   <si>
     <t>Continuação dos wireframes e WorkShop Cosmos</t>
+  </si>
+  <si>
+    <t>Finalização de cadastro de chamados web, refatorando SPA, finalização cadastro mobile e SplashScreen, tabela de chamados BD</t>
+  </si>
+  <si>
+    <t>Projeto teste para exportar em .PDF, testes com bibliotecas para realizar requisições a outras APIs com C#, alinhamento das conclusões sobre a API Zabbix</t>
+  </si>
+  <si>
+    <t>Tela Login Web, rotas do projeto react web, calculadora de preços, correção de telas para os testes de UX, componentes barra de progresso, lista e formulário de cadastro, testes de UX</t>
+  </si>
+  <si>
+    <t>Alterações wireframes, identidade visual e funcionalidades</t>
   </si>
 </sst>
 </file>
@@ -1476,6 +1488,18 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1484,18 +1508,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1963,10 +1975,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1978,7 +1990,8 @@
     <col min="17" max="17" width="15.77734375" style="78" customWidth="1"/>
     <col min="18" max="22" width="20.77734375" customWidth="1"/>
     <col min="23" max="23" width="35.77734375" customWidth="1"/>
-    <col min="24" max="26" width="20.77734375" customWidth="1"/>
+    <col min="24" max="24" width="30.77734375" customWidth="1"/>
+    <col min="25" max="26" width="20.77734375" customWidth="1"/>
     <col min="27" max="27" width="15.77734375" customWidth="1"/>
     <col min="28" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
@@ -1993,7 +2006,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2273,7 +2286,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2383,7 +2396,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2671,10 +2684,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2738,31 +2751,33 @@
       <c r="W4" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="X4" s="94"/>
+      <c r="X4" s="94" t="s">
+        <v>204</v>
+      </c>
       <c r="Y4" s="94"/>
       <c r="Z4" s="94"/>
       <c r="AA4" s="94"/>
-      <c r="AV4" s="99" t="s">
+      <c r="AV4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="99" t="s">
+      <c r="AW4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="99" t="s">
+      <c r="BT4" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="99" t="s">
+      <c r="BW4" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="99" t="s">
+      <c r="CO4" s="97" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2824,21 +2839,23 @@
       <c r="W5" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="X5" s="94"/>
+      <c r="X5" s="94" t="s">
+        <v>205</v>
+      </c>
       <c r="Y5" s="94"/>
       <c r="Z5" s="94"/>
       <c r="AA5" s="94"/>
-      <c r="AV5" s="99"/>
-      <c r="AW5" s="99"/>
-      <c r="BT5" s="99"/>
-      <c r="BW5" s="99"/>
-      <c r="CO5" s="99"/>
+      <c r="AV5" s="97"/>
+      <c r="AW5" s="97"/>
+      <c r="BT5" s="97"/>
+      <c r="BW5" s="97"/>
+      <c r="CO5" s="97"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="95" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2902,21 +2919,23 @@
       <c r="W6" s="94" t="s">
         <v>202</v>
       </c>
-      <c r="X6" s="94"/>
+      <c r="X6" s="94" t="s">
+        <v>206</v>
+      </c>
       <c r="Y6" s="94"/>
       <c r="Z6" s="94"/>
       <c r="AA6" s="94"/>
-      <c r="AV6" s="99"/>
-      <c r="AW6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BW6" s="99"/>
-      <c r="CO6" s="99"/>
+      <c r="AV6" s="97"/>
+      <c r="AW6" s="97"/>
+      <c r="BT6" s="97"/>
+      <c r="BW6" s="97"/>
+      <c r="CO6" s="97"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -2980,33 +2999,35 @@
       <c r="W7" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="X7" s="94"/>
+      <c r="X7" s="94" t="s">
+        <v>207</v>
+      </c>
       <c r="Y7" s="94"/>
       <c r="Z7" s="94"/>
       <c r="AA7" s="94"/>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="CO7" s="99"/>
+      <c r="AV7" s="97"/>
+      <c r="AW7" s="97"/>
+      <c r="BT7" s="97"/>
+      <c r="BW7" s="97"/>
+      <c r="CO7" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 12-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E1EDFB-79CC-420F-A673-A6EA3F78DA55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -27,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="212">
   <si>
     <t>REDES</t>
   </si>
@@ -737,11 +736,23 @@
   <si>
     <t>Alterações wireframes, identidade visual e funcionalidades</t>
   </si>
+  <si>
+    <t>Cadastro chamados mobile, resolução de conflitos ao juntar as telas web, cadastro de chamados API</t>
+  </si>
+  <si>
+    <t>Finalização dos testes com a API Zabbix</t>
+  </si>
+  <si>
+    <t>Prototipação das telas, componente modal, ajuste CRUD usuários e início CRUD agenda API, Banner apresentação final, estudo drag and drop</t>
+  </si>
+  <si>
+    <t>Wireframes e documentação das telas, incluindo funcionalidades sobre as mesmas.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1488,18 +1499,6 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1508,6 +1507,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1971,14 +1982,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
+      <selection pane="bottomRight" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2017,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2286,7 +2297,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2396,7 +2407,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2684,10 +2695,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2754,30 +2765,32 @@
       <c r="X4" s="94" t="s">
         <v>204</v>
       </c>
-      <c r="Y4" s="94"/>
+      <c r="Y4" s="94" t="s">
+        <v>208</v>
+      </c>
       <c r="Z4" s="94"/>
       <c r="AA4" s="94"/>
-      <c r="AV4" s="97" t="s">
+      <c r="AV4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="97" t="s">
+      <c r="AW4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="97" t="s">
+      <c r="BT4" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="97" t="s">
+      <c r="BW4" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="97" t="s">
+      <c r="CO4" s="99" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2842,20 +2855,22 @@
       <c r="X5" s="94" t="s">
         <v>205</v>
       </c>
-      <c r="Y5" s="94"/>
+      <c r="Y5" s="94" t="s">
+        <v>209</v>
+      </c>
       <c r="Z5" s="94"/>
       <c r="AA5" s="94"/>
-      <c r="AV5" s="97"/>
-      <c r="AW5" s="97"/>
-      <c r="BT5" s="97"/>
-      <c r="BW5" s="97"/>
-      <c r="CO5" s="97"/>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="96"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2922,20 +2937,22 @@
       <c r="X6" s="94" t="s">
         <v>206</v>
       </c>
-      <c r="Y6" s="94"/>
+      <c r="Y6" s="94" t="s">
+        <v>210</v>
+      </c>
       <c r="Z6" s="94"/>
       <c r="AA6" s="94"/>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97"/>
-      <c r="BT6" s="97"/>
-      <c r="BW6" s="97"/>
-      <c r="CO6" s="97"/>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3002,32 +3019,34 @@
       <c r="X7" s="94" t="s">
         <v>207</v>
       </c>
-      <c r="Y7" s="94"/>
+      <c r="Y7" s="94" t="s">
+        <v>211</v>
+      </c>
       <c r="Z7" s="94"/>
       <c r="AA7" s="94"/>
-      <c r="AV7" s="97"/>
-      <c r="AW7" s="97"/>
-      <c r="BT7" s="97"/>
-      <c r="BW7" s="97"/>
-      <c r="CO7" s="97"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3036,7 +3055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F2A229-C49C-4272-9B33-7396812FE142}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16615,7 +16634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona daily realizada em 13-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="216">
   <si>
     <t>REDES</t>
   </si>
@@ -747,6 +747,18 @@
   </si>
   <si>
     <t>Wireframes e documentação das telas, incluindo funcionalidades sobre as mesmas.</t>
+  </si>
+  <si>
+    <t>Estilização menu web, lista de usuários web, menu mobile, tela cadastro chamados (falta funcionalidade) mobile, hospedagem API Azure, cadastro de chamados API</t>
+  </si>
+  <si>
+    <t>Alinhamento com o grupo de redes para a reunião, passo a passo como coletar dados da API Zabbix</t>
+  </si>
+  <si>
+    <t>Modal aviso e confirmação, listar por id, listar usuário API, teste de Endpoins API, estudo drag and drop, finalização testes de UX</t>
+  </si>
+  <si>
+    <t>Finalização wireframe mobile, montagem apresentação, finalização documentação telas, funcionalidades e regras de negócio, ajuste user stories</t>
   </si>
 </sst>
 </file>
@@ -1499,6 +1511,18 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1507,18 +1531,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1989,7 +2001,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W4" sqref="W4"/>
+      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2014,8 @@
     <col min="18" max="22" width="20.77734375" customWidth="1"/>
     <col min="23" max="23" width="35.77734375" customWidth="1"/>
     <col min="24" max="24" width="30.77734375" customWidth="1"/>
-    <col min="25" max="26" width="20.77734375" customWidth="1"/>
+    <col min="25" max="25" width="20.77734375" customWidth="1"/>
+    <col min="26" max="26" width="25.77734375" customWidth="1"/>
     <col min="27" max="27" width="15.77734375" customWidth="1"/>
     <col min="28" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
@@ -2017,7 +2030,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2297,7 +2310,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2407,7 +2420,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2695,10 +2708,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2768,29 +2781,31 @@
       <c r="Y4" s="94" t="s">
         <v>208</v>
       </c>
-      <c r="Z4" s="94"/>
+      <c r="Z4" s="94" t="s">
+        <v>212</v>
+      </c>
       <c r="AA4" s="94"/>
-      <c r="AV4" s="99" t="s">
+      <c r="AV4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="99" t="s">
+      <c r="AW4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="99" t="s">
+      <c r="BT4" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="99" t="s">
+      <c r="BW4" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="99" t="s">
+      <c r="CO4" s="97" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2858,19 +2873,21 @@
       <c r="Y5" s="94" t="s">
         <v>209</v>
       </c>
-      <c r="Z5" s="94"/>
+      <c r="Z5" s="94" t="s">
+        <v>213</v>
+      </c>
       <c r="AA5" s="94"/>
-      <c r="AV5" s="99"/>
-      <c r="AW5" s="99"/>
-      <c r="BT5" s="99"/>
-      <c r="BW5" s="99"/>
-      <c r="CO5" s="99"/>
+      <c r="AV5" s="97"/>
+      <c r="AW5" s="97"/>
+      <c r="BT5" s="97"/>
+      <c r="BW5" s="97"/>
+      <c r="CO5" s="97"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="95" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2940,19 +2957,21 @@
       <c r="Y6" s="94" t="s">
         <v>210</v>
       </c>
-      <c r="Z6" s="94"/>
+      <c r="Z6" s="94" t="s">
+        <v>214</v>
+      </c>
       <c r="AA6" s="94"/>
-      <c r="AV6" s="99"/>
-      <c r="AW6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BW6" s="99"/>
-      <c r="CO6" s="99"/>
+      <c r="AV6" s="97"/>
+      <c r="AW6" s="97"/>
+      <c r="BT6" s="97"/>
+      <c r="BW6" s="97"/>
+      <c r="CO6" s="97"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3022,31 +3041,33 @@
       <c r="Y7" s="94" t="s">
         <v>211</v>
       </c>
-      <c r="Z7" s="94"/>
+      <c r="Z7" s="94" t="s">
+        <v>215</v>
+      </c>
       <c r="AA7" s="94"/>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="CO7" s="99"/>
+      <c r="AV7" s="97"/>
+      <c r="AW7" s="97"/>
+      <c r="BT7" s="97"/>
+      <c r="BW7" s="97"/>
+      <c r="CO7" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 16-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="217">
   <si>
     <t>REDES</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>Finalização wireframe mobile, montagem apresentação, finalização documentação telas, funcionalidades e regras de negócio, ajuste user stories</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente</t>
   </si>
 </sst>
 </file>
@@ -1511,18 +1514,6 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1531,6 +1522,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2001,7 +2004,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2030,7 +2033,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2310,7 +2313,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2420,7 +2423,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2708,10 +2711,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2784,28 +2787,30 @@
       <c r="Z4" s="94" t="s">
         <v>212</v>
       </c>
-      <c r="AA4" s="94"/>
-      <c r="AV4" s="97" t="s">
+      <c r="AA4" s="94" t="s">
+        <v>216</v>
+      </c>
+      <c r="AV4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="97" t="s">
+      <c r="AW4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="97" t="s">
+      <c r="BT4" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="97" t="s">
+      <c r="BW4" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="97" t="s">
+      <c r="CO4" s="99" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2876,18 +2881,20 @@
       <c r="Z5" s="94" t="s">
         <v>213</v>
       </c>
-      <c r="AA5" s="94"/>
-      <c r="AV5" s="97"/>
-      <c r="AW5" s="97"/>
-      <c r="BT5" s="97"/>
-      <c r="BW5" s="97"/>
-      <c r="CO5" s="97"/>
+      <c r="AA5" s="94" t="s">
+        <v>216</v>
+      </c>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="96"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2960,18 +2967,20 @@
       <c r="Z6" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="AA6" s="94"/>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97"/>
-      <c r="BT6" s="97"/>
-      <c r="BW6" s="97"/>
-      <c r="CO6" s="97"/>
+      <c r="AA6" s="94" t="s">
+        <v>216</v>
+      </c>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3044,30 +3053,32 @@
       <c r="Z7" s="94" t="s">
         <v>215</v>
       </c>
-      <c r="AA7" s="94"/>
-      <c r="AV7" s="97"/>
-      <c r="AW7" s="97"/>
-      <c r="BT7" s="97"/>
-      <c r="BW7" s="97"/>
-      <c r="CO7" s="97"/>
+      <c r="AA7" s="94" t="s">
+        <v>216</v>
+      </c>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Incrementa informacoes da daily de 16-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="220">
   <si>
     <t>REDES</t>
   </si>
@@ -761,7 +761,16 @@
     <t>Finalização wireframe mobile, montagem apresentação, finalização documentação telas, funcionalidades e regras de negócio, ajuste user stories</t>
   </si>
   <si>
-    <t>Reunião com o cliente</t>
+    <t>Reunião com o cliente. Entrega das telas, feedback do cliente positivo. Acrescida uma tela de anexo</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente. Entrega do projeto 1, o qual vai sofrer mais alterações. Demonstraram das requisições do projeto 2. Feedback do cliente positivo</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente. Entrega dos layouts e teste de UX com o cliente. Alterações solicitadas</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente. Entrega dos wireframes e user stories revisadas. Validações pendentes</t>
   </si>
 </sst>
 </file>
@@ -1514,6 +1523,18 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1522,18 +1543,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2018,8 +2027,7 @@
     <col min="23" max="23" width="35.77734375" customWidth="1"/>
     <col min="24" max="24" width="30.77734375" customWidth="1"/>
     <col min="25" max="25" width="20.77734375" customWidth="1"/>
-    <col min="26" max="26" width="25.77734375" customWidth="1"/>
-    <col min="27" max="27" width="15.77734375" customWidth="1"/>
+    <col min="26" max="27" width="25.77734375" customWidth="1"/>
     <col min="28" max="47" width="5.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -2033,7 +2041,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2313,7 +2321,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2423,7 +2431,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2711,10 +2719,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2790,27 +2798,27 @@
       <c r="AA4" s="94" t="s">
         <v>216</v>
       </c>
-      <c r="AV4" s="99" t="s">
+      <c r="AV4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="99" t="s">
+      <c r="AW4" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="99" t="s">
+      <c r="BT4" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="99" t="s">
+      <c r="BW4" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="99" t="s">
+      <c r="CO4" s="97" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2882,19 +2890,19 @@
         <v>213</v>
       </c>
       <c r="AA5" s="94" t="s">
-        <v>216</v>
-      </c>
-      <c r="AV5" s="99"/>
-      <c r="AW5" s="99"/>
-      <c r="BT5" s="99"/>
-      <c r="BW5" s="99"/>
-      <c r="CO5" s="99"/>
+        <v>217</v>
+      </c>
+      <c r="AV5" s="97"/>
+      <c r="AW5" s="97"/>
+      <c r="BT5" s="97"/>
+      <c r="BW5" s="97"/>
+      <c r="CO5" s="97"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="95" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2968,19 +2976,19 @@
         <v>214</v>
       </c>
       <c r="AA6" s="94" t="s">
-        <v>216</v>
-      </c>
-      <c r="AV6" s="99"/>
-      <c r="AW6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BW6" s="99"/>
-      <c r="CO6" s="99"/>
+        <v>218</v>
+      </c>
+      <c r="AV6" s="97"/>
+      <c r="AW6" s="97"/>
+      <c r="BT6" s="97"/>
+      <c r="BW6" s="97"/>
+      <c r="CO6" s="97"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3054,31 +3062,31 @@
         <v>215</v>
       </c>
       <c r="AA7" s="94" t="s">
-        <v>216</v>
-      </c>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="CO7" s="99"/>
+        <v>219</v>
+      </c>
+      <c r="AV7" s="97"/>
+      <c r="AW7" s="97"/>
+      <c r="BT7" s="97"/>
+      <c r="BW7" s="97"/>
+      <c r="CO7" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 17-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3007318A-8B47-4F93-B0CF-F1B6D43AE447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="224">
   <si>
     <t>REDES</t>
   </si>
@@ -772,12 +773,24 @@
   <si>
     <t>Reunião com o cliente. Entrega dos wireframes e user stories revisadas. Validações pendentes</t>
   </si>
+  <si>
+    <t>Sprint review, planejamento da sprint e construção da ata de reunião</t>
+  </si>
+  <si>
+    <t>Planejamento da sprint e definição da estrutura das telas do site</t>
+  </si>
+  <si>
+    <t>Alinhamento dos resultados da reunião, navbar, dashboard, listagem de jornadas na API, alterações no componente de cadastro</t>
+  </si>
+  <si>
+    <t>Sprint review, planning da sprint e funcionalidades e telas do administrador com a Space Needle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -906,6 +919,12 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1287,7 +1306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1523,18 +1542,6 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1543,6 +1550,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1614,6 +1633,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1690,12 +1721,12 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF9B54D0"/>
+      <color rgb="FFCB3D3D"/>
+      <color rgb="FFFFD966"/>
       <color rgb="FF5B2484"/>
-      <color rgb="FF9B54D0"/>
       <color rgb="FF7C7C7C"/>
       <color rgb="FF548235"/>
-      <color rgb="FFCB3D3D"/>
-      <color rgb="FFFFD966"/>
       <color rgb="FFB47EDC"/>
     </mruColors>
   </colors>
@@ -2006,14 +2037,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
+      <selection pane="bottomRight" activeCell="AQ5" sqref="AQ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2059,8 @@
     <col min="24" max="24" width="30.77734375" customWidth="1"/>
     <col min="25" max="25" width="20.77734375" customWidth="1"/>
     <col min="26" max="27" width="25.77734375" customWidth="1"/>
-    <col min="28" max="47" width="5.77734375" customWidth="1"/>
+    <col min="28" max="37" width="20.77734375" customWidth="1"/>
+    <col min="38" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="71" width="5.77734375" customWidth="1"/>
@@ -2041,7 +2073,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="95" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2321,7 +2353,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2431,7 +2463,7 @@
       <c r="CR2" s="98"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2510,7 +2542,7 @@
       <c r="AA3" s="88">
         <v>13</v>
       </c>
-      <c r="AB3" s="87">
+      <c r="AB3" s="88">
         <v>16</v>
       </c>
       <c r="AC3" s="87">
@@ -2522,10 +2554,10 @@
       <c r="AE3" s="87">
         <v>19</v>
       </c>
-      <c r="AF3" s="87">
+      <c r="AF3" s="88">
         <v>20</v>
       </c>
-      <c r="AG3" s="87">
+      <c r="AG3" s="88">
         <v>23</v>
       </c>
       <c r="AH3" s="87">
@@ -2537,10 +2569,10 @@
       <c r="AJ3" s="87">
         <v>26</v>
       </c>
-      <c r="AK3" s="87">
+      <c r="AK3" s="88">
         <v>27</v>
       </c>
-      <c r="AL3" s="87">
+      <c r="AL3" s="88">
         <v>30</v>
       </c>
       <c r="AM3" s="87">
@@ -2552,10 +2584,10 @@
       <c r="AO3" s="87">
         <v>3</v>
       </c>
-      <c r="AP3" s="87">
+      <c r="AP3" s="88">
         <v>4</v>
       </c>
-      <c r="AQ3" s="87">
+      <c r="AQ3" s="88">
         <v>7</v>
       </c>
       <c r="AR3" s="87">
@@ -2567,7 +2599,7 @@
       <c r="AT3" s="87">
         <v>10</v>
       </c>
-      <c r="AU3" s="87">
+      <c r="AU3" s="88">
         <v>11</v>
       </c>
       <c r="AV3" s="83">
@@ -2719,10 +2751,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2798,27 +2830,49 @@
       <c r="AA4" s="94" t="s">
         <v>216</v>
       </c>
-      <c r="AV4" s="97" t="s">
+      <c r="AB4" s="126" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC4" s="126"/>
+      <c r="AD4" s="126"/>
+      <c r="AE4" s="126"/>
+      <c r="AF4" s="126"/>
+      <c r="AG4" s="126"/>
+      <c r="AH4" s="126"/>
+      <c r="AI4" s="126"/>
+      <c r="AJ4" s="126"/>
+      <c r="AK4" s="126"/>
+      <c r="AL4" s="127"/>
+      <c r="AM4" s="127"/>
+      <c r="AN4" s="127"/>
+      <c r="AO4" s="127"/>
+      <c r="AP4" s="127"/>
+      <c r="AQ4" s="127"/>
+      <c r="AR4" s="127"/>
+      <c r="AS4" s="127"/>
+      <c r="AT4" s="127"/>
+      <c r="AU4" s="128"/>
+      <c r="AV4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="97" t="s">
+      <c r="AW4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="97" t="s">
+      <c r="BT4" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="97" t="s">
+      <c r="BW4" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="97" t="s">
+      <c r="CO4" s="99" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2892,17 +2946,39 @@
       <c r="AA5" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="AV5" s="97"/>
-      <c r="AW5" s="97"/>
-      <c r="BT5" s="97"/>
-      <c r="BW5" s="97"/>
-      <c r="CO5" s="97"/>
+      <c r="AB5" s="126" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC5" s="126"/>
+      <c r="AD5" s="126"/>
+      <c r="AE5" s="126"/>
+      <c r="AF5" s="126"/>
+      <c r="AG5" s="126"/>
+      <c r="AH5" s="126"/>
+      <c r="AI5" s="126"/>
+      <c r="AJ5" s="126"/>
+      <c r="AK5" s="126"/>
+      <c r="AL5" s="127"/>
+      <c r="AM5" s="127"/>
+      <c r="AN5" s="127"/>
+      <c r="AO5" s="127"/>
+      <c r="AP5" s="127"/>
+      <c r="AQ5" s="127"/>
+      <c r="AR5" s="127"/>
+      <c r="AS5" s="127"/>
+      <c r="AT5" s="127"/>
+      <c r="AU5" s="129"/>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="96"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -2978,17 +3054,39 @@
       <c r="AA6" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97"/>
-      <c r="BT6" s="97"/>
-      <c r="BW6" s="97"/>
-      <c r="CO6" s="97"/>
+      <c r="AB6" s="126" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC6" s="126"/>
+      <c r="AD6" s="126"/>
+      <c r="AE6" s="126"/>
+      <c r="AF6" s="126"/>
+      <c r="AG6" s="126"/>
+      <c r="AH6" s="126"/>
+      <c r="AI6" s="126"/>
+      <c r="AJ6" s="126"/>
+      <c r="AK6" s="126"/>
+      <c r="AL6" s="127"/>
+      <c r="AM6" s="127"/>
+      <c r="AN6" s="127"/>
+      <c r="AO6" s="127"/>
+      <c r="AP6" s="127"/>
+      <c r="AQ6" s="127"/>
+      <c r="AR6" s="127"/>
+      <c r="AS6" s="127"/>
+      <c r="AT6" s="127"/>
+      <c r="AU6" s="128"/>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3064,29 +3162,51 @@
       <c r="AA7" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="AV7" s="97"/>
-      <c r="AW7" s="97"/>
-      <c r="BT7" s="97"/>
-      <c r="BW7" s="97"/>
-      <c r="CO7" s="97"/>
+      <c r="AB7" s="126" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC7" s="126"/>
+      <c r="AD7" s="126"/>
+      <c r="AE7" s="126"/>
+      <c r="AF7" s="126"/>
+      <c r="AG7" s="126"/>
+      <c r="AH7" s="126"/>
+      <c r="AI7" s="126"/>
+      <c r="AJ7" s="126"/>
+      <c r="AK7" s="126"/>
+      <c r="AL7" s="127"/>
+      <c r="AM7" s="127"/>
+      <c r="AN7" s="127"/>
+      <c r="AO7" s="127"/>
+      <c r="AP7" s="127"/>
+      <c r="AQ7" s="127"/>
+      <c r="AR7" s="127"/>
+      <c r="AS7" s="127"/>
+      <c r="AT7" s="127"/>
+      <c r="AU7" s="128"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3095,7 +3215,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16674,11 +16794,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AO4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AD12" sqref="AD12"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 18-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3007318A-8B47-4F93-B0CF-F1B6D43AE447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A10EFCF-B176-43B7-B2DE-EE4A4BA0F24A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="228">
   <si>
     <t>REDES</t>
   </si>
@@ -784,6 +784,18 @@
   </si>
   <si>
     <t>Sprint review, planning da sprint e funcionalidades e telas do administrador com a Space Needle</t>
+  </si>
+  <si>
+    <t>Configuração DevOps, estudo API Zabbix, integração com GLPI (login chamados e token), tela lista de usuários web, cadastro de chamados API</t>
+  </si>
+  <si>
+    <t>Layouts baixa fidelidade telas, modelagem banco de dados, página login web, definição de telas</t>
+  </si>
+  <si>
+    <t>Dashboard lista agendas encerradas, navbar, estudo drag and drop, JSON false, página cadastro</t>
+  </si>
+  <si>
+    <t>Planning da sprint, distribuição de tarefas, store points, wireframe administrador</t>
   </si>
 </sst>
 </file>
@@ -1542,6 +1554,30 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1550,18 +1586,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1633,18 +1657,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2044,7 +2056,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ5" sqref="AQ5"/>
+      <selection pane="bottomRight" activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2071,9 @@
     <col min="24" max="24" width="30.77734375" customWidth="1"/>
     <col min="25" max="25" width="20.77734375" customWidth="1"/>
     <col min="26" max="27" width="25.77734375" customWidth="1"/>
-    <col min="28" max="37" width="20.77734375" customWidth="1"/>
+    <col min="28" max="28" width="20.77734375" customWidth="1"/>
+    <col min="29" max="29" width="25.77734375" customWidth="1"/>
+    <col min="30" max="37" width="20.77734375" customWidth="1"/>
     <col min="38" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -2073,7 +2087,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="103" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2353,117 +2367,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="104"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="102" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98" t="s">
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="98"/>
-      <c r="W2" s="98"/>
-      <c r="X2" s="98"/>
-      <c r="Y2" s="98"/>
-      <c r="Z2" s="98"/>
-      <c r="AA2" s="98"/>
-      <c r="AB2" s="98"/>
-      <c r="AC2" s="98"/>
-      <c r="AD2" s="98"/>
-      <c r="AE2" s="98"/>
-      <c r="AF2" s="98"/>
-      <c r="AG2" s="98"/>
-      <c r="AH2" s="98"/>
-      <c r="AI2" s="98"/>
-      <c r="AJ2" s="98"/>
-      <c r="AK2" s="98"/>
-      <c r="AL2" s="98"/>
-      <c r="AM2" s="98" t="s">
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="102"/>
+      <c r="Y2" s="102"/>
+      <c r="Z2" s="102"/>
+      <c r="AA2" s="102"/>
+      <c r="AB2" s="102"/>
+      <c r="AC2" s="102"/>
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="102"/>
+      <c r="AF2" s="102"/>
+      <c r="AG2" s="102"/>
+      <c r="AH2" s="102"/>
+      <c r="AI2" s="102"/>
+      <c r="AJ2" s="102"/>
+      <c r="AK2" s="102"/>
+      <c r="AL2" s="102"/>
+      <c r="AM2" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="98"/>
-      <c r="AO2" s="98"/>
-      <c r="AP2" s="98"/>
-      <c r="AQ2" s="98"/>
-      <c r="AR2" s="98"/>
-      <c r="AS2" s="98"/>
-      <c r="AT2" s="98"/>
-      <c r="AU2" s="98"/>
-      <c r="AV2" s="98"/>
-      <c r="AW2" s="98"/>
-      <c r="AX2" s="98"/>
-      <c r="AY2" s="98"/>
-      <c r="AZ2" s="98"/>
-      <c r="BA2" s="98"/>
-      <c r="BB2" s="98"/>
-      <c r="BC2" s="98"/>
-      <c r="BD2" s="98"/>
-      <c r="BE2" s="98"/>
-      <c r="BF2" s="98"/>
-      <c r="BG2" s="98"/>
-      <c r="BH2" s="98"/>
-      <c r="BI2" s="98"/>
-      <c r="BJ2" s="98" t="s">
+      <c r="AN2" s="102"/>
+      <c r="AO2" s="102"/>
+      <c r="AP2" s="102"/>
+      <c r="AQ2" s="102"/>
+      <c r="AR2" s="102"/>
+      <c r="AS2" s="102"/>
+      <c r="AT2" s="102"/>
+      <c r="AU2" s="102"/>
+      <c r="AV2" s="102"/>
+      <c r="AW2" s="102"/>
+      <c r="AX2" s="102"/>
+      <c r="AY2" s="102"/>
+      <c r="AZ2" s="102"/>
+      <c r="BA2" s="102"/>
+      <c r="BB2" s="102"/>
+      <c r="BC2" s="102"/>
+      <c r="BD2" s="102"/>
+      <c r="BE2" s="102"/>
+      <c r="BF2" s="102"/>
+      <c r="BG2" s="102"/>
+      <c r="BH2" s="102"/>
+      <c r="BI2" s="102"/>
+      <c r="BJ2" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="98"/>
-      <c r="BL2" s="98"/>
-      <c r="BM2" s="98"/>
-      <c r="BN2" s="98"/>
-      <c r="BO2" s="98"/>
-      <c r="BP2" s="98"/>
-      <c r="BQ2" s="98"/>
-      <c r="BR2" s="98"/>
-      <c r="BS2" s="98"/>
-      <c r="BT2" s="98"/>
-      <c r="BU2" s="98"/>
-      <c r="BV2" s="98"/>
-      <c r="BW2" s="98"/>
-      <c r="BX2" s="98"/>
-      <c r="BY2" s="98"/>
-      <c r="BZ2" s="98"/>
-      <c r="CA2" s="98"/>
-      <c r="CB2" s="98"/>
-      <c r="CC2" s="98"/>
-      <c r="CD2" s="98"/>
-      <c r="CE2" s="98" t="s">
+      <c r="BK2" s="102"/>
+      <c r="BL2" s="102"/>
+      <c r="BM2" s="102"/>
+      <c r="BN2" s="102"/>
+      <c r="BO2" s="102"/>
+      <c r="BP2" s="102"/>
+      <c r="BQ2" s="102"/>
+      <c r="BR2" s="102"/>
+      <c r="BS2" s="102"/>
+      <c r="BT2" s="102"/>
+      <c r="BU2" s="102"/>
+      <c r="BV2" s="102"/>
+      <c r="BW2" s="102"/>
+      <c r="BX2" s="102"/>
+      <c r="BY2" s="102"/>
+      <c r="BZ2" s="102"/>
+      <c r="CA2" s="102"/>
+      <c r="CB2" s="102"/>
+      <c r="CC2" s="102"/>
+      <c r="CD2" s="102"/>
+      <c r="CE2" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="98"/>
-      <c r="CG2" s="98"/>
-      <c r="CH2" s="98"/>
-      <c r="CI2" s="98"/>
-      <c r="CJ2" s="98"/>
-      <c r="CK2" s="98"/>
-      <c r="CL2" s="98"/>
-      <c r="CM2" s="98"/>
-      <c r="CN2" s="98"/>
-      <c r="CO2" s="98"/>
-      <c r="CP2" s="98"/>
-      <c r="CQ2" s="98"/>
-      <c r="CR2" s="98"/>
+      <c r="CF2" s="102"/>
+      <c r="CG2" s="102"/>
+      <c r="CH2" s="102"/>
+      <c r="CI2" s="102"/>
+      <c r="CJ2" s="102"/>
+      <c r="CK2" s="102"/>
+      <c r="CL2" s="102"/>
+      <c r="CM2" s="102"/>
+      <c r="CN2" s="102"/>
+      <c r="CO2" s="102"/>
+      <c r="CP2" s="102"/>
+      <c r="CQ2" s="102"/>
+      <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="105"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2751,10 +2765,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2830,49 +2844,51 @@
       <c r="AA4" s="94" t="s">
         <v>216</v>
       </c>
-      <c r="AB4" s="126" t="s">
+      <c r="AB4" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="AC4" s="126"/>
-      <c r="AD4" s="126"/>
-      <c r="AE4" s="126"/>
-      <c r="AF4" s="126"/>
-      <c r="AG4" s="126"/>
-      <c r="AH4" s="126"/>
-      <c r="AI4" s="126"/>
-      <c r="AJ4" s="126"/>
-      <c r="AK4" s="126"/>
-      <c r="AL4" s="127"/>
-      <c r="AM4" s="127"/>
-      <c r="AN4" s="127"/>
-      <c r="AO4" s="127"/>
-      <c r="AP4" s="127"/>
-      <c r="AQ4" s="127"/>
-      <c r="AR4" s="127"/>
-      <c r="AS4" s="127"/>
-      <c r="AT4" s="127"/>
-      <c r="AU4" s="128"/>
-      <c r="AV4" s="99" t="s">
+      <c r="AC4" s="95" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="95"/>
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
+      <c r="AL4" s="96"/>
+      <c r="AM4" s="96"/>
+      <c r="AN4" s="96"/>
+      <c r="AO4" s="96"/>
+      <c r="AP4" s="96"/>
+      <c r="AQ4" s="96"/>
+      <c r="AR4" s="96"/>
+      <c r="AS4" s="96"/>
+      <c r="AT4" s="96"/>
+      <c r="AU4" s="97"/>
+      <c r="AV4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="99" t="s">
+      <c r="AW4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="99" t="s">
+      <c r="BT4" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="99" t="s">
+      <c r="BW4" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="99" t="s">
+      <c r="CO4" s="101" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2946,39 +2962,41 @@
       <c r="AA5" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="AB5" s="126" t="s">
+      <c r="AB5" s="95" t="s">
         <v>221</v>
       </c>
-      <c r="AC5" s="126"/>
-      <c r="AD5" s="126"/>
-      <c r="AE5" s="126"/>
-      <c r="AF5" s="126"/>
-      <c r="AG5" s="126"/>
-      <c r="AH5" s="126"/>
-      <c r="AI5" s="126"/>
-      <c r="AJ5" s="126"/>
-      <c r="AK5" s="126"/>
-      <c r="AL5" s="127"/>
-      <c r="AM5" s="127"/>
-      <c r="AN5" s="127"/>
-      <c r="AO5" s="127"/>
-      <c r="AP5" s="127"/>
-      <c r="AQ5" s="127"/>
-      <c r="AR5" s="127"/>
-      <c r="AS5" s="127"/>
-      <c r="AT5" s="127"/>
-      <c r="AU5" s="129"/>
-      <c r="AV5" s="99"/>
-      <c r="AW5" s="99"/>
-      <c r="BT5" s="99"/>
-      <c r="BW5" s="99"/>
-      <c r="CO5" s="99"/>
+      <c r="AC5" s="95" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
+      <c r="AI5" s="95"/>
+      <c r="AJ5" s="95"/>
+      <c r="AK5" s="95"/>
+      <c r="AL5" s="96"/>
+      <c r="AM5" s="96"/>
+      <c r="AN5" s="96"/>
+      <c r="AO5" s="96"/>
+      <c r="AP5" s="96"/>
+      <c r="AQ5" s="96"/>
+      <c r="AR5" s="96"/>
+      <c r="AS5" s="96"/>
+      <c r="AT5" s="96"/>
+      <c r="AU5" s="98"/>
+      <c r="AV5" s="101"/>
+      <c r="AW5" s="101"/>
+      <c r="BT5" s="101"/>
+      <c r="BW5" s="101"/>
+      <c r="CO5" s="101"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3054,39 +3072,41 @@
       <c r="AA6" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="AB6" s="126" t="s">
+      <c r="AB6" s="95" t="s">
         <v>222</v>
       </c>
-      <c r="AC6" s="126"/>
-      <c r="AD6" s="126"/>
-      <c r="AE6" s="126"/>
-      <c r="AF6" s="126"/>
-      <c r="AG6" s="126"/>
-      <c r="AH6" s="126"/>
-      <c r="AI6" s="126"/>
-      <c r="AJ6" s="126"/>
-      <c r="AK6" s="126"/>
-      <c r="AL6" s="127"/>
-      <c r="AM6" s="127"/>
-      <c r="AN6" s="127"/>
-      <c r="AO6" s="127"/>
-      <c r="AP6" s="127"/>
-      <c r="AQ6" s="127"/>
-      <c r="AR6" s="127"/>
-      <c r="AS6" s="127"/>
-      <c r="AT6" s="127"/>
-      <c r="AU6" s="128"/>
-      <c r="AV6" s="99"/>
-      <c r="AW6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BW6" s="99"/>
-      <c r="CO6" s="99"/>
+      <c r="AC6" s="95" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD6" s="95"/>
+      <c r="AE6" s="95"/>
+      <c r="AF6" s="95"/>
+      <c r="AG6" s="95"/>
+      <c r="AH6" s="95"/>
+      <c r="AI6" s="95"/>
+      <c r="AJ6" s="95"/>
+      <c r="AK6" s="95"/>
+      <c r="AL6" s="96"/>
+      <c r="AM6" s="96"/>
+      <c r="AN6" s="96"/>
+      <c r="AO6" s="96"/>
+      <c r="AP6" s="96"/>
+      <c r="AQ6" s="96"/>
+      <c r="AR6" s="96"/>
+      <c r="AS6" s="96"/>
+      <c r="AT6" s="96"/>
+      <c r="AU6" s="97"/>
+      <c r="AV6" s="101"/>
+      <c r="AW6" s="101"/>
+      <c r="BT6" s="101"/>
+      <c r="BW6" s="101"/>
+      <c r="CO6" s="101"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3162,51 +3182,53 @@
       <c r="AA7" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="AB7" s="126" t="s">
+      <c r="AB7" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="AC7" s="126"/>
-      <c r="AD7" s="126"/>
-      <c r="AE7" s="126"/>
-      <c r="AF7" s="126"/>
-      <c r="AG7" s="126"/>
-      <c r="AH7" s="126"/>
-      <c r="AI7" s="126"/>
-      <c r="AJ7" s="126"/>
-      <c r="AK7" s="126"/>
-      <c r="AL7" s="127"/>
-      <c r="AM7" s="127"/>
-      <c r="AN7" s="127"/>
-      <c r="AO7" s="127"/>
-      <c r="AP7" s="127"/>
-      <c r="AQ7" s="127"/>
-      <c r="AR7" s="127"/>
-      <c r="AS7" s="127"/>
-      <c r="AT7" s="127"/>
-      <c r="AU7" s="128"/>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="CO7" s="99"/>
+      <c r="AC7" s="95" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="95"/>
+      <c r="AG7" s="95"/>
+      <c r="AH7" s="95"/>
+      <c r="AI7" s="95"/>
+      <c r="AJ7" s="95"/>
+      <c r="AK7" s="95"/>
+      <c r="AL7" s="96"/>
+      <c r="AM7" s="96"/>
+      <c r="AN7" s="96"/>
+      <c r="AO7" s="96"/>
+      <c r="AP7" s="96"/>
+      <c r="AQ7" s="96"/>
+      <c r="AR7" s="96"/>
+      <c r="AS7" s="96"/>
+      <c r="AT7" s="96"/>
+      <c r="AU7" s="97"/>
+      <c r="AV7" s="101"/>
+      <c r="AW7" s="101"/>
+      <c r="BT7" s="101"/>
+      <c r="BW7" s="101"/>
+      <c r="CO7" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3289,36 +3311,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="110" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="119" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="115"/>
+      <c r="G2" s="119"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="116" t="s">
+      <c r="I2" s="120" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="116"/>
+      <c r="J2" s="120"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="117" t="s">
+      <c r="L2" s="121" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="117"/>
+      <c r="M2" s="121"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="118" t="s">
+      <c r="O2" s="122" t="s">
         <v>170</v>
       </c>
-      <c r="P2" s="118"/>
+      <c r="P2" s="122"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="102" t="s">
+      <c r="R2" s="106" t="s">
         <v>171</v>
       </c>
-      <c r="S2" s="102"/>
+      <c r="S2" s="106"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -3352,24 +3374,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="118"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="102"/>
+      <c r="R3" s="106"/>
+      <c r="S3" s="106"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -3403,24 +3425,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="117"/>
-      <c r="M4" s="117"/>
+      <c r="L4" s="121"/>
+      <c r="M4" s="121"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118"/>
+      <c r="O4" s="122"/>
+      <c r="P4" s="122"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
+      <c r="R4" s="106"/>
+      <c r="S4" s="106"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -3458,20 +3480,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="117"/>
-      <c r="M5" s="117"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
+      <c r="O5" s="122"/>
+      <c r="P5" s="122"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="102"/>
-      <c r="S5" s="102"/>
+      <c r="R5" s="106"/>
+      <c r="S5" s="106"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -3505,26 +3527,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="111" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="118"/>
+      <c r="O6" s="122"/>
+      <c r="P6" s="122"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="102"/>
-      <c r="S6" s="102"/>
+      <c r="R6" s="106"/>
+      <c r="S6" s="106"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -3558,24 +3580,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
+      <c r="B7" s="112"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
+      <c r="I7" s="120"/>
+      <c r="J7" s="120"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="118"/>
-      <c r="P7" s="118"/>
+      <c r="O7" s="122"/>
+      <c r="P7" s="122"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="102"/>
-      <c r="S7" s="102"/>
+      <c r="R7" s="106"/>
+      <c r="S7" s="106"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -3609,24 +3631,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="112"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="115"/>
-      <c r="G8" s="115"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="117"/>
-      <c r="M8" s="117"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="118"/>
-      <c r="P8" s="118"/>
+      <c r="O8" s="122"/>
+      <c r="P8" s="122"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="102"/>
-      <c r="S8" s="102"/>
+      <c r="R8" s="106"/>
+      <c r="S8" s="106"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -3660,24 +3682,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="115"/>
-      <c r="G9" s="115"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="119"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="117"/>
-      <c r="M9" s="117"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="118"/>
-      <c r="P9" s="118"/>
+      <c r="O9" s="122"/>
+      <c r="P9" s="122"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="102"/>
-      <c r="S9" s="102"/>
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -3711,24 +3733,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="115"/>
-      <c r="G10" s="115"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
+      <c r="L10" s="121"/>
+      <c r="M10" s="121"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="118"/>
-      <c r="P10" s="118"/>
+      <c r="O10" s="122"/>
+      <c r="P10" s="122"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="102"/>
-      <c r="S10" s="102"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="106"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -3817,25 +3839,25 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="103" t="s">
+      <c r="F12" s="107" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="103"/>
+      <c r="G12" s="107"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="104" t="s">
+      <c r="I12" s="108" t="s">
         <v>173</v>
       </c>
-      <c r="J12" s="104"/>
+      <c r="J12" s="108"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="105" t="s">
+      <c r="L12" s="109" t="s">
         <v>174</v>
       </c>
-      <c r="M12" s="105"/>
+      <c r="M12" s="109"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="109" t="s">
+      <c r="O12" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="P12" s="110"/>
+      <c r="P12" s="114"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -3876,17 +3898,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
+      <c r="I13" s="108"/>
+      <c r="J13" s="108"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="109"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="112"/>
+      <c r="O13" s="115"/>
+      <c r="P13" s="116"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -3927,17 +3949,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="111"/>
-      <c r="P14" s="112"/>
+      <c r="O14" s="115"/>
+      <c r="P14" s="116"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -3978,17 +4000,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="103"/>
-      <c r="G15" s="103"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="107"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="104"/>
-      <c r="J15" s="104"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="108"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="109"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="111"/>
-      <c r="P15" s="112"/>
+      <c r="O15" s="115"/>
+      <c r="P15" s="116"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -4029,17 +4051,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="107"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="104"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="108"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
+      <c r="L16" s="109"/>
+      <c r="M16" s="109"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="111"/>
-      <c r="P16" s="112"/>
+      <c r="O16" s="115"/>
+      <c r="P16" s="116"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -4080,17 +4102,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="104"/>
-      <c r="J17" s="104"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="108"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="105"/>
+      <c r="L17" s="109"/>
+      <c r="M17" s="109"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="111"/>
-      <c r="P17" s="112"/>
+      <c r="O17" s="115"/>
+      <c r="P17" s="116"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -4131,17 +4153,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
+      <c r="F18" s="107"/>
+      <c r="G18" s="107"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="104"/>
-      <c r="J18" s="104"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="108"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="111"/>
-      <c r="P18" s="112"/>
+      <c r="O18" s="115"/>
+      <c r="P18" s="116"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -4182,17 +4204,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="103"/>
-      <c r="G19" s="103"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="107"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="104"/>
-      <c r="J19" s="104"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="105"/>
-      <c r="M19" s="105"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="111"/>
-      <c r="P19" s="112"/>
+      <c r="O19" s="115"/>
+      <c r="P19" s="116"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -4233,17 +4255,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="107"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="104"/>
-      <c r="J20" s="104"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="108"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="105"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="109"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="113"/>
-      <c r="P20" s="114"/>
+      <c r="O20" s="117"/>
+      <c r="P20" s="118"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -16816,7 +16838,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -17156,7 +17178,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121"/>
+      <c r="A2" s="125"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -17482,15 +17504,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="122"/>
-      <c r="DH2" s="122"/>
-      <c r="DI2" s="122"/>
-      <c r="DJ2" s="122"/>
+      <c r="DG2" s="126"/>
+      <c r="DH2" s="126"/>
+      <c r="DI2" s="126"/>
+      <c r="DJ2" s="126"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="121"/>
+      <c r="A3" s="125"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -17827,7 +17849,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="127" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -17969,7 +17991,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -18109,7 +18131,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -18249,7 +18271,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="123"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -18387,7 +18409,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="123"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -18527,7 +18549,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="128" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -18669,7 +18691,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="124"/>
+      <c r="B10" s="128"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -18809,7 +18831,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="129" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -18939,7 +18961,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="125"/>
+      <c r="B12" s="129"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -19077,7 +19099,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="125"/>
+      <c r="B13" s="129"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -19217,7 +19239,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="125"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -19353,7 +19375,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="125"/>
+      <c r="B15" s="129"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -19489,7 +19511,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="125"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -19625,7 +19647,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="125"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -19761,7 +19783,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="129"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -19901,7 +19923,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="125"/>
+      <c r="B19" s="129"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -20037,7 +20059,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="125"/>
+      <c r="B20" s="129"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -20173,7 +20195,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="123" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -20307,7 +20329,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="119"/>
+      <c r="B22" s="123"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -20443,7 +20465,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="119"/>
+      <c r="B23" s="123"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -20575,7 +20597,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="119"/>
+      <c r="B24" s="123"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -20709,7 +20731,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="119"/>
+      <c r="B25" s="123"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -20853,7 +20875,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="120" t="s">
+      <c r="B26" s="124" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -20987,7 +21009,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="120"/>
+      <c r="B27" s="124"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -21127,7 +21149,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="120"/>
+      <c r="B28" s="124"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -21259,7 +21281,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="120"/>
+      <c r="B29" s="124"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -21387,7 +21409,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="120"/>
+      <c r="B30" s="124"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -21513,7 +21535,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="120"/>
+      <c r="B31" s="124"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 19 e 20-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A10EFCF-B176-43B7-B2DE-EE4A4BA0F24A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0996EC9B-4B90-4057-84F5-EFD529F412C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="236">
   <si>
     <t>REDES</t>
   </si>
@@ -796,6 +796,30 @@
   </si>
   <si>
     <t>Planning da sprint, distribuição de tarefas, store points, wireframe administrador</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da arquitetura do software, organização DevOps, agendamento reunião com o cliente para 20-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layout de alta fidelidade tela login e últimos relatórios, </t>
+  </si>
+  <si>
+    <t>Dashboard lista de agendas encerradas, navbar, página cadastro, finalização JSON false</t>
+  </si>
+  <si>
+    <t>Configuração do ambiente web, criação guideline, diagrama de classes, modelagem do banco de dados, estudo gremlin</t>
+  </si>
+  <si>
+    <t>Entrega modelagem banco de dados, diagrama de classes, trello, DevOps, baixa fidelidade, configuração rotas web, guideline, estudo CRUD gremlin, estudo integração da api com o gremlin</t>
+  </si>
+  <si>
+    <t>Tela de cadastro, lista de jornadas com validação, estudo drag and drop, navbar, alterações banco de dados</t>
+  </si>
+  <si>
+    <t>Layout de alta fidelidade últimos relatórios, testes integração API com Zabbix</t>
+  </si>
+  <si>
+    <t>Integração da API com gLPI Login, lista de chamados web, tela lista e edição de usuários web</t>
   </si>
 </sst>
 </file>
@@ -1566,18 +1590,6 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1586,6 +1598,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1733,6 +1757,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFF9F9F9"/>
+      <color rgb="FFDCDCDC"/>
       <color rgb="FF9B54D0"/>
       <color rgb="FFCB3D3D"/>
       <color rgb="FFFFD966"/>
@@ -2056,7 +2082,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AD7" sqref="AD7"/>
+      <selection pane="bottomRight" activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2073,7 +2099,9 @@
     <col min="26" max="27" width="25.77734375" customWidth="1"/>
     <col min="28" max="28" width="20.77734375" customWidth="1"/>
     <col min="29" max="29" width="25.77734375" customWidth="1"/>
-    <col min="30" max="37" width="20.77734375" customWidth="1"/>
+    <col min="30" max="30" width="20.77734375" customWidth="1"/>
+    <col min="31" max="31" width="30.77734375" customWidth="1"/>
+    <col min="32" max="37" width="20.77734375" customWidth="1"/>
     <col min="38" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -2087,7 +2115,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2367,7 +2395,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2477,7 +2505,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="105"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2765,10 +2793,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2850,8 +2878,12 @@
       <c r="AC4" s="95" t="s">
         <v>224</v>
       </c>
-      <c r="AD4" s="95"/>
-      <c r="AE4" s="95"/>
+      <c r="AD4" s="95" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE4" s="95" t="s">
+        <v>235</v>
+      </c>
       <c r="AF4" s="95"/>
       <c r="AG4" s="95"/>
       <c r="AH4" s="95"/>
@@ -2868,27 +2900,27 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="101" t="s">
+      <c r="AV4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="101" t="s">
+      <c r="AW4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="101" t="s">
+      <c r="BT4" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="101" t="s">
+      <c r="BW4" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="101" t="s">
+      <c r="CO4" s="103" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -2968,8 +3000,12 @@
       <c r="AC5" s="95" t="s">
         <v>225</v>
       </c>
-      <c r="AD5" s="95"/>
-      <c r="AE5" s="95"/>
+      <c r="AD5" s="95" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE5" s="95" t="s">
+        <v>234</v>
+      </c>
       <c r="AF5" s="95"/>
       <c r="AG5" s="95"/>
       <c r="AH5" s="95"/>
@@ -2986,17 +3022,17 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="BT5" s="101"/>
-      <c r="BW5" s="101"/>
-      <c r="CO5" s="101"/>
+      <c r="AV5" s="103"/>
+      <c r="AW5" s="103"/>
+      <c r="BT5" s="103"/>
+      <c r="BW5" s="103"/>
+      <c r="CO5" s="103"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3078,8 +3114,12 @@
       <c r="AC6" s="95" t="s">
         <v>226</v>
       </c>
-      <c r="AD6" s="95"/>
-      <c r="AE6" s="95"/>
+      <c r="AD6" s="95" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE6" s="95" t="s">
+        <v>233</v>
+      </c>
       <c r="AF6" s="95"/>
       <c r="AG6" s="95"/>
       <c r="AH6" s="95"/>
@@ -3096,17 +3136,17 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="BT6" s="101"/>
-      <c r="BW6" s="101"/>
-      <c r="CO6" s="101"/>
+      <c r="AV6" s="103"/>
+      <c r="AW6" s="103"/>
+      <c r="BT6" s="103"/>
+      <c r="BW6" s="103"/>
+      <c r="CO6" s="103"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3188,8 +3228,12 @@
       <c r="AC7" s="95" t="s">
         <v>227</v>
       </c>
-      <c r="AD7" s="95"/>
-      <c r="AE7" s="95"/>
+      <c r="AD7" s="95" t="s">
+        <v>231</v>
+      </c>
+      <c r="AE7" s="95" t="s">
+        <v>232</v>
+      </c>
       <c r="AF7" s="95"/>
       <c r="AG7" s="95"/>
       <c r="AH7" s="95"/>
@@ -3206,29 +3250,29 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="101"/>
-      <c r="AW7" s="101"/>
-      <c r="BT7" s="101"/>
-      <c r="BW7" s="101"/>
-      <c r="CO7" s="101"/>
+      <c r="AV7" s="103"/>
+      <c r="AW7" s="103"/>
+      <c r="BT7" s="103"/>
+      <c r="BW7" s="103"/>
+      <c r="CO7" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 23-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0996EC9B-4B90-4057-84F5-EFD529F412C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -27,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="240">
   <si>
     <t>REDES</t>
   </si>
@@ -798,9 +797,6 @@
     <t>Planning da sprint, distribuição de tarefas, store points, wireframe administrador</t>
   </si>
   <si>
-    <t>Desenvolvimento da arquitetura do software, organização DevOps, agendamento reunião com o cliente para 20-09</t>
-  </si>
-  <si>
     <t xml:space="preserve">Layout de alta fidelidade tela login e últimos relatórios, </t>
   </si>
   <si>
@@ -820,12 +816,27 @@
   </si>
   <si>
     <t>Integração da API com gLPI Login, lista de chamados web, tela lista e edição de usuários web</t>
+  </si>
+  <si>
+    <t>Cadastro de usuário via GLPi API, retornar token no Login API, página web editar usuário, lista de chamados web</t>
+  </si>
+  <si>
+    <t>Layout alta fidelidade home, documentação modelagem banco de dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correção métodos de listagem, dashboard, estudo drag and drop, navbar e merge com telas de cadastro com navbar </t>
+  </si>
+  <si>
+    <t>Estudo gremlin local, domain e métodos na interface e repositório do bloco, guideline</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da arquitetura do software, organização DevOps, agendamento reunião com o cliente para 27-09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1590,6 +1601,18 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1598,18 +1621,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2075,14 +2086,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AE5" sqref="AE5"/>
+      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2115,7 +2126,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="103" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2395,7 +2406,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="104"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2505,7 +2516,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="105"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2793,10 +2804,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="105"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2879,12 +2890,14 @@
         <v>224</v>
       </c>
       <c r="AD4" s="95" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="AE4" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF4" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="AF4" s="95"/>
       <c r="AG4" s="95"/>
       <c r="AH4" s="95"/>
       <c r="AI4" s="95"/>
@@ -2900,27 +2913,27 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="103" t="s">
+      <c r="AV4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="103" t="s">
+      <c r="AW4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="103" t="s">
+      <c r="BT4" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="103" t="s">
+      <c r="BW4" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="103" t="s">
+      <c r="CO4" s="101" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="105"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3001,12 +3014,14 @@
         <v>225</v>
       </c>
       <c r="AD5" s="95" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AE5" s="95" t="s">
-        <v>234</v>
-      </c>
-      <c r="AF5" s="95"/>
+        <v>233</v>
+      </c>
+      <c r="AF5" s="95" t="s">
+        <v>236</v>
+      </c>
       <c r="AG5" s="95"/>
       <c r="AH5" s="95"/>
       <c r="AI5" s="95"/>
@@ -3022,17 +3037,17 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="103"/>
-      <c r="AW5" s="103"/>
-      <c r="BT5" s="103"/>
-      <c r="BW5" s="103"/>
-      <c r="CO5" s="103"/>
+      <c r="AV5" s="101"/>
+      <c r="AW5" s="101"/>
+      <c r="BT5" s="101"/>
+      <c r="BW5" s="101"/>
+      <c r="CO5" s="101"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3115,12 +3130,14 @@
         <v>226</v>
       </c>
       <c r="AD6" s="95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AE6" s="95" t="s">
-        <v>233</v>
-      </c>
-      <c r="AF6" s="95"/>
+        <v>232</v>
+      </c>
+      <c r="AF6" s="95" t="s">
+        <v>237</v>
+      </c>
       <c r="AG6" s="95"/>
       <c r="AH6" s="95"/>
       <c r="AI6" s="95"/>
@@ -3136,17 +3153,17 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="103"/>
-      <c r="AW6" s="103"/>
-      <c r="BT6" s="103"/>
-      <c r="BW6" s="103"/>
-      <c r="CO6" s="103"/>
+      <c r="AV6" s="101"/>
+      <c r="AW6" s="101"/>
+      <c r="BT6" s="101"/>
+      <c r="BW6" s="101"/>
+      <c r="CO6" s="101"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3229,12 +3246,14 @@
         <v>227</v>
       </c>
       <c r="AD7" s="95" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE7" s="95" t="s">
         <v>231</v>
       </c>
-      <c r="AE7" s="95" t="s">
-        <v>232</v>
-      </c>
-      <c r="AF7" s="95"/>
+      <c r="AF7" s="95" t="s">
+        <v>238</v>
+      </c>
       <c r="AG7" s="95"/>
       <c r="AH7" s="95"/>
       <c r="AI7" s="95"/>
@@ -3250,29 +3269,29 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="103"/>
-      <c r="AW7" s="103"/>
-      <c r="BT7" s="103"/>
-      <c r="BW7" s="103"/>
-      <c r="CO7" s="103"/>
+      <c r="AV7" s="101"/>
+      <c r="AW7" s="101"/>
+      <c r="BT7" s="101"/>
+      <c r="BW7" s="101"/>
+      <c r="CO7" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3281,7 +3300,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16860,7 +16879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona daily realizada em 24-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="244">
   <si>
     <t>REDES</t>
   </si>
@@ -831,6 +831,18 @@
   </si>
   <si>
     <t>Desenvolvimento da arquitetura do software, organização DevOps, agendamento reunião com o cliente para 27-09</t>
+  </si>
+  <si>
+    <t>Continuidade Login API com GLPi, criação de submenu web, editar usuário mobile, modal com informações na tela Login mobile, listar usuários mobile</t>
+  </si>
+  <si>
+    <t>Fluxo de funcionalidade e layout alta fidelidade home, tela Login web</t>
+  </si>
+  <si>
+    <t>Correção dos selects da dashboard e finalização navbar</t>
+  </si>
+  <si>
+    <t>Conexão API com gremlin, finalização guideline, mockagem de dados no banco, repositório genérico</t>
   </si>
 </sst>
 </file>
@@ -1601,18 +1613,6 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1621,6 +1621,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2090,10 +2102,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2112,7 +2124,9 @@
     <col min="29" max="29" width="25.77734375" customWidth="1"/>
     <col min="30" max="30" width="20.77734375" customWidth="1"/>
     <col min="31" max="31" width="30.77734375" customWidth="1"/>
-    <col min="32" max="37" width="20.77734375" customWidth="1"/>
+    <col min="32" max="32" width="20.77734375" customWidth="1"/>
+    <col min="33" max="33" width="25.77734375" customWidth="1"/>
+    <col min="34" max="37" width="20.77734375" customWidth="1"/>
     <col min="38" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -2126,7 +2140,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2406,7 +2420,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2516,7 +2530,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="105"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2804,10 +2818,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2898,7 +2912,9 @@
       <c r="AF4" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="AG4" s="95"/>
+      <c r="AG4" s="95" t="s">
+        <v>240</v>
+      </c>
       <c r="AH4" s="95"/>
       <c r="AI4" s="95"/>
       <c r="AJ4" s="95"/>
@@ -2913,27 +2929,27 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="101" t="s">
+      <c r="AV4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="101" t="s">
+      <c r="AW4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="101" t="s">
+      <c r="BT4" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="101" t="s">
+      <c r="BW4" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="101" t="s">
+      <c r="CO4" s="103" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3022,7 +3038,9 @@
       <c r="AF5" s="95" t="s">
         <v>236</v>
       </c>
-      <c r="AG5" s="95"/>
+      <c r="AG5" s="95" t="s">
+        <v>241</v>
+      </c>
       <c r="AH5" s="95"/>
       <c r="AI5" s="95"/>
       <c r="AJ5" s="95"/>
@@ -3037,17 +3055,17 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="BT5" s="101"/>
-      <c r="BW5" s="101"/>
-      <c r="CO5" s="101"/>
+      <c r="AV5" s="103"/>
+      <c r="AW5" s="103"/>
+      <c r="BT5" s="103"/>
+      <c r="BW5" s="103"/>
+      <c r="CO5" s="103"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3138,7 +3156,9 @@
       <c r="AF6" s="95" t="s">
         <v>237</v>
       </c>
-      <c r="AG6" s="95"/>
+      <c r="AG6" s="95" t="s">
+        <v>242</v>
+      </c>
       <c r="AH6" s="95"/>
       <c r="AI6" s="95"/>
       <c r="AJ6" s="95"/>
@@ -3153,17 +3173,17 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="BT6" s="101"/>
-      <c r="BW6" s="101"/>
-      <c r="CO6" s="101"/>
+      <c r="AV6" s="103"/>
+      <c r="AW6" s="103"/>
+      <c r="BT6" s="103"/>
+      <c r="BW6" s="103"/>
+      <c r="CO6" s="103"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3254,7 +3274,9 @@
       <c r="AF7" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="AG7" s="95"/>
+      <c r="AG7" s="95" t="s">
+        <v>243</v>
+      </c>
       <c r="AH7" s="95"/>
       <c r="AI7" s="95"/>
       <c r="AJ7" s="95"/>
@@ -3269,29 +3291,29 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="101"/>
-      <c r="AW7" s="101"/>
-      <c r="BT7" s="101"/>
-      <c r="BW7" s="101"/>
-      <c r="CO7" s="101"/>
+      <c r="AV7" s="103"/>
+      <c r="AW7" s="103"/>
+      <c r="BT7" s="103"/>
+      <c r="BW7" s="103"/>
+      <c r="CO7" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 25 e 26-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A516C0B5-B9AE-457C-8DD7-7D35BFFFAA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="252">
   <si>
     <t>REDES</t>
   </si>
@@ -843,12 +844,36 @@
   </si>
   <si>
     <t>Conexão API com gremlin, finalização guideline, mockagem de dados no banco, repositório genérico</t>
+  </si>
+  <si>
+    <t>Finalizou Login API GLPi, listar Chamados API, estudo httpclient, cadastro Chamados API, editar usuário mobile</t>
+  </si>
+  <si>
+    <t>Integração API com Zabbix, layout de alta fidelidade Login</t>
+  </si>
+  <si>
+    <t>Estudo drag and drop, construção modais justificativa, dashboard, função sair na navbar, listagens para select no componente de cadastro</t>
+  </si>
+  <si>
+    <t>Listar dados do cosmos usando API gremlin e componentes da página blocos</t>
+  </si>
+  <si>
+    <t>Conexão API com gremlin, estudo comandos básicos gremlin, layout alta fidelidade criação e listagem de bloco e HTML e CSS dessas páginas</t>
+  </si>
+  <si>
+    <t>Listar chamados e usuários, Cadastro de chamados e usuários, Cadastro de usuário e de chamado, fluxo de telas mobile</t>
+  </si>
+  <si>
+    <t>Página Login, layout de alta fidelidade login, home e empresas, métodos de Login e listar HostGroup</t>
+  </si>
+  <si>
+    <t>Componente de cadastro, finalização navbar, redirecionamento página não encontrada, lista de agendas componentizadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1613,6 +1638,18 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1621,18 +1658,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2098,14 +2123,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AK4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AH6" sqref="AH6"/>
+      <selection pane="bottomRight" activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2125,8 +2150,8 @@
     <col min="30" max="30" width="20.77734375" customWidth="1"/>
     <col min="31" max="31" width="30.77734375" customWidth="1"/>
     <col min="32" max="32" width="20.77734375" customWidth="1"/>
-    <col min="33" max="33" width="25.77734375" customWidth="1"/>
-    <col min="34" max="37" width="20.77734375" customWidth="1"/>
+    <col min="33" max="35" width="25.77734375" customWidth="1"/>
+    <col min="36" max="37" width="20.77734375" customWidth="1"/>
     <col min="38" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -2140,7 +2165,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="103" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2420,7 +2445,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="104"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2530,7 +2555,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="105"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2818,10 +2843,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="105"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2915,8 +2940,12 @@
       <c r="AG4" s="95" t="s">
         <v>240</v>
       </c>
-      <c r="AH4" s="95"/>
-      <c r="AI4" s="95"/>
+      <c r="AH4" s="95" t="s">
+        <v>244</v>
+      </c>
+      <c r="AI4" s="95" t="s">
+        <v>249</v>
+      </c>
       <c r="AJ4" s="95"/>
       <c r="AK4" s="95"/>
       <c r="AL4" s="96"/>
@@ -2929,27 +2958,27 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="103" t="s">
+      <c r="AV4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="103" t="s">
+      <c r="AW4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="103" t="s">
+      <c r="BT4" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="103" t="s">
+      <c r="BW4" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="103" t="s">
+      <c r="CO4" s="101" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="105"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3041,8 +3070,12 @@
       <c r="AG5" s="95" t="s">
         <v>241</v>
       </c>
-      <c r="AH5" s="95"/>
-      <c r="AI5" s="95"/>
+      <c r="AH5" s="95" t="s">
+        <v>245</v>
+      </c>
+      <c r="AI5" s="95" t="s">
+        <v>250</v>
+      </c>
       <c r="AJ5" s="95"/>
       <c r="AK5" s="95"/>
       <c r="AL5" s="96"/>
@@ -3055,17 +3088,17 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="103"/>
-      <c r="AW5" s="103"/>
-      <c r="BT5" s="103"/>
-      <c r="BW5" s="103"/>
-      <c r="CO5" s="103"/>
+      <c r="AV5" s="101"/>
+      <c r="AW5" s="101"/>
+      <c r="BT5" s="101"/>
+      <c r="BW5" s="101"/>
+      <c r="CO5" s="101"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3159,8 +3192,12 @@
       <c r="AG6" s="95" t="s">
         <v>242</v>
       </c>
-      <c r="AH6" s="95"/>
-      <c r="AI6" s="95"/>
+      <c r="AH6" s="95" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI6" s="95" t="s">
+        <v>251</v>
+      </c>
       <c r="AJ6" s="95"/>
       <c r="AK6" s="95"/>
       <c r="AL6" s="96"/>
@@ -3173,17 +3210,17 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="103"/>
-      <c r="AW6" s="103"/>
-      <c r="BT6" s="103"/>
-      <c r="BW6" s="103"/>
-      <c r="CO6" s="103"/>
+      <c r="AV6" s="101"/>
+      <c r="AW6" s="101"/>
+      <c r="BT6" s="101"/>
+      <c r="BW6" s="101"/>
+      <c r="CO6" s="101"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3277,8 +3314,12 @@
       <c r="AG7" s="95" t="s">
         <v>243</v>
       </c>
-      <c r="AH7" s="95"/>
-      <c r="AI7" s="95"/>
+      <c r="AH7" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="AI7" s="95" t="s">
+        <v>247</v>
+      </c>
       <c r="AJ7" s="95"/>
       <c r="AK7" s="95"/>
       <c r="AL7" s="96"/>
@@ -3291,29 +3332,29 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="103"/>
-      <c r="AW7" s="103"/>
-      <c r="BT7" s="103"/>
-      <c r="BW7" s="103"/>
-      <c r="CO7" s="103"/>
+      <c r="AV7" s="101"/>
+      <c r="AW7" s="101"/>
+      <c r="BT7" s="101"/>
+      <c r="BW7" s="101"/>
+      <c r="CO7" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3322,7 +3363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16901,7 +16942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona daily realizada em 27-09
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A516C0B5-B9AE-457C-8DD7-7D35BFFFAA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -27,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="256">
   <si>
     <t>REDES</t>
   </si>
@@ -868,12 +867,24 @@
   </si>
   <si>
     <t>Componente de cadastro, finalização navbar, redirecionamento página não encontrada, lista de agendas componentizadas</t>
+  </si>
+  <si>
+    <t>Integração API com GLPi finalizando listar e cadastrar usuários, listar e cadastrar chamados e Login, listar chamados Web, ajustes gerais mobile</t>
+  </si>
+  <si>
+    <t>Wireframe e alta fidelidade da página de relatórios, reunião com a equipe de redes, html e css login e layout de alta fidelidade página empresas</t>
+  </si>
+  <si>
+    <t>Componente card dashboard, construção modais, cadastro jornada e clientes, máscaras de inputs, refatoração código Front</t>
+  </si>
+  <si>
+    <t>Html e css página lista de blocos e cadastro de blocos, listar, lisitar por id e cadastro de blocos API gremlin, documentação API</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1638,18 +1649,6 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1658,6 +1657,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2123,14 +2134,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AK4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AJ7" sqref="AJ7"/>
+      <selection pane="bottomRight" activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2150,8 +2161,8 @@
     <col min="30" max="30" width="20.77734375" customWidth="1"/>
     <col min="31" max="31" width="30.77734375" customWidth="1"/>
     <col min="32" max="32" width="20.77734375" customWidth="1"/>
-    <col min="33" max="35" width="25.77734375" customWidth="1"/>
-    <col min="36" max="37" width="20.77734375" customWidth="1"/>
+    <col min="33" max="36" width="25.77734375" customWidth="1"/>
+    <col min="37" max="37" width="20.77734375" customWidth="1"/>
     <col min="38" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
@@ -2165,7 +2176,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2445,7 +2456,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2555,7 +2566,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="105"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2843,10 +2854,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2946,7 +2957,9 @@
       <c r="AI4" s="95" t="s">
         <v>249</v>
       </c>
-      <c r="AJ4" s="95"/>
+      <c r="AJ4" s="95" t="s">
+        <v>252</v>
+      </c>
       <c r="AK4" s="95"/>
       <c r="AL4" s="96"/>
       <c r="AM4" s="96"/>
@@ -2958,27 +2971,27 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="101" t="s">
+      <c r="AV4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="101" t="s">
+      <c r="AW4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="101" t="s">
+      <c r="BT4" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="101" t="s">
+      <c r="BW4" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="101" t="s">
+      <c r="CO4" s="103" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3076,7 +3089,9 @@
       <c r="AI5" s="95" t="s">
         <v>250</v>
       </c>
-      <c r="AJ5" s="95"/>
+      <c r="AJ5" s="95" t="s">
+        <v>253</v>
+      </c>
       <c r="AK5" s="95"/>
       <c r="AL5" s="96"/>
       <c r="AM5" s="96"/>
@@ -3088,17 +3103,17 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="BT5" s="101"/>
-      <c r="BW5" s="101"/>
-      <c r="CO5" s="101"/>
+      <c r="AV5" s="103"/>
+      <c r="AW5" s="103"/>
+      <c r="BT5" s="103"/>
+      <c r="BW5" s="103"/>
+      <c r="CO5" s="103"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3198,7 +3213,9 @@
       <c r="AI6" s="95" t="s">
         <v>251</v>
       </c>
-      <c r="AJ6" s="95"/>
+      <c r="AJ6" s="95" t="s">
+        <v>254</v>
+      </c>
       <c r="AK6" s="95"/>
       <c r="AL6" s="96"/>
       <c r="AM6" s="96"/>
@@ -3210,17 +3227,17 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="BT6" s="101"/>
-      <c r="BW6" s="101"/>
-      <c r="CO6" s="101"/>
+      <c r="AV6" s="103"/>
+      <c r="AW6" s="103"/>
+      <c r="BT6" s="103"/>
+      <c r="BW6" s="103"/>
+      <c r="CO6" s="103"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3320,7 +3337,9 @@
       <c r="AI7" s="95" t="s">
         <v>247</v>
       </c>
-      <c r="AJ7" s="95"/>
+      <c r="AJ7" s="95" t="s">
+        <v>255</v>
+      </c>
       <c r="AK7" s="95"/>
       <c r="AL7" s="96"/>
       <c r="AM7" s="96"/>
@@ -3332,29 +3351,29 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="101"/>
-      <c r="AW7" s="101"/>
-      <c r="BT7" s="101"/>
-      <c r="BW7" s="101"/>
-      <c r="CO7" s="101"/>
+      <c r="AV7" s="103"/>
+      <c r="AW7" s="103"/>
+      <c r="BT7" s="103"/>
+      <c r="BW7" s="103"/>
+      <c r="CO7" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3363,7 +3382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16942,7 +16961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 30-09 e 01-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="261">
   <si>
     <t>REDES</t>
   </si>
@@ -879,6 +879,21 @@
   </si>
   <si>
     <t>Html e css página lista de blocos e cadastro de blocos, listar, lisitar por id e cadastro de blocos API gremlin, documentação API</t>
+  </si>
+  <si>
+    <t>Ajustes no código para reunião com o cliente</t>
+  </si>
+  <si>
+    <t>Wireframe e alta fidelidade da página de relatórios, preparação da apresentação, página Login</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente, ajustes nos modais e demais páginas</t>
+  </si>
+  <si>
+    <t>Finalização CRUD do bloco, estilização página listagem de blocos e cadastro de blocos.</t>
+  </si>
+  <si>
+    <t>Reunião com a coordenação da escola para esclarecer o andamento dos projetos.</t>
   </si>
 </sst>
 </file>
@@ -1649,6 +1664,18 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1657,18 +1684,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2141,7 +2156,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AK7" sqref="AK7"/>
+      <selection pane="bottomRight" activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2176,7 +2191,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="103" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2456,7 +2471,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="104"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2566,7 +2581,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="105"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2854,10 +2869,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="105"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2960,8 +2975,12 @@
       <c r="AJ4" s="95" t="s">
         <v>252</v>
       </c>
-      <c r="AK4" s="95"/>
-      <c r="AL4" s="96"/>
+      <c r="AK4" s="95" t="s">
+        <v>256</v>
+      </c>
+      <c r="AL4" s="96" t="s">
+        <v>260</v>
+      </c>
       <c r="AM4" s="96"/>
       <c r="AN4" s="96"/>
       <c r="AO4" s="96"/>
@@ -2971,27 +2990,27 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="103" t="s">
+      <c r="AV4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="103" t="s">
+      <c r="AW4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="103" t="s">
+      <c r="BT4" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="103" t="s">
+      <c r="BW4" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="103" t="s">
+      <c r="CO4" s="101" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="105"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3092,8 +3111,12 @@
       <c r="AJ5" s="95" t="s">
         <v>253</v>
       </c>
-      <c r="AK5" s="95"/>
-      <c r="AL5" s="96"/>
+      <c r="AK5" s="95" t="s">
+        <v>257</v>
+      </c>
+      <c r="AL5" s="96" t="s">
+        <v>260</v>
+      </c>
       <c r="AM5" s="96"/>
       <c r="AN5" s="96"/>
       <c r="AO5" s="96"/>
@@ -3103,17 +3126,17 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="103"/>
-      <c r="AW5" s="103"/>
-      <c r="BT5" s="103"/>
-      <c r="BW5" s="103"/>
-      <c r="CO5" s="103"/>
+      <c r="AV5" s="101"/>
+      <c r="AW5" s="101"/>
+      <c r="BT5" s="101"/>
+      <c r="BW5" s="101"/>
+      <c r="CO5" s="101"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3216,8 +3239,12 @@
       <c r="AJ6" s="95" t="s">
         <v>254</v>
       </c>
-      <c r="AK6" s="95"/>
-      <c r="AL6" s="96"/>
+      <c r="AK6" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="AL6" s="96" t="s">
+        <v>260</v>
+      </c>
       <c r="AM6" s="96"/>
       <c r="AN6" s="96"/>
       <c r="AO6" s="96"/>
@@ -3227,17 +3254,17 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="103"/>
-      <c r="AW6" s="103"/>
-      <c r="BT6" s="103"/>
-      <c r="BW6" s="103"/>
-      <c r="CO6" s="103"/>
+      <c r="AV6" s="101"/>
+      <c r="AW6" s="101"/>
+      <c r="BT6" s="101"/>
+      <c r="BW6" s="101"/>
+      <c r="CO6" s="101"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3340,8 +3367,12 @@
       <c r="AJ7" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="AK7" s="95"/>
-      <c r="AL7" s="96"/>
+      <c r="AK7" s="95" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL7" s="96" t="s">
+        <v>260</v>
+      </c>
       <c r="AM7" s="96"/>
       <c r="AN7" s="96"/>
       <c r="AO7" s="96"/>
@@ -3351,29 +3382,29 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="103"/>
-      <c r="AW7" s="103"/>
-      <c r="BT7" s="103"/>
-      <c r="BW7" s="103"/>
-      <c r="CO7" s="103"/>
+      <c r="AV7" s="101"/>
+      <c r="AW7" s="101"/>
+      <c r="BT7" s="101"/>
+      <c r="BW7" s="101"/>
+      <c r="CO7" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Altera duracao das sprints
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="260">
   <si>
     <t>REDES</t>
   </si>
@@ -635,9 +635,6 @@
   </si>
   <si>
     <t>SPRINT 8</t>
-  </si>
-  <si>
-    <t>SPRINT 9</t>
   </si>
   <si>
     <t>Funcionalidades (Login e Cadastro) no Front-End Web e Mobile, fazendo a chamada para a API</t>
@@ -1040,7 +1037,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1263,8 +1260,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2F75B5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF8F00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1352,49 +1367,61 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
+        <color rgb="FFF9F9F9"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FFF9F9F9"/>
+      </right>
       <top style="thin">
-        <color theme="0"/>
+        <color rgb="FFF9F9F9"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFF9F9F9"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="0"/>
+        <color rgb="FFF9F9F9"/>
       </right>
       <top style="thin">
-        <color theme="0"/>
+        <color rgb="FFF9F9F9"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFF9F9F9"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
+        <color rgb="FFF9F9F9"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFF9F9F9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF9F9F9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFF9F9F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF9F9F9"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="0"/>
+        <color rgb="FFF9F9F9"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color theme="0"/>
@@ -1404,9 +1431,46 @@
     <border>
       <left/>
       <right style="thin">
+        <color rgb="FFF9F9F9"/>
+      </right>
+      <top style="thin">
         <color theme="0"/>
-      </right>
-      <top/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFF9F9F9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFF9F9F9"/>
+      </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
@@ -1416,7 +1480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1664,18 +1728,6 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1684,6 +1736,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1704,24 +1768,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1756,6 +1802,66 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1831,15 +1937,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFBF8F00"/>
+      <color rgb="FF2F75B5"/>
+      <color rgb="FF9B54D0"/>
+      <color rgb="FF548235"/>
       <color rgb="FFF9F9F9"/>
+      <color rgb="FFCB3D3D"/>
       <color rgb="FFDCDCDC"/>
-      <color rgb="FF9B54D0"/>
-      <color rgb="FFCB3D3D"/>
       <color rgb="FFFFD966"/>
       <color rgb="FF5B2484"/>
       <color rgb="FF7C7C7C"/>
-      <color rgb="FF548235"/>
-      <color rgb="FFB47EDC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2153,10 +2260,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AK4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AM4" sqref="AM4"/>
+      <selection pane="bottomRight" activeCell="CL6" sqref="CL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2191,7 +2298,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2471,7 +2578,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2581,7 +2688,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="105"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2729,136 +2836,136 @@
       <c r="AX3" s="87">
         <v>16</v>
       </c>
-      <c r="AY3" s="87">
+      <c r="AY3" s="126">
         <v>17</v>
       </c>
-      <c r="AZ3" s="87">
+      <c r="AZ3" s="130">
         <v>18</v>
       </c>
-      <c r="BA3" s="87">
+      <c r="BA3" s="130">
         <v>21</v>
       </c>
-      <c r="BB3" s="87">
+      <c r="BB3" s="126">
         <v>22</v>
       </c>
-      <c r="BC3" s="87">
+      <c r="BC3" s="126">
         <v>23</v>
       </c>
-      <c r="BD3" s="87">
+      <c r="BD3" s="126">
         <v>24</v>
       </c>
-      <c r="BE3" s="87">
+      <c r="BE3" s="130">
         <v>25</v>
       </c>
-      <c r="BF3" s="87">
+      <c r="BF3" s="130">
         <v>28</v>
       </c>
-      <c r="BG3" s="87">
+      <c r="BG3" s="126">
         <v>29</v>
       </c>
-      <c r="BH3" s="87">
+      <c r="BH3" s="126">
         <v>30</v>
       </c>
-      <c r="BI3" s="87">
+      <c r="BI3" s="126">
         <v>31</v>
       </c>
-      <c r="BJ3" s="87">
+      <c r="BJ3" s="130">
         <v>1</v>
       </c>
-      <c r="BK3" s="87">
+      <c r="BK3" s="130">
         <v>4</v>
       </c>
-      <c r="BL3" s="87">
+      <c r="BL3" s="126">
         <v>5</v>
       </c>
-      <c r="BM3" s="87">
+      <c r="BM3" s="126">
         <v>6</v>
       </c>
-      <c r="BN3" s="87">
+      <c r="BN3" s="126">
         <v>7</v>
       </c>
-      <c r="BO3" s="87">
+      <c r="BO3" s="130">
         <v>8</v>
       </c>
-      <c r="BP3" s="87">
+      <c r="BP3" s="130">
         <v>11</v>
       </c>
-      <c r="BQ3" s="87">
+      <c r="BQ3" s="126">
         <v>12</v>
       </c>
-      <c r="BR3" s="87">
+      <c r="BR3" s="126">
         <v>13</v>
       </c>
-      <c r="BS3" s="87">
+      <c r="BS3" s="126">
         <v>14</v>
       </c>
       <c r="BT3" s="83">
         <v>15</v>
       </c>
-      <c r="BU3" s="87">
+      <c r="BU3" s="130">
         <v>18</v>
       </c>
-      <c r="BV3" s="87">
+      <c r="BV3" s="126">
         <v>19</v>
       </c>
       <c r="BW3" s="83">
         <v>20</v>
       </c>
-      <c r="BX3" s="87">
+      <c r="BX3" s="126">
         <v>21</v>
       </c>
-      <c r="BY3" s="87">
+      <c r="BY3" s="130">
         <v>22</v>
       </c>
-      <c r="BZ3" s="87">
+      <c r="BZ3" s="130">
         <v>25</v>
       </c>
-      <c r="CA3" s="87">
+      <c r="CA3" s="126">
         <v>26</v>
       </c>
-      <c r="CB3" s="87">
+      <c r="CB3" s="126">
         <v>27</v>
       </c>
-      <c r="CC3" s="87">
+      <c r="CC3" s="126">
         <v>28</v>
       </c>
-      <c r="CD3" s="87">
+      <c r="CD3" s="130">
         <v>29</v>
       </c>
-      <c r="CE3" s="87">
+      <c r="CE3" s="130">
         <v>2</v>
       </c>
-      <c r="CF3" s="87">
+      <c r="CF3" s="126">
         <v>3</v>
       </c>
-      <c r="CG3" s="87">
+      <c r="CG3" s="126">
         <v>4</v>
       </c>
-      <c r="CH3" s="87">
+      <c r="CH3" s="126">
         <v>5</v>
       </c>
-      <c r="CI3" s="87">
+      <c r="CI3" s="130">
         <v>6</v>
       </c>
-      <c r="CJ3" s="87">
+      <c r="CJ3" s="130">
         <v>9</v>
       </c>
-      <c r="CK3" s="87">
+      <c r="CK3" s="126">
         <v>10</v>
       </c>
-      <c r="CL3" s="87">
+      <c r="CL3" s="126">
         <v>11</v>
       </c>
-      <c r="CM3" s="87">
+      <c r="CM3" s="126">
         <v>12</v>
       </c>
-      <c r="CN3" s="87">
+      <c r="CN3" s="130">
         <v>13</v>
       </c>
       <c r="CO3" s="83">
         <v>14</v>
       </c>
-      <c r="CP3" s="85">
+      <c r="CP3" s="131">
         <v>16</v>
       </c>
       <c r="CQ3" s="85">
@@ -2869,10 +2976,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -2913,73 +3020,73 @@
         <v>161</v>
       </c>
       <c r="P4" s="93" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q4" s="93" t="s">
+        <v>178</v>
+      </c>
+      <c r="R4" s="94" t="s">
         <v>179</v>
       </c>
-      <c r="R4" s="94" t="s">
-        <v>180</v>
-      </c>
       <c r="S4" s="94" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T4" s="94" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U4" s="94" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="V4" s="94" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="W4" s="94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X4" s="94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Y4" s="94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z4" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AA4" s="94" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB4" s="95" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AC4" s="95" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AD4" s="95" t="s">
+        <v>238</v>
+      </c>
+      <c r="AE4" s="95" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF4" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG4" s="95" t="s">
         <v>239</v>
       </c>
-      <c r="AE4" s="95" t="s">
-        <v>234</v>
-      </c>
-      <c r="AF4" s="95" t="s">
-        <v>235</v>
-      </c>
-      <c r="AG4" s="95" t="s">
-        <v>240</v>
-      </c>
       <c r="AH4" s="95" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AI4" s="95" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AJ4" s="95" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AK4" s="95" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AL4" s="96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AM4" s="96"/>
       <c r="AN4" s="96"/>
@@ -2990,27 +3097,68 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="101" t="s">
+      <c r="AV4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="101" t="s">
+      <c r="AW4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="101" t="s">
+      <c r="AX4" s="125"/>
+      <c r="AY4" s="127"/>
+      <c r="AZ4" s="127"/>
+      <c r="BA4" s="127"/>
+      <c r="BB4" s="127"/>
+      <c r="BC4" s="127"/>
+      <c r="BD4" s="127"/>
+      <c r="BE4" s="127"/>
+      <c r="BF4" s="129"/>
+      <c r="BG4" s="129"/>
+      <c r="BH4" s="129"/>
+      <c r="BI4" s="129"/>
+      <c r="BJ4" s="129"/>
+      <c r="BK4" s="129"/>
+      <c r="BL4" s="129"/>
+      <c r="BM4" s="129"/>
+      <c r="BN4" s="129"/>
+      <c r="BO4" s="129"/>
+      <c r="BP4" s="132"/>
+      <c r="BQ4" s="132"/>
+      <c r="BR4" s="132"/>
+      <c r="BS4" s="134"/>
+      <c r="BT4" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="101" t="s">
+      <c r="BU4" s="139"/>
+      <c r="BV4" s="140"/>
+      <c r="BW4" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="101" t="s">
+      <c r="BX4" s="135"/>
+      <c r="BY4" s="132"/>
+      <c r="BZ4" s="141"/>
+      <c r="CA4" s="141"/>
+      <c r="CB4" s="141"/>
+      <c r="CC4" s="141"/>
+      <c r="CD4" s="141"/>
+      <c r="CE4" s="141"/>
+      <c r="CF4" s="141"/>
+      <c r="CG4" s="141"/>
+      <c r="CH4" s="141"/>
+      <c r="CI4" s="141"/>
+      <c r="CJ4" s="142"/>
+      <c r="CK4" s="142"/>
+      <c r="CL4" s="142"/>
+      <c r="CM4" s="142"/>
+      <c r="CN4" s="143"/>
+      <c r="CO4" s="103" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3052,70 +3200,70 @@
       </c>
       <c r="P5" s="93"/>
       <c r="Q5" s="93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R5" s="94" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S5" s="94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T5" s="94" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U5" s="94" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V5" s="94" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="W5" s="94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="X5" s="94" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y5" s="94" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z5" s="94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AA5" s="94" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AB5" s="95" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AC5" s="95" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AD5" s="95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AE5" s="95" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AF5" s="95" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AG5" s="95" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AH5" s="95" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AI5" s="95" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AJ5" s="95" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AK5" s="95" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AL5" s="96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AM5" s="96"/>
       <c r="AN5" s="96"/>
@@ -3126,17 +3274,58 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="BT5" s="101"/>
-      <c r="BW5" s="101"/>
-      <c r="CO5" s="101"/>
+      <c r="AV5" s="103"/>
+      <c r="AW5" s="103"/>
+      <c r="AX5" s="128"/>
+      <c r="AY5" s="127"/>
+      <c r="AZ5" s="127"/>
+      <c r="BA5" s="127"/>
+      <c r="BB5" s="127"/>
+      <c r="BC5" s="127"/>
+      <c r="BD5" s="127"/>
+      <c r="BE5" s="127"/>
+      <c r="BF5" s="129"/>
+      <c r="BG5" s="129"/>
+      <c r="BH5" s="129"/>
+      <c r="BI5" s="129"/>
+      <c r="BJ5" s="129"/>
+      <c r="BK5" s="129"/>
+      <c r="BL5" s="129"/>
+      <c r="BM5" s="129"/>
+      <c r="BN5" s="129"/>
+      <c r="BO5" s="129"/>
+      <c r="BP5" s="132"/>
+      <c r="BQ5" s="132"/>
+      <c r="BR5" s="132"/>
+      <c r="BS5" s="134"/>
+      <c r="BT5" s="103"/>
+      <c r="BU5" s="137"/>
+      <c r="BV5" s="138"/>
+      <c r="BW5" s="103"/>
+      <c r="BX5" s="136"/>
+      <c r="BY5" s="132"/>
+      <c r="BZ5" s="141"/>
+      <c r="CA5" s="141"/>
+      <c r="CB5" s="141"/>
+      <c r="CC5" s="141"/>
+      <c r="CD5" s="141"/>
+      <c r="CE5" s="141"/>
+      <c r="CF5" s="141"/>
+      <c r="CG5" s="141"/>
+      <c r="CH5" s="141"/>
+      <c r="CI5" s="141"/>
+      <c r="CJ5" s="142"/>
+      <c r="CK5" s="142"/>
+      <c r="CL5" s="142"/>
+      <c r="CM5" s="142"/>
+      <c r="CN5" s="143"/>
+      <c r="CO5" s="103"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3177,73 +3366,73 @@
         <v>163</v>
       </c>
       <c r="P6" s="93" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q6" s="93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R6" s="94" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S6" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T6" s="94" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U6" s="94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V6" s="94" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="W6" s="94" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X6" s="94" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y6" s="94" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Z6" s="94" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AA6" s="94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB6" s="95" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AC6" s="95" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AD6" s="95" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AE6" s="95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AF6" s="95" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG6" s="95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AH6" s="95" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AI6" s="95" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AJ6" s="95" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AK6" s="95" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AL6" s="96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AM6" s="96"/>
       <c r="AN6" s="96"/>
@@ -3254,17 +3443,58 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="BT6" s="101"/>
-      <c r="BW6" s="101"/>
-      <c r="CO6" s="101"/>
+      <c r="AV6" s="103"/>
+      <c r="AW6" s="103"/>
+      <c r="AX6" s="128"/>
+      <c r="AY6" s="127"/>
+      <c r="AZ6" s="127"/>
+      <c r="BA6" s="127"/>
+      <c r="BB6" s="127"/>
+      <c r="BC6" s="127"/>
+      <c r="BD6" s="127"/>
+      <c r="BE6" s="127"/>
+      <c r="BF6" s="129"/>
+      <c r="BG6" s="129"/>
+      <c r="BH6" s="129"/>
+      <c r="BI6" s="129"/>
+      <c r="BJ6" s="129"/>
+      <c r="BK6" s="129"/>
+      <c r="BL6" s="129"/>
+      <c r="BM6" s="129"/>
+      <c r="BN6" s="129"/>
+      <c r="BO6" s="129"/>
+      <c r="BP6" s="132"/>
+      <c r="BQ6" s="132"/>
+      <c r="BR6" s="132"/>
+      <c r="BS6" s="134"/>
+      <c r="BT6" s="103"/>
+      <c r="BU6" s="137"/>
+      <c r="BV6" s="138"/>
+      <c r="BW6" s="103"/>
+      <c r="BX6" s="136"/>
+      <c r="BY6" s="132"/>
+      <c r="BZ6" s="141"/>
+      <c r="CA6" s="141"/>
+      <c r="CB6" s="141"/>
+      <c r="CC6" s="141"/>
+      <c r="CD6" s="141"/>
+      <c r="CE6" s="141"/>
+      <c r="CF6" s="141"/>
+      <c r="CG6" s="141"/>
+      <c r="CH6" s="141"/>
+      <c r="CI6" s="141"/>
+      <c r="CJ6" s="142"/>
+      <c r="CK6" s="142"/>
+      <c r="CL6" s="142"/>
+      <c r="CM6" s="142"/>
+      <c r="CN6" s="143"/>
+      <c r="CO6" s="103"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3305,73 +3535,73 @@
         <v>164</v>
       </c>
       <c r="P7" s="93" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q7" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="Q7" s="93" t="s">
-        <v>179</v>
-      </c>
       <c r="R7" s="94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S7" s="94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T7" s="94" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U7" s="94" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V7" s="94" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="W7" s="94" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X7" s="94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y7" s="94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Z7" s="94" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AA7" s="94" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AB7" s="95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AC7" s="95" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AD7" s="95" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE7" s="95" t="s">
         <v>230</v>
       </c>
-      <c r="AE7" s="95" t="s">
-        <v>231</v>
-      </c>
       <c r="AF7" s="95" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AG7" s="95" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AH7" s="95" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AI7" s="95" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AJ7" s="95" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AK7" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="AL7" s="96" t="s">
         <v>259</v>
-      </c>
-      <c r="AL7" s="96" t="s">
-        <v>260</v>
       </c>
       <c r="AM7" s="96"/>
       <c r="AN7" s="96"/>
@@ -3382,29 +3612,70 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="101"/>
-      <c r="AW7" s="101"/>
-      <c r="BT7" s="101"/>
-      <c r="BW7" s="101"/>
-      <c r="CO7" s="101"/>
+      <c r="AV7" s="103"/>
+      <c r="AW7" s="103"/>
+      <c r="AX7" s="128"/>
+      <c r="AY7" s="127"/>
+      <c r="AZ7" s="127"/>
+      <c r="BA7" s="127"/>
+      <c r="BB7" s="127"/>
+      <c r="BC7" s="127"/>
+      <c r="BD7" s="127"/>
+      <c r="BE7" s="127"/>
+      <c r="BF7" s="129"/>
+      <c r="BG7" s="129"/>
+      <c r="BH7" s="129"/>
+      <c r="BI7" s="129"/>
+      <c r="BJ7" s="129"/>
+      <c r="BK7" s="129"/>
+      <c r="BL7" s="129"/>
+      <c r="BM7" s="129"/>
+      <c r="BN7" s="129"/>
+      <c r="BO7" s="129"/>
+      <c r="BP7" s="132"/>
+      <c r="BQ7" s="132"/>
+      <c r="BR7" s="132"/>
+      <c r="BS7" s="133"/>
+      <c r="BT7" s="103"/>
+      <c r="BU7" s="137"/>
+      <c r="BV7" s="138"/>
+      <c r="BW7" s="103"/>
+      <c r="BX7" s="136"/>
+      <c r="BY7" s="132"/>
+      <c r="BZ7" s="141"/>
+      <c r="CA7" s="141"/>
+      <c r="CB7" s="141"/>
+      <c r="CC7" s="141"/>
+      <c r="CD7" s="141"/>
+      <c r="CE7" s="141"/>
+      <c r="CF7" s="141"/>
+      <c r="CG7" s="141"/>
+      <c r="CH7" s="141"/>
+      <c r="CI7" s="141"/>
+      <c r="CJ7" s="142"/>
+      <c r="CK7" s="142"/>
+      <c r="CL7" s="142"/>
+      <c r="CM7" s="142"/>
+      <c r="CN7" s="143"/>
+      <c r="CO7" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3417,7 +3688,7 @@
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3493,25 +3764,25 @@
       <c r="C2" s="110"/>
       <c r="D2" s="110"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="119" t="s">
+      <c r="F2" s="113" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="119"/>
+      <c r="G2" s="113"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="120" t="s">
+      <c r="I2" s="114" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="120"/>
+      <c r="J2" s="114"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="121" t="s">
+      <c r="L2" s="115" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="121"/>
+      <c r="M2" s="115"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="122" t="s">
+      <c r="O2" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="P2" s="122"/>
+      <c r="P2" s="116"/>
       <c r="Q2" s="89"/>
       <c r="R2" s="106" t="s">
         <v>171</v>
@@ -3554,17 +3825,17 @@
       <c r="C3" s="110"/>
       <c r="D3" s="110"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="116"/>
       <c r="Q3" s="89"/>
       <c r="R3" s="106"/>
       <c r="S3" s="106"/>
@@ -3605,17 +3876,17 @@
       <c r="C4" s="110"/>
       <c r="D4" s="110"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="121"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="115"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="122"/>
-      <c r="P4" s="122"/>
+      <c r="O4" s="116"/>
+      <c r="P4" s="116"/>
       <c r="Q4" s="89"/>
       <c r="R4" s="106"/>
       <c r="S4" s="106"/>
@@ -3656,17 +3927,17 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="121"/>
-      <c r="M5" s="121"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="122"/>
-      <c r="P5" s="122"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
       <c r="Q5" s="89"/>
       <c r="R5" s="106"/>
       <c r="S5" s="106"/>
@@ -3709,17 +3980,17 @@
       <c r="C6" s="112"/>
       <c r="D6" s="112"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="121"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="115"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="122"/>
-      <c r="P6" s="122"/>
+      <c r="O6" s="116"/>
+      <c r="P6" s="116"/>
       <c r="Q6" s="89"/>
       <c r="R6" s="106"/>
       <c r="S6" s="106"/>
@@ -3760,17 +4031,17 @@
       <c r="C7" s="112"/>
       <c r="D7" s="112"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="121"/>
-      <c r="M7" s="121"/>
+      <c r="L7" s="115"/>
+      <c r="M7" s="115"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="122"/>
-      <c r="P7" s="122"/>
+      <c r="O7" s="116"/>
+      <c r="P7" s="116"/>
       <c r="Q7" s="89"/>
       <c r="R7" s="106"/>
       <c r="S7" s="106"/>
@@ -3811,17 +4082,17 @@
       <c r="C8" s="112"/>
       <c r="D8" s="112"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="114"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="121"/>
-      <c r="M8" s="121"/>
+      <c r="L8" s="115"/>
+      <c r="M8" s="115"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="122"/>
-      <c r="P8" s="122"/>
+      <c r="O8" s="116"/>
+      <c r="P8" s="116"/>
       <c r="Q8" s="89"/>
       <c r="R8" s="106"/>
       <c r="S8" s="106"/>
@@ -3862,17 +4133,17 @@
       <c r="C9" s="112"/>
       <c r="D9" s="112"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="120"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="121"/>
-      <c r="M9" s="121"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="122"/>
-      <c r="P9" s="122"/>
+      <c r="O9" s="116"/>
+      <c r="P9" s="116"/>
       <c r="Q9" s="89"/>
       <c r="R9" s="106"/>
       <c r="S9" s="106"/>
@@ -3913,17 +4184,17 @@
       <c r="C10" s="112"/>
       <c r="D10" s="112"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="120"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="114"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="121"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="115"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="122"/>
-      <c r="P10" s="122"/>
+      <c r="O10" s="116"/>
+      <c r="P10" s="116"/>
       <c r="Q10" s="89"/>
       <c r="R10" s="106"/>
       <c r="S10" s="106"/>
@@ -4030,10 +4301,8 @@
       </c>
       <c r="M12" s="109"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="P12" s="114"/>
+      <c r="O12" s="124"/>
+      <c r="P12" s="124"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4083,8 +4352,8 @@
       <c r="L13" s="109"/>
       <c r="M13" s="109"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="115"/>
-      <c r="P13" s="116"/>
+      <c r="O13" s="124"/>
+      <c r="P13" s="124"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4134,8 +4403,8 @@
       <c r="L14" s="109"/>
       <c r="M14" s="109"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="115"/>
-      <c r="P14" s="116"/>
+      <c r="O14" s="124"/>
+      <c r="P14" s="124"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4185,8 +4454,8 @@
       <c r="L15" s="109"/>
       <c r="M15" s="109"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="115"/>
-      <c r="P15" s="116"/>
+      <c r="O15" s="124"/>
+      <c r="P15" s="124"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -4236,8 +4505,8 @@
       <c r="L16" s="109"/>
       <c r="M16" s="109"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="115"/>
-      <c r="P16" s="116"/>
+      <c r="O16" s="124"/>
+      <c r="P16" s="124"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -4287,8 +4556,8 @@
       <c r="L17" s="109"/>
       <c r="M17" s="109"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="115"/>
-      <c r="P17" s="116"/>
+      <c r="O17" s="124"/>
+      <c r="P17" s="124"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -4338,8 +4607,8 @@
       <c r="L18" s="109"/>
       <c r="M18" s="109"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="115"/>
-      <c r="P18" s="116"/>
+      <c r="O18" s="124"/>
+      <c r="P18" s="124"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -4389,8 +4658,8 @@
       <c r="L19" s="109"/>
       <c r="M19" s="109"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="115"/>
-      <c r="P19" s="116"/>
+      <c r="O19" s="124"/>
+      <c r="P19" s="124"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -4440,8 +4709,8 @@
       <c r="L20" s="109"/>
       <c r="M20" s="109"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="117"/>
-      <c r="P20" s="118"/>
+      <c r="O20" s="124"/>
+      <c r="P20" s="124"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -16987,7 +17256,7 @@
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17014,7 +17283,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="119" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -17354,7 +17623,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="125"/>
+      <c r="A2" s="119"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -17680,15 +17949,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="126"/>
-      <c r="DH2" s="126"/>
-      <c r="DI2" s="126"/>
-      <c r="DJ2" s="126"/>
+      <c r="DG2" s="120"/>
+      <c r="DH2" s="120"/>
+      <c r="DI2" s="120"/>
+      <c r="DJ2" s="120"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="125"/>
+      <c r="A3" s="119"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18025,7 +18294,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="121" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18167,7 +18436,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="127"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -18307,7 +18576,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="127"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -18447,7 +18716,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="127"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -18585,7 +18854,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="127"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -18725,7 +18994,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="122" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -18867,7 +19136,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="128"/>
+      <c r="B10" s="122"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19007,7 +19276,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="129" t="s">
+      <c r="B11" s="123" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19137,7 +19406,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="129"/>
+      <c r="B12" s="123"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -19275,7 +19544,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="129"/>
+      <c r="B13" s="123"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -19415,7 +19684,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="129"/>
+      <c r="B14" s="123"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -19551,7 +19820,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="129"/>
+      <c r="B15" s="123"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -19687,7 +19956,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="129"/>
+      <c r="B16" s="123"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -19823,7 +20092,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="129"/>
+      <c r="B17" s="123"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -19959,7 +20228,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="129"/>
+      <c r="B18" s="123"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20099,7 +20368,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="129"/>
+      <c r="B19" s="123"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -20235,7 +20504,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="129"/>
+      <c r="B20" s="123"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -20371,7 +20640,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="123" t="s">
+      <c r="B21" s="117" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -20505,7 +20774,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="123"/>
+      <c r="B22" s="117"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -20641,7 +20910,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="123"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -20773,7 +21042,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="123"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -20907,7 +21176,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="123"/>
+      <c r="B25" s="117"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21051,7 +21320,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="124" t="s">
+      <c r="B26" s="118" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -21185,7 +21454,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="124"/>
+      <c r="B27" s="118"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -21325,7 +21594,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="124"/>
+      <c r="B28" s="118"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -21457,7 +21726,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="124"/>
+      <c r="B29" s="118"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -21585,7 +21854,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="124"/>
+      <c r="B30" s="118"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -21711,7 +21980,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="124"/>
+      <c r="B31" s="118"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 02-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607835C1-8DBF-43A1-B412-C81578E355A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="264">
   <si>
     <t>REDES</t>
   </si>
@@ -891,12 +892,24 @@
   </si>
   <si>
     <t>Reunião com a coordenação da escola para esclarecer o andamento dos projetos.</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente. Sprint Review</t>
+  </si>
+  <si>
+    <t>Planning, preparação de reunião, implantação do JWT, métodos login, listagem de hostgroup e host, conexão com o banco de dados</t>
+  </si>
+  <si>
+    <t>Planning. Configuração projeto mobile, finalização de modais, ajuste nas validações da API, login na API e Web. Documentação e casos de uso</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente. Planning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1728,84 +1741,6 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1862,6 +1797,84 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2256,14 +2269,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="AK4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CL6" sqref="CL6"/>
+      <selection pane="bottomRight" activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2284,8 +2297,9 @@
     <col min="31" max="31" width="30.77734375" customWidth="1"/>
     <col min="32" max="32" width="20.77734375" customWidth="1"/>
     <col min="33" max="36" width="25.77734375" customWidth="1"/>
-    <col min="37" max="37" width="20.77734375" customWidth="1"/>
-    <col min="38" max="47" width="15.77734375" customWidth="1"/>
+    <col min="37" max="38" width="20.77734375" customWidth="1"/>
+    <col min="39" max="39" width="25.77734375" customWidth="1"/>
+    <col min="40" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="71" width="5.77734375" customWidth="1"/>
@@ -2298,7 +2312,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="122" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2578,117 +2592,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="123"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="121" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102" t="s">
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="102"/>
-      <c r="T2" s="102"/>
-      <c r="U2" s="102"/>
-      <c r="V2" s="102"/>
-      <c r="W2" s="102"/>
-      <c r="X2" s="102"/>
-      <c r="Y2" s="102"/>
-      <c r="Z2" s="102"/>
-      <c r="AA2" s="102"/>
-      <c r="AB2" s="102"/>
-      <c r="AC2" s="102"/>
-      <c r="AD2" s="102"/>
-      <c r="AE2" s="102"/>
-      <c r="AF2" s="102"/>
-      <c r="AG2" s="102"/>
-      <c r="AH2" s="102"/>
-      <c r="AI2" s="102"/>
-      <c r="AJ2" s="102"/>
-      <c r="AK2" s="102"/>
-      <c r="AL2" s="102"/>
-      <c r="AM2" s="102" t="s">
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="121"/>
+      <c r="Z2" s="121"/>
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="121"/>
+      <c r="AF2" s="121"/>
+      <c r="AG2" s="121"/>
+      <c r="AH2" s="121"/>
+      <c r="AI2" s="121"/>
+      <c r="AJ2" s="121"/>
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="102"/>
-      <c r="AO2" s="102"/>
-      <c r="AP2" s="102"/>
-      <c r="AQ2" s="102"/>
-      <c r="AR2" s="102"/>
-      <c r="AS2" s="102"/>
-      <c r="AT2" s="102"/>
-      <c r="AU2" s="102"/>
-      <c r="AV2" s="102"/>
-      <c r="AW2" s="102"/>
-      <c r="AX2" s="102"/>
-      <c r="AY2" s="102"/>
-      <c r="AZ2" s="102"/>
-      <c r="BA2" s="102"/>
-      <c r="BB2" s="102"/>
-      <c r="BC2" s="102"/>
-      <c r="BD2" s="102"/>
-      <c r="BE2" s="102"/>
-      <c r="BF2" s="102"/>
-      <c r="BG2" s="102"/>
-      <c r="BH2" s="102"/>
-      <c r="BI2" s="102"/>
-      <c r="BJ2" s="102" t="s">
+      <c r="AN2" s="121"/>
+      <c r="AO2" s="121"/>
+      <c r="AP2" s="121"/>
+      <c r="AQ2" s="121"/>
+      <c r="AR2" s="121"/>
+      <c r="AS2" s="121"/>
+      <c r="AT2" s="121"/>
+      <c r="AU2" s="121"/>
+      <c r="AV2" s="121"/>
+      <c r="AW2" s="121"/>
+      <c r="AX2" s="121"/>
+      <c r="AY2" s="121"/>
+      <c r="AZ2" s="121"/>
+      <c r="BA2" s="121"/>
+      <c r="BB2" s="121"/>
+      <c r="BC2" s="121"/>
+      <c r="BD2" s="121"/>
+      <c r="BE2" s="121"/>
+      <c r="BF2" s="121"/>
+      <c r="BG2" s="121"/>
+      <c r="BH2" s="121"/>
+      <c r="BI2" s="121"/>
+      <c r="BJ2" s="121" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="102"/>
-      <c r="BL2" s="102"/>
-      <c r="BM2" s="102"/>
-      <c r="BN2" s="102"/>
-      <c r="BO2" s="102"/>
-      <c r="BP2" s="102"/>
-      <c r="BQ2" s="102"/>
-      <c r="BR2" s="102"/>
-      <c r="BS2" s="102"/>
-      <c r="BT2" s="102"/>
-      <c r="BU2" s="102"/>
-      <c r="BV2" s="102"/>
-      <c r="BW2" s="102"/>
-      <c r="BX2" s="102"/>
-      <c r="BY2" s="102"/>
-      <c r="BZ2" s="102"/>
-      <c r="CA2" s="102"/>
-      <c r="CB2" s="102"/>
-      <c r="CC2" s="102"/>
-      <c r="CD2" s="102"/>
-      <c r="CE2" s="102" t="s">
+      <c r="BK2" s="121"/>
+      <c r="BL2" s="121"/>
+      <c r="BM2" s="121"/>
+      <c r="BN2" s="121"/>
+      <c r="BO2" s="121"/>
+      <c r="BP2" s="121"/>
+      <c r="BQ2" s="121"/>
+      <c r="BR2" s="121"/>
+      <c r="BS2" s="121"/>
+      <c r="BT2" s="121"/>
+      <c r="BU2" s="121"/>
+      <c r="BV2" s="121"/>
+      <c r="BW2" s="121"/>
+      <c r="BX2" s="121"/>
+      <c r="BY2" s="121"/>
+      <c r="BZ2" s="121"/>
+      <c r="CA2" s="121"/>
+      <c r="CB2" s="121"/>
+      <c r="CC2" s="121"/>
+      <c r="CD2" s="121"/>
+      <c r="CE2" s="121" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="102"/>
-      <c r="CG2" s="102"/>
-      <c r="CH2" s="102"/>
-      <c r="CI2" s="102"/>
-      <c r="CJ2" s="102"/>
-      <c r="CK2" s="102"/>
-      <c r="CL2" s="102"/>
-      <c r="CM2" s="102"/>
-      <c r="CN2" s="102"/>
-      <c r="CO2" s="102"/>
-      <c r="CP2" s="102"/>
-      <c r="CQ2" s="102"/>
-      <c r="CR2" s="102"/>
+      <c r="CF2" s="121"/>
+      <c r="CG2" s="121"/>
+      <c r="CH2" s="121"/>
+      <c r="CI2" s="121"/>
+      <c r="CJ2" s="121"/>
+      <c r="CK2" s="121"/>
+      <c r="CL2" s="121"/>
+      <c r="CM2" s="121"/>
+      <c r="CN2" s="121"/>
+      <c r="CO2" s="121"/>
+      <c r="CP2" s="121"/>
+      <c r="CQ2" s="121"/>
+      <c r="CR2" s="121"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="124"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2836,136 +2850,136 @@
       <c r="AX3" s="87">
         <v>16</v>
       </c>
-      <c r="AY3" s="126">
+      <c r="AY3" s="100">
         <v>17</v>
       </c>
-      <c r="AZ3" s="130">
+      <c r="AZ3" s="104">
         <v>18</v>
       </c>
-      <c r="BA3" s="130">
+      <c r="BA3" s="104">
         <v>21</v>
       </c>
-      <c r="BB3" s="126">
+      <c r="BB3" s="100">
         <v>22</v>
       </c>
-      <c r="BC3" s="126">
+      <c r="BC3" s="100">
         <v>23</v>
       </c>
-      <c r="BD3" s="126">
+      <c r="BD3" s="100">
         <v>24</v>
       </c>
-      <c r="BE3" s="130">
+      <c r="BE3" s="104">
         <v>25</v>
       </c>
-      <c r="BF3" s="130">
+      <c r="BF3" s="104">
         <v>28</v>
       </c>
-      <c r="BG3" s="126">
+      <c r="BG3" s="100">
         <v>29</v>
       </c>
-      <c r="BH3" s="126">
+      <c r="BH3" s="100">
         <v>30</v>
       </c>
-      <c r="BI3" s="126">
+      <c r="BI3" s="100">
         <v>31</v>
       </c>
-      <c r="BJ3" s="130">
+      <c r="BJ3" s="104">
         <v>1</v>
       </c>
-      <c r="BK3" s="130">
+      <c r="BK3" s="104">
         <v>4</v>
       </c>
-      <c r="BL3" s="126">
+      <c r="BL3" s="100">
         <v>5</v>
       </c>
-      <c r="BM3" s="126">
+      <c r="BM3" s="100">
         <v>6</v>
       </c>
-      <c r="BN3" s="126">
+      <c r="BN3" s="100">
         <v>7</v>
       </c>
-      <c r="BO3" s="130">
+      <c r="BO3" s="104">
         <v>8</v>
       </c>
-      <c r="BP3" s="130">
+      <c r="BP3" s="104">
         <v>11</v>
       </c>
-      <c r="BQ3" s="126">
+      <c r="BQ3" s="100">
         <v>12</v>
       </c>
-      <c r="BR3" s="126">
+      <c r="BR3" s="100">
         <v>13</v>
       </c>
-      <c r="BS3" s="126">
+      <c r="BS3" s="100">
         <v>14</v>
       </c>
       <c r="BT3" s="83">
         <v>15</v>
       </c>
-      <c r="BU3" s="130">
+      <c r="BU3" s="104">
         <v>18</v>
       </c>
-      <c r="BV3" s="126">
+      <c r="BV3" s="100">
         <v>19</v>
       </c>
       <c r="BW3" s="83">
         <v>20</v>
       </c>
-      <c r="BX3" s="126">
+      <c r="BX3" s="100">
         <v>21</v>
       </c>
-      <c r="BY3" s="130">
+      <c r="BY3" s="104">
         <v>22</v>
       </c>
-      <c r="BZ3" s="130">
+      <c r="BZ3" s="104">
         <v>25</v>
       </c>
-      <c r="CA3" s="126">
+      <c r="CA3" s="100">
         <v>26</v>
       </c>
-      <c r="CB3" s="126">
+      <c r="CB3" s="100">
         <v>27</v>
       </c>
-      <c r="CC3" s="126">
+      <c r="CC3" s="100">
         <v>28</v>
       </c>
-      <c r="CD3" s="130">
+      <c r="CD3" s="104">
         <v>29</v>
       </c>
-      <c r="CE3" s="130">
+      <c r="CE3" s="104">
         <v>2</v>
       </c>
-      <c r="CF3" s="126">
+      <c r="CF3" s="100">
         <v>3</v>
       </c>
-      <c r="CG3" s="126">
+      <c r="CG3" s="100">
         <v>4</v>
       </c>
-      <c r="CH3" s="126">
+      <c r="CH3" s="100">
         <v>5</v>
       </c>
-      <c r="CI3" s="130">
+      <c r="CI3" s="104">
         <v>6</v>
       </c>
-      <c r="CJ3" s="130">
+      <c r="CJ3" s="104">
         <v>9</v>
       </c>
-      <c r="CK3" s="126">
+      <c r="CK3" s="100">
         <v>10</v>
       </c>
-      <c r="CL3" s="126">
+      <c r="CL3" s="100">
         <v>11</v>
       </c>
-      <c r="CM3" s="126">
+      <c r="CM3" s="100">
         <v>12</v>
       </c>
-      <c r="CN3" s="130">
+      <c r="CN3" s="104">
         <v>13</v>
       </c>
       <c r="CO3" s="83">
         <v>14</v>
       </c>
-      <c r="CP3" s="131">
+      <c r="CP3" s="105">
         <v>16</v>
       </c>
       <c r="CQ3" s="85">
@@ -2976,10 +2990,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="118" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="105"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -3088,7 +3102,9 @@
       <c r="AL4" s="96" t="s">
         <v>259</v>
       </c>
-      <c r="AM4" s="96"/>
+      <c r="AM4" s="96" t="s">
+        <v>260</v>
+      </c>
       <c r="AN4" s="96"/>
       <c r="AO4" s="96"/>
       <c r="AP4" s="96"/>
@@ -3097,68 +3113,68 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="103" t="s">
+      <c r="AV4" s="120" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="103" t="s">
+      <c r="AW4" s="120" t="s">
         <v>112</v>
       </c>
-      <c r="AX4" s="125"/>
-      <c r="AY4" s="127"/>
-      <c r="AZ4" s="127"/>
-      <c r="BA4" s="127"/>
-      <c r="BB4" s="127"/>
-      <c r="BC4" s="127"/>
-      <c r="BD4" s="127"/>
-      <c r="BE4" s="127"/>
-      <c r="BF4" s="129"/>
-      <c r="BG4" s="129"/>
-      <c r="BH4" s="129"/>
-      <c r="BI4" s="129"/>
-      <c r="BJ4" s="129"/>
-      <c r="BK4" s="129"/>
-      <c r="BL4" s="129"/>
-      <c r="BM4" s="129"/>
-      <c r="BN4" s="129"/>
-      <c r="BO4" s="129"/>
-      <c r="BP4" s="132"/>
-      <c r="BQ4" s="132"/>
-      <c r="BR4" s="132"/>
-      <c r="BS4" s="134"/>
-      <c r="BT4" s="103" t="s">
+      <c r="AX4" s="99"/>
+      <c r="AY4" s="101"/>
+      <c r="AZ4" s="101"/>
+      <c r="BA4" s="101"/>
+      <c r="BB4" s="101"/>
+      <c r="BC4" s="101"/>
+      <c r="BD4" s="101"/>
+      <c r="BE4" s="101"/>
+      <c r="BF4" s="103"/>
+      <c r="BG4" s="103"/>
+      <c r="BH4" s="103"/>
+      <c r="BI4" s="103"/>
+      <c r="BJ4" s="103"/>
+      <c r="BK4" s="103"/>
+      <c r="BL4" s="103"/>
+      <c r="BM4" s="103"/>
+      <c r="BN4" s="103"/>
+      <c r="BO4" s="103"/>
+      <c r="BP4" s="106"/>
+      <c r="BQ4" s="106"/>
+      <c r="BR4" s="106"/>
+      <c r="BS4" s="108"/>
+      <c r="BT4" s="120" t="s">
         <v>113</v>
       </c>
-      <c r="BU4" s="139"/>
-      <c r="BV4" s="140"/>
-      <c r="BW4" s="103" t="s">
+      <c r="BU4" s="113"/>
+      <c r="BV4" s="114"/>
+      <c r="BW4" s="120" t="s">
         <v>114</v>
       </c>
-      <c r="BX4" s="135"/>
-      <c r="BY4" s="132"/>
-      <c r="BZ4" s="141"/>
-      <c r="CA4" s="141"/>
-      <c r="CB4" s="141"/>
-      <c r="CC4" s="141"/>
-      <c r="CD4" s="141"/>
-      <c r="CE4" s="141"/>
-      <c r="CF4" s="141"/>
-      <c r="CG4" s="141"/>
-      <c r="CH4" s="141"/>
-      <c r="CI4" s="141"/>
-      <c r="CJ4" s="142"/>
-      <c r="CK4" s="142"/>
-      <c r="CL4" s="142"/>
-      <c r="CM4" s="142"/>
-      <c r="CN4" s="143"/>
-      <c r="CO4" s="103" t="s">
+      <c r="BX4" s="109"/>
+      <c r="BY4" s="106"/>
+      <c r="BZ4" s="115"/>
+      <c r="CA4" s="115"/>
+      <c r="CB4" s="115"/>
+      <c r="CC4" s="115"/>
+      <c r="CD4" s="115"/>
+      <c r="CE4" s="115"/>
+      <c r="CF4" s="115"/>
+      <c r="CG4" s="115"/>
+      <c r="CH4" s="115"/>
+      <c r="CI4" s="115"/>
+      <c r="CJ4" s="116"/>
+      <c r="CK4" s="116"/>
+      <c r="CL4" s="116"/>
+      <c r="CM4" s="116"/>
+      <c r="CN4" s="117"/>
+      <c r="CO4" s="120" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="118" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="105"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3265,7 +3281,9 @@
       <c r="AL5" s="96" t="s">
         <v>259</v>
       </c>
-      <c r="AM5" s="96"/>
+      <c r="AM5" s="96" t="s">
+        <v>261</v>
+      </c>
       <c r="AN5" s="96"/>
       <c r="AO5" s="96"/>
       <c r="AP5" s="96"/>
@@ -3274,58 +3292,58 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="103"/>
-      <c r="AW5" s="103"/>
-      <c r="AX5" s="128"/>
-      <c r="AY5" s="127"/>
-      <c r="AZ5" s="127"/>
-      <c r="BA5" s="127"/>
-      <c r="BB5" s="127"/>
-      <c r="BC5" s="127"/>
-      <c r="BD5" s="127"/>
-      <c r="BE5" s="127"/>
-      <c r="BF5" s="129"/>
-      <c r="BG5" s="129"/>
-      <c r="BH5" s="129"/>
-      <c r="BI5" s="129"/>
-      <c r="BJ5" s="129"/>
-      <c r="BK5" s="129"/>
-      <c r="BL5" s="129"/>
-      <c r="BM5" s="129"/>
-      <c r="BN5" s="129"/>
-      <c r="BO5" s="129"/>
-      <c r="BP5" s="132"/>
-      <c r="BQ5" s="132"/>
-      <c r="BR5" s="132"/>
-      <c r="BS5" s="134"/>
-      <c r="BT5" s="103"/>
-      <c r="BU5" s="137"/>
-      <c r="BV5" s="138"/>
-      <c r="BW5" s="103"/>
-      <c r="BX5" s="136"/>
-      <c r="BY5" s="132"/>
-      <c r="BZ5" s="141"/>
-      <c r="CA5" s="141"/>
-      <c r="CB5" s="141"/>
-      <c r="CC5" s="141"/>
-      <c r="CD5" s="141"/>
-      <c r="CE5" s="141"/>
-      <c r="CF5" s="141"/>
-      <c r="CG5" s="141"/>
-      <c r="CH5" s="141"/>
-      <c r="CI5" s="141"/>
-      <c r="CJ5" s="142"/>
-      <c r="CK5" s="142"/>
-      <c r="CL5" s="142"/>
-      <c r="CM5" s="142"/>
-      <c r="CN5" s="143"/>
-      <c r="CO5" s="103"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
+      <c r="AX5" s="102"/>
+      <c r="AY5" s="101"/>
+      <c r="AZ5" s="101"/>
+      <c r="BA5" s="101"/>
+      <c r="BB5" s="101"/>
+      <c r="BC5" s="101"/>
+      <c r="BD5" s="101"/>
+      <c r="BE5" s="101"/>
+      <c r="BF5" s="103"/>
+      <c r="BG5" s="103"/>
+      <c r="BH5" s="103"/>
+      <c r="BI5" s="103"/>
+      <c r="BJ5" s="103"/>
+      <c r="BK5" s="103"/>
+      <c r="BL5" s="103"/>
+      <c r="BM5" s="103"/>
+      <c r="BN5" s="103"/>
+      <c r="BO5" s="103"/>
+      <c r="BP5" s="106"/>
+      <c r="BQ5" s="106"/>
+      <c r="BR5" s="106"/>
+      <c r="BS5" s="108"/>
+      <c r="BT5" s="120"/>
+      <c r="BU5" s="111"/>
+      <c r="BV5" s="112"/>
+      <c r="BW5" s="120"/>
+      <c r="BX5" s="110"/>
+      <c r="BY5" s="106"/>
+      <c r="BZ5" s="115"/>
+      <c r="CA5" s="115"/>
+      <c r="CB5" s="115"/>
+      <c r="CC5" s="115"/>
+      <c r="CD5" s="115"/>
+      <c r="CE5" s="115"/>
+      <c r="CF5" s="115"/>
+      <c r="CG5" s="115"/>
+      <c r="CH5" s="115"/>
+      <c r="CI5" s="115"/>
+      <c r="CJ5" s="116"/>
+      <c r="CK5" s="116"/>
+      <c r="CL5" s="116"/>
+      <c r="CM5" s="116"/>
+      <c r="CN5" s="117"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="118" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3434,7 +3452,9 @@
       <c r="AL6" s="96" t="s">
         <v>259</v>
       </c>
-      <c r="AM6" s="96"/>
+      <c r="AM6" s="96" t="s">
+        <v>262</v>
+      </c>
       <c r="AN6" s="96"/>
       <c r="AO6" s="96"/>
       <c r="AP6" s="96"/>
@@ -3443,58 +3463,58 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="103"/>
-      <c r="AW6" s="103"/>
-      <c r="AX6" s="128"/>
-      <c r="AY6" s="127"/>
-      <c r="AZ6" s="127"/>
-      <c r="BA6" s="127"/>
-      <c r="BB6" s="127"/>
-      <c r="BC6" s="127"/>
-      <c r="BD6" s="127"/>
-      <c r="BE6" s="127"/>
-      <c r="BF6" s="129"/>
-      <c r="BG6" s="129"/>
-      <c r="BH6" s="129"/>
-      <c r="BI6" s="129"/>
-      <c r="BJ6" s="129"/>
-      <c r="BK6" s="129"/>
-      <c r="BL6" s="129"/>
-      <c r="BM6" s="129"/>
-      <c r="BN6" s="129"/>
-      <c r="BO6" s="129"/>
-      <c r="BP6" s="132"/>
-      <c r="BQ6" s="132"/>
-      <c r="BR6" s="132"/>
-      <c r="BS6" s="134"/>
-      <c r="BT6" s="103"/>
-      <c r="BU6" s="137"/>
-      <c r="BV6" s="138"/>
-      <c r="BW6" s="103"/>
-      <c r="BX6" s="136"/>
-      <c r="BY6" s="132"/>
-      <c r="BZ6" s="141"/>
-      <c r="CA6" s="141"/>
-      <c r="CB6" s="141"/>
-      <c r="CC6" s="141"/>
-      <c r="CD6" s="141"/>
-      <c r="CE6" s="141"/>
-      <c r="CF6" s="141"/>
-      <c r="CG6" s="141"/>
-      <c r="CH6" s="141"/>
-      <c r="CI6" s="141"/>
-      <c r="CJ6" s="142"/>
-      <c r="CK6" s="142"/>
-      <c r="CL6" s="142"/>
-      <c r="CM6" s="142"/>
-      <c r="CN6" s="143"/>
-      <c r="CO6" s="103"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
+      <c r="AX6" s="102"/>
+      <c r="AY6" s="101"/>
+      <c r="AZ6" s="101"/>
+      <c r="BA6" s="101"/>
+      <c r="BB6" s="101"/>
+      <c r="BC6" s="101"/>
+      <c r="BD6" s="101"/>
+      <c r="BE6" s="101"/>
+      <c r="BF6" s="103"/>
+      <c r="BG6" s="103"/>
+      <c r="BH6" s="103"/>
+      <c r="BI6" s="103"/>
+      <c r="BJ6" s="103"/>
+      <c r="BK6" s="103"/>
+      <c r="BL6" s="103"/>
+      <c r="BM6" s="103"/>
+      <c r="BN6" s="103"/>
+      <c r="BO6" s="103"/>
+      <c r="BP6" s="106"/>
+      <c r="BQ6" s="106"/>
+      <c r="BR6" s="106"/>
+      <c r="BS6" s="108"/>
+      <c r="BT6" s="120"/>
+      <c r="BU6" s="111"/>
+      <c r="BV6" s="112"/>
+      <c r="BW6" s="120"/>
+      <c r="BX6" s="110"/>
+      <c r="BY6" s="106"/>
+      <c r="BZ6" s="115"/>
+      <c r="CA6" s="115"/>
+      <c r="CB6" s="115"/>
+      <c r="CC6" s="115"/>
+      <c r="CD6" s="115"/>
+      <c r="CE6" s="115"/>
+      <c r="CF6" s="115"/>
+      <c r="CG6" s="115"/>
+      <c r="CH6" s="115"/>
+      <c r="CI6" s="115"/>
+      <c r="CJ6" s="116"/>
+      <c r="CK6" s="116"/>
+      <c r="CL6" s="116"/>
+      <c r="CM6" s="116"/>
+      <c r="CN6" s="117"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3603,7 +3623,9 @@
       <c r="AL7" s="96" t="s">
         <v>259</v>
       </c>
-      <c r="AM7" s="96"/>
+      <c r="AM7" s="96" t="s">
+        <v>263</v>
+      </c>
       <c r="AN7" s="96"/>
       <c r="AO7" s="96"/>
       <c r="AP7" s="96"/>
@@ -3612,70 +3634,70 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="103"/>
-      <c r="AW7" s="103"/>
-      <c r="AX7" s="128"/>
-      <c r="AY7" s="127"/>
-      <c r="AZ7" s="127"/>
-      <c r="BA7" s="127"/>
-      <c r="BB7" s="127"/>
-      <c r="BC7" s="127"/>
-      <c r="BD7" s="127"/>
-      <c r="BE7" s="127"/>
-      <c r="BF7" s="129"/>
-      <c r="BG7" s="129"/>
-      <c r="BH7" s="129"/>
-      <c r="BI7" s="129"/>
-      <c r="BJ7" s="129"/>
-      <c r="BK7" s="129"/>
-      <c r="BL7" s="129"/>
-      <c r="BM7" s="129"/>
-      <c r="BN7" s="129"/>
-      <c r="BO7" s="129"/>
-      <c r="BP7" s="132"/>
-      <c r="BQ7" s="132"/>
-      <c r="BR7" s="132"/>
-      <c r="BS7" s="133"/>
-      <c r="BT7" s="103"/>
-      <c r="BU7" s="137"/>
-      <c r="BV7" s="138"/>
-      <c r="BW7" s="103"/>
-      <c r="BX7" s="136"/>
-      <c r="BY7" s="132"/>
-      <c r="BZ7" s="141"/>
-      <c r="CA7" s="141"/>
-      <c r="CB7" s="141"/>
-      <c r="CC7" s="141"/>
-      <c r="CD7" s="141"/>
-      <c r="CE7" s="141"/>
-      <c r="CF7" s="141"/>
-      <c r="CG7" s="141"/>
-      <c r="CH7" s="141"/>
-      <c r="CI7" s="141"/>
-      <c r="CJ7" s="142"/>
-      <c r="CK7" s="142"/>
-      <c r="CL7" s="142"/>
-      <c r="CM7" s="142"/>
-      <c r="CN7" s="143"/>
-      <c r="CO7" s="103"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
+      <c r="AX7" s="102"/>
+      <c r="AY7" s="101"/>
+      <c r="AZ7" s="101"/>
+      <c r="BA7" s="101"/>
+      <c r="BB7" s="101"/>
+      <c r="BC7" s="101"/>
+      <c r="BD7" s="101"/>
+      <c r="BE7" s="101"/>
+      <c r="BF7" s="103"/>
+      <c r="BG7" s="103"/>
+      <c r="BH7" s="103"/>
+      <c r="BI7" s="103"/>
+      <c r="BJ7" s="103"/>
+      <c r="BK7" s="103"/>
+      <c r="BL7" s="103"/>
+      <c r="BM7" s="103"/>
+      <c r="BN7" s="103"/>
+      <c r="BO7" s="103"/>
+      <c r="BP7" s="106"/>
+      <c r="BQ7" s="106"/>
+      <c r="BR7" s="106"/>
+      <c r="BS7" s="107"/>
+      <c r="BT7" s="120"/>
+      <c r="BU7" s="111"/>
+      <c r="BV7" s="112"/>
+      <c r="BW7" s="120"/>
+      <c r="BX7" s="110"/>
+      <c r="BY7" s="106"/>
+      <c r="BZ7" s="115"/>
+      <c r="CA7" s="115"/>
+      <c r="CB7" s="115"/>
+      <c r="CC7" s="115"/>
+      <c r="CD7" s="115"/>
+      <c r="CE7" s="115"/>
+      <c r="CF7" s="115"/>
+      <c r="CG7" s="115"/>
+      <c r="CH7" s="115"/>
+      <c r="CI7" s="115"/>
+      <c r="CJ7" s="116"/>
+      <c r="CK7" s="116"/>
+      <c r="CL7" s="116"/>
+      <c r="CM7" s="116"/>
+      <c r="CN7" s="117"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3684,7 +3706,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -3758,36 +3780,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="129" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="133" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="113"/>
+      <c r="G2" s="133"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="114"/>
+      <c r="J2" s="134"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="115" t="s">
+      <c r="L2" s="135" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="115"/>
+      <c r="M2" s="135"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="116" t="s">
+      <c r="O2" s="136" t="s">
         <v>170</v>
       </c>
-      <c r="P2" s="116"/>
+      <c r="P2" s="136"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="106" t="s">
+      <c r="R2" s="125" t="s">
         <v>171</v>
       </c>
-      <c r="S2" s="106"/>
+      <c r="S2" s="125"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -3821,24 +3843,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
+      <c r="R3" s="125"/>
+      <c r="S3" s="125"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -3872,24 +3894,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="114"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
+      <c r="L4" s="135"/>
+      <c r="M4" s="135"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="116"/>
-      <c r="P4" s="116"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="125"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -3927,20 +3949,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
+      <c r="R5" s="125"/>
+      <c r="S5" s="125"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -3974,26 +3996,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="130" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="116"/>
-      <c r="P6" s="116"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="136"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
+      <c r="R6" s="125"/>
+      <c r="S6" s="125"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4027,24 +4049,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="114"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="115"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="116"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
+      <c r="R7" s="125"/>
+      <c r="S7" s="125"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4078,24 +4100,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="113"/>
-      <c r="G8" s="113"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="114"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="115"/>
-      <c r="M8" s="115"/>
+      <c r="L8" s="135"/>
+      <c r="M8" s="135"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
+      <c r="O8" s="136"/>
+      <c r="P8" s="136"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4129,24 +4151,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="113"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="114"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="115"/>
-      <c r="M9" s="115"/>
+      <c r="L9" s="135"/>
+      <c r="M9" s="135"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
+      <c r="O9" s="136"/>
+      <c r="P9" s="136"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
+      <c r="R9" s="125"/>
+      <c r="S9" s="125"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4180,24 +4202,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="112"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="113"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="114"/>
-      <c r="J10" s="114"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="115"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="116"/>
+      <c r="O10" s="136"/>
+      <c r="P10" s="136"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="106"/>
+      <c r="R10" s="125"/>
+      <c r="S10" s="125"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4286,23 +4308,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="107" t="s">
+      <c r="F12" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="107"/>
+      <c r="G12" s="126"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="108" t="s">
+      <c r="I12" s="127" t="s">
         <v>173</v>
       </c>
-      <c r="J12" s="108"/>
+      <c r="J12" s="127"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="109" t="s">
+      <c r="L12" s="128" t="s">
         <v>174</v>
       </c>
-      <c r="M12" s="109"/>
+      <c r="M12" s="128"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
+      <c r="O12" s="132"/>
+      <c r="P12" s="132"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4343,17 +4365,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="108"/>
-      <c r="J13" s="108"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="109"/>
-      <c r="M13" s="109"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="128"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="124"/>
-      <c r="P13" s="124"/>
+      <c r="O13" s="132"/>
+      <c r="P13" s="132"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4394,17 +4416,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="107"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="108"/>
-      <c r="J14" s="108"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="109"/>
+      <c r="L14" s="128"/>
+      <c r="M14" s="128"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="124"/>
+      <c r="O14" s="132"/>
+      <c r="P14" s="132"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4445,17 +4467,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="107"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="126"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="108"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="109"/>
-      <c r="M15" s="109"/>
+      <c r="L15" s="128"/>
+      <c r="M15" s="128"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="124"/>
-      <c r="P15" s="124"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="132"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -4496,17 +4518,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="107"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="109"/>
-      <c r="M16" s="109"/>
+      <c r="L16" s="128"/>
+      <c r="M16" s="128"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="124"/>
-      <c r="P16" s="124"/>
+      <c r="O16" s="132"/>
+      <c r="P16" s="132"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -4547,17 +4569,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="107"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="108"/>
-      <c r="J17" s="108"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="109"/>
-      <c r="M17" s="109"/>
+      <c r="L17" s="128"/>
+      <c r="M17" s="128"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
+      <c r="O17" s="132"/>
+      <c r="P17" s="132"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -4598,17 +4620,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="107"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="109"/>
-      <c r="M18" s="109"/>
+      <c r="L18" s="128"/>
+      <c r="M18" s="128"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="124"/>
-      <c r="P18" s="124"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="132"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -4649,17 +4671,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="107"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="127"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="109"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="128"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="124"/>
-      <c r="P19" s="124"/>
+      <c r="O19" s="132"/>
+      <c r="P19" s="132"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -4700,17 +4722,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="126"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="108"/>
-      <c r="J20" s="108"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="127"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="109"/>
+      <c r="L20" s="128"/>
+      <c r="M20" s="128"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="124"/>
-      <c r="P20" s="124"/>
+      <c r="O20" s="132"/>
+      <c r="P20" s="132"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17261,7 +17283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -17283,7 +17305,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="139" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -17623,7 +17645,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119"/>
+      <c r="A2" s="139"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -17949,15 +17971,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="120"/>
-      <c r="DH2" s="120"/>
-      <c r="DI2" s="120"/>
-      <c r="DJ2" s="120"/>
+      <c r="DG2" s="140"/>
+      <c r="DH2" s="140"/>
+      <c r="DI2" s="140"/>
+      <c r="DJ2" s="140"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="119"/>
+      <c r="A3" s="139"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18294,7 +18316,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="141" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18436,7 +18458,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="121"/>
+      <c r="B5" s="141"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -18576,7 +18598,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="121"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -18716,7 +18738,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="121"/>
+      <c r="B7" s="141"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -18854,7 +18876,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="121"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -18994,7 +19016,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="142" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19136,7 +19158,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="122"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19276,7 +19298,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="143" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19406,7 +19428,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="123"/>
+      <c r="B12" s="143"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -19544,7 +19566,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="123"/>
+      <c r="B13" s="143"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -19684,7 +19706,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="123"/>
+      <c r="B14" s="143"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -19820,7 +19842,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="123"/>
+      <c r="B15" s="143"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -19956,7 +19978,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="123"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20092,7 +20114,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="123"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20228,7 +20250,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="123"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20368,7 +20390,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="123"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -20504,7 +20526,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="123"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -20640,7 +20662,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="137" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -20774,7 +20796,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="117"/>
+      <c r="B22" s="137"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -20910,7 +20932,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="117"/>
+      <c r="B23" s="137"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21042,7 +21064,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="117"/>
+      <c r="B24" s="137"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21176,7 +21198,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="117"/>
+      <c r="B25" s="137"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21320,7 +21342,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="118" t="s">
+      <c r="B26" s="138" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -21454,7 +21476,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="118"/>
+      <c r="B27" s="138"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -21594,7 +21616,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="118"/>
+      <c r="B28" s="138"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -21726,7 +21748,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="118"/>
+      <c r="B29" s="138"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -21854,7 +21876,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="118"/>
+      <c r="B30" s="138"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -21980,7 +22002,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="118"/>
+      <c r="B31" s="138"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 03-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607835C1-8DBF-43A1-B412-C81578E355A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6707C3-C9E7-41B6-824B-252C15677646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="268">
   <si>
     <t>REDES</t>
   </si>
@@ -904,6 +904,18 @@
   </si>
   <si>
     <t>Reunião com o cliente. Planning</t>
+  </si>
+  <si>
+    <t>Planning e ajuste menu mobile</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente. Divisão de tarefas</t>
+  </si>
+  <si>
+    <t>Dashboard, página passo a paso inicial, listagem prospectores e vendedores API, documentação, ajustar calendário de cadastro de agenda para formato 24h</t>
+  </si>
+  <si>
+    <t>Planning. Configuração cosmos db emulator, listagem de blocos</t>
   </si>
 </sst>
 </file>
@@ -1798,18 +1810,6 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1818,6 +1818,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2273,10 +2285,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AK4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AI4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AN7" sqref="AN7"/>
+      <selection pane="bottomRight" activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2298,8 +2310,8 @@
     <col min="32" max="32" width="20.77734375" customWidth="1"/>
     <col min="33" max="36" width="25.77734375" customWidth="1"/>
     <col min="37" max="38" width="20.77734375" customWidth="1"/>
-    <col min="39" max="39" width="25.77734375" customWidth="1"/>
-    <col min="40" max="47" width="15.77734375" customWidth="1"/>
+    <col min="39" max="40" width="25.77734375" customWidth="1"/>
+    <col min="41" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="71" width="5.77734375" customWidth="1"/>
@@ -2312,7 +2324,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="118" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2592,7 +2604,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123"/>
+      <c r="A2" s="119"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2702,7 +2714,7 @@
       <c r="CR2" s="121"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="124"/>
+      <c r="A3" s="120"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2990,10 +3002,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="119"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -3105,7 +3117,9 @@
       <c r="AM4" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="AN4" s="96"/>
+      <c r="AN4" s="96" t="s">
+        <v>264</v>
+      </c>
       <c r="AO4" s="96"/>
       <c r="AP4" s="96"/>
       <c r="AQ4" s="96"/>
@@ -3113,10 +3127,10 @@
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="122" t="s">
         <v>112</v>
       </c>
       <c r="AX4" s="99"/>
@@ -3141,12 +3155,12 @@
       <c r="BQ4" s="106"/>
       <c r="BR4" s="106"/>
       <c r="BS4" s="108"/>
-      <c r="BT4" s="120" t="s">
+      <c r="BT4" s="122" t="s">
         <v>113</v>
       </c>
       <c r="BU4" s="113"/>
       <c r="BV4" s="114"/>
-      <c r="BW4" s="120" t="s">
+      <c r="BW4" s="122" t="s">
         <v>114</v>
       </c>
       <c r="BX4" s="109"/>
@@ -3166,15 +3180,15 @@
       <c r="CL4" s="116"/>
       <c r="CM4" s="116"/>
       <c r="CN4" s="117"/>
-      <c r="CO4" s="120" t="s">
+      <c r="CO4" s="122" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="119"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3284,7 +3298,9 @@
       <c r="AM5" s="96" t="s">
         <v>261</v>
       </c>
-      <c r="AN5" s="96"/>
+      <c r="AN5" s="96" t="s">
+        <v>265</v>
+      </c>
       <c r="AO5" s="96"/>
       <c r="AP5" s="96"/>
       <c r="AQ5" s="96"/>
@@ -3292,8 +3308,8 @@
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
+      <c r="AV5" s="122"/>
+      <c r="AW5" s="122"/>
       <c r="AX5" s="102"/>
       <c r="AY5" s="101"/>
       <c r="AZ5" s="101"/>
@@ -3316,10 +3332,10 @@
       <c r="BQ5" s="106"/>
       <c r="BR5" s="106"/>
       <c r="BS5" s="108"/>
-      <c r="BT5" s="120"/>
+      <c r="BT5" s="122"/>
       <c r="BU5" s="111"/>
       <c r="BV5" s="112"/>
-      <c r="BW5" s="120"/>
+      <c r="BW5" s="122"/>
       <c r="BX5" s="110"/>
       <c r="BY5" s="106"/>
       <c r="BZ5" s="115"/>
@@ -3337,13 +3353,13 @@
       <c r="CL5" s="116"/>
       <c r="CM5" s="116"/>
       <c r="CN5" s="117"/>
-      <c r="CO5" s="120"/>
+      <c r="CO5" s="122"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="123" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="119"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3455,7 +3471,9 @@
       <c r="AM6" s="96" t="s">
         <v>262</v>
       </c>
-      <c r="AN6" s="96"/>
+      <c r="AN6" s="96" t="s">
+        <v>266</v>
+      </c>
       <c r="AO6" s="96"/>
       <c r="AP6" s="96"/>
       <c r="AQ6" s="96"/>
@@ -3463,8 +3481,8 @@
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
+      <c r="AV6" s="122"/>
+      <c r="AW6" s="122"/>
       <c r="AX6" s="102"/>
       <c r="AY6" s="101"/>
       <c r="AZ6" s="101"/>
@@ -3487,10 +3505,10 @@
       <c r="BQ6" s="106"/>
       <c r="BR6" s="106"/>
       <c r="BS6" s="108"/>
-      <c r="BT6" s="120"/>
+      <c r="BT6" s="122"/>
       <c r="BU6" s="111"/>
       <c r="BV6" s="112"/>
-      <c r="BW6" s="120"/>
+      <c r="BW6" s="122"/>
       <c r="BX6" s="110"/>
       <c r="BY6" s="106"/>
       <c r="BZ6" s="115"/>
@@ -3508,13 +3526,13 @@
       <c r="CL6" s="116"/>
       <c r="CM6" s="116"/>
       <c r="CN6" s="117"/>
-      <c r="CO6" s="120"/>
+      <c r="CO6" s="122"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="123" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="119"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3626,7 +3644,9 @@
       <c r="AM7" s="96" t="s">
         <v>263</v>
       </c>
-      <c r="AN7" s="96"/>
+      <c r="AN7" s="96" t="s">
+        <v>267</v>
+      </c>
       <c r="AO7" s="96"/>
       <c r="AP7" s="96"/>
       <c r="AQ7" s="96"/>
@@ -3634,8 +3654,8 @@
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
+      <c r="AV7" s="122"/>
+      <c r="AW7" s="122"/>
       <c r="AX7" s="102"/>
       <c r="AY7" s="101"/>
       <c r="AZ7" s="101"/>
@@ -3658,10 +3678,10 @@
       <c r="BQ7" s="106"/>
       <c r="BR7" s="106"/>
       <c r="BS7" s="107"/>
-      <c r="BT7" s="120"/>
+      <c r="BT7" s="122"/>
       <c r="BU7" s="111"/>
       <c r="BV7" s="112"/>
-      <c r="BW7" s="120"/>
+      <c r="BW7" s="122"/>
       <c r="BX7" s="110"/>
       <c r="BY7" s="106"/>
       <c r="BZ7" s="115"/>
@@ -3679,25 +3699,25 @@
       <c r="CL7" s="116"/>
       <c r="CM7" s="116"/>
       <c r="CN7" s="117"/>
-      <c r="CO7" s="120"/>
+      <c r="CO7" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 04-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6707C3-C9E7-41B6-824B-252C15677646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -27,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="272">
   <si>
     <t>REDES</t>
   </si>
@@ -916,12 +915,24 @@
   </si>
   <si>
     <t>Planning. Configuração cosmos db emulator, listagem de blocos</t>
+  </si>
+  <si>
+    <t>Planning. Estudo requisições para o banco de dados. Ajuste lista de usuários mobile. Teste de requisições API com o Postman</t>
+  </si>
+  <si>
+    <t>Layouts de alta fidelidade e HTML + CSS das páginas</t>
+  </si>
+  <si>
+    <t>Página Dashboard, gerar senha automática no cadastro de usuário, alteração listagem de usuários, ajuste no relógio e calendário no cadastro, descomponentização, passo a passo</t>
+  </si>
+  <si>
+    <t>Planning. Diagrama de classe levels, configuração cosmos db emulator, layout alta fidelidade recompensas, ajuste listagem de blocos web</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1810,6 +1821,18 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1818,18 +1841,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2281,14 +2292,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AI4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AM4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AO7" sqref="AO7"/>
+      <selection pane="bottomRight" activeCell="AP6" sqref="AP6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2310,8 +2321,8 @@
     <col min="32" max="32" width="20.77734375" customWidth="1"/>
     <col min="33" max="36" width="25.77734375" customWidth="1"/>
     <col min="37" max="38" width="20.77734375" customWidth="1"/>
-    <col min="39" max="40" width="25.77734375" customWidth="1"/>
-    <col min="41" max="47" width="15.77734375" customWidth="1"/>
+    <col min="39" max="41" width="25.77734375" customWidth="1"/>
+    <col min="42" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="71" width="5.77734375" customWidth="1"/>
@@ -2324,7 +2335,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="122" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2604,7 +2615,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="119"/>
+      <c r="A2" s="123"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2714,7 +2725,7 @@
       <c r="CR2" s="121"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="120"/>
+      <c r="A3" s="124"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3002,10 +3013,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="118" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="124"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -3120,17 +3131,19 @@
       <c r="AN4" s="96" t="s">
         <v>264</v>
       </c>
-      <c r="AO4" s="96"/>
+      <c r="AO4" s="96" t="s">
+        <v>268</v>
+      </c>
       <c r="AP4" s="96"/>
       <c r="AQ4" s="96"/>
       <c r="AR4" s="96"/>
       <c r="AS4" s="96"/>
       <c r="AT4" s="96"/>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="122" t="s">
+      <c r="AV4" s="120" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="122" t="s">
+      <c r="AW4" s="120" t="s">
         <v>112</v>
       </c>
       <c r="AX4" s="99"/>
@@ -3155,12 +3168,12 @@
       <c r="BQ4" s="106"/>
       <c r="BR4" s="106"/>
       <c r="BS4" s="108"/>
-      <c r="BT4" s="122" t="s">
+      <c r="BT4" s="120" t="s">
         <v>113</v>
       </c>
       <c r="BU4" s="113"/>
       <c r="BV4" s="114"/>
-      <c r="BW4" s="122" t="s">
+      <c r="BW4" s="120" t="s">
         <v>114</v>
       </c>
       <c r="BX4" s="109"/>
@@ -3180,15 +3193,15 @@
       <c r="CL4" s="116"/>
       <c r="CM4" s="116"/>
       <c r="CN4" s="117"/>
-      <c r="CO4" s="122" t="s">
+      <c r="CO4" s="120" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="123" t="s">
+      <c r="A5" s="118" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="124"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3301,15 +3314,17 @@
       <c r="AN5" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="AO5" s="96"/>
+      <c r="AO5" s="96" t="s">
+        <v>269</v>
+      </c>
       <c r="AP5" s="96"/>
       <c r="AQ5" s="96"/>
       <c r="AR5" s="96"/>
       <c r="AS5" s="96"/>
       <c r="AT5" s="96"/>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="122"/>
-      <c r="AW5" s="122"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
       <c r="AX5" s="102"/>
       <c r="AY5" s="101"/>
       <c r="AZ5" s="101"/>
@@ -3332,10 +3347,10 @@
       <c r="BQ5" s="106"/>
       <c r="BR5" s="106"/>
       <c r="BS5" s="108"/>
-      <c r="BT5" s="122"/>
+      <c r="BT5" s="120"/>
       <c r="BU5" s="111"/>
       <c r="BV5" s="112"/>
-      <c r="BW5" s="122"/>
+      <c r="BW5" s="120"/>
       <c r="BX5" s="110"/>
       <c r="BY5" s="106"/>
       <c r="BZ5" s="115"/>
@@ -3353,13 +3368,13 @@
       <c r="CL5" s="116"/>
       <c r="CM5" s="116"/>
       <c r="CN5" s="117"/>
-      <c r="CO5" s="122"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="123" t="s">
+      <c r="A6" s="118" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="124"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3474,15 +3489,17 @@
       <c r="AN6" s="96" t="s">
         <v>266</v>
       </c>
-      <c r="AO6" s="96"/>
+      <c r="AO6" s="96" t="s">
+        <v>270</v>
+      </c>
       <c r="AP6" s="96"/>
       <c r="AQ6" s="96"/>
       <c r="AR6" s="96"/>
       <c r="AS6" s="96"/>
       <c r="AT6" s="96"/>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="122"/>
-      <c r="AW6" s="122"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
       <c r="AX6" s="102"/>
       <c r="AY6" s="101"/>
       <c r="AZ6" s="101"/>
@@ -3505,10 +3522,10 @@
       <c r="BQ6" s="106"/>
       <c r="BR6" s="106"/>
       <c r="BS6" s="108"/>
-      <c r="BT6" s="122"/>
+      <c r="BT6" s="120"/>
       <c r="BU6" s="111"/>
       <c r="BV6" s="112"/>
-      <c r="BW6" s="122"/>
+      <c r="BW6" s="120"/>
       <c r="BX6" s="110"/>
       <c r="BY6" s="106"/>
       <c r="BZ6" s="115"/>
@@ -3526,13 +3543,13 @@
       <c r="CL6" s="116"/>
       <c r="CM6" s="116"/>
       <c r="CN6" s="117"/>
-      <c r="CO6" s="122"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="124"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3647,15 +3664,17 @@
       <c r="AN7" s="96" t="s">
         <v>267</v>
       </c>
-      <c r="AO7" s="96"/>
+      <c r="AO7" s="96" t="s">
+        <v>271</v>
+      </c>
       <c r="AP7" s="96"/>
       <c r="AQ7" s="96"/>
       <c r="AR7" s="96"/>
       <c r="AS7" s="96"/>
       <c r="AT7" s="96"/>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="122"/>
-      <c r="AW7" s="122"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
       <c r="AX7" s="102"/>
       <c r="AY7" s="101"/>
       <c r="AZ7" s="101"/>
@@ -3678,10 +3697,10 @@
       <c r="BQ7" s="106"/>
       <c r="BR7" s="106"/>
       <c r="BS7" s="107"/>
-      <c r="BT7" s="122"/>
+      <c r="BT7" s="120"/>
       <c r="BU7" s="111"/>
       <c r="BV7" s="112"/>
-      <c r="BW7" s="122"/>
+      <c r="BW7" s="120"/>
       <c r="BX7" s="110"/>
       <c r="BY7" s="106"/>
       <c r="BZ7" s="115"/>
@@ -3699,25 +3718,25 @@
       <c r="CL7" s="116"/>
       <c r="CM7" s="116"/>
       <c r="CN7" s="117"/>
-      <c r="CO7" s="122"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3726,7 +3745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -17303,7 +17322,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona daily realizada em 11-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13E8290-DBC2-42E4-8DE0-6225092665EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="278">
   <si>
     <t>REDES</t>
   </si>
@@ -927,12 +928,30 @@
   </si>
   <si>
     <t>Planning. Diagrama de classe levels, configuração cosmos db emulator, layout alta fidelidade recompensas, ajuste listagem de blocos web</t>
+  </si>
+  <si>
+    <t>Não foi possível realizar a daily devido às atividades do SAEP</t>
+  </si>
+  <si>
+    <t>Prova SAEP</t>
+  </si>
+  <si>
+    <t>Edição logout web, ajustes login web e lista de chamados web. Editar usuário API</t>
+  </si>
+  <si>
+    <t>Implementando gráfcos na página relatórios, listagem de hostgroups, documentação do projeto II</t>
+  </si>
+  <si>
+    <t>Métodos para envio de senha por e-mail ao realizar cadastro, páginas de confirmação e alterar senha. Funcionalidades de listagem e cadastro nos modais. Funcionalidade de cadastro genérico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layout de alta de fidelidade levels, loading e sweet alert, diagrama de classes e modelagem banco de dados. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1821,18 +1840,6 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1841,6 +1848,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2292,14 +2311,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AM4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP6" sqref="AP6"/>
+      <selection pane="bottomRight" activeCell="AU7" sqref="AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2322,7 +2341,9 @@
     <col min="33" max="36" width="25.77734375" customWidth="1"/>
     <col min="37" max="38" width="20.77734375" customWidth="1"/>
     <col min="39" max="41" width="25.77734375" customWidth="1"/>
-    <col min="42" max="47" width="15.77734375" customWidth="1"/>
+    <col min="42" max="45" width="15.77734375" customWidth="1"/>
+    <col min="46" max="46" width="35.77734375" customWidth="1"/>
+    <col min="47" max="47" width="15.77734375" customWidth="1"/>
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="71" width="5.77734375" customWidth="1"/>
@@ -2335,7 +2356,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="118" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2615,7 +2636,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123"/>
+      <c r="A2" s="119"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2725,7 +2746,7 @@
       <c r="CR2" s="121"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="124"/>
+      <c r="A3" s="120"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3013,10 +3034,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="119"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="91" t="s">
         <v>118</v>
       </c>
@@ -3134,16 +3155,26 @@
       <c r="AO4" s="96" t="s">
         <v>268</v>
       </c>
-      <c r="AP4" s="96"/>
-      <c r="AQ4" s="96"/>
-      <c r="AR4" s="96"/>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="96"/>
+      <c r="AP4" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AQ4" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AR4" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AS4" s="96" t="s">
+        <v>273</v>
+      </c>
+      <c r="AT4" s="96" t="s">
+        <v>274</v>
+      </c>
       <c r="AU4" s="97"/>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="122" t="s">
         <v>112</v>
       </c>
       <c r="AX4" s="99"/>
@@ -3168,12 +3199,12 @@
       <c r="BQ4" s="106"/>
       <c r="BR4" s="106"/>
       <c r="BS4" s="108"/>
-      <c r="BT4" s="120" t="s">
+      <c r="BT4" s="122" t="s">
         <v>113</v>
       </c>
       <c r="BU4" s="113"/>
       <c r="BV4" s="114"/>
-      <c r="BW4" s="120" t="s">
+      <c r="BW4" s="122" t="s">
         <v>114</v>
       </c>
       <c r="BX4" s="109"/>
@@ -3193,15 +3224,15 @@
       <c r="CL4" s="116"/>
       <c r="CM4" s="116"/>
       <c r="CN4" s="117"/>
-      <c r="CO4" s="120" t="s">
+      <c r="CO4" s="122" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="119"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="91" t="s">
         <v>118</v>
       </c>
@@ -3317,14 +3348,24 @@
       <c r="AO5" s="96" t="s">
         <v>269</v>
       </c>
-      <c r="AP5" s="96"/>
-      <c r="AQ5" s="96"/>
-      <c r="AR5" s="96"/>
-      <c r="AS5" s="96"/>
-      <c r="AT5" s="96"/>
+      <c r="AP5" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AQ5" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AR5" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AS5" s="96" t="s">
+        <v>273</v>
+      </c>
+      <c r="AT5" s="96" t="s">
+        <v>275</v>
+      </c>
       <c r="AU5" s="98"/>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
+      <c r="AV5" s="122"/>
+      <c r="AW5" s="122"/>
       <c r="AX5" s="102"/>
       <c r="AY5" s="101"/>
       <c r="AZ5" s="101"/>
@@ -3347,10 +3388,10 @@
       <c r="BQ5" s="106"/>
       <c r="BR5" s="106"/>
       <c r="BS5" s="108"/>
-      <c r="BT5" s="120"/>
+      <c r="BT5" s="122"/>
       <c r="BU5" s="111"/>
       <c r="BV5" s="112"/>
-      <c r="BW5" s="120"/>
+      <c r="BW5" s="122"/>
       <c r="BX5" s="110"/>
       <c r="BY5" s="106"/>
       <c r="BZ5" s="115"/>
@@ -3368,13 +3409,13 @@
       <c r="CL5" s="116"/>
       <c r="CM5" s="116"/>
       <c r="CN5" s="117"/>
-      <c r="CO5" s="120"/>
+      <c r="CO5" s="122"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="123" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="119"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="91" t="s">
         <v>118</v>
       </c>
@@ -3492,14 +3533,24 @@
       <c r="AO6" s="96" t="s">
         <v>270</v>
       </c>
-      <c r="AP6" s="96"/>
-      <c r="AQ6" s="96"/>
-      <c r="AR6" s="96"/>
-      <c r="AS6" s="96"/>
-      <c r="AT6" s="96"/>
+      <c r="AP6" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AQ6" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AR6" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AS6" s="96" t="s">
+        <v>273</v>
+      </c>
+      <c r="AT6" s="96" t="s">
+        <v>276</v>
+      </c>
       <c r="AU6" s="97"/>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
+      <c r="AV6" s="122"/>
+      <c r="AW6" s="122"/>
       <c r="AX6" s="102"/>
       <c r="AY6" s="101"/>
       <c r="AZ6" s="101"/>
@@ -3522,10 +3573,10 @@
       <c r="BQ6" s="106"/>
       <c r="BR6" s="106"/>
       <c r="BS6" s="108"/>
-      <c r="BT6" s="120"/>
+      <c r="BT6" s="122"/>
       <c r="BU6" s="111"/>
       <c r="BV6" s="112"/>
-      <c r="BW6" s="120"/>
+      <c r="BW6" s="122"/>
       <c r="BX6" s="110"/>
       <c r="BY6" s="106"/>
       <c r="BZ6" s="115"/>
@@ -3543,13 +3594,13 @@
       <c r="CL6" s="116"/>
       <c r="CM6" s="116"/>
       <c r="CN6" s="117"/>
-      <c r="CO6" s="120"/>
+      <c r="CO6" s="122"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="123" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="119"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="91" t="s">
         <v>118</v>
       </c>
@@ -3667,14 +3718,24 @@
       <c r="AO7" s="96" t="s">
         <v>271</v>
       </c>
-      <c r="AP7" s="96"/>
-      <c r="AQ7" s="96"/>
-      <c r="AR7" s="96"/>
-      <c r="AS7" s="96"/>
-      <c r="AT7" s="96"/>
+      <c r="AP7" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AQ7" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AR7" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="AS7" s="96" t="s">
+        <v>273</v>
+      </c>
+      <c r="AT7" s="96" t="s">
+        <v>277</v>
+      </c>
       <c r="AU7" s="97"/>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
+      <c r="AV7" s="122"/>
+      <c r="AW7" s="122"/>
       <c r="AX7" s="102"/>
       <c r="AY7" s="101"/>
       <c r="AZ7" s="101"/>
@@ -3697,10 +3758,10 @@
       <c r="BQ7" s="106"/>
       <c r="BR7" s="106"/>
       <c r="BS7" s="107"/>
-      <c r="BT7" s="120"/>
+      <c r="BT7" s="122"/>
       <c r="BU7" s="111"/>
       <c r="BV7" s="112"/>
-      <c r="BW7" s="120"/>
+      <c r="BW7" s="122"/>
       <c r="BX7" s="110"/>
       <c r="BY7" s="106"/>
       <c r="BZ7" s="115"/>
@@ -3718,25 +3779,25 @@
       <c r="CL7" s="116"/>
       <c r="CM7" s="116"/>
       <c r="CN7" s="117"/>
-      <c r="CO7" s="120"/>
+      <c r="CO7" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3745,7 +3806,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -17322,7 +17383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona daily realizada em 18-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB55161-2A07-47A3-B3E6-53CAC7E36A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="290">
   <si>
     <t>REDES</t>
   </si>
@@ -969,12 +970,24 @@
   </si>
   <si>
     <t>Alinhamento das funcionalidades do levels, configuração do cosmos emulator, tela criação de level, CRUD achtievements API, aprimoramento feedback para o usuário, ajuste no cadastro de data de blocos</t>
+  </si>
+  <si>
+    <t>Lista de chamados e de usuários API, lista de chamados web, validação de input no cadastro de chamado e usuário mobile, solicitação de cadastro de usuário</t>
+  </si>
+  <si>
+    <t>Funcionalidade logout, contagem de computador por host e filtro de pesquisa na listagem de web</t>
+  </si>
+  <si>
+    <t>Correção de erros na dashboard, estudo Hooks, estilização página de listagem de funcionários, criação dos endpoints para cadastro, alteração e confirmação de senha</t>
+  </si>
+  <si>
+    <t>Estilização página criar novo level, modelagem do achievement do banco de dados, documentação, layout de alta fidelidade level, listagem do level web</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1809,9 +1822,6 @@
     <xf numFmtId="0" fontId="12" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1857,6 +1867,21 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1865,18 +1890,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1935,7 +1948,7 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2331,14 +2344,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="AU4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AX8" sqref="AX8"/>
+      <selection pane="bottomRight" activeCell="BA7" sqref="BA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2366,7 +2379,8 @@
     <col min="48" max="48" width="3.77734375" style="79" customWidth="1"/>
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="50" width="30.77734375" customWidth="1"/>
-    <col min="51" max="71" width="5.77734375" customWidth="1"/>
+    <col min="51" max="51" width="25.77734375" customWidth="1"/>
+    <col min="52" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2376,7 +2390,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="120" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2656,7 +2670,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="117"/>
+      <c r="A2" s="121"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2766,7 +2780,7 @@
       <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="118"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -2917,10 +2931,10 @@
       <c r="AY3" s="99">
         <v>17</v>
       </c>
-      <c r="AZ3" s="102">
+      <c r="AZ3" s="101">
         <v>18</v>
       </c>
-      <c r="BA3" s="102">
+      <c r="BA3" s="101">
         <v>21</v>
       </c>
       <c r="BB3" s="99">
@@ -2932,10 +2946,10 @@
       <c r="BD3" s="99">
         <v>24</v>
       </c>
-      <c r="BE3" s="102">
+      <c r="BE3" s="101">
         <v>25</v>
       </c>
-      <c r="BF3" s="102">
+      <c r="BF3" s="101">
         <v>28</v>
       </c>
       <c r="BG3" s="99">
@@ -2947,10 +2961,10 @@
       <c r="BI3" s="99">
         <v>31</v>
       </c>
-      <c r="BJ3" s="102">
+      <c r="BJ3" s="101">
         <v>1</v>
       </c>
-      <c r="BK3" s="102">
+      <c r="BK3" s="101">
         <v>4</v>
       </c>
       <c r="BL3" s="99">
@@ -2962,10 +2976,10 @@
       <c r="BN3" s="99">
         <v>7</v>
       </c>
-      <c r="BO3" s="102">
+      <c r="BO3" s="101">
         <v>8</v>
       </c>
-      <c r="BP3" s="102">
+      <c r="BP3" s="101">
         <v>11</v>
       </c>
       <c r="BQ3" s="99">
@@ -2980,7 +2994,7 @@
       <c r="BT3" s="83">
         <v>15</v>
       </c>
-      <c r="BU3" s="102">
+      <c r="BU3" s="101">
         <v>18</v>
       </c>
       <c r="BV3" s="99">
@@ -2992,10 +3006,10 @@
       <c r="BX3" s="99">
         <v>21</v>
       </c>
-      <c r="BY3" s="102">
+      <c r="BY3" s="101">
         <v>22</v>
       </c>
-      <c r="BZ3" s="102">
+      <c r="BZ3" s="101">
         <v>25</v>
       </c>
       <c r="CA3" s="99">
@@ -3007,10 +3021,10 @@
       <c r="CC3" s="99">
         <v>28</v>
       </c>
-      <c r="CD3" s="102">
+      <c r="CD3" s="101">
         <v>29</v>
       </c>
-      <c r="CE3" s="102">
+      <c r="CE3" s="101">
         <v>2</v>
       </c>
       <c r="CF3" s="99">
@@ -3022,10 +3036,10 @@
       <c r="CH3" s="99">
         <v>5</v>
       </c>
-      <c r="CI3" s="102">
+      <c r="CI3" s="101">
         <v>6</v>
       </c>
-      <c r="CJ3" s="102">
+      <c r="CJ3" s="101">
         <v>9</v>
       </c>
       <c r="CK3" s="99">
@@ -3037,13 +3051,13 @@
       <c r="CM3" s="99">
         <v>12</v>
       </c>
-      <c r="CN3" s="102">
+      <c r="CN3" s="101">
         <v>13</v>
       </c>
       <c r="CO3" s="83">
         <v>14</v>
       </c>
-      <c r="CP3" s="103">
+      <c r="CP3" s="102">
         <v>16</v>
       </c>
       <c r="CQ3" s="85">
@@ -3054,10 +3068,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3193,70 +3207,72 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="118" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="118" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
         <v>282</v>
       </c>
-      <c r="AY4" s="100"/>
-      <c r="AZ4" s="100"/>
-      <c r="BA4" s="100"/>
-      <c r="BB4" s="100"/>
-      <c r="BC4" s="100"/>
-      <c r="BD4" s="100"/>
-      <c r="BE4" s="100"/>
-      <c r="BF4" s="101"/>
-      <c r="BG4" s="101"/>
-      <c r="BH4" s="101"/>
-      <c r="BI4" s="101"/>
-      <c r="BJ4" s="101"/>
-      <c r="BK4" s="101"/>
-      <c r="BL4" s="101"/>
-      <c r="BM4" s="101"/>
-      <c r="BN4" s="101"/>
-      <c r="BO4" s="101"/>
-      <c r="BP4" s="104"/>
-      <c r="BQ4" s="104"/>
-      <c r="BR4" s="104"/>
-      <c r="BS4" s="106"/>
-      <c r="BT4" s="120" t="s">
+      <c r="AY4" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="AZ4" s="142"/>
+      <c r="BA4" s="142"/>
+      <c r="BB4" s="142"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="142"/>
+      <c r="BE4" s="142"/>
+      <c r="BF4" s="100"/>
+      <c r="BG4" s="100"/>
+      <c r="BH4" s="100"/>
+      <c r="BI4" s="100"/>
+      <c r="BJ4" s="100"/>
+      <c r="BK4" s="100"/>
+      <c r="BL4" s="100"/>
+      <c r="BM4" s="100"/>
+      <c r="BN4" s="100"/>
+      <c r="BO4" s="100"/>
+      <c r="BP4" s="103"/>
+      <c r="BQ4" s="103"/>
+      <c r="BR4" s="103"/>
+      <c r="BS4" s="105"/>
+      <c r="BT4" s="118" t="s">
         <v>112</v>
       </c>
-      <c r="BU4" s="111"/>
-      <c r="BV4" s="112"/>
-      <c r="BW4" s="120" t="s">
+      <c r="BU4" s="110"/>
+      <c r="BV4" s="111"/>
+      <c r="BW4" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="107"/>
-      <c r="BY4" s="104"/>
-      <c r="BZ4" s="113"/>
-      <c r="CA4" s="113"/>
-      <c r="CB4" s="113"/>
-      <c r="CC4" s="113"/>
-      <c r="CD4" s="113"/>
-      <c r="CE4" s="113"/>
-      <c r="CF4" s="113"/>
-      <c r="CG4" s="113"/>
-      <c r="CH4" s="113"/>
-      <c r="CI4" s="113"/>
-      <c r="CJ4" s="114"/>
-      <c r="CK4" s="114"/>
-      <c r="CL4" s="114"/>
-      <c r="CM4" s="114"/>
-      <c r="CN4" s="115"/>
-      <c r="CO4" s="120" t="s">
+      <c r="BX4" s="106"/>
+      <c r="BY4" s="103"/>
+      <c r="BZ4" s="112"/>
+      <c r="CA4" s="112"/>
+      <c r="CB4" s="112"/>
+      <c r="CC4" s="112"/>
+      <c r="CD4" s="112"/>
+      <c r="CE4" s="112"/>
+      <c r="CF4" s="112"/>
+      <c r="CG4" s="112"/>
+      <c r="CH4" s="112"/>
+      <c r="CI4" s="112"/>
+      <c r="CJ4" s="113"/>
+      <c r="CK4" s="113"/>
+      <c r="CL4" s="113"/>
+      <c r="CM4" s="113"/>
+      <c r="CN4" s="114"/>
+      <c r="CO4" s="118" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3390,60 +3406,62 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
-      <c r="AX5" s="142" t="s">
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
-      <c r="AY5" s="100"/>
-      <c r="AZ5" s="100"/>
-      <c r="BA5" s="100"/>
-      <c r="BB5" s="100"/>
-      <c r="BC5" s="100"/>
-      <c r="BD5" s="100"/>
-      <c r="BE5" s="100"/>
-      <c r="BF5" s="101"/>
-      <c r="BG5" s="101"/>
-      <c r="BH5" s="101"/>
-      <c r="BI5" s="101"/>
-      <c r="BJ5" s="101"/>
-      <c r="BK5" s="101"/>
-      <c r="BL5" s="101"/>
-      <c r="BM5" s="101"/>
-      <c r="BN5" s="101"/>
-      <c r="BO5" s="101"/>
-      <c r="BP5" s="104"/>
-      <c r="BQ5" s="104"/>
-      <c r="BR5" s="104"/>
-      <c r="BS5" s="106"/>
-      <c r="BT5" s="120"/>
-      <c r="BU5" s="109"/>
-      <c r="BV5" s="110"/>
-      <c r="BW5" s="120"/>
-      <c r="BX5" s="108"/>
-      <c r="BY5" s="104"/>
-      <c r="BZ5" s="113"/>
-      <c r="CA5" s="113"/>
-      <c r="CB5" s="113"/>
-      <c r="CC5" s="113"/>
-      <c r="CD5" s="113"/>
-      <c r="CE5" s="113"/>
-      <c r="CF5" s="113"/>
-      <c r="CG5" s="113"/>
-      <c r="CH5" s="113"/>
-      <c r="CI5" s="113"/>
-      <c r="CJ5" s="114"/>
-      <c r="CK5" s="114"/>
-      <c r="CL5" s="114"/>
-      <c r="CM5" s="114"/>
-      <c r="CN5" s="115"/>
-      <c r="CO5" s="120"/>
+      <c r="AY5" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="AZ5" s="142"/>
+      <c r="BA5" s="142"/>
+      <c r="BB5" s="142"/>
+      <c r="BC5" s="142"/>
+      <c r="BD5" s="142"/>
+      <c r="BE5" s="142"/>
+      <c r="BF5" s="100"/>
+      <c r="BG5" s="100"/>
+      <c r="BH5" s="100"/>
+      <c r="BI5" s="100"/>
+      <c r="BJ5" s="100"/>
+      <c r="BK5" s="100"/>
+      <c r="BL5" s="100"/>
+      <c r="BM5" s="100"/>
+      <c r="BN5" s="100"/>
+      <c r="BO5" s="100"/>
+      <c r="BP5" s="103"/>
+      <c r="BQ5" s="103"/>
+      <c r="BR5" s="103"/>
+      <c r="BS5" s="105"/>
+      <c r="BT5" s="118"/>
+      <c r="BU5" s="108"/>
+      <c r="BV5" s="109"/>
+      <c r="BW5" s="118"/>
+      <c r="BX5" s="107"/>
+      <c r="BY5" s="103"/>
+      <c r="BZ5" s="112"/>
+      <c r="CA5" s="112"/>
+      <c r="CB5" s="112"/>
+      <c r="CC5" s="112"/>
+      <c r="CD5" s="112"/>
+      <c r="CE5" s="112"/>
+      <c r="CF5" s="112"/>
+      <c r="CG5" s="112"/>
+      <c r="CH5" s="112"/>
+      <c r="CI5" s="112"/>
+      <c r="CJ5" s="113"/>
+      <c r="CK5" s="113"/>
+      <c r="CL5" s="113"/>
+      <c r="CM5" s="113"/>
+      <c r="CN5" s="114"/>
+      <c r="CO5" s="118"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3579,60 +3597,62 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
-      <c r="AX6" s="142" t="s">
+      <c r="AV6" s="118"/>
+      <c r="AW6" s="118"/>
+      <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
-      <c r="AY6" s="100"/>
-      <c r="AZ6" s="100"/>
-      <c r="BA6" s="100"/>
-      <c r="BB6" s="100"/>
-      <c r="BC6" s="100"/>
-      <c r="BD6" s="100"/>
-      <c r="BE6" s="100"/>
-      <c r="BF6" s="101"/>
-      <c r="BG6" s="101"/>
-      <c r="BH6" s="101"/>
-      <c r="BI6" s="101"/>
-      <c r="BJ6" s="101"/>
-      <c r="BK6" s="101"/>
-      <c r="BL6" s="101"/>
-      <c r="BM6" s="101"/>
-      <c r="BN6" s="101"/>
-      <c r="BO6" s="101"/>
-      <c r="BP6" s="104"/>
-      <c r="BQ6" s="104"/>
-      <c r="BR6" s="104"/>
-      <c r="BS6" s="106"/>
-      <c r="BT6" s="120"/>
-      <c r="BU6" s="109"/>
-      <c r="BV6" s="110"/>
-      <c r="BW6" s="120"/>
-      <c r="BX6" s="108"/>
-      <c r="BY6" s="104"/>
-      <c r="BZ6" s="113"/>
-      <c r="CA6" s="113"/>
-      <c r="CB6" s="113"/>
-      <c r="CC6" s="113"/>
-      <c r="CD6" s="113"/>
-      <c r="CE6" s="113"/>
-      <c r="CF6" s="113"/>
-      <c r="CG6" s="113"/>
-      <c r="CH6" s="113"/>
-      <c r="CI6" s="113"/>
-      <c r="CJ6" s="114"/>
-      <c r="CK6" s="114"/>
-      <c r="CL6" s="114"/>
-      <c r="CM6" s="114"/>
-      <c r="CN6" s="115"/>
-      <c r="CO6" s="120"/>
+      <c r="AY6" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="AZ6" s="142"/>
+      <c r="BA6" s="142"/>
+      <c r="BB6" s="142"/>
+      <c r="BC6" s="142"/>
+      <c r="BD6" s="142"/>
+      <c r="BE6" s="142"/>
+      <c r="BF6" s="100"/>
+      <c r="BG6" s="100"/>
+      <c r="BH6" s="100"/>
+      <c r="BI6" s="100"/>
+      <c r="BJ6" s="100"/>
+      <c r="BK6" s="100"/>
+      <c r="BL6" s="100"/>
+      <c r="BM6" s="100"/>
+      <c r="BN6" s="100"/>
+      <c r="BO6" s="100"/>
+      <c r="BP6" s="103"/>
+      <c r="BQ6" s="103"/>
+      <c r="BR6" s="103"/>
+      <c r="BS6" s="105"/>
+      <c r="BT6" s="118"/>
+      <c r="BU6" s="108"/>
+      <c r="BV6" s="109"/>
+      <c r="BW6" s="118"/>
+      <c r="BX6" s="107"/>
+      <c r="BY6" s="103"/>
+      <c r="BZ6" s="112"/>
+      <c r="CA6" s="112"/>
+      <c r="CB6" s="112"/>
+      <c r="CC6" s="112"/>
+      <c r="CD6" s="112"/>
+      <c r="CE6" s="112"/>
+      <c r="CF6" s="112"/>
+      <c r="CG6" s="112"/>
+      <c r="CH6" s="112"/>
+      <c r="CI6" s="112"/>
+      <c r="CJ6" s="113"/>
+      <c r="CK6" s="113"/>
+      <c r="CL6" s="113"/>
+      <c r="CM6" s="113"/>
+      <c r="CN6" s="114"/>
+      <c r="CO6" s="118"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3768,72 +3788,74 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
-      <c r="AX7" s="142" t="s">
+      <c r="AV7" s="118"/>
+      <c r="AW7" s="118"/>
+      <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
-      <c r="AY7" s="100"/>
-      <c r="AZ7" s="100"/>
-      <c r="BA7" s="100"/>
-      <c r="BB7" s="100"/>
-      <c r="BC7" s="100"/>
-      <c r="BD7" s="100"/>
-      <c r="BE7" s="100"/>
-      <c r="BF7" s="101"/>
-      <c r="BG7" s="101"/>
-      <c r="BH7" s="101"/>
-      <c r="BI7" s="101"/>
-      <c r="BJ7" s="101"/>
-      <c r="BK7" s="101"/>
-      <c r="BL7" s="101"/>
-      <c r="BM7" s="101"/>
-      <c r="BN7" s="101"/>
-      <c r="BO7" s="101"/>
-      <c r="BP7" s="104"/>
-      <c r="BQ7" s="104"/>
-      <c r="BR7" s="104"/>
-      <c r="BS7" s="105"/>
-      <c r="BT7" s="120"/>
-      <c r="BU7" s="109"/>
-      <c r="BV7" s="110"/>
-      <c r="BW7" s="120"/>
-      <c r="BX7" s="108"/>
-      <c r="BY7" s="104"/>
-      <c r="BZ7" s="113"/>
-      <c r="CA7" s="113"/>
-      <c r="CB7" s="113"/>
-      <c r="CC7" s="113"/>
-      <c r="CD7" s="113"/>
-      <c r="CE7" s="113"/>
-      <c r="CF7" s="113"/>
-      <c r="CG7" s="113"/>
-      <c r="CH7" s="113"/>
-      <c r="CI7" s="113"/>
-      <c r="CJ7" s="114"/>
-      <c r="CK7" s="114"/>
-      <c r="CL7" s="114"/>
-      <c r="CM7" s="114"/>
-      <c r="CN7" s="115"/>
-      <c r="CO7" s="120"/>
+      <c r="AY7" s="142" t="s">
+        <v>289</v>
+      </c>
+      <c r="AZ7" s="142"/>
+      <c r="BA7" s="142"/>
+      <c r="BB7" s="142"/>
+      <c r="BC7" s="142"/>
+      <c r="BD7" s="142"/>
+      <c r="BE7" s="142"/>
+      <c r="BF7" s="100"/>
+      <c r="BG7" s="100"/>
+      <c r="BH7" s="100"/>
+      <c r="BI7" s="100"/>
+      <c r="BJ7" s="100"/>
+      <c r="BK7" s="100"/>
+      <c r="BL7" s="100"/>
+      <c r="BM7" s="100"/>
+      <c r="BN7" s="100"/>
+      <c r="BO7" s="100"/>
+      <c r="BP7" s="103"/>
+      <c r="BQ7" s="103"/>
+      <c r="BR7" s="103"/>
+      <c r="BS7" s="104"/>
+      <c r="BT7" s="118"/>
+      <c r="BU7" s="108"/>
+      <c r="BV7" s="109"/>
+      <c r="BW7" s="118"/>
+      <c r="BX7" s="107"/>
+      <c r="BY7" s="103"/>
+      <c r="BZ7" s="112"/>
+      <c r="CA7" s="112"/>
+      <c r="CB7" s="112"/>
+      <c r="CC7" s="112"/>
+      <c r="CD7" s="112"/>
+      <c r="CE7" s="112"/>
+      <c r="CF7" s="112"/>
+      <c r="CG7" s="112"/>
+      <c r="CH7" s="112"/>
+      <c r="CI7" s="112"/>
+      <c r="CJ7" s="113"/>
+      <c r="CK7" s="113"/>
+      <c r="CL7" s="113"/>
+      <c r="CM7" s="113"/>
+      <c r="CN7" s="114"/>
+      <c r="CO7" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3842,7 +3864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW265"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -17419,7 +17441,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Adiciona daily realizada em 21-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB55161-2A07-47A3-B3E6-53CAC7E36A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2218D81A-4CD3-46CF-9C82-83C618A6AA91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="294">
   <si>
     <t>REDES</t>
   </si>
@@ -982,6 +982,18 @@
   </si>
   <si>
     <t>Estilização página criar novo level, modelagem do achievement do banco de dados, documentação, layout de alta fidelidade level, listagem do level web</t>
+  </si>
+  <si>
+    <t>Ajustes na listagem de chamados API, estudo GLPI reabrir chamado. Estilização componentes lista de chamados Web. Solicitação de cadastro de usuário API</t>
+  </si>
+  <si>
+    <t>Contagem de computador por host API</t>
+  </si>
+  <si>
+    <t>Correção de erros na dshboard, estilização página de listagem de funcionários, correção de preenchimento do array de busca de endereço através do CEP, validação de inputs de cadastro de usuáros, clientes e agendas</t>
+  </si>
+  <si>
+    <t>Estilização e funcionalidades página criar novo level, layout de alta fidelidade level e documentação</t>
   </si>
 </sst>
 </file>
@@ -1870,17 +1882,8 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1890,6 +1893,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1946,9 +1961,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2348,10 +2360,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AU4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BA7" sqref="BA7"/>
+      <selection pane="bottomRight" activeCell="AZ8" sqref="AZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2380,7 +2392,8 @@
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="50" width="30.77734375" customWidth="1"/>
     <col min="51" max="51" width="25.77734375" customWidth="1"/>
-    <col min="52" max="71" width="5.77734375" customWidth="1"/>
+    <col min="52" max="52" width="35.77734375" customWidth="1"/>
+    <col min="53" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2390,7 +2403,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="117" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2670,117 +2683,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121"/>
+      <c r="A2" s="118"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="120" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="119" t="s">
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="119"/>
-      <c r="T2" s="119"/>
-      <c r="U2" s="119"/>
-      <c r="V2" s="119"/>
-      <c r="W2" s="119"/>
-      <c r="X2" s="119"/>
-      <c r="Y2" s="119"/>
-      <c r="Z2" s="119"/>
-      <c r="AA2" s="119"/>
-      <c r="AB2" s="119"/>
-      <c r="AC2" s="119"/>
-      <c r="AD2" s="119"/>
-      <c r="AE2" s="119"/>
-      <c r="AF2" s="119"/>
-      <c r="AG2" s="119"/>
-      <c r="AH2" s="119"/>
-      <c r="AI2" s="119"/>
-      <c r="AJ2" s="119"/>
-      <c r="AK2" s="119"/>
-      <c r="AL2" s="119"/>
-      <c r="AM2" s="119" t="s">
+      <c r="S2" s="120"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="120"/>
+      <c r="V2" s="120"/>
+      <c r="W2" s="120"/>
+      <c r="X2" s="120"/>
+      <c r="Y2" s="120"/>
+      <c r="Z2" s="120"/>
+      <c r="AA2" s="120"/>
+      <c r="AB2" s="120"/>
+      <c r="AC2" s="120"/>
+      <c r="AD2" s="120"/>
+      <c r="AE2" s="120"/>
+      <c r="AF2" s="120"/>
+      <c r="AG2" s="120"/>
+      <c r="AH2" s="120"/>
+      <c r="AI2" s="120"/>
+      <c r="AJ2" s="120"/>
+      <c r="AK2" s="120"/>
+      <c r="AL2" s="120"/>
+      <c r="AM2" s="120" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="119"/>
-      <c r="AO2" s="119"/>
-      <c r="AP2" s="119"/>
-      <c r="AQ2" s="119"/>
-      <c r="AR2" s="119"/>
-      <c r="AS2" s="119"/>
-      <c r="AT2" s="119"/>
-      <c r="AU2" s="119"/>
-      <c r="AV2" s="119"/>
-      <c r="AW2" s="119"/>
-      <c r="AX2" s="119"/>
-      <c r="AY2" s="119"/>
-      <c r="AZ2" s="119"/>
-      <c r="BA2" s="119"/>
-      <c r="BB2" s="119"/>
-      <c r="BC2" s="119"/>
-      <c r="BD2" s="119"/>
-      <c r="BE2" s="119"/>
-      <c r="BF2" s="119"/>
-      <c r="BG2" s="119"/>
-      <c r="BH2" s="119"/>
-      <c r="BI2" s="119"/>
-      <c r="BJ2" s="119" t="s">
+      <c r="AN2" s="120"/>
+      <c r="AO2" s="120"/>
+      <c r="AP2" s="120"/>
+      <c r="AQ2" s="120"/>
+      <c r="AR2" s="120"/>
+      <c r="AS2" s="120"/>
+      <c r="AT2" s="120"/>
+      <c r="AU2" s="120"/>
+      <c r="AV2" s="120"/>
+      <c r="AW2" s="120"/>
+      <c r="AX2" s="120"/>
+      <c r="AY2" s="120"/>
+      <c r="AZ2" s="120"/>
+      <c r="BA2" s="120"/>
+      <c r="BB2" s="120"/>
+      <c r="BC2" s="120"/>
+      <c r="BD2" s="120"/>
+      <c r="BE2" s="120"/>
+      <c r="BF2" s="120"/>
+      <c r="BG2" s="120"/>
+      <c r="BH2" s="120"/>
+      <c r="BI2" s="120"/>
+      <c r="BJ2" s="120" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="119"/>
-      <c r="BL2" s="119"/>
-      <c r="BM2" s="119"/>
-      <c r="BN2" s="119"/>
-      <c r="BO2" s="119"/>
-      <c r="BP2" s="119"/>
-      <c r="BQ2" s="119"/>
-      <c r="BR2" s="119"/>
-      <c r="BS2" s="119"/>
-      <c r="BT2" s="119"/>
-      <c r="BU2" s="119"/>
-      <c r="BV2" s="119"/>
-      <c r="BW2" s="119"/>
-      <c r="BX2" s="119"/>
-      <c r="BY2" s="119"/>
-      <c r="BZ2" s="119"/>
-      <c r="CA2" s="119"/>
-      <c r="CB2" s="119"/>
-      <c r="CC2" s="119"/>
-      <c r="CD2" s="119"/>
-      <c r="CE2" s="119" t="s">
+      <c r="BK2" s="120"/>
+      <c r="BL2" s="120"/>
+      <c r="BM2" s="120"/>
+      <c r="BN2" s="120"/>
+      <c r="BO2" s="120"/>
+      <c r="BP2" s="120"/>
+      <c r="BQ2" s="120"/>
+      <c r="BR2" s="120"/>
+      <c r="BS2" s="120"/>
+      <c r="BT2" s="120"/>
+      <c r="BU2" s="120"/>
+      <c r="BV2" s="120"/>
+      <c r="BW2" s="120"/>
+      <c r="BX2" s="120"/>
+      <c r="BY2" s="120"/>
+      <c r="BZ2" s="120"/>
+      <c r="CA2" s="120"/>
+      <c r="CB2" s="120"/>
+      <c r="CC2" s="120"/>
+      <c r="CD2" s="120"/>
+      <c r="CE2" s="120" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="119"/>
-      <c r="CG2" s="119"/>
-      <c r="CH2" s="119"/>
-      <c r="CI2" s="119"/>
-      <c r="CJ2" s="119"/>
-      <c r="CK2" s="119"/>
-      <c r="CL2" s="119"/>
-      <c r="CM2" s="119"/>
-      <c r="CN2" s="119"/>
-      <c r="CO2" s="119"/>
-      <c r="CP2" s="119"/>
-      <c r="CQ2" s="119"/>
-      <c r="CR2" s="119"/>
+      <c r="CF2" s="120"/>
+      <c r="CG2" s="120"/>
+      <c r="CH2" s="120"/>
+      <c r="CI2" s="120"/>
+      <c r="CJ2" s="120"/>
+      <c r="CK2" s="120"/>
+      <c r="CL2" s="120"/>
+      <c r="CM2" s="120"/>
+      <c r="CN2" s="120"/>
+      <c r="CO2" s="120"/>
+      <c r="CP2" s="120"/>
+      <c r="CQ2" s="120"/>
+      <c r="CR2" s="120"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="122"/>
+      <c r="A3" s="119"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3068,10 +3081,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3207,24 +3220,26 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="118" t="s">
+      <c r="AV4" s="121" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="118" t="s">
+      <c r="AW4" s="121" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
         <v>282</v>
       </c>
-      <c r="AY4" s="142" t="s">
+      <c r="AY4" s="116" t="s">
         <v>286</v>
       </c>
-      <c r="AZ4" s="142"/>
-      <c r="BA4" s="142"/>
-      <c r="BB4" s="142"/>
-      <c r="BC4" s="142"/>
-      <c r="BD4" s="142"/>
-      <c r="BE4" s="142"/>
+      <c r="AZ4" s="116" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA4" s="116"/>
+      <c r="BB4" s="116"/>
+      <c r="BC4" s="116"/>
+      <c r="BD4" s="116"/>
+      <c r="BE4" s="116"/>
       <c r="BF4" s="100"/>
       <c r="BG4" s="100"/>
       <c r="BH4" s="100"/>
@@ -3239,12 +3254,12 @@
       <c r="BQ4" s="103"/>
       <c r="BR4" s="103"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="118" t="s">
+      <c r="BT4" s="121" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="110"/>
       <c r="BV4" s="111"/>
-      <c r="BW4" s="118" t="s">
+      <c r="BW4" s="121" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="106"/>
@@ -3264,15 +3279,15 @@
       <c r="CL4" s="113"/>
       <c r="CM4" s="113"/>
       <c r="CN4" s="114"/>
-      <c r="CO4" s="118" t="s">
+      <c r="CO4" s="121" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="117"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3406,20 +3421,22 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
+      <c r="AV5" s="121"/>
+      <c r="AW5" s="121"/>
       <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
-      <c r="AY5" s="142" t="s">
+      <c r="AY5" s="116" t="s">
         <v>287</v>
       </c>
-      <c r="AZ5" s="142"/>
-      <c r="BA5" s="142"/>
-      <c r="BB5" s="142"/>
-      <c r="BC5" s="142"/>
-      <c r="BD5" s="142"/>
-      <c r="BE5" s="142"/>
+      <c r="AZ5" s="116" t="s">
+        <v>291</v>
+      </c>
+      <c r="BA5" s="116"/>
+      <c r="BB5" s="116"/>
+      <c r="BC5" s="116"/>
+      <c r="BD5" s="116"/>
+      <c r="BE5" s="116"/>
       <c r="BF5" s="100"/>
       <c r="BG5" s="100"/>
       <c r="BH5" s="100"/>
@@ -3434,10 +3451,10 @@
       <c r="BQ5" s="103"/>
       <c r="BR5" s="103"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="118"/>
+      <c r="BT5" s="121"/>
       <c r="BU5" s="108"/>
       <c r="BV5" s="109"/>
-      <c r="BW5" s="118"/>
+      <c r="BW5" s="121"/>
       <c r="BX5" s="107"/>
       <c r="BY5" s="103"/>
       <c r="BZ5" s="112"/>
@@ -3455,13 +3472,13 @@
       <c r="CL5" s="113"/>
       <c r="CM5" s="113"/>
       <c r="CN5" s="114"/>
-      <c r="CO5" s="118"/>
+      <c r="CO5" s="121"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="122" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="117"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3597,20 +3614,22 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="118"/>
-      <c r="AW6" s="118"/>
+      <c r="AV6" s="121"/>
+      <c r="AW6" s="121"/>
       <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
-      <c r="AY6" s="142" t="s">
+      <c r="AY6" s="116" t="s">
         <v>288</v>
       </c>
-      <c r="AZ6" s="142"/>
-      <c r="BA6" s="142"/>
-      <c r="BB6" s="142"/>
-      <c r="BC6" s="142"/>
-      <c r="BD6" s="142"/>
-      <c r="BE6" s="142"/>
+      <c r="AZ6" s="116" t="s">
+        <v>292</v>
+      </c>
+      <c r="BA6" s="116"/>
+      <c r="BB6" s="116"/>
+      <c r="BC6" s="116"/>
+      <c r="BD6" s="116"/>
+      <c r="BE6" s="116"/>
       <c r="BF6" s="100"/>
       <c r="BG6" s="100"/>
       <c r="BH6" s="100"/>
@@ -3625,10 +3644,10 @@
       <c r="BQ6" s="103"/>
       <c r="BR6" s="103"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="118"/>
+      <c r="BT6" s="121"/>
       <c r="BU6" s="108"/>
       <c r="BV6" s="109"/>
-      <c r="BW6" s="118"/>
+      <c r="BW6" s="121"/>
       <c r="BX6" s="107"/>
       <c r="BY6" s="103"/>
       <c r="BZ6" s="112"/>
@@ -3646,13 +3665,13 @@
       <c r="CL6" s="113"/>
       <c r="CM6" s="113"/>
       <c r="CN6" s="114"/>
-      <c r="CO6" s="118"/>
+      <c r="CO6" s="121"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="122" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="123"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3788,20 +3807,22 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="118"/>
-      <c r="AW7" s="118"/>
+      <c r="AV7" s="121"/>
+      <c r="AW7" s="121"/>
       <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
-      <c r="AY7" s="142" t="s">
+      <c r="AY7" s="116" t="s">
         <v>289</v>
       </c>
-      <c r="AZ7" s="142"/>
-      <c r="BA7" s="142"/>
-      <c r="BB7" s="142"/>
-      <c r="BC7" s="142"/>
-      <c r="BD7" s="142"/>
-      <c r="BE7" s="142"/>
+      <c r="AZ7" s="116" t="s">
+        <v>293</v>
+      </c>
+      <c r="BA7" s="116"/>
+      <c r="BB7" s="116"/>
+      <c r="BC7" s="116"/>
+      <c r="BD7" s="116"/>
+      <c r="BE7" s="116"/>
       <c r="BF7" s="100"/>
       <c r="BG7" s="100"/>
       <c r="BH7" s="100"/>
@@ -3816,10 +3837,10 @@
       <c r="BQ7" s="103"/>
       <c r="BR7" s="103"/>
       <c r="BS7" s="104"/>
-      <c r="BT7" s="118"/>
+      <c r="BT7" s="121"/>
       <c r="BU7" s="108"/>
       <c r="BV7" s="109"/>
-      <c r="BW7" s="118"/>
+      <c r="BW7" s="121"/>
       <c r="BX7" s="107"/>
       <c r="BY7" s="103"/>
       <c r="BZ7" s="112"/>
@@ -3837,25 +3858,25 @@
       <c r="CL7" s="113"/>
       <c r="CM7" s="113"/>
       <c r="CN7" s="114"/>
-      <c r="CO7" s="118"/>
+      <c r="CO7" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3938,36 +3959,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="128" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="131" t="s">
+      <c r="F2" s="132" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="131"/>
+      <c r="G2" s="132"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="132" t="s">
+      <c r="I2" s="133" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="132"/>
+      <c r="J2" s="133"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="133" t="s">
+      <c r="L2" s="134" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="133"/>
+      <c r="M2" s="134"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="134" t="s">
+      <c r="O2" s="135" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="134"/>
+      <c r="P2" s="135"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="123" t="s">
+      <c r="R2" s="124" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="123"/>
+      <c r="S2" s="124"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4001,24 +4022,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="123"/>
-      <c r="S3" s="123"/>
+      <c r="R3" s="124"/>
+      <c r="S3" s="124"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4052,24 +4073,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="134"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="134"/>
-      <c r="P4" s="134"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
+      <c r="R4" s="124"/>
+      <c r="S4" s="124"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4107,20 +4128,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="132"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="132"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="133"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="134"/>
-      <c r="P5" s="134"/>
+      <c r="O5" s="135"/>
+      <c r="P5" s="135"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="123"/>
-      <c r="S5" s="123"/>
+      <c r="R5" s="124"/>
+      <c r="S5" s="124"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4154,26 +4175,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="129" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="133"/>
-      <c r="M6" s="133"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
+      <c r="R6" s="124"/>
+      <c r="S6" s="124"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4207,24 +4228,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="131"/>
-      <c r="G7" s="131"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="132"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
+      <c r="L7" s="134"/>
+      <c r="M7" s="134"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="134"/>
-      <c r="P7" s="134"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="123"/>
-      <c r="S7" s="123"/>
+      <c r="R7" s="124"/>
+      <c r="S7" s="124"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4258,24 +4279,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
+      <c r="B8" s="130"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="130"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="133"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="133"/>
+      <c r="L8" s="134"/>
+      <c r="M8" s="134"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="134"/>
+      <c r="O8" s="135"/>
+      <c r="P8" s="135"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="123"/>
-      <c r="S8" s="123"/>
+      <c r="R8" s="124"/>
+      <c r="S8" s="124"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4309,24 +4330,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
+      <c r="B9" s="130"/>
+      <c r="C9" s="130"/>
+      <c r="D9" s="130"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="131"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="132"/>
+      <c r="I9" s="133"/>
+      <c r="J9" s="133"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="133"/>
-      <c r="M9" s="133"/>
+      <c r="L9" s="134"/>
+      <c r="M9" s="134"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="134"/>
-      <c r="P9" s="134"/>
+      <c r="O9" s="135"/>
+      <c r="P9" s="135"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="123"/>
-      <c r="S9" s="123"/>
+      <c r="R9" s="124"/>
+      <c r="S9" s="124"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4360,24 +4381,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
+      <c r="B10" s="130"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="130"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="133"/>
+      <c r="L10" s="134"/>
+      <c r="M10" s="134"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="134"/>
-      <c r="P10" s="134"/>
+      <c r="O10" s="135"/>
+      <c r="P10" s="135"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="123"/>
-      <c r="S10" s="123"/>
+      <c r="R10" s="124"/>
+      <c r="S10" s="124"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4466,23 +4487,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="124" t="s">
+      <c r="F12" s="125" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="124"/>
+      <c r="G12" s="125"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="125" t="s">
+      <c r="I12" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="125"/>
+      <c r="J12" s="126"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="126" t="s">
+      <c r="L12" s="127" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="126"/>
+      <c r="M12" s="127"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="130"/>
-      <c r="P12" s="130"/>
+      <c r="O12" s="131"/>
+      <c r="P12" s="131"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4523,17 +4544,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="125"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="125"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="126"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="126"/>
-      <c r="M13" s="126"/>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="130"/>
-      <c r="P13" s="130"/>
+      <c r="O13" s="131"/>
+      <c r="P13" s="131"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4574,17 +4595,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="124"/>
+      <c r="F14" s="125"/>
+      <c r="G14" s="125"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="125"/>
+      <c r="I14" s="126"/>
+      <c r="J14" s="126"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="126"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="130"/>
-      <c r="P14" s="130"/>
+      <c r="O14" s="131"/>
+      <c r="P14" s="131"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4625,17 +4646,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
+      <c r="F15" s="125"/>
+      <c r="G15" s="125"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="125"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="126"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="126"/>
-      <c r="M15" s="126"/>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="130"/>
-      <c r="P15" s="130"/>
+      <c r="O15" s="131"/>
+      <c r="P15" s="131"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -4676,17 +4697,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="124"/>
-      <c r="G16" s="124"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="125"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="126"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="126"/>
-      <c r="M16" s="126"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="130"/>
-      <c r="P16" s="130"/>
+      <c r="O16" s="131"/>
+      <c r="P16" s="131"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -4727,17 +4748,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="124"/>
+      <c r="F17" s="125"/>
+      <c r="G17" s="125"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="125"/>
-      <c r="J17" s="125"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="126"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="126"/>
-      <c r="M17" s="126"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="130"/>
-      <c r="P17" s="130"/>
+      <c r="O17" s="131"/>
+      <c r="P17" s="131"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -4778,17 +4799,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="124"/>
+      <c r="F18" s="125"/>
+      <c r="G18" s="125"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="125"/>
+      <c r="I18" s="126"/>
+      <c r="J18" s="126"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="126"/>
-      <c r="M18" s="126"/>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="130"/>
-      <c r="P18" s="130"/>
+      <c r="O18" s="131"/>
+      <c r="P18" s="131"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -4829,17 +4850,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="124"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="125"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="125"/>
-      <c r="J19" s="125"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="126"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="126"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="130"/>
-      <c r="P19" s="130"/>
+      <c r="O19" s="131"/>
+      <c r="P19" s="131"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -4880,17 +4901,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="124"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="125"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="125"/>
-      <c r="J20" s="125"/>
+      <c r="I20" s="126"/>
+      <c r="J20" s="126"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="126"/>
-      <c r="M20" s="126"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="127"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="130"/>
+      <c r="O20" s="131"/>
+      <c r="P20" s="131"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17463,7 +17484,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -17803,7 +17824,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="137"/>
+      <c r="A2" s="138"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18129,15 +18150,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="138"/>
-      <c r="DH2" s="138"/>
-      <c r="DI2" s="138"/>
-      <c r="DJ2" s="138"/>
+      <c r="DG2" s="139"/>
+      <c r="DH2" s="139"/>
+      <c r="DI2" s="139"/>
+      <c r="DJ2" s="139"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="137"/>
+      <c r="A3" s="138"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18474,7 +18495,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="140" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18616,7 +18637,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="139"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -18756,7 +18777,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="139"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -18896,7 +18917,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="139"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19034,7 +19055,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="139"/>
+      <c r="B8" s="140"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19174,7 +19195,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="141" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19316,7 +19337,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="140"/>
+      <c r="B10" s="141"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19456,7 +19477,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="142" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19586,7 +19607,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="141"/>
+      <c r="B12" s="142"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -19724,7 +19745,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="141"/>
+      <c r="B13" s="142"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -19864,7 +19885,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="141"/>
+      <c r="B14" s="142"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20000,7 +20021,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="141"/>
+      <c r="B15" s="142"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20136,7 +20157,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="142"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20272,7 +20293,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="142"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20408,7 +20429,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="141"/>
+      <c r="B18" s="142"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20548,7 +20569,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="141"/>
+      <c r="B19" s="142"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -20684,7 +20705,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="141"/>
+      <c r="B20" s="142"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -20820,7 +20841,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="136" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -20954,7 +20975,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="135"/>
+      <c r="B22" s="136"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21090,7 +21111,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="135"/>
+      <c r="B23" s="136"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21222,7 +21243,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="135"/>
+      <c r="B24" s="136"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21356,7 +21377,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="135"/>
+      <c r="B25" s="136"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21500,7 +21521,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="136" t="s">
+      <c r="B26" s="137" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -21634,7 +21655,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="136"/>
+      <c r="B27" s="137"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -21774,7 +21795,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="136"/>
+      <c r="B28" s="137"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -21906,7 +21927,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="136"/>
+      <c r="B29" s="137"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22034,7 +22055,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="136"/>
+      <c r="B30" s="137"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22160,7 +22181,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="136"/>
+      <c r="B31" s="137"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 22-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2218D81A-4CD3-46CF-9C82-83C618A6AA91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BD7D47-71B3-4A72-A952-69740CCEB79C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="298">
   <si>
     <t>REDES</t>
   </si>
@@ -994,6 +994,18 @@
   </si>
   <si>
     <t>Estilização e funcionalidades página criar novo level, layout de alta fidelidade level e documentação</t>
+  </si>
+  <si>
+    <t>Busca processamento dos chamados API, planejamento reabrir chamado GLPI. Cadastro de usuário Mobile, Logoout Mobile, Rotas para renderização, tela listar chamados Mobile, Solicitação de cadastro de usuário API e listagem de usuários inativos API</t>
+  </si>
+  <si>
+    <t>Documentação e junção dos arquivos dos outros integrantes do grupo</t>
+  </si>
+  <si>
+    <t>Integração das funcionalidades desenvolvidas por outros integrantes do grupo, ajustes Dashboard, ajuste na listagem de funcionários, cadastro de agendas, tela de listagem geral (clientes, funcionários etc)</t>
+  </si>
+  <si>
+    <t>Altera renderização de componentes na criação de um leve. Pesquisa de como fazer um join no gremlin. Ajustes na API</t>
   </si>
 </sst>
 </file>
@@ -1885,6 +1897,18 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1893,18 +1917,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2363,7 +2375,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AZ8" sqref="AZ8"/>
+      <selection pane="bottomRight" activeCell="BA8" sqref="BA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2392,8 +2404,8 @@
     <col min="49" max="49" width="3.77734375" style="80" customWidth="1"/>
     <col min="50" max="50" width="30.77734375" customWidth="1"/>
     <col min="51" max="51" width="25.77734375" customWidth="1"/>
-    <col min="52" max="52" width="35.77734375" customWidth="1"/>
-    <col min="53" max="71" width="5.77734375" customWidth="1"/>
+    <col min="52" max="53" width="35.77734375" customWidth="1"/>
+    <col min="54" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2403,7 +2415,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="121" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2683,7 +2695,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="118"/>
+      <c r="A2" s="122"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2793,7 +2805,7 @@
       <c r="CR2" s="120"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="119"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3081,10 +3093,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="117" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="123"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3220,10 +3232,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="121" t="s">
+      <c r="AV4" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="121" t="s">
+      <c r="AW4" s="119" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3235,7 +3247,9 @@
       <c r="AZ4" s="116" t="s">
         <v>290</v>
       </c>
-      <c r="BA4" s="116"/>
+      <c r="BA4" s="116" t="s">
+        <v>294</v>
+      </c>
       <c r="BB4" s="116"/>
       <c r="BC4" s="116"/>
       <c r="BD4" s="116"/>
@@ -3254,12 +3268,12 @@
       <c r="BQ4" s="103"/>
       <c r="BR4" s="103"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="121" t="s">
+      <c r="BT4" s="119" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="110"/>
       <c r="BV4" s="111"/>
-      <c r="BW4" s="121" t="s">
+      <c r="BW4" s="119" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="106"/>
@@ -3279,15 +3293,15 @@
       <c r="CL4" s="113"/>
       <c r="CM4" s="113"/>
       <c r="CN4" s="114"/>
-      <c r="CO4" s="121" t="s">
+      <c r="CO4" s="119" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="117" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3421,8 +3435,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="121"/>
-      <c r="AW5" s="121"/>
+      <c r="AV5" s="119"/>
+      <c r="AW5" s="119"/>
       <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
@@ -3432,7 +3446,9 @@
       <c r="AZ5" s="116" t="s">
         <v>291</v>
       </c>
-      <c r="BA5" s="116"/>
+      <c r="BA5" s="116" t="s">
+        <v>295</v>
+      </c>
       <c r="BB5" s="116"/>
       <c r="BC5" s="116"/>
       <c r="BD5" s="116"/>
@@ -3451,10 +3467,10 @@
       <c r="BQ5" s="103"/>
       <c r="BR5" s="103"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="121"/>
+      <c r="BT5" s="119"/>
       <c r="BU5" s="108"/>
       <c r="BV5" s="109"/>
-      <c r="BW5" s="121"/>
+      <c r="BW5" s="119"/>
       <c r="BX5" s="107"/>
       <c r="BY5" s="103"/>
       <c r="BZ5" s="112"/>
@@ -3472,13 +3488,13 @@
       <c r="CL5" s="113"/>
       <c r="CM5" s="113"/>
       <c r="CN5" s="114"/>
-      <c r="CO5" s="121"/>
+      <c r="CO5" s="119"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="117" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3614,8 +3630,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="121"/>
-      <c r="AW6" s="121"/>
+      <c r="AV6" s="119"/>
+      <c r="AW6" s="119"/>
       <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
@@ -3625,7 +3641,9 @@
       <c r="AZ6" s="116" t="s">
         <v>292</v>
       </c>
-      <c r="BA6" s="116"/>
+      <c r="BA6" s="116" t="s">
+        <v>296</v>
+      </c>
       <c r="BB6" s="116"/>
       <c r="BC6" s="116"/>
       <c r="BD6" s="116"/>
@@ -3644,10 +3662,10 @@
       <c r="BQ6" s="103"/>
       <c r="BR6" s="103"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="121"/>
+      <c r="BT6" s="119"/>
       <c r="BU6" s="108"/>
       <c r="BV6" s="109"/>
-      <c r="BW6" s="121"/>
+      <c r="BW6" s="119"/>
       <c r="BX6" s="107"/>
       <c r="BY6" s="103"/>
       <c r="BZ6" s="112"/>
@@ -3665,13 +3683,13 @@
       <c r="CL6" s="113"/>
       <c r="CM6" s="113"/>
       <c r="CN6" s="114"/>
-      <c r="CO6" s="121"/>
+      <c r="CO6" s="119"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="123"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3807,8 +3825,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="121"/>
-      <c r="AW7" s="121"/>
+      <c r="AV7" s="119"/>
+      <c r="AW7" s="119"/>
       <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
@@ -3818,7 +3836,9 @@
       <c r="AZ7" s="116" t="s">
         <v>293</v>
       </c>
-      <c r="BA7" s="116"/>
+      <c r="BA7" s="116" t="s">
+        <v>297</v>
+      </c>
       <c r="BB7" s="116"/>
       <c r="BC7" s="116"/>
       <c r="BD7" s="116"/>
@@ -3837,10 +3857,10 @@
       <c r="BQ7" s="103"/>
       <c r="BR7" s="103"/>
       <c r="BS7" s="104"/>
-      <c r="BT7" s="121"/>
+      <c r="BT7" s="119"/>
       <c r="BU7" s="108"/>
       <c r="BV7" s="109"/>
-      <c r="BW7" s="121"/>
+      <c r="BW7" s="119"/>
       <c r="BX7" s="107"/>
       <c r="BY7" s="103"/>
       <c r="BZ7" s="112"/>
@@ -3858,25 +3878,25 @@
       <c r="CL7" s="113"/>
       <c r="CM7" s="113"/>
       <c r="CN7" s="114"/>
-      <c r="CO7" s="121"/>
+      <c r="CO7" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 23-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BD7D47-71B3-4A72-A952-69740CCEB79C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCDE813-370D-4C12-9BB9-1133A83963CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="302">
   <si>
     <t>REDES</t>
   </si>
@@ -1006,6 +1006,18 @@
   </si>
   <si>
     <t>Altera renderização de componentes na criação de um leve. Pesquisa de como fazer um join no gremlin. Ajustes na API</t>
+  </si>
+  <si>
+    <t>Confirmação de cadastro de usuário API, método reabrir chamado API, responsividade Mobile, editar usuário Mobile, loading Mobile, renderização condicional baseado no usuário logado</t>
+  </si>
+  <si>
+    <t>Busca de soluções para reduzir o tempo de requisições Zabbix</t>
+  </si>
+  <si>
+    <t>Dashboard implementação drag, finalização do passo a passo de cadastro inicial, finalização de cadastro de agendas e decomposição do que listar na página de listagem geral, página de cadastro de cliente e usuário</t>
+  </si>
+  <si>
+    <t>Tela listagem de levels, modal para editar e deletar bloco genérico, funcionalidade deletar bloco na tela editar level</t>
   </si>
 </sst>
 </file>
@@ -1897,18 +1909,6 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1917,6 +1917,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2375,7 +2387,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BA8" sqref="BA8"/>
+      <selection pane="bottomRight" activeCell="BC4" sqref="BC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2405,7 +2417,8 @@
     <col min="50" max="50" width="30.77734375" customWidth="1"/>
     <col min="51" max="51" width="25.77734375" customWidth="1"/>
     <col min="52" max="53" width="35.77734375" customWidth="1"/>
-    <col min="54" max="71" width="5.77734375" customWidth="1"/>
+    <col min="54" max="54" width="30.77734375" customWidth="1"/>
+    <col min="55" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2415,7 +2428,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="117" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2695,7 +2708,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="122"/>
+      <c r="A2" s="118"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2805,7 +2818,7 @@
       <c r="CR2" s="120"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="123"/>
+      <c r="A3" s="119"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3093,10 +3106,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3232,10 +3245,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="119" t="s">
+      <c r="AV4" s="121" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="119" t="s">
+      <c r="AW4" s="121" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3250,7 +3263,9 @@
       <c r="BA4" s="116" t="s">
         <v>294</v>
       </c>
-      <c r="BB4" s="116"/>
+      <c r="BB4" s="116" t="s">
+        <v>298</v>
+      </c>
       <c r="BC4" s="116"/>
       <c r="BD4" s="116"/>
       <c r="BE4" s="116"/>
@@ -3268,12 +3283,12 @@
       <c r="BQ4" s="103"/>
       <c r="BR4" s="103"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="119" t="s">
+      <c r="BT4" s="121" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="110"/>
       <c r="BV4" s="111"/>
-      <c r="BW4" s="119" t="s">
+      <c r="BW4" s="121" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="106"/>
@@ -3293,15 +3308,15 @@
       <c r="CL4" s="113"/>
       <c r="CM4" s="113"/>
       <c r="CN4" s="114"/>
-      <c r="CO4" s="119" t="s">
+      <c r="CO4" s="121" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3435,8 +3450,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="119"/>
-      <c r="AW5" s="119"/>
+      <c r="AV5" s="121"/>
+      <c r="AW5" s="121"/>
       <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
@@ -3449,7 +3464,9 @@
       <c r="BA5" s="116" t="s">
         <v>295</v>
       </c>
-      <c r="BB5" s="116"/>
+      <c r="BB5" s="116" t="s">
+        <v>299</v>
+      </c>
       <c r="BC5" s="116"/>
       <c r="BD5" s="116"/>
       <c r="BE5" s="116"/>
@@ -3467,10 +3484,10 @@
       <c r="BQ5" s="103"/>
       <c r="BR5" s="103"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="119"/>
+      <c r="BT5" s="121"/>
       <c r="BU5" s="108"/>
       <c r="BV5" s="109"/>
-      <c r="BW5" s="119"/>
+      <c r="BW5" s="121"/>
       <c r="BX5" s="107"/>
       <c r="BY5" s="103"/>
       <c r="BZ5" s="112"/>
@@ -3488,13 +3505,13 @@
       <c r="CL5" s="113"/>
       <c r="CM5" s="113"/>
       <c r="CN5" s="114"/>
-      <c r="CO5" s="119"/>
+      <c r="CO5" s="121"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="122" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="118"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3630,8 +3647,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="119"/>
-      <c r="AW6" s="119"/>
+      <c r="AV6" s="121"/>
+      <c r="AW6" s="121"/>
       <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
@@ -3644,7 +3661,9 @@
       <c r="BA6" s="116" t="s">
         <v>296</v>
       </c>
-      <c r="BB6" s="116"/>
+      <c r="BB6" s="116" t="s">
+        <v>300</v>
+      </c>
       <c r="BC6" s="116"/>
       <c r="BD6" s="116"/>
       <c r="BE6" s="116"/>
@@ -3662,10 +3681,10 @@
       <c r="BQ6" s="103"/>
       <c r="BR6" s="103"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="119"/>
+      <c r="BT6" s="121"/>
       <c r="BU6" s="108"/>
       <c r="BV6" s="109"/>
-      <c r="BW6" s="119"/>
+      <c r="BW6" s="121"/>
       <c r="BX6" s="107"/>
       <c r="BY6" s="103"/>
       <c r="BZ6" s="112"/>
@@ -3683,13 +3702,13 @@
       <c r="CL6" s="113"/>
       <c r="CM6" s="113"/>
       <c r="CN6" s="114"/>
-      <c r="CO6" s="119"/>
+      <c r="CO6" s="121"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="122" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="123"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3825,8 +3844,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="119"/>
-      <c r="AW7" s="119"/>
+      <c r="AV7" s="121"/>
+      <c r="AW7" s="121"/>
       <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
@@ -3839,7 +3858,9 @@
       <c r="BA7" s="116" t="s">
         <v>297</v>
       </c>
-      <c r="BB7" s="116"/>
+      <c r="BB7" s="116" t="s">
+        <v>301</v>
+      </c>
       <c r="BC7" s="116"/>
       <c r="BD7" s="116"/>
       <c r="BE7" s="116"/>
@@ -3857,10 +3878,10 @@
       <c r="BQ7" s="103"/>
       <c r="BR7" s="103"/>
       <c r="BS7" s="104"/>
-      <c r="BT7" s="119"/>
+      <c r="BT7" s="121"/>
       <c r="BU7" s="108"/>
       <c r="BV7" s="109"/>
-      <c r="BW7" s="119"/>
+      <c r="BW7" s="121"/>
       <c r="BX7" s="107"/>
       <c r="BY7" s="103"/>
       <c r="BZ7" s="112"/>
@@ -3878,25 +3899,25 @@
       <c r="CL7" s="113"/>
       <c r="CM7" s="113"/>
       <c r="CN7" s="114"/>
-      <c r="CO7" s="119"/>
+      <c r="CO7" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 24, 25 e 28-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCDE813-370D-4C12-9BB9-1133A83963CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF02C14-4D39-4AB7-9EEC-FB2A169EE3EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="311">
   <si>
     <t>REDES</t>
   </si>
@@ -1018,6 +1018,33 @@
   </si>
   <si>
     <t>Tela listagem de levels, modal para editar e deletar bloco genérico, funcionalidade deletar bloco na tela editar level</t>
+  </si>
+  <si>
+    <t>Ajustes e preparação para a reunião com o cliente</t>
+  </si>
+  <si>
+    <t>Dashboard implementação drag, ajustes nos métodos de cadastro na API, cadastro de cliente, página listagem geral e exportar para excel</t>
+  </si>
+  <si>
+    <t>Tela listagem de levels, correção na criação e edição de um level na tela, ajustes no styleguide</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente alocado</t>
+  </si>
+  <si>
+    <t>Estudo de como exportar para PDF</t>
+  </si>
+  <si>
+    <t>Listagem de levels com blocos, achievements e categorias e estudo azure blobs</t>
+  </si>
+  <si>
+    <t>Início da planning</t>
+  </si>
+  <si>
+    <t>Estudo de como exportar para PDF, aprimoramento na exibição da lista de dados</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente</t>
   </si>
 </sst>
 </file>
@@ -1909,6 +1936,18 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1917,18 +1956,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2384,10 +2411,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BC4" sqref="BC4"/>
+      <selection pane="bottomRight" activeCell="BE4" sqref="BE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2418,7 +2445,8 @@
     <col min="51" max="51" width="25.77734375" customWidth="1"/>
     <col min="52" max="53" width="35.77734375" customWidth="1"/>
     <col min="54" max="54" width="30.77734375" customWidth="1"/>
-    <col min="55" max="71" width="5.77734375" customWidth="1"/>
+    <col min="55" max="57" width="20.77734375" customWidth="1"/>
+    <col min="58" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2428,7 +2456,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="121" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2708,7 +2736,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="118"/>
+      <c r="A2" s="122"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2818,7 +2846,7 @@
       <c r="CR2" s="120"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="119"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3106,10 +3134,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="117" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="123"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3245,10 +3273,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="121" t="s">
+      <c r="AV4" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="121" t="s">
+      <c r="AW4" s="119" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3266,9 +3294,15 @@
       <c r="BB4" s="116" t="s">
         <v>298</v>
       </c>
-      <c r="BC4" s="116"/>
-      <c r="BD4" s="116"/>
-      <c r="BE4" s="116"/>
+      <c r="BC4" s="116" t="s">
+        <v>302</v>
+      </c>
+      <c r="BD4" s="116" t="s">
+        <v>305</v>
+      </c>
+      <c r="BE4" s="116" t="s">
+        <v>308</v>
+      </c>
       <c r="BF4" s="100"/>
       <c r="BG4" s="100"/>
       <c r="BH4" s="100"/>
@@ -3283,12 +3317,12 @@
       <c r="BQ4" s="103"/>
       <c r="BR4" s="103"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="121" t="s">
+      <c r="BT4" s="119" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="110"/>
       <c r="BV4" s="111"/>
-      <c r="BW4" s="121" t="s">
+      <c r="BW4" s="119" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="106"/>
@@ -3308,15 +3342,15 @@
       <c r="CL4" s="113"/>
       <c r="CM4" s="113"/>
       <c r="CN4" s="114"/>
-      <c r="CO4" s="121" t="s">
+      <c r="CO4" s="119" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="117" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3450,8 +3484,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="121"/>
-      <c r="AW5" s="121"/>
+      <c r="AV5" s="119"/>
+      <c r="AW5" s="119"/>
       <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
@@ -3467,9 +3501,15 @@
       <c r="BB5" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="BC5" s="116"/>
-      <c r="BD5" s="116"/>
-      <c r="BE5" s="116"/>
+      <c r="BC5" s="116" t="s">
+        <v>299</v>
+      </c>
+      <c r="BD5" s="116" t="s">
+        <v>306</v>
+      </c>
+      <c r="BE5" s="116" t="s">
+        <v>309</v>
+      </c>
       <c r="BF5" s="100"/>
       <c r="BG5" s="100"/>
       <c r="BH5" s="100"/>
@@ -3484,10 +3524,10 @@
       <c r="BQ5" s="103"/>
       <c r="BR5" s="103"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="121"/>
+      <c r="BT5" s="119"/>
       <c r="BU5" s="108"/>
       <c r="BV5" s="109"/>
-      <c r="BW5" s="121"/>
+      <c r="BW5" s="119"/>
       <c r="BX5" s="107"/>
       <c r="BY5" s="103"/>
       <c r="BZ5" s="112"/>
@@ -3505,13 +3545,13 @@
       <c r="CL5" s="113"/>
       <c r="CM5" s="113"/>
       <c r="CN5" s="114"/>
-      <c r="CO5" s="121"/>
+      <c r="CO5" s="119"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="117" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3647,8 +3687,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="121"/>
-      <c r="AW6" s="121"/>
+      <c r="AV6" s="119"/>
+      <c r="AW6" s="119"/>
       <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
@@ -3664,9 +3704,15 @@
       <c r="BB6" s="116" t="s">
         <v>300</v>
       </c>
-      <c r="BC6" s="116"/>
-      <c r="BD6" s="116"/>
-      <c r="BE6" s="116"/>
+      <c r="BC6" s="116" t="s">
+        <v>303</v>
+      </c>
+      <c r="BD6" s="116" t="s">
+        <v>302</v>
+      </c>
+      <c r="BE6" s="116" t="s">
+        <v>310</v>
+      </c>
       <c r="BF6" s="100"/>
       <c r="BG6" s="100"/>
       <c r="BH6" s="100"/>
@@ -3681,10 +3727,10 @@
       <c r="BQ6" s="103"/>
       <c r="BR6" s="103"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="121"/>
+      <c r="BT6" s="119"/>
       <c r="BU6" s="108"/>
       <c r="BV6" s="109"/>
-      <c r="BW6" s="121"/>
+      <c r="BW6" s="119"/>
       <c r="BX6" s="107"/>
       <c r="BY6" s="103"/>
       <c r="BZ6" s="112"/>
@@ -3702,13 +3748,13 @@
       <c r="CL6" s="113"/>
       <c r="CM6" s="113"/>
       <c r="CN6" s="114"/>
-      <c r="CO6" s="121"/>
+      <c r="CO6" s="119"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="123"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3844,8 +3890,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="121"/>
-      <c r="AW7" s="121"/>
+      <c r="AV7" s="119"/>
+      <c r="AW7" s="119"/>
       <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
@@ -3861,9 +3907,15 @@
       <c r="BB7" s="116" t="s">
         <v>301</v>
       </c>
-      <c r="BC7" s="116"/>
-      <c r="BD7" s="116"/>
-      <c r="BE7" s="116"/>
+      <c r="BC7" s="116" t="s">
+        <v>304</v>
+      </c>
+      <c r="BD7" s="116" t="s">
+        <v>307</v>
+      </c>
+      <c r="BE7" s="116" t="s">
+        <v>310</v>
+      </c>
       <c r="BF7" s="100"/>
       <c r="BG7" s="100"/>
       <c r="BH7" s="100"/>
@@ -3878,10 +3930,10 @@
       <c r="BQ7" s="103"/>
       <c r="BR7" s="103"/>
       <c r="BS7" s="104"/>
-      <c r="BT7" s="121"/>
+      <c r="BT7" s="119"/>
       <c r="BU7" s="108"/>
       <c r="BV7" s="109"/>
-      <c r="BW7" s="121"/>
+      <c r="BW7" s="119"/>
       <c r="BX7" s="107"/>
       <c r="BY7" s="103"/>
       <c r="BZ7" s="112"/>
@@ -3899,25 +3951,25 @@
       <c r="CL7" s="113"/>
       <c r="CM7" s="113"/>
       <c r="CN7" s="114"/>
-      <c r="CO7" s="121"/>
+      <c r="CO7" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 29-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF02C14-4D39-4AB7-9EEC-FB2A169EE3EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49E09DC-CC7D-4AF0-80B8-457362D4E1C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="315">
   <si>
     <t>REDES</t>
   </si>
@@ -1045,6 +1045,18 @@
   </si>
   <si>
     <t>Reunião com o cliente</t>
+  </si>
+  <si>
+    <t>Planning e Sprint Review</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente, início da Planning e Sprint Review</t>
+  </si>
+  <si>
+    <t>Integração do que foi desenvolvido individualmente por cada membro, hospedagem API</t>
+  </si>
+  <si>
+    <t>Alinhamento das tarefas e pendências com o cliente e início da Planning</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1936,18 +1948,6 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1956,6 +1956,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2012,6 +2024,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2411,10 +2426,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BA4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BD4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BE4" sqref="BE4"/>
+      <selection pane="bottomRight" activeCell="BG4" sqref="BG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2445,8 +2460,8 @@
     <col min="51" max="51" width="25.77734375" customWidth="1"/>
     <col min="52" max="53" width="35.77734375" customWidth="1"/>
     <col min="54" max="54" width="30.77734375" customWidth="1"/>
-    <col min="55" max="57" width="20.77734375" customWidth="1"/>
-    <col min="58" max="71" width="5.77734375" customWidth="1"/>
+    <col min="55" max="58" width="20.77734375" customWidth="1"/>
+    <col min="59" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2456,7 +2471,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="117" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2736,7 +2751,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="122"/>
+      <c r="A2" s="118"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2846,7 +2861,7 @@
       <c r="CR2" s="120"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="123"/>
+      <c r="A3" s="119"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3134,10 +3149,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3273,10 +3288,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="119" t="s">
+      <c r="AV4" s="121" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="119" t="s">
+      <c r="AW4" s="121" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3303,11 +3318,13 @@
       <c r="BE4" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="BF4" s="100"/>
-      <c r="BG4" s="100"/>
-      <c r="BH4" s="100"/>
-      <c r="BI4" s="100"/>
-      <c r="BJ4" s="100"/>
+      <c r="BF4" s="143" t="s">
+        <v>311</v>
+      </c>
+      <c r="BG4" s="143"/>
+      <c r="BH4" s="143"/>
+      <c r="BI4" s="143"/>
+      <c r="BJ4" s="143"/>
       <c r="BK4" s="100"/>
       <c r="BL4" s="100"/>
       <c r="BM4" s="100"/>
@@ -3317,12 +3334,12 @@
       <c r="BQ4" s="103"/>
       <c r="BR4" s="103"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="119" t="s">
+      <c r="BT4" s="121" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="110"/>
       <c r="BV4" s="111"/>
-      <c r="BW4" s="119" t="s">
+      <c r="BW4" s="121" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="106"/>
@@ -3342,15 +3359,15 @@
       <c r="CL4" s="113"/>
       <c r="CM4" s="113"/>
       <c r="CN4" s="114"/>
-      <c r="CO4" s="119" t="s">
+      <c r="CO4" s="121" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3484,8 +3501,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="119"/>
-      <c r="AW5" s="119"/>
+      <c r="AV5" s="121"/>
+      <c r="AW5" s="121"/>
       <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
@@ -3510,11 +3527,13 @@
       <c r="BE5" s="116" t="s">
         <v>309</v>
       </c>
-      <c r="BF5" s="100"/>
-      <c r="BG5" s="100"/>
-      <c r="BH5" s="100"/>
-      <c r="BI5" s="100"/>
-      <c r="BJ5" s="100"/>
+      <c r="BF5" s="143" t="s">
+        <v>312</v>
+      </c>
+      <c r="BG5" s="143"/>
+      <c r="BH5" s="143"/>
+      <c r="BI5" s="143"/>
+      <c r="BJ5" s="143"/>
       <c r="BK5" s="100"/>
       <c r="BL5" s="100"/>
       <c r="BM5" s="100"/>
@@ -3524,10 +3543,10 @@
       <c r="BQ5" s="103"/>
       <c r="BR5" s="103"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="119"/>
+      <c r="BT5" s="121"/>
       <c r="BU5" s="108"/>
       <c r="BV5" s="109"/>
-      <c r="BW5" s="119"/>
+      <c r="BW5" s="121"/>
       <c r="BX5" s="107"/>
       <c r="BY5" s="103"/>
       <c r="BZ5" s="112"/>
@@ -3545,13 +3564,13 @@
       <c r="CL5" s="113"/>
       <c r="CM5" s="113"/>
       <c r="CN5" s="114"/>
-      <c r="CO5" s="119"/>
+      <c r="CO5" s="121"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="122" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="118"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3687,8 +3706,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="119"/>
-      <c r="AW6" s="119"/>
+      <c r="AV6" s="121"/>
+      <c r="AW6" s="121"/>
       <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
@@ -3713,11 +3732,13 @@
       <c r="BE6" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="BF6" s="100"/>
-      <c r="BG6" s="100"/>
-      <c r="BH6" s="100"/>
-      <c r="BI6" s="100"/>
-      <c r="BJ6" s="100"/>
+      <c r="BF6" s="143" t="s">
+        <v>313</v>
+      </c>
+      <c r="BG6" s="143"/>
+      <c r="BH6" s="143"/>
+      <c r="BI6" s="143"/>
+      <c r="BJ6" s="143"/>
       <c r="BK6" s="100"/>
       <c r="BL6" s="100"/>
       <c r="BM6" s="100"/>
@@ -3727,10 +3748,10 @@
       <c r="BQ6" s="103"/>
       <c r="BR6" s="103"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="119"/>
+      <c r="BT6" s="121"/>
       <c r="BU6" s="108"/>
       <c r="BV6" s="109"/>
-      <c r="BW6" s="119"/>
+      <c r="BW6" s="121"/>
       <c r="BX6" s="107"/>
       <c r="BY6" s="103"/>
       <c r="BZ6" s="112"/>
@@ -3748,13 +3769,13 @@
       <c r="CL6" s="113"/>
       <c r="CM6" s="113"/>
       <c r="CN6" s="114"/>
-      <c r="CO6" s="119"/>
+      <c r="CO6" s="121"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="122" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="123"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3890,8 +3911,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="119"/>
-      <c r="AW7" s="119"/>
+      <c r="AV7" s="121"/>
+      <c r="AW7" s="121"/>
       <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
@@ -3916,11 +3937,13 @@
       <c r="BE7" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="BF7" s="100"/>
-      <c r="BG7" s="100"/>
-      <c r="BH7" s="100"/>
-      <c r="BI7" s="100"/>
-      <c r="BJ7" s="100"/>
+      <c r="BF7" s="143" t="s">
+        <v>314</v>
+      </c>
+      <c r="BG7" s="143"/>
+      <c r="BH7" s="143"/>
+      <c r="BI7" s="143"/>
+      <c r="BJ7" s="143"/>
       <c r="BK7" s="100"/>
       <c r="BL7" s="100"/>
       <c r="BM7" s="100"/>
@@ -3930,10 +3953,10 @@
       <c r="BQ7" s="103"/>
       <c r="BR7" s="103"/>
       <c r="BS7" s="104"/>
-      <c r="BT7" s="119"/>
+      <c r="BT7" s="121"/>
       <c r="BU7" s="108"/>
       <c r="BV7" s="109"/>
-      <c r="BW7" s="119"/>
+      <c r="BW7" s="121"/>
       <c r="BX7" s="107"/>
       <c r="BY7" s="103"/>
       <c r="BZ7" s="112"/>
@@ -3951,25 +3974,25 @@
       <c r="CL7" s="113"/>
       <c r="CM7" s="113"/>
       <c r="CN7" s="114"/>
-      <c r="CO7" s="119"/>
+      <c r="CO7" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 30-10
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49E09DC-CC7D-4AF0-80B8-457362D4E1C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0FDC5-536A-45A1-901B-F284931DF07E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="319">
   <si>
     <t>REDES</t>
   </si>
@@ -1057,6 +1057,18 @@
   </si>
   <si>
     <t>Alinhamento das tarefas e pendências com o cliente e início da Planning</t>
+  </si>
+  <si>
+    <t>Levantamento do pronto para a versão beta. Validação de campos Login API e Mobile, Loading no botão de login Mobile, validação nos campos de cadastro de usuário Mobile, estilização lista de chamados Mobile. Responsividade WEB.</t>
+  </si>
+  <si>
+    <t>Levantamento do pronto para a versão beta. Integração back-end e front-end</t>
+  </si>
+  <si>
+    <t>Levantamento do pronto para a versão beta. Apresentação pro cliente com o sistema integrado</t>
+  </si>
+  <si>
+    <t>Levantamento do pronto para a versão beta e planning</t>
   </si>
 </sst>
 </file>
@@ -1948,6 +1960,21 @@
     <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1956,18 +1983,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2024,9 +2039,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2429,7 +2441,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="BD4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BG4" sqref="BG4"/>
+      <selection pane="bottomRight" activeCell="BG8" sqref="BG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2461,7 +2473,8 @@
     <col min="52" max="53" width="35.77734375" customWidth="1"/>
     <col min="54" max="54" width="30.77734375" customWidth="1"/>
     <col min="55" max="58" width="20.77734375" customWidth="1"/>
-    <col min="59" max="71" width="5.77734375" customWidth="1"/>
+    <col min="59" max="59" width="30.77734375" customWidth="1"/>
+    <col min="60" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2471,7 +2484,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="122" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2751,117 +2764,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="118"/>
+      <c r="A2" s="123"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="121" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120" t="s">
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="120"/>
-      <c r="AA2" s="120"/>
-      <c r="AB2" s="120"/>
-      <c r="AC2" s="120"/>
-      <c r="AD2" s="120"/>
-      <c r="AE2" s="120"/>
-      <c r="AF2" s="120"/>
-      <c r="AG2" s="120"/>
-      <c r="AH2" s="120"/>
-      <c r="AI2" s="120"/>
-      <c r="AJ2" s="120"/>
-      <c r="AK2" s="120"/>
-      <c r="AL2" s="120"/>
-      <c r="AM2" s="120" t="s">
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="121"/>
+      <c r="Z2" s="121"/>
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="121"/>
+      <c r="AF2" s="121"/>
+      <c r="AG2" s="121"/>
+      <c r="AH2" s="121"/>
+      <c r="AI2" s="121"/>
+      <c r="AJ2" s="121"/>
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="120"/>
-      <c r="AO2" s="120"/>
-      <c r="AP2" s="120"/>
-      <c r="AQ2" s="120"/>
-      <c r="AR2" s="120"/>
-      <c r="AS2" s="120"/>
-      <c r="AT2" s="120"/>
-      <c r="AU2" s="120"/>
-      <c r="AV2" s="120"/>
-      <c r="AW2" s="120"/>
-      <c r="AX2" s="120"/>
-      <c r="AY2" s="120"/>
-      <c r="AZ2" s="120"/>
-      <c r="BA2" s="120"/>
-      <c r="BB2" s="120"/>
-      <c r="BC2" s="120"/>
-      <c r="BD2" s="120"/>
-      <c r="BE2" s="120"/>
-      <c r="BF2" s="120"/>
-      <c r="BG2" s="120"/>
-      <c r="BH2" s="120"/>
-      <c r="BI2" s="120"/>
-      <c r="BJ2" s="120" t="s">
+      <c r="AN2" s="121"/>
+      <c r="AO2" s="121"/>
+      <c r="AP2" s="121"/>
+      <c r="AQ2" s="121"/>
+      <c r="AR2" s="121"/>
+      <c r="AS2" s="121"/>
+      <c r="AT2" s="121"/>
+      <c r="AU2" s="121"/>
+      <c r="AV2" s="121"/>
+      <c r="AW2" s="121"/>
+      <c r="AX2" s="121"/>
+      <c r="AY2" s="121"/>
+      <c r="AZ2" s="121"/>
+      <c r="BA2" s="121"/>
+      <c r="BB2" s="121"/>
+      <c r="BC2" s="121"/>
+      <c r="BD2" s="121"/>
+      <c r="BE2" s="121"/>
+      <c r="BF2" s="121"/>
+      <c r="BG2" s="121"/>
+      <c r="BH2" s="121"/>
+      <c r="BI2" s="121"/>
+      <c r="BJ2" s="121" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="120"/>
-      <c r="BL2" s="120"/>
-      <c r="BM2" s="120"/>
-      <c r="BN2" s="120"/>
-      <c r="BO2" s="120"/>
-      <c r="BP2" s="120"/>
-      <c r="BQ2" s="120"/>
-      <c r="BR2" s="120"/>
-      <c r="BS2" s="120"/>
-      <c r="BT2" s="120"/>
-      <c r="BU2" s="120"/>
-      <c r="BV2" s="120"/>
-      <c r="BW2" s="120"/>
-      <c r="BX2" s="120"/>
-      <c r="BY2" s="120"/>
-      <c r="BZ2" s="120"/>
-      <c r="CA2" s="120"/>
-      <c r="CB2" s="120"/>
-      <c r="CC2" s="120"/>
-      <c r="CD2" s="120"/>
-      <c r="CE2" s="120" t="s">
+      <c r="BK2" s="121"/>
+      <c r="BL2" s="121"/>
+      <c r="BM2" s="121"/>
+      <c r="BN2" s="121"/>
+      <c r="BO2" s="121"/>
+      <c r="BP2" s="121"/>
+      <c r="BQ2" s="121"/>
+      <c r="BR2" s="121"/>
+      <c r="BS2" s="121"/>
+      <c r="BT2" s="121"/>
+      <c r="BU2" s="121"/>
+      <c r="BV2" s="121"/>
+      <c r="BW2" s="121"/>
+      <c r="BX2" s="121"/>
+      <c r="BY2" s="121"/>
+      <c r="BZ2" s="121"/>
+      <c r="CA2" s="121"/>
+      <c r="CB2" s="121"/>
+      <c r="CC2" s="121"/>
+      <c r="CD2" s="121"/>
+      <c r="CE2" s="121" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="120"/>
-      <c r="CG2" s="120"/>
-      <c r="CH2" s="120"/>
-      <c r="CI2" s="120"/>
-      <c r="CJ2" s="120"/>
-      <c r="CK2" s="120"/>
-      <c r="CL2" s="120"/>
-      <c r="CM2" s="120"/>
-      <c r="CN2" s="120"/>
-      <c r="CO2" s="120"/>
-      <c r="CP2" s="120"/>
-      <c r="CQ2" s="120"/>
-      <c r="CR2" s="120"/>
+      <c r="CF2" s="121"/>
+      <c r="CG2" s="121"/>
+      <c r="CH2" s="121"/>
+      <c r="CI2" s="121"/>
+      <c r="CJ2" s="121"/>
+      <c r="CK2" s="121"/>
+      <c r="CL2" s="121"/>
+      <c r="CM2" s="121"/>
+      <c r="CN2" s="121"/>
+      <c r="CO2" s="121"/>
+      <c r="CP2" s="121"/>
+      <c r="CQ2" s="121"/>
+      <c r="CR2" s="121"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="119"/>
+      <c r="A3" s="124"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3149,10 +3162,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="118" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="123"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3288,10 +3301,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="121" t="s">
+      <c r="AV4" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="121" t="s">
+      <c r="AW4" s="120" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3318,13 +3331,15 @@
       <c r="BE4" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="BF4" s="143" t="s">
+      <c r="BF4" s="117" t="s">
         <v>311</v>
       </c>
-      <c r="BG4" s="143"/>
-      <c r="BH4" s="143"/>
-      <c r="BI4" s="143"/>
-      <c r="BJ4" s="143"/>
+      <c r="BG4" s="117" t="s">
+        <v>315</v>
+      </c>
+      <c r="BH4" s="117"/>
+      <c r="BI4" s="117"/>
+      <c r="BJ4" s="117"/>
       <c r="BK4" s="100"/>
       <c r="BL4" s="100"/>
       <c r="BM4" s="100"/>
@@ -3334,12 +3349,12 @@
       <c r="BQ4" s="103"/>
       <c r="BR4" s="103"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="121" t="s">
+      <c r="BT4" s="120" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="110"/>
       <c r="BV4" s="111"/>
-      <c r="BW4" s="121" t="s">
+      <c r="BW4" s="120" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="106"/>
@@ -3359,15 +3374,15 @@
       <c r="CL4" s="113"/>
       <c r="CM4" s="113"/>
       <c r="CN4" s="114"/>
-      <c r="CO4" s="121" t="s">
+      <c r="CO4" s="120" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3501,8 +3516,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="121"/>
-      <c r="AW5" s="121"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
       <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
@@ -3527,13 +3542,15 @@
       <c r="BE5" s="116" t="s">
         <v>309</v>
       </c>
-      <c r="BF5" s="143" t="s">
+      <c r="BF5" s="117" t="s">
         <v>312</v>
       </c>
-      <c r="BG5" s="143"/>
-      <c r="BH5" s="143"/>
-      <c r="BI5" s="143"/>
-      <c r="BJ5" s="143"/>
+      <c r="BG5" s="117" t="s">
+        <v>316</v>
+      </c>
+      <c r="BH5" s="117"/>
+      <c r="BI5" s="117"/>
+      <c r="BJ5" s="117"/>
       <c r="BK5" s="100"/>
       <c r="BL5" s="100"/>
       <c r="BM5" s="100"/>
@@ -3543,10 +3560,10 @@
       <c r="BQ5" s="103"/>
       <c r="BR5" s="103"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="121"/>
+      <c r="BT5" s="120"/>
       <c r="BU5" s="108"/>
       <c r="BV5" s="109"/>
-      <c r="BW5" s="121"/>
+      <c r="BW5" s="120"/>
       <c r="BX5" s="107"/>
       <c r="BY5" s="103"/>
       <c r="BZ5" s="112"/>
@@ -3564,13 +3581,13 @@
       <c r="CL5" s="113"/>
       <c r="CM5" s="113"/>
       <c r="CN5" s="114"/>
-      <c r="CO5" s="121"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="118" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3706,8 +3723,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="121"/>
-      <c r="AW6" s="121"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
       <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
@@ -3732,13 +3749,15 @@
       <c r="BE6" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="BF6" s="143" t="s">
+      <c r="BF6" s="117" t="s">
         <v>313</v>
       </c>
-      <c r="BG6" s="143"/>
-      <c r="BH6" s="143"/>
-      <c r="BI6" s="143"/>
-      <c r="BJ6" s="143"/>
+      <c r="BG6" s="117" t="s">
+        <v>317</v>
+      </c>
+      <c r="BH6" s="117"/>
+      <c r="BI6" s="117"/>
+      <c r="BJ6" s="117"/>
       <c r="BK6" s="100"/>
       <c r="BL6" s="100"/>
       <c r="BM6" s="100"/>
@@ -3748,10 +3767,10 @@
       <c r="BQ6" s="103"/>
       <c r="BR6" s="103"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="121"/>
+      <c r="BT6" s="120"/>
       <c r="BU6" s="108"/>
       <c r="BV6" s="109"/>
-      <c r="BW6" s="121"/>
+      <c r="BW6" s="120"/>
       <c r="BX6" s="107"/>
       <c r="BY6" s="103"/>
       <c r="BZ6" s="112"/>
@@ -3769,13 +3788,13 @@
       <c r="CL6" s="113"/>
       <c r="CM6" s="113"/>
       <c r="CN6" s="114"/>
-      <c r="CO6" s="121"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="118" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="123"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3911,8 +3930,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="121"/>
-      <c r="AW7" s="121"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
       <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
@@ -3937,13 +3956,15 @@
       <c r="BE7" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="BF7" s="143" t="s">
+      <c r="BF7" s="117" t="s">
         <v>314</v>
       </c>
-      <c r="BG7" s="143"/>
-      <c r="BH7" s="143"/>
-      <c r="BI7" s="143"/>
-      <c r="BJ7" s="143"/>
+      <c r="BG7" s="117" t="s">
+        <v>318</v>
+      </c>
+      <c r="BH7" s="117"/>
+      <c r="BI7" s="117"/>
+      <c r="BJ7" s="117"/>
       <c r="BK7" s="100"/>
       <c r="BL7" s="100"/>
       <c r="BM7" s="100"/>
@@ -3953,10 +3974,10 @@
       <c r="BQ7" s="103"/>
       <c r="BR7" s="103"/>
       <c r="BS7" s="104"/>
-      <c r="BT7" s="121"/>
+      <c r="BT7" s="120"/>
       <c r="BU7" s="108"/>
       <c r="BV7" s="109"/>
-      <c r="BW7" s="121"/>
+      <c r="BW7" s="120"/>
       <c r="BX7" s="107"/>
       <c r="BY7" s="103"/>
       <c r="BZ7" s="112"/>
@@ -3974,25 +3995,25 @@
       <c r="CL7" s="113"/>
       <c r="CM7" s="113"/>
       <c r="CN7" s="114"/>
-      <c r="CO7" s="121"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4075,36 +4096,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="129" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="133" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="132"/>
+      <c r="G2" s="133"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="133" t="s">
+      <c r="I2" s="134" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="133"/>
+      <c r="J2" s="134"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="134" t="s">
+      <c r="L2" s="135" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="134"/>
+      <c r="M2" s="135"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="135" t="s">
+      <c r="O2" s="136" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="135"/>
+      <c r="P2" s="136"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="124" t="s">
+      <c r="R2" s="125" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="124"/>
+      <c r="S2" s="125"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4138,24 +4159,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="124"/>
-      <c r="S3" s="124"/>
+      <c r="R3" s="125"/>
+      <c r="S3" s="125"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4189,24 +4210,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="134"/>
-      <c r="M4" s="134"/>
+      <c r="L4" s="135"/>
+      <c r="M4" s="135"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="135"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="125"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4244,20 +4265,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="134"/>
-      <c r="M5" s="134"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="135"/>
-      <c r="P5" s="135"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="124"/>
+      <c r="R5" s="125"/>
+      <c r="S5" s="125"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4291,26 +4312,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="130" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="130"/>
-      <c r="D6" s="130"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="136"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
+      <c r="R6" s="125"/>
+      <c r="S6" s="125"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4344,24 +4365,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="133"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="134"/>
-      <c r="M7" s="134"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="124"/>
-      <c r="S7" s="124"/>
+      <c r="R7" s="125"/>
+      <c r="S7" s="125"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4395,24 +4416,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="130"/>
-      <c r="C8" s="130"/>
-      <c r="D8" s="130"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="133"/>
-      <c r="J8" s="133"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="134"/>
-      <c r="M8" s="134"/>
+      <c r="L8" s="135"/>
+      <c r="M8" s="135"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="135"/>
-      <c r="P8" s="135"/>
+      <c r="O8" s="136"/>
+      <c r="P8" s="136"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="124"/>
-      <c r="S8" s="124"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4446,24 +4467,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="130"/>
-      <c r="C9" s="130"/>
-      <c r="D9" s="130"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="132"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="133"/>
-      <c r="J9" s="133"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="134"/>
-      <c r="M9" s="134"/>
+      <c r="L9" s="135"/>
+      <c r="M9" s="135"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="135"/>
-      <c r="P9" s="135"/>
+      <c r="O9" s="136"/>
+      <c r="P9" s="136"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="124"/>
-      <c r="S9" s="124"/>
+      <c r="R9" s="125"/>
+      <c r="S9" s="125"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4497,24 +4518,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="130"/>
-      <c r="C10" s="130"/>
-      <c r="D10" s="130"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="133"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="134"/>
-      <c r="M10" s="134"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="135"/>
-      <c r="P10" s="135"/>
+      <c r="O10" s="136"/>
+      <c r="P10" s="136"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="124"/>
+      <c r="R10" s="125"/>
+      <c r="S10" s="125"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4603,23 +4624,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="125" t="s">
+      <c r="F12" s="126" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="125"/>
+      <c r="G12" s="126"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="126" t="s">
+      <c r="I12" s="127" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="126"/>
+      <c r="J12" s="127"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="127" t="s">
+      <c r="L12" s="128" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="127"/>
+      <c r="M12" s="128"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="131"/>
-      <c r="P12" s="131"/>
+      <c r="O12" s="132"/>
+      <c r="P12" s="132"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4660,17 +4681,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="125"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="126"/>
-      <c r="J13" s="126"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="127"/>
-      <c r="M13" s="127"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="128"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="131"/>
-      <c r="P13" s="131"/>
+      <c r="O13" s="132"/>
+      <c r="P13" s="132"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4711,17 +4732,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="125"/>
-      <c r="G14" s="125"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="126"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="127"/>
-      <c r="M14" s="127"/>
+      <c r="L14" s="128"/>
+      <c r="M14" s="128"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="131"/>
-      <c r="P14" s="131"/>
+      <c r="O14" s="132"/>
+      <c r="P14" s="132"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4762,17 +4783,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="125"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="126"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="126"/>
-      <c r="J15" s="126"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="127"/>
-      <c r="M15" s="127"/>
+      <c r="L15" s="128"/>
+      <c r="M15" s="128"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="131"/>
-      <c r="P15" s="131"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="132"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -4813,17 +4834,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="125"/>
-      <c r="G16" s="125"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="126"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="127"/>
-      <c r="M16" s="127"/>
+      <c r="L16" s="128"/>
+      <c r="M16" s="128"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="131"/>
-      <c r="P16" s="131"/>
+      <c r="O16" s="132"/>
+      <c r="P16" s="132"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -4864,17 +4885,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="125"/>
-      <c r="G17" s="125"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="126"/>
-      <c r="J17" s="126"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
+      <c r="L17" s="128"/>
+      <c r="M17" s="128"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="131"/>
-      <c r="P17" s="131"/>
+      <c r="O17" s="132"/>
+      <c r="P17" s="132"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -4915,17 +4936,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="125"/>
-      <c r="G18" s="125"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="126"/>
-      <c r="J18" s="126"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="127"/>
-      <c r="M18" s="127"/>
+      <c r="L18" s="128"/>
+      <c r="M18" s="128"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="131"/>
-      <c r="P18" s="131"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="132"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -4966,17 +4987,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="125"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="126"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="127"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="127"/>
-      <c r="M19" s="127"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="128"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="131"/>
-      <c r="P19" s="131"/>
+      <c r="O19" s="132"/>
+      <c r="P19" s="132"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5017,17 +5038,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="125"/>
-      <c r="G20" s="125"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="126"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="126"/>
-      <c r="J20" s="126"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="127"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="127"/>
-      <c r="M20" s="127"/>
+      <c r="L20" s="128"/>
+      <c r="M20" s="128"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="131"/>
-      <c r="P20" s="131"/>
+      <c r="O20" s="132"/>
+      <c r="P20" s="132"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17600,7 +17621,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -17940,7 +17961,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="138"/>
+      <c r="A2" s="139"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18266,15 +18287,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="139"/>
-      <c r="DH2" s="139"/>
-      <c r="DI2" s="139"/>
-      <c r="DJ2" s="139"/>
+      <c r="DG2" s="140"/>
+      <c r="DH2" s="140"/>
+      <c r="DI2" s="140"/>
+      <c r="DJ2" s="140"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="138"/>
+      <c r="A3" s="139"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18611,7 +18632,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="141" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18753,7 +18774,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="140"/>
+      <c r="B5" s="141"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -18893,7 +18914,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="140"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19033,7 +19054,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="140"/>
+      <c r="B7" s="141"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19171,7 +19192,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="140"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19311,7 +19332,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="142" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19453,7 +19474,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="141"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19593,7 +19614,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="142" t="s">
+      <c r="B11" s="143" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19723,7 +19744,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="142"/>
+      <c r="B12" s="143"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -19861,7 +19882,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="142"/>
+      <c r="B13" s="143"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20001,7 +20022,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="142"/>
+      <c r="B14" s="143"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20137,7 +20158,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="142"/>
+      <c r="B15" s="143"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20273,7 +20294,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="142"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20409,7 +20430,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="142"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20545,7 +20566,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20685,7 +20706,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="142"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -20821,7 +20842,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="142"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -20957,7 +20978,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="137" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21091,7 +21112,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="136"/>
+      <c r="B22" s="137"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21227,7 +21248,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="136"/>
+      <c r="B23" s="137"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21359,7 +21380,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="136"/>
+      <c r="B24" s="137"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21493,7 +21514,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="136"/>
+      <c r="B25" s="137"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21637,7 +21658,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="137" t="s">
+      <c r="B26" s="138" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -21771,7 +21792,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="137"/>
+      <c r="B27" s="138"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -21911,7 +21932,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="137"/>
+      <c r="B28" s="138"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22043,7 +22064,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="137"/>
+      <c r="B29" s="138"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22171,7 +22192,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="137"/>
+      <c r="B30" s="138"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22297,7 +22318,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="137"/>
+      <c r="B31" s="138"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 31-10 e 01-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0FDC5-536A-45A1-901B-F284931DF07E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D37A9BD-A742-483D-9326-4F31B154AB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="327">
   <si>
     <t>REDES</t>
   </si>
@@ -1069,6 +1069,30 @@
   </si>
   <si>
     <t>Levantamento do pronto para a versão beta e planning</t>
+  </si>
+  <si>
+    <t>Validação dos campos no cadastro de usuário, de chamados, edição de usuário e reabertura de chamados API, Responsividade WEB, editar solicitação de cadastro de usuário API</t>
+  </si>
+  <si>
+    <t>Definição do layout para exibição dos gráficos (relatório) e impressão, integração da API com o banco de dados do cliente. Integração back-end e front-end</t>
+  </si>
+  <si>
+    <t>Planning, dashboard, testes de endpoints, método de exportar usuário em planilha, alteração cadastro usuário, listagem geral na página de exportação</t>
+  </si>
+  <si>
+    <t>Refatoração API incluindo Achievements, estudo blobs, layout de alta fidelidade de achievements</t>
+  </si>
+  <si>
+    <t>Responsividade WEB, deletar usuário API, ajuste de permissões API, estilização da lista de chamados Mobile com filtro, responsividade WEB</t>
+  </si>
+  <si>
+    <t>Definição do layout para exibição dos gráficos (relatório) e impressão, integração back-end e front-end</t>
+  </si>
+  <si>
+    <t>Drag and drop, estilização dashboard, feedback de cadastro, select para listagem</t>
+  </si>
+  <si>
+    <t>Endpoints de listagem API, estudo blobs, estilização página de achievements</t>
   </si>
 </sst>
 </file>
@@ -1963,18 +1987,6 @@
     <xf numFmtId="0" fontId="12" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1983,6 +1995,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2441,7 +2465,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="BD4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BG8" sqref="BG8"/>
+      <selection pane="bottomRight" activeCell="BL7" sqref="BL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2474,7 +2498,9 @@
     <col min="54" max="54" width="30.77734375" customWidth="1"/>
     <col min="55" max="58" width="20.77734375" customWidth="1"/>
     <col min="59" max="59" width="30.77734375" customWidth="1"/>
-    <col min="60" max="71" width="5.77734375" customWidth="1"/>
+    <col min="60" max="60" width="25.77734375" customWidth="1"/>
+    <col min="61" max="61" width="20.77734375" customWidth="1"/>
+    <col min="62" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2484,7 +2510,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="118" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2764,7 +2790,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123"/>
+      <c r="A2" s="119"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2874,7 +2900,7 @@
       <c r="CR2" s="121"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="124"/>
+      <c r="A3" s="120"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3162,10 +3188,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="119"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3301,10 +3327,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="122" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="122" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3337,8 +3363,12 @@
       <c r="BG4" s="117" t="s">
         <v>315</v>
       </c>
-      <c r="BH4" s="117"/>
-      <c r="BI4" s="117"/>
+      <c r="BH4" s="117" t="s">
+        <v>319</v>
+      </c>
+      <c r="BI4" s="117" t="s">
+        <v>323</v>
+      </c>
       <c r="BJ4" s="117"/>
       <c r="BK4" s="100"/>
       <c r="BL4" s="100"/>
@@ -3349,12 +3379,12 @@
       <c r="BQ4" s="103"/>
       <c r="BR4" s="103"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="120" t="s">
+      <c r="BT4" s="122" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="110"/>
       <c r="BV4" s="111"/>
-      <c r="BW4" s="120" t="s">
+      <c r="BW4" s="122" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="106"/>
@@ -3374,15 +3404,15 @@
       <c r="CL4" s="113"/>
       <c r="CM4" s="113"/>
       <c r="CN4" s="114"/>
-      <c r="CO4" s="120" t="s">
+      <c r="CO4" s="122" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="123" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="119"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3516,8 +3546,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
+      <c r="AV5" s="122"/>
+      <c r="AW5" s="122"/>
       <c r="AX5" s="115" t="s">
         <v>283</v>
       </c>
@@ -3548,8 +3578,12 @@
       <c r="BG5" s="117" t="s">
         <v>316</v>
       </c>
-      <c r="BH5" s="117"/>
-      <c r="BI5" s="117"/>
+      <c r="BH5" s="117" t="s">
+        <v>320</v>
+      </c>
+      <c r="BI5" s="117" t="s">
+        <v>324</v>
+      </c>
       <c r="BJ5" s="117"/>
       <c r="BK5" s="100"/>
       <c r="BL5" s="100"/>
@@ -3560,10 +3594,10 @@
       <c r="BQ5" s="103"/>
       <c r="BR5" s="103"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="120"/>
+      <c r="BT5" s="122"/>
       <c r="BU5" s="108"/>
       <c r="BV5" s="109"/>
-      <c r="BW5" s="120"/>
+      <c r="BW5" s="122"/>
       <c r="BX5" s="107"/>
       <c r="BY5" s="103"/>
       <c r="BZ5" s="112"/>
@@ -3581,13 +3615,13 @@
       <c r="CL5" s="113"/>
       <c r="CM5" s="113"/>
       <c r="CN5" s="114"/>
-      <c r="CO5" s="120"/>
+      <c r="CO5" s="122"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="119"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3723,8 +3757,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
+      <c r="AV6" s="122"/>
+      <c r="AW6" s="122"/>
       <c r="AX6" s="115" t="s">
         <v>284</v>
       </c>
@@ -3755,8 +3789,12 @@
       <c r="BG6" s="117" t="s">
         <v>317</v>
       </c>
-      <c r="BH6" s="117"/>
-      <c r="BI6" s="117"/>
+      <c r="BH6" s="117" t="s">
+        <v>321</v>
+      </c>
+      <c r="BI6" s="117" t="s">
+        <v>325</v>
+      </c>
       <c r="BJ6" s="117"/>
       <c r="BK6" s="100"/>
       <c r="BL6" s="100"/>
@@ -3767,10 +3805,10 @@
       <c r="BQ6" s="103"/>
       <c r="BR6" s="103"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="120"/>
+      <c r="BT6" s="122"/>
       <c r="BU6" s="108"/>
       <c r="BV6" s="109"/>
-      <c r="BW6" s="120"/>
+      <c r="BW6" s="122"/>
       <c r="BX6" s="107"/>
       <c r="BY6" s="103"/>
       <c r="BZ6" s="112"/>
@@ -3788,13 +3826,13 @@
       <c r="CL6" s="113"/>
       <c r="CM6" s="113"/>
       <c r="CN6" s="114"/>
-      <c r="CO6" s="120"/>
+      <c r="CO6" s="122"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="123" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="119"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3930,8 +3968,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
+      <c r="AV7" s="122"/>
+      <c r="AW7" s="122"/>
       <c r="AX7" s="115" t="s">
         <v>285</v>
       </c>
@@ -3962,8 +4000,12 @@
       <c r="BG7" s="117" t="s">
         <v>318</v>
       </c>
-      <c r="BH7" s="117"/>
-      <c r="BI7" s="117"/>
+      <c r="BH7" s="117" t="s">
+        <v>322</v>
+      </c>
+      <c r="BI7" s="117" t="s">
+        <v>326</v>
+      </c>
       <c r="BJ7" s="117"/>
       <c r="BK7" s="100"/>
       <c r="BL7" s="100"/>
@@ -3974,10 +4016,10 @@
       <c r="BQ7" s="103"/>
       <c r="BR7" s="103"/>
       <c r="BS7" s="104"/>
-      <c r="BT7" s="120"/>
+      <c r="BT7" s="122"/>
       <c r="BU7" s="108"/>
       <c r="BV7" s="109"/>
-      <c r="BW7" s="120"/>
+      <c r="BW7" s="122"/>
       <c r="BX7" s="107"/>
       <c r="BY7" s="103"/>
       <c r="BZ7" s="112"/>
@@ -3995,25 +4037,25 @@
       <c r="CL7" s="113"/>
       <c r="CM7" s="113"/>
       <c r="CN7" s="114"/>
-      <c r="CO7" s="120"/>
+      <c r="CO7" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 07-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D37A9BD-A742-483D-9326-4F31B154AB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C3AD13-3BA4-4069-975A-DB835A7615E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="331">
   <si>
     <t>REDES</t>
   </si>
@@ -1093,6 +1093,18 @@
   </si>
   <si>
     <t>Endpoints de listagem API, estudo blobs, estilização página de achievements</t>
+  </si>
+  <si>
+    <t>Início de testes unitários e adicionado filtro nas listagens</t>
+  </si>
+  <si>
+    <t>Exportar relatórios para PDF, tela editar usuário, migração de database first para codefirst</t>
+  </si>
+  <si>
+    <t>Configuração de ambiente para projeto Mobile, tela de listagem geral e edição de dados</t>
+  </si>
+  <si>
+    <t>Estilização página Achievements, refatoração de listagens, método de adicionar e remover Achievement do Bloco</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1251,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1474,12 +1486,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBF8F00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -1682,7 +1688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1933,50 +1939,11 @@
     <xf numFmtId="0" fontId="12" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1987,6 +1954,18 @@
     <xf numFmtId="0" fontId="12" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1995,18 +1974,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2064,6 +2031,39 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2139,10 +2139,10 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF2F75B5"/>
+      <color rgb="FF548235"/>
       <color rgb="FFBF8F00"/>
-      <color rgb="FF2F75B5"/>
       <color rgb="FF9B54D0"/>
-      <color rgb="FF548235"/>
       <color rgb="FFF9F9F9"/>
       <color rgb="FFCB3D3D"/>
       <color rgb="FFDCDCDC"/>
@@ -2462,10 +2462,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BD4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BG4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BL7" sqref="BL7"/>
+      <selection pane="bottomRight" activeCell="BO6" sqref="BO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2500,7 +2500,9 @@
     <col min="59" max="59" width="30.77734375" customWidth="1"/>
     <col min="60" max="60" width="25.77734375" customWidth="1"/>
     <col min="61" max="61" width="20.77734375" customWidth="1"/>
-    <col min="62" max="71" width="5.77734375" customWidth="1"/>
+    <col min="62" max="64" width="15.77734375" customWidth="1"/>
+    <col min="65" max="65" width="20.77734375" customWidth="1"/>
+    <col min="66" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2510,7 +2512,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="109" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2790,117 +2792,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="119"/>
+      <c r="A2" s="110"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="121" t="s">
+      <c r="C2" s="108" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
-      <c r="Q2" s="121"/>
-      <c r="R2" s="121" t="s">
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="121"/>
-      <c r="T2" s="121"/>
-      <c r="U2" s="121"/>
-      <c r="V2" s="121"/>
-      <c r="W2" s="121"/>
-      <c r="X2" s="121"/>
-      <c r="Y2" s="121"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="121"/>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="121"/>
-      <c r="AD2" s="121"/>
-      <c r="AE2" s="121"/>
-      <c r="AF2" s="121"/>
-      <c r="AG2" s="121"/>
-      <c r="AH2" s="121"/>
-      <c r="AI2" s="121"/>
-      <c r="AJ2" s="121"/>
-      <c r="AK2" s="121"/>
-      <c r="AL2" s="121"/>
-      <c r="AM2" s="121" t="s">
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="108"/>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
+      <c r="AA2" s="108"/>
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="108"/>
+      <c r="AD2" s="108"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="108"/>
+      <c r="AG2" s="108"/>
+      <c r="AH2" s="108"/>
+      <c r="AI2" s="108"/>
+      <c r="AJ2" s="108"/>
+      <c r="AK2" s="108"/>
+      <c r="AL2" s="108"/>
+      <c r="AM2" s="108" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="121"/>
-      <c r="AO2" s="121"/>
-      <c r="AP2" s="121"/>
-      <c r="AQ2" s="121"/>
-      <c r="AR2" s="121"/>
-      <c r="AS2" s="121"/>
-      <c r="AT2" s="121"/>
-      <c r="AU2" s="121"/>
-      <c r="AV2" s="121"/>
-      <c r="AW2" s="121"/>
-      <c r="AX2" s="121"/>
-      <c r="AY2" s="121"/>
-      <c r="AZ2" s="121"/>
-      <c r="BA2" s="121"/>
-      <c r="BB2" s="121"/>
-      <c r="BC2" s="121"/>
-      <c r="BD2" s="121"/>
-      <c r="BE2" s="121"/>
-      <c r="BF2" s="121"/>
-      <c r="BG2" s="121"/>
-      <c r="BH2" s="121"/>
-      <c r="BI2" s="121"/>
-      <c r="BJ2" s="121" t="s">
+      <c r="AN2" s="108"/>
+      <c r="AO2" s="108"/>
+      <c r="AP2" s="108"/>
+      <c r="AQ2" s="108"/>
+      <c r="AR2" s="108"/>
+      <c r="AS2" s="108"/>
+      <c r="AT2" s="108"/>
+      <c r="AU2" s="108"/>
+      <c r="AV2" s="108"/>
+      <c r="AW2" s="108"/>
+      <c r="AX2" s="108"/>
+      <c r="AY2" s="108"/>
+      <c r="AZ2" s="108"/>
+      <c r="BA2" s="108"/>
+      <c r="BB2" s="108"/>
+      <c r="BC2" s="108"/>
+      <c r="BD2" s="108"/>
+      <c r="BE2" s="108"/>
+      <c r="BF2" s="108"/>
+      <c r="BG2" s="108"/>
+      <c r="BH2" s="108"/>
+      <c r="BI2" s="108"/>
+      <c r="BJ2" s="108" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="121"/>
-      <c r="BL2" s="121"/>
-      <c r="BM2" s="121"/>
-      <c r="BN2" s="121"/>
-      <c r="BO2" s="121"/>
-      <c r="BP2" s="121"/>
-      <c r="BQ2" s="121"/>
-      <c r="BR2" s="121"/>
-      <c r="BS2" s="121"/>
-      <c r="BT2" s="121"/>
-      <c r="BU2" s="121"/>
-      <c r="BV2" s="121"/>
-      <c r="BW2" s="121"/>
-      <c r="BX2" s="121"/>
-      <c r="BY2" s="121"/>
-      <c r="BZ2" s="121"/>
-      <c r="CA2" s="121"/>
-      <c r="CB2" s="121"/>
-      <c r="CC2" s="121"/>
-      <c r="CD2" s="121"/>
-      <c r="CE2" s="121" t="s">
+      <c r="BK2" s="108"/>
+      <c r="BL2" s="108"/>
+      <c r="BM2" s="108"/>
+      <c r="BN2" s="108"/>
+      <c r="BO2" s="108"/>
+      <c r="BP2" s="108"/>
+      <c r="BQ2" s="108"/>
+      <c r="BR2" s="108"/>
+      <c r="BS2" s="108"/>
+      <c r="BT2" s="108"/>
+      <c r="BU2" s="108"/>
+      <c r="BV2" s="108"/>
+      <c r="BW2" s="108"/>
+      <c r="BX2" s="108"/>
+      <c r="BY2" s="108"/>
+      <c r="BZ2" s="108"/>
+      <c r="CA2" s="108"/>
+      <c r="CB2" s="108"/>
+      <c r="CC2" s="108"/>
+      <c r="CD2" s="108"/>
+      <c r="CE2" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="121"/>
-      <c r="CG2" s="121"/>
-      <c r="CH2" s="121"/>
-      <c r="CI2" s="121"/>
-      <c r="CJ2" s="121"/>
-      <c r="CK2" s="121"/>
-      <c r="CL2" s="121"/>
-      <c r="CM2" s="121"/>
-      <c r="CN2" s="121"/>
-      <c r="CO2" s="121"/>
-      <c r="CP2" s="121"/>
-      <c r="CQ2" s="121"/>
-      <c r="CR2" s="121"/>
+      <c r="CF2" s="108"/>
+      <c r="CG2" s="108"/>
+      <c r="CH2" s="108"/>
+      <c r="CI2" s="108"/>
+      <c r="CJ2" s="108"/>
+      <c r="CK2" s="108"/>
+      <c r="CL2" s="108"/>
+      <c r="CM2" s="108"/>
+      <c r="CN2" s="108"/>
+      <c r="CO2" s="108"/>
+      <c r="CP2" s="108"/>
+      <c r="CQ2" s="108"/>
+      <c r="CR2" s="108"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="120"/>
+      <c r="A3" s="111"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3051,10 +3053,10 @@
       <c r="AY3" s="99">
         <v>17</v>
       </c>
-      <c r="AZ3" s="101">
+      <c r="AZ3" s="100">
         <v>18</v>
       </c>
-      <c r="BA3" s="101">
+      <c r="BA3" s="100">
         <v>21</v>
       </c>
       <c r="BB3" s="99">
@@ -3066,10 +3068,10 @@
       <c r="BD3" s="99">
         <v>24</v>
       </c>
-      <c r="BE3" s="101">
+      <c r="BE3" s="100">
         <v>25</v>
       </c>
-      <c r="BF3" s="101">
+      <c r="BF3" s="100">
         <v>28</v>
       </c>
       <c r="BG3" s="99">
@@ -3081,10 +3083,10 @@
       <c r="BI3" s="99">
         <v>31</v>
       </c>
-      <c r="BJ3" s="101">
+      <c r="BJ3" s="100">
         <v>1</v>
       </c>
-      <c r="BK3" s="101">
+      <c r="BK3" s="100">
         <v>4</v>
       </c>
       <c r="BL3" s="99">
@@ -3096,10 +3098,10 @@
       <c r="BN3" s="99">
         <v>7</v>
       </c>
-      <c r="BO3" s="101">
+      <c r="BO3" s="100">
         <v>8</v>
       </c>
-      <c r="BP3" s="101">
+      <c r="BP3" s="100">
         <v>11</v>
       </c>
       <c r="BQ3" s="99">
@@ -3114,7 +3116,7 @@
       <c r="BT3" s="83">
         <v>15</v>
       </c>
-      <c r="BU3" s="101">
+      <c r="BU3" s="100">
         <v>18</v>
       </c>
       <c r="BV3" s="99">
@@ -3126,10 +3128,10 @@
       <c r="BX3" s="99">
         <v>21</v>
       </c>
-      <c r="BY3" s="101">
+      <c r="BY3" s="100">
         <v>22</v>
       </c>
-      <c r="BZ3" s="101">
+      <c r="BZ3" s="100">
         <v>25</v>
       </c>
       <c r="CA3" s="99">
@@ -3141,10 +3143,10 @@
       <c r="CC3" s="99">
         <v>28</v>
       </c>
-      <c r="CD3" s="101">
+      <c r="CD3" s="100">
         <v>29</v>
       </c>
-      <c r="CE3" s="101">
+      <c r="CE3" s="100">
         <v>2</v>
       </c>
       <c r="CF3" s="99">
@@ -3156,10 +3158,10 @@
       <c r="CH3" s="99">
         <v>5</v>
       </c>
-      <c r="CI3" s="101">
+      <c r="CI3" s="100">
         <v>6</v>
       </c>
-      <c r="CJ3" s="101">
+      <c r="CJ3" s="100">
         <v>9</v>
       </c>
       <c r="CK3" s="99">
@@ -3171,13 +3173,13 @@
       <c r="CM3" s="99">
         <v>12</v>
       </c>
-      <c r="CN3" s="101">
+      <c r="CN3" s="100">
         <v>13</v>
       </c>
       <c r="CO3" s="83">
         <v>14</v>
       </c>
-      <c r="CP3" s="102">
+      <c r="CP3" s="101">
         <v>16</v>
       </c>
       <c r="CQ3" s="85">
@@ -3188,10 +3190,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="124"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3327,92 +3329,100 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="122" t="s">
+      <c r="AV4" s="107" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="122" t="s">
+      <c r="AW4" s="107" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
         <v>282</v>
       </c>
-      <c r="AY4" s="116" t="s">
+      <c r="AY4" s="103" t="s">
         <v>286</v>
       </c>
-      <c r="AZ4" s="116" t="s">
+      <c r="AZ4" s="103" t="s">
         <v>290</v>
       </c>
-      <c r="BA4" s="116" t="s">
+      <c r="BA4" s="103" t="s">
         <v>294</v>
       </c>
-      <c r="BB4" s="116" t="s">
+      <c r="BB4" s="103" t="s">
         <v>298</v>
       </c>
-      <c r="BC4" s="116" t="s">
+      <c r="BC4" s="103" t="s">
         <v>302</v>
       </c>
-      <c r="BD4" s="116" t="s">
+      <c r="BD4" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="BE4" s="116" t="s">
+      <c r="BE4" s="103" t="s">
         <v>308</v>
       </c>
-      <c r="BF4" s="117" t="s">
+      <c r="BF4" s="104" t="s">
         <v>311</v>
       </c>
-      <c r="BG4" s="117" t="s">
+      <c r="BG4" s="104" t="s">
         <v>315</v>
       </c>
-      <c r="BH4" s="117" t="s">
+      <c r="BH4" s="104" t="s">
         <v>319</v>
       </c>
-      <c r="BI4" s="117" t="s">
+      <c r="BI4" s="104" t="s">
         <v>323</v>
       </c>
-      <c r="BJ4" s="117"/>
-      <c r="BK4" s="100"/>
-      <c r="BL4" s="100"/>
-      <c r="BM4" s="100"/>
-      <c r="BN4" s="100"/>
-      <c r="BO4" s="100"/>
-      <c r="BP4" s="103"/>
-      <c r="BQ4" s="103"/>
-      <c r="BR4" s="103"/>
-      <c r="BS4" s="105"/>
-      <c r="BT4" s="122" t="s">
+      <c r="BJ4" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BK4" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BL4" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BM4" s="104" t="s">
+        <v>327</v>
+      </c>
+      <c r="BN4" s="104"/>
+      <c r="BO4" s="104"/>
+      <c r="BP4" s="104"/>
+      <c r="BQ4" s="104"/>
+      <c r="BR4" s="104"/>
+      <c r="BS4" s="131"/>
+      <c r="BT4" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="BU4" s="110"/>
-      <c r="BV4" s="111"/>
-      <c r="BW4" s="122" t="s">
+      <c r="BU4" s="133"/>
+      <c r="BV4" s="134"/>
+      <c r="BW4" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="106"/>
-      <c r="BY4" s="103"/>
-      <c r="BZ4" s="112"/>
-      <c r="CA4" s="112"/>
-      <c r="CB4" s="112"/>
-      <c r="CC4" s="112"/>
-      <c r="CD4" s="112"/>
-      <c r="CE4" s="112"/>
-      <c r="CF4" s="112"/>
-      <c r="CG4" s="112"/>
-      <c r="CH4" s="112"/>
-      <c r="CI4" s="112"/>
-      <c r="CJ4" s="113"/>
-      <c r="CK4" s="113"/>
-      <c r="CL4" s="113"/>
-      <c r="CM4" s="113"/>
-      <c r="CN4" s="114"/>
-      <c r="CO4" s="122" t="s">
+      <c r="BX4" s="137"/>
+      <c r="BY4" s="138"/>
+      <c r="BZ4" s="138"/>
+      <c r="CA4" s="138"/>
+      <c r="CB4" s="138"/>
+      <c r="CC4" s="138"/>
+      <c r="CD4" s="138"/>
+      <c r="CE4" s="140"/>
+      <c r="CF4" s="140"/>
+      <c r="CG4" s="140"/>
+      <c r="CH4" s="140"/>
+      <c r="CI4" s="140"/>
+      <c r="CJ4" s="140"/>
+      <c r="CK4" s="140"/>
+      <c r="CL4" s="140"/>
+      <c r="CM4" s="140"/>
+      <c r="CN4" s="141"/>
+      <c r="CO4" s="107" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="123" t="s">
+      <c r="A5" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="124"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3546,82 +3556,90 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="122"/>
-      <c r="AW5" s="122"/>
-      <c r="AX5" s="115" t="s">
+      <c r="AV5" s="107"/>
+      <c r="AW5" s="107"/>
+      <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
-      <c r="AY5" s="116" t="s">
+      <c r="AY5" s="103" t="s">
         <v>287</v>
       </c>
-      <c r="AZ5" s="116" t="s">
+      <c r="AZ5" s="103" t="s">
         <v>291</v>
       </c>
-      <c r="BA5" s="116" t="s">
+      <c r="BA5" s="103" t="s">
         <v>295</v>
       </c>
-      <c r="BB5" s="116" t="s">
+      <c r="BB5" s="103" t="s">
         <v>299</v>
       </c>
-      <c r="BC5" s="116" t="s">
+      <c r="BC5" s="103" t="s">
         <v>299</v>
       </c>
-      <c r="BD5" s="116" t="s">
+      <c r="BD5" s="103" t="s">
         <v>306</v>
       </c>
-      <c r="BE5" s="116" t="s">
+      <c r="BE5" s="103" t="s">
         <v>309</v>
       </c>
-      <c r="BF5" s="117" t="s">
+      <c r="BF5" s="104" t="s">
         <v>312</v>
       </c>
-      <c r="BG5" s="117" t="s">
+      <c r="BG5" s="104" t="s">
         <v>316</v>
       </c>
-      <c r="BH5" s="117" t="s">
+      <c r="BH5" s="104" t="s">
         <v>320</v>
       </c>
-      <c r="BI5" s="117" t="s">
+      <c r="BI5" s="104" t="s">
         <v>324</v>
       </c>
-      <c r="BJ5" s="117"/>
-      <c r="BK5" s="100"/>
-      <c r="BL5" s="100"/>
-      <c r="BM5" s="100"/>
-      <c r="BN5" s="100"/>
-      <c r="BO5" s="100"/>
-      <c r="BP5" s="103"/>
-      <c r="BQ5" s="103"/>
-      <c r="BR5" s="103"/>
-      <c r="BS5" s="105"/>
-      <c r="BT5" s="122"/>
-      <c r="BU5" s="108"/>
-      <c r="BV5" s="109"/>
-      <c r="BW5" s="122"/>
-      <c r="BX5" s="107"/>
-      <c r="BY5" s="103"/>
-      <c r="BZ5" s="112"/>
-      <c r="CA5" s="112"/>
-      <c r="CB5" s="112"/>
-      <c r="CC5" s="112"/>
-      <c r="CD5" s="112"/>
-      <c r="CE5" s="112"/>
-      <c r="CF5" s="112"/>
-      <c r="CG5" s="112"/>
-      <c r="CH5" s="112"/>
-      <c r="CI5" s="112"/>
-      <c r="CJ5" s="113"/>
-      <c r="CK5" s="113"/>
-      <c r="CL5" s="113"/>
-      <c r="CM5" s="113"/>
-      <c r="CN5" s="114"/>
-      <c r="CO5" s="122"/>
+      <c r="BJ5" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BK5" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BL5" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BM5" s="104" t="s">
+        <v>328</v>
+      </c>
+      <c r="BN5" s="104"/>
+      <c r="BO5" s="104"/>
+      <c r="BP5" s="104"/>
+      <c r="BQ5" s="104"/>
+      <c r="BR5" s="104"/>
+      <c r="BS5" s="131"/>
+      <c r="BT5" s="107"/>
+      <c r="BU5" s="135"/>
+      <c r="BV5" s="136"/>
+      <c r="BW5" s="107"/>
+      <c r="BX5" s="139"/>
+      <c r="BY5" s="138"/>
+      <c r="BZ5" s="138"/>
+      <c r="CA5" s="138"/>
+      <c r="CB5" s="138"/>
+      <c r="CC5" s="138"/>
+      <c r="CD5" s="138"/>
+      <c r="CE5" s="140"/>
+      <c r="CF5" s="140"/>
+      <c r="CG5" s="140"/>
+      <c r="CH5" s="140"/>
+      <c r="CI5" s="140"/>
+      <c r="CJ5" s="140"/>
+      <c r="CK5" s="140"/>
+      <c r="CL5" s="140"/>
+      <c r="CM5" s="140"/>
+      <c r="CN5" s="141"/>
+      <c r="CO5" s="107"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="123" t="s">
+      <c r="A6" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="124"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3757,82 +3775,90 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="122"/>
-      <c r="AW6" s="122"/>
-      <c r="AX6" s="115" t="s">
+      <c r="AV6" s="107"/>
+      <c r="AW6" s="107"/>
+      <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
-      <c r="AY6" s="116" t="s">
+      <c r="AY6" s="103" t="s">
         <v>288</v>
       </c>
-      <c r="AZ6" s="116" t="s">
+      <c r="AZ6" s="103" t="s">
         <v>292</v>
       </c>
-      <c r="BA6" s="116" t="s">
+      <c r="BA6" s="103" t="s">
         <v>296</v>
       </c>
-      <c r="BB6" s="116" t="s">
+      <c r="BB6" s="103" t="s">
         <v>300</v>
       </c>
-      <c r="BC6" s="116" t="s">
+      <c r="BC6" s="103" t="s">
         <v>303</v>
       </c>
-      <c r="BD6" s="116" t="s">
+      <c r="BD6" s="103" t="s">
         <v>302</v>
       </c>
-      <c r="BE6" s="116" t="s">
+      <c r="BE6" s="103" t="s">
         <v>310</v>
       </c>
-      <c r="BF6" s="117" t="s">
+      <c r="BF6" s="104" t="s">
         <v>313</v>
       </c>
-      <c r="BG6" s="117" t="s">
+      <c r="BG6" s="104" t="s">
         <v>317</v>
       </c>
-      <c r="BH6" s="117" t="s">
+      <c r="BH6" s="104" t="s">
         <v>321</v>
       </c>
-      <c r="BI6" s="117" t="s">
+      <c r="BI6" s="104" t="s">
         <v>325</v>
       </c>
-      <c r="BJ6" s="117"/>
-      <c r="BK6" s="100"/>
-      <c r="BL6" s="100"/>
-      <c r="BM6" s="100"/>
-      <c r="BN6" s="100"/>
-      <c r="BO6" s="100"/>
-      <c r="BP6" s="103"/>
-      <c r="BQ6" s="103"/>
-      <c r="BR6" s="103"/>
-      <c r="BS6" s="105"/>
-      <c r="BT6" s="122"/>
-      <c r="BU6" s="108"/>
-      <c r="BV6" s="109"/>
-      <c r="BW6" s="122"/>
-      <c r="BX6" s="107"/>
-      <c r="BY6" s="103"/>
-      <c r="BZ6" s="112"/>
-      <c r="CA6" s="112"/>
-      <c r="CB6" s="112"/>
-      <c r="CC6" s="112"/>
-      <c r="CD6" s="112"/>
-      <c r="CE6" s="112"/>
-      <c r="CF6" s="112"/>
-      <c r="CG6" s="112"/>
-      <c r="CH6" s="112"/>
-      <c r="CI6" s="112"/>
-      <c r="CJ6" s="113"/>
-      <c r="CK6" s="113"/>
-      <c r="CL6" s="113"/>
-      <c r="CM6" s="113"/>
-      <c r="CN6" s="114"/>
-      <c r="CO6" s="122"/>
+      <c r="BJ6" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BK6" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BL6" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BM6" s="104" t="s">
+        <v>329</v>
+      </c>
+      <c r="BN6" s="104"/>
+      <c r="BO6" s="104"/>
+      <c r="BP6" s="104"/>
+      <c r="BQ6" s="104"/>
+      <c r="BR6" s="104"/>
+      <c r="BS6" s="131"/>
+      <c r="BT6" s="107"/>
+      <c r="BU6" s="135"/>
+      <c r="BV6" s="136"/>
+      <c r="BW6" s="107"/>
+      <c r="BX6" s="139"/>
+      <c r="BY6" s="138"/>
+      <c r="BZ6" s="138"/>
+      <c r="CA6" s="138"/>
+      <c r="CB6" s="138"/>
+      <c r="CC6" s="138"/>
+      <c r="CD6" s="138"/>
+      <c r="CE6" s="140"/>
+      <c r="CF6" s="140"/>
+      <c r="CG6" s="140"/>
+      <c r="CH6" s="140"/>
+      <c r="CI6" s="140"/>
+      <c r="CJ6" s="140"/>
+      <c r="CK6" s="140"/>
+      <c r="CL6" s="140"/>
+      <c r="CM6" s="140"/>
+      <c r="CN6" s="141"/>
+      <c r="CO6" s="107"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="105" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="124"/>
+      <c r="B7" s="106"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3968,94 +3994,102 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="122"/>
-      <c r="AW7" s="122"/>
-      <c r="AX7" s="115" t="s">
+      <c r="AV7" s="107"/>
+      <c r="AW7" s="107"/>
+      <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="AY7" s="116" t="s">
+      <c r="AY7" s="103" t="s">
         <v>289</v>
       </c>
-      <c r="AZ7" s="116" t="s">
+      <c r="AZ7" s="103" t="s">
         <v>293</v>
       </c>
-      <c r="BA7" s="116" t="s">
+      <c r="BA7" s="103" t="s">
         <v>297</v>
       </c>
-      <c r="BB7" s="116" t="s">
+      <c r="BB7" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="BC7" s="116" t="s">
+      <c r="BC7" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="BD7" s="116" t="s">
+      <c r="BD7" s="103" t="s">
         <v>307</v>
       </c>
-      <c r="BE7" s="116" t="s">
+      <c r="BE7" s="103" t="s">
         <v>310</v>
       </c>
-      <c r="BF7" s="117" t="s">
+      <c r="BF7" s="104" t="s">
         <v>314</v>
       </c>
-      <c r="BG7" s="117" t="s">
+      <c r="BG7" s="104" t="s">
         <v>318</v>
       </c>
-      <c r="BH7" s="117" t="s">
+      <c r="BH7" s="104" t="s">
         <v>322</v>
       </c>
-      <c r="BI7" s="117" t="s">
+      <c r="BI7" s="104" t="s">
         <v>326</v>
       </c>
-      <c r="BJ7" s="117"/>
-      <c r="BK7" s="100"/>
-      <c r="BL7" s="100"/>
-      <c r="BM7" s="100"/>
-      <c r="BN7" s="100"/>
-      <c r="BO7" s="100"/>
-      <c r="BP7" s="103"/>
-      <c r="BQ7" s="103"/>
-      <c r="BR7" s="103"/>
-      <c r="BS7" s="104"/>
-      <c r="BT7" s="122"/>
-      <c r="BU7" s="108"/>
-      <c r="BV7" s="109"/>
-      <c r="BW7" s="122"/>
-      <c r="BX7" s="107"/>
-      <c r="BY7" s="103"/>
-      <c r="BZ7" s="112"/>
-      <c r="CA7" s="112"/>
-      <c r="CB7" s="112"/>
-      <c r="CC7" s="112"/>
-      <c r="CD7" s="112"/>
-      <c r="CE7" s="112"/>
-      <c r="CF7" s="112"/>
-      <c r="CG7" s="112"/>
-      <c r="CH7" s="112"/>
-      <c r="CI7" s="112"/>
-      <c r="CJ7" s="113"/>
-      <c r="CK7" s="113"/>
-      <c r="CL7" s="113"/>
-      <c r="CM7" s="113"/>
-      <c r="CN7" s="114"/>
-      <c r="CO7" s="122"/>
+      <c r="BJ7" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BK7" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BL7" s="104" t="s">
+        <v>271</v>
+      </c>
+      <c r="BM7" s="104" t="s">
+        <v>330</v>
+      </c>
+      <c r="BN7" s="104"/>
+      <c r="BO7" s="104"/>
+      <c r="BP7" s="104"/>
+      <c r="BQ7" s="104"/>
+      <c r="BR7" s="104"/>
+      <c r="BS7" s="132"/>
+      <c r="BT7" s="107"/>
+      <c r="BU7" s="135"/>
+      <c r="BV7" s="136"/>
+      <c r="BW7" s="107"/>
+      <c r="BX7" s="139"/>
+      <c r="BY7" s="138"/>
+      <c r="BZ7" s="138"/>
+      <c r="CA7" s="138"/>
+      <c r="CB7" s="138"/>
+      <c r="CC7" s="138"/>
+      <c r="CD7" s="138"/>
+      <c r="CE7" s="140"/>
+      <c r="CF7" s="140"/>
+      <c r="CG7" s="140"/>
+      <c r="CH7" s="140"/>
+      <c r="CI7" s="140"/>
+      <c r="CJ7" s="140"/>
+      <c r="CK7" s="140"/>
+      <c r="CL7" s="140"/>
+      <c r="CM7" s="140"/>
+      <c r="CN7" s="141"/>
+      <c r="CO7" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4138,36 +4172,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="133" t="s">
+      <c r="F2" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="133"/>
+      <c r="G2" s="120"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="134" t="s">
+      <c r="I2" s="121" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="134"/>
+      <c r="J2" s="121"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="135" t="s">
+      <c r="L2" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="135"/>
+      <c r="M2" s="122"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="136" t="s">
+      <c r="O2" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="136"/>
+      <c r="P2" s="123"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="125" t="s">
+      <c r="R2" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="125"/>
+      <c r="S2" s="112"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4201,24 +4235,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="133"/>
-      <c r="G3" s="133"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="136"/>
-      <c r="P3" s="136"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="123"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="125"/>
-      <c r="S3" s="125"/>
+      <c r="R3" s="112"/>
+      <c r="S3" s="112"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4252,24 +4286,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="129"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="129"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="135"/>
-      <c r="M4" s="135"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="136"/>
-      <c r="P4" s="136"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4307,20 +4341,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="135"/>
-      <c r="M5" s="135"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="122"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="136"/>
-      <c r="P5" s="136"/>
+      <c r="O5" s="123"/>
+      <c r="P5" s="123"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="125"/>
-      <c r="S5" s="125"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="112"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4354,26 +4388,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="117" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="133"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="136"/>
-      <c r="P6" s="136"/>
+      <c r="O6" s="123"/>
+      <c r="P6" s="123"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="125"/>
-      <c r="S6" s="125"/>
+      <c r="R6" s="112"/>
+      <c r="S6" s="112"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4407,24 +4441,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="131"/>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="133"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="135"/>
-      <c r="M7" s="135"/>
+      <c r="L7" s="122"/>
+      <c r="M7" s="122"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="136"/>
-      <c r="P7" s="136"/>
+      <c r="O7" s="123"/>
+      <c r="P7" s="123"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="125"/>
-      <c r="S7" s="125"/>
+      <c r="R7" s="112"/>
+      <c r="S7" s="112"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4458,24 +4492,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="135"/>
-      <c r="M8" s="135"/>
+      <c r="L8" s="122"/>
+      <c r="M8" s="122"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="136"/>
-      <c r="P8" s="136"/>
+      <c r="O8" s="123"/>
+      <c r="P8" s="123"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="125"/>
-      <c r="S8" s="125"/>
+      <c r="R8" s="112"/>
+      <c r="S8" s="112"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4509,24 +4543,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="120"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="134"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="135"/>
-      <c r="M9" s="135"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="136"/>
-      <c r="P9" s="136"/>
+      <c r="O9" s="123"/>
+      <c r="P9" s="123"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="125"/>
-      <c r="S9" s="125"/>
+      <c r="R9" s="112"/>
+      <c r="S9" s="112"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4560,24 +4594,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="133"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="134"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="135"/>
-      <c r="M10" s="135"/>
+      <c r="L10" s="122"/>
+      <c r="M10" s="122"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="136"/>
-      <c r="P10" s="136"/>
+      <c r="O10" s="123"/>
+      <c r="P10" s="123"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="125"/>
-      <c r="S10" s="125"/>
+      <c r="R10" s="112"/>
+      <c r="S10" s="112"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4666,23 +4700,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="126" t="s">
+      <c r="F12" s="113" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="126"/>
+      <c r="G12" s="113"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="127" t="s">
+      <c r="I12" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="127"/>
+      <c r="J12" s="114"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="128" t="s">
+      <c r="L12" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="128"/>
+      <c r="M12" s="115"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="132"/>
-      <c r="P12" s="132"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4723,17 +4757,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="126"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="127"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="128"/>
-      <c r="M13" s="128"/>
+      <c r="L13" s="115"/>
+      <c r="M13" s="115"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="132"/>
-      <c r="P13" s="132"/>
+      <c r="O13" s="119"/>
+      <c r="P13" s="119"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4774,17 +4808,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="127"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="114"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="128"/>
-      <c r="M14" s="128"/>
+      <c r="L14" s="115"/>
+      <c r="M14" s="115"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="132"/>
-      <c r="P14" s="132"/>
+      <c r="O14" s="119"/>
+      <c r="P14" s="119"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4825,17 +4859,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="126"/>
-      <c r="G15" s="126"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="127"/>
-      <c r="J15" s="127"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="114"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="128"/>
-      <c r="M15" s="128"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="115"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="132"/>
-      <c r="P15" s="132"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="119"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -4876,17 +4910,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="128"/>
-      <c r="M16" s="128"/>
+      <c r="L16" s="115"/>
+      <c r="M16" s="115"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="132"/>
-      <c r="P16" s="132"/>
+      <c r="O16" s="119"/>
+      <c r="P16" s="119"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -4927,17 +4961,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="126"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="127"/>
+      <c r="I17" s="114"/>
+      <c r="J17" s="114"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="128"/>
-      <c r="M17" s="128"/>
+      <c r="L17" s="115"/>
+      <c r="M17" s="115"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="132"/>
-      <c r="P17" s="132"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -4978,17 +5012,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="113"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="127"/>
-      <c r="J18" s="127"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="128"/>
-      <c r="M18" s="128"/>
+      <c r="L18" s="115"/>
+      <c r="M18" s="115"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="132"/>
-      <c r="P18" s="132"/>
+      <c r="O18" s="119"/>
+      <c r="P18" s="119"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -5029,17 +5063,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="127"/>
-      <c r="J19" s="127"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="114"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="128"/>
-      <c r="M19" s="128"/>
+      <c r="L19" s="115"/>
+      <c r="M19" s="115"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="132"/>
-      <c r="P19" s="132"/>
+      <c r="O19" s="119"/>
+      <c r="P19" s="119"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5080,17 +5114,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
+      <c r="F20" s="113"/>
+      <c r="G20" s="113"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="127"/>
-      <c r="J20" s="127"/>
+      <c r="I20" s="114"/>
+      <c r="J20" s="114"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="128"/>
-      <c r="M20" s="128"/>
+      <c r="L20" s="115"/>
+      <c r="M20" s="115"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="132"/>
-      <c r="P20" s="132"/>
+      <c r="O20" s="119"/>
+      <c r="P20" s="119"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17663,7 +17697,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="126" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -18003,7 +18037,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="139"/>
+      <c r="A2" s="126"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18329,15 +18363,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="140"/>
-      <c r="DH2" s="140"/>
-      <c r="DI2" s="140"/>
-      <c r="DJ2" s="140"/>
+      <c r="DG2" s="127"/>
+      <c r="DH2" s="127"/>
+      <c r="DI2" s="127"/>
+      <c r="DJ2" s="127"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="139"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18674,7 +18708,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="128" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18816,7 +18850,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="141"/>
+      <c r="B5" s="128"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -18956,7 +18990,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="141"/>
+      <c r="B6" s="128"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19096,7 +19130,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="128"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19234,7 +19268,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="141"/>
+      <c r="B8" s="128"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19374,7 +19408,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="142" t="s">
+      <c r="B9" s="129" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19516,7 +19550,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="142"/>
+      <c r="B10" s="129"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19656,7 +19690,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="130" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19786,7 +19820,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="143"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -19924,7 +19958,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="143"/>
+      <c r="B13" s="130"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20064,7 +20098,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="143"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20200,7 +20234,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="143"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20336,7 +20370,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="143"/>
+      <c r="B16" s="130"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20472,7 +20506,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="143"/>
+      <c r="B17" s="130"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20608,7 +20642,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="143"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20748,7 +20782,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="143"/>
+      <c r="B19" s="130"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -20884,7 +20918,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="143"/>
+      <c r="B20" s="130"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -21020,7 +21054,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="137" t="s">
+      <c r="B21" s="124" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21154,7 +21188,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="137"/>
+      <c r="B22" s="124"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21290,7 +21324,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="137"/>
+      <c r="B23" s="124"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21422,7 +21456,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="137"/>
+      <c r="B24" s="124"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21556,7 +21590,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="137"/>
+      <c r="B25" s="124"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21700,7 +21734,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="138" t="s">
+      <c r="B26" s="125" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -21834,7 +21868,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="138"/>
+      <c r="B27" s="125"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -21974,7 +22008,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="138"/>
+      <c r="B28" s="125"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22106,7 +22140,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="138"/>
+      <c r="B29" s="125"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22234,7 +22268,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="138"/>
+      <c r="B30" s="125"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22360,7 +22394,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="138"/>
+      <c r="B31" s="125"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 08-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C3AD13-3BA4-4069-975A-DB835A7615E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389B1183-E2DF-4CEB-90B9-3398DDFAA0B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="335">
   <si>
     <t>REDES</t>
   </si>
@@ -1105,6 +1105,18 @@
   </si>
   <si>
     <t>Estilização página Achievements, refatoração de listagens, método de adicionar e remover Achievement do Bloco</t>
+  </si>
+  <si>
+    <t>Correção de Login WEB, nome de usuário logaddo no menu, teste unitário de usuário, filtro nas listagens, validação dos campos de Login</t>
+  </si>
+  <si>
+    <t>Modal de exportação de relatórios, exportar relatórios para PDF, migração de database first para code first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuração de ambiente para projeto Mobile, teste de requisições API, </t>
+  </si>
+  <si>
+    <t>Organização dos repositórios e merges com a master e divisão de tarefas</t>
   </si>
 </sst>
 </file>
@@ -1954,17 +1966,38 @@
     <xf numFmtId="0" fontId="12" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1974,6 +2007,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2031,39 +2076,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2462,10 +2474,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BG4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BN4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BO6" sqref="BO6"/>
+      <selection pane="bottomRight" activeCell="BP5" sqref="BP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2501,8 +2513,8 @@
     <col min="60" max="60" width="25.77734375" customWidth="1"/>
     <col min="61" max="61" width="20.77734375" customWidth="1"/>
     <col min="62" max="64" width="15.77734375" customWidth="1"/>
-    <col min="65" max="65" width="20.77734375" customWidth="1"/>
-    <col min="66" max="71" width="5.77734375" customWidth="1"/>
+    <col min="65" max="66" width="20.77734375" customWidth="1"/>
+    <col min="67" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2512,7 +2524,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="116" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2792,117 +2804,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="110"/>
+      <c r="A2" s="117"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="119" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="119"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="108"/>
-      <c r="X2" s="108"/>
-      <c r="Y2" s="108"/>
-      <c r="Z2" s="108"/>
-      <c r="AA2" s="108"/>
-      <c r="AB2" s="108"/>
-      <c r="AC2" s="108"/>
-      <c r="AD2" s="108"/>
-      <c r="AE2" s="108"/>
-      <c r="AF2" s="108"/>
-      <c r="AG2" s="108"/>
-      <c r="AH2" s="108"/>
-      <c r="AI2" s="108"/>
-      <c r="AJ2" s="108"/>
-      <c r="AK2" s="108"/>
-      <c r="AL2" s="108"/>
-      <c r="AM2" s="108" t="s">
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
+      <c r="AA2" s="119"/>
+      <c r="AB2" s="119"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="119"/>
+      <c r="AE2" s="119"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="119"/>
+      <c r="AH2" s="119"/>
+      <c r="AI2" s="119"/>
+      <c r="AJ2" s="119"/>
+      <c r="AK2" s="119"/>
+      <c r="AL2" s="119"/>
+      <c r="AM2" s="119" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="108"/>
-      <c r="AO2" s="108"/>
-      <c r="AP2" s="108"/>
-      <c r="AQ2" s="108"/>
-      <c r="AR2" s="108"/>
-      <c r="AS2" s="108"/>
-      <c r="AT2" s="108"/>
-      <c r="AU2" s="108"/>
-      <c r="AV2" s="108"/>
-      <c r="AW2" s="108"/>
-      <c r="AX2" s="108"/>
-      <c r="AY2" s="108"/>
-      <c r="AZ2" s="108"/>
-      <c r="BA2" s="108"/>
-      <c r="BB2" s="108"/>
-      <c r="BC2" s="108"/>
-      <c r="BD2" s="108"/>
-      <c r="BE2" s="108"/>
-      <c r="BF2" s="108"/>
-      <c r="BG2" s="108"/>
-      <c r="BH2" s="108"/>
-      <c r="BI2" s="108"/>
-      <c r="BJ2" s="108" t="s">
+      <c r="AN2" s="119"/>
+      <c r="AO2" s="119"/>
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="119"/>
+      <c r="AR2" s="119"/>
+      <c r="AS2" s="119"/>
+      <c r="AT2" s="119"/>
+      <c r="AU2" s="119"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="119"/>
+      <c r="AX2" s="119"/>
+      <c r="AY2" s="119"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="119"/>
+      <c r="BB2" s="119"/>
+      <c r="BC2" s="119"/>
+      <c r="BD2" s="119"/>
+      <c r="BE2" s="119"/>
+      <c r="BF2" s="119"/>
+      <c r="BG2" s="119"/>
+      <c r="BH2" s="119"/>
+      <c r="BI2" s="119"/>
+      <c r="BJ2" s="119" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="108"/>
-      <c r="BL2" s="108"/>
-      <c r="BM2" s="108"/>
-      <c r="BN2" s="108"/>
-      <c r="BO2" s="108"/>
-      <c r="BP2" s="108"/>
-      <c r="BQ2" s="108"/>
-      <c r="BR2" s="108"/>
-      <c r="BS2" s="108"/>
-      <c r="BT2" s="108"/>
-      <c r="BU2" s="108"/>
-      <c r="BV2" s="108"/>
-      <c r="BW2" s="108"/>
-      <c r="BX2" s="108"/>
-      <c r="BY2" s="108"/>
-      <c r="BZ2" s="108"/>
-      <c r="CA2" s="108"/>
-      <c r="CB2" s="108"/>
-      <c r="CC2" s="108"/>
-      <c r="CD2" s="108"/>
-      <c r="CE2" s="108" t="s">
+      <c r="BK2" s="119"/>
+      <c r="BL2" s="119"/>
+      <c r="BM2" s="119"/>
+      <c r="BN2" s="119"/>
+      <c r="BO2" s="119"/>
+      <c r="BP2" s="119"/>
+      <c r="BQ2" s="119"/>
+      <c r="BR2" s="119"/>
+      <c r="BS2" s="119"/>
+      <c r="BT2" s="119"/>
+      <c r="BU2" s="119"/>
+      <c r="BV2" s="119"/>
+      <c r="BW2" s="119"/>
+      <c r="BX2" s="119"/>
+      <c r="BY2" s="119"/>
+      <c r="BZ2" s="119"/>
+      <c r="CA2" s="119"/>
+      <c r="CB2" s="119"/>
+      <c r="CC2" s="119"/>
+      <c r="CD2" s="119"/>
+      <c r="CE2" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="108"/>
-      <c r="CG2" s="108"/>
-      <c r="CH2" s="108"/>
-      <c r="CI2" s="108"/>
-      <c r="CJ2" s="108"/>
-      <c r="CK2" s="108"/>
-      <c r="CL2" s="108"/>
-      <c r="CM2" s="108"/>
-      <c r="CN2" s="108"/>
-      <c r="CO2" s="108"/>
-      <c r="CP2" s="108"/>
-      <c r="CQ2" s="108"/>
-      <c r="CR2" s="108"/>
+      <c r="CF2" s="119"/>
+      <c r="CG2" s="119"/>
+      <c r="CH2" s="119"/>
+      <c r="CI2" s="119"/>
+      <c r="CJ2" s="119"/>
+      <c r="CK2" s="119"/>
+      <c r="CL2" s="119"/>
+      <c r="CM2" s="119"/>
+      <c r="CN2" s="119"/>
+      <c r="CO2" s="119"/>
+      <c r="CP2" s="119"/>
+      <c r="CQ2" s="119"/>
+      <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3190,10 +3202,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="106"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3329,10 +3341,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="107" t="s">
+      <c r="AV4" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="107" t="s">
+      <c r="AW4" s="120" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3383,46 +3395,48 @@
       <c r="BM4" s="104" t="s">
         <v>327</v>
       </c>
-      <c r="BN4" s="104"/>
+      <c r="BN4" s="104" t="s">
+        <v>331</v>
+      </c>
       <c r="BO4" s="104"/>
       <c r="BP4" s="104"/>
       <c r="BQ4" s="104"/>
       <c r="BR4" s="104"/>
-      <c r="BS4" s="131"/>
-      <c r="BT4" s="107" t="s">
+      <c r="BS4" s="105"/>
+      <c r="BT4" s="120" t="s">
         <v>112</v>
       </c>
-      <c r="BU4" s="133"/>
-      <c r="BV4" s="134"/>
-      <c r="BW4" s="107" t="s">
+      <c r="BU4" s="107"/>
+      <c r="BV4" s="108"/>
+      <c r="BW4" s="120" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="137"/>
-      <c r="BY4" s="138"/>
-      <c r="BZ4" s="138"/>
-      <c r="CA4" s="138"/>
-      <c r="CB4" s="138"/>
-      <c r="CC4" s="138"/>
-      <c r="CD4" s="138"/>
-      <c r="CE4" s="140"/>
-      <c r="CF4" s="140"/>
-      <c r="CG4" s="140"/>
-      <c r="CH4" s="140"/>
-      <c r="CI4" s="140"/>
-      <c r="CJ4" s="140"/>
-      <c r="CK4" s="140"/>
-      <c r="CL4" s="140"/>
-      <c r="CM4" s="140"/>
-      <c r="CN4" s="141"/>
-      <c r="CO4" s="107" t="s">
+      <c r="BX4" s="111"/>
+      <c r="BY4" s="112"/>
+      <c r="BZ4" s="112"/>
+      <c r="CA4" s="112"/>
+      <c r="CB4" s="112"/>
+      <c r="CC4" s="112"/>
+      <c r="CD4" s="112"/>
+      <c r="CE4" s="114"/>
+      <c r="CF4" s="114"/>
+      <c r="CG4" s="114"/>
+      <c r="CH4" s="114"/>
+      <c r="CI4" s="114"/>
+      <c r="CJ4" s="114"/>
+      <c r="CK4" s="114"/>
+      <c r="CL4" s="114"/>
+      <c r="CM4" s="114"/>
+      <c r="CN4" s="115"/>
+      <c r="CO4" s="120" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="106"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3556,8 +3570,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="107"/>
-      <c r="AW5" s="107"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3606,40 +3620,42 @@
       <c r="BM5" s="104" t="s">
         <v>328</v>
       </c>
-      <c r="BN5" s="104"/>
+      <c r="BN5" s="104" t="s">
+        <v>332</v>
+      </c>
       <c r="BO5" s="104"/>
       <c r="BP5" s="104"/>
       <c r="BQ5" s="104"/>
       <c r="BR5" s="104"/>
-      <c r="BS5" s="131"/>
-      <c r="BT5" s="107"/>
-      <c r="BU5" s="135"/>
-      <c r="BV5" s="136"/>
-      <c r="BW5" s="107"/>
-      <c r="BX5" s="139"/>
-      <c r="BY5" s="138"/>
-      <c r="BZ5" s="138"/>
-      <c r="CA5" s="138"/>
-      <c r="CB5" s="138"/>
-      <c r="CC5" s="138"/>
-      <c r="CD5" s="138"/>
-      <c r="CE5" s="140"/>
-      <c r="CF5" s="140"/>
-      <c r="CG5" s="140"/>
-      <c r="CH5" s="140"/>
-      <c r="CI5" s="140"/>
-      <c r="CJ5" s="140"/>
-      <c r="CK5" s="140"/>
-      <c r="CL5" s="140"/>
-      <c r="CM5" s="140"/>
-      <c r="CN5" s="141"/>
-      <c r="CO5" s="107"/>
+      <c r="BS5" s="105"/>
+      <c r="BT5" s="120"/>
+      <c r="BU5" s="109"/>
+      <c r="BV5" s="110"/>
+      <c r="BW5" s="120"/>
+      <c r="BX5" s="113"/>
+      <c r="BY5" s="112"/>
+      <c r="BZ5" s="112"/>
+      <c r="CA5" s="112"/>
+      <c r="CB5" s="112"/>
+      <c r="CC5" s="112"/>
+      <c r="CD5" s="112"/>
+      <c r="CE5" s="114"/>
+      <c r="CF5" s="114"/>
+      <c r="CG5" s="114"/>
+      <c r="CH5" s="114"/>
+      <c r="CI5" s="114"/>
+      <c r="CJ5" s="114"/>
+      <c r="CK5" s="114"/>
+      <c r="CL5" s="114"/>
+      <c r="CM5" s="114"/>
+      <c r="CN5" s="115"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="105" t="s">
+      <c r="A6" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="106"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3775,8 +3791,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="107"/>
-      <c r="AW6" s="107"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3825,40 +3841,42 @@
       <c r="BM6" s="104" t="s">
         <v>329</v>
       </c>
-      <c r="BN6" s="104"/>
+      <c r="BN6" s="104" t="s">
+        <v>333</v>
+      </c>
       <c r="BO6" s="104"/>
       <c r="BP6" s="104"/>
       <c r="BQ6" s="104"/>
       <c r="BR6" s="104"/>
-      <c r="BS6" s="131"/>
-      <c r="BT6" s="107"/>
-      <c r="BU6" s="135"/>
-      <c r="BV6" s="136"/>
-      <c r="BW6" s="107"/>
-      <c r="BX6" s="139"/>
-      <c r="BY6" s="138"/>
-      <c r="BZ6" s="138"/>
-      <c r="CA6" s="138"/>
-      <c r="CB6" s="138"/>
-      <c r="CC6" s="138"/>
-      <c r="CD6" s="138"/>
-      <c r="CE6" s="140"/>
-      <c r="CF6" s="140"/>
-      <c r="CG6" s="140"/>
-      <c r="CH6" s="140"/>
-      <c r="CI6" s="140"/>
-      <c r="CJ6" s="140"/>
-      <c r="CK6" s="140"/>
-      <c r="CL6" s="140"/>
-      <c r="CM6" s="140"/>
-      <c r="CN6" s="141"/>
-      <c r="CO6" s="107"/>
+      <c r="BS6" s="105"/>
+      <c r="BT6" s="120"/>
+      <c r="BU6" s="109"/>
+      <c r="BV6" s="110"/>
+      <c r="BW6" s="120"/>
+      <c r="BX6" s="113"/>
+      <c r="BY6" s="112"/>
+      <c r="BZ6" s="112"/>
+      <c r="CA6" s="112"/>
+      <c r="CB6" s="112"/>
+      <c r="CC6" s="112"/>
+      <c r="CD6" s="112"/>
+      <c r="CE6" s="114"/>
+      <c r="CF6" s="114"/>
+      <c r="CG6" s="114"/>
+      <c r="CH6" s="114"/>
+      <c r="CI6" s="114"/>
+      <c r="CJ6" s="114"/>
+      <c r="CK6" s="114"/>
+      <c r="CL6" s="114"/>
+      <c r="CM6" s="114"/>
+      <c r="CN6" s="115"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="105" t="s">
+      <c r="A7" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="106"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -3994,8 +4012,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="107"/>
-      <c r="AW7" s="107"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4044,52 +4062,54 @@
       <c r="BM7" s="104" t="s">
         <v>330</v>
       </c>
-      <c r="BN7" s="104"/>
+      <c r="BN7" s="104" t="s">
+        <v>334</v>
+      </c>
       <c r="BO7" s="104"/>
       <c r="BP7" s="104"/>
       <c r="BQ7" s="104"/>
       <c r="BR7" s="104"/>
-      <c r="BS7" s="132"/>
-      <c r="BT7" s="107"/>
-      <c r="BU7" s="135"/>
-      <c r="BV7" s="136"/>
-      <c r="BW7" s="107"/>
-      <c r="BX7" s="139"/>
-      <c r="BY7" s="138"/>
-      <c r="BZ7" s="138"/>
-      <c r="CA7" s="138"/>
-      <c r="CB7" s="138"/>
-      <c r="CC7" s="138"/>
-      <c r="CD7" s="138"/>
-      <c r="CE7" s="140"/>
-      <c r="CF7" s="140"/>
-      <c r="CG7" s="140"/>
-      <c r="CH7" s="140"/>
-      <c r="CI7" s="140"/>
-      <c r="CJ7" s="140"/>
-      <c r="CK7" s="140"/>
-      <c r="CL7" s="140"/>
-      <c r="CM7" s="140"/>
-      <c r="CN7" s="141"/>
-      <c r="CO7" s="107"/>
+      <c r="BS7" s="106"/>
+      <c r="BT7" s="120"/>
+      <c r="BU7" s="109"/>
+      <c r="BV7" s="110"/>
+      <c r="BW7" s="120"/>
+      <c r="BX7" s="113"/>
+      <c r="BY7" s="112"/>
+      <c r="BZ7" s="112"/>
+      <c r="CA7" s="112"/>
+      <c r="CB7" s="112"/>
+      <c r="CC7" s="112"/>
+      <c r="CD7" s="112"/>
+      <c r="CE7" s="114"/>
+      <c r="CF7" s="114"/>
+      <c r="CG7" s="114"/>
+      <c r="CH7" s="114"/>
+      <c r="CI7" s="114"/>
+      <c r="CJ7" s="114"/>
+      <c r="CK7" s="114"/>
+      <c r="CL7" s="114"/>
+      <c r="CM7" s="114"/>
+      <c r="CN7" s="115"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4172,36 +4192,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="127" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="120" t="s">
+      <c r="F2" s="131" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="120"/>
+      <c r="G2" s="131"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="132" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="121"/>
+      <c r="J2" s="132"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="122" t="s">
+      <c r="L2" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="122"/>
+      <c r="M2" s="133"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="123" t="s">
+      <c r="O2" s="134" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="123"/>
+      <c r="P2" s="134"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="112" t="s">
+      <c r="R2" s="123" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="112"/>
+      <c r="S2" s="123"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4235,24 +4255,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="123"/>
-      <c r="P3" s="123"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="112"/>
-      <c r="S3" s="112"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4286,24 +4306,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="122"/>
-      <c r="M4" s="122"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="123"/>
-      <c r="P4" s="123"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4341,20 +4361,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="121"/>
-      <c r="J5" s="121"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="122"/>
-      <c r="M5" s="122"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="123"/>
-      <c r="P5" s="123"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4388,26 +4408,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="122"/>
-      <c r="M6" s="122"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="123"/>
-      <c r="P6" s="123"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="112"/>
-      <c r="S6" s="112"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4441,24 +4461,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="122"/>
-      <c r="M7" s="122"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="133"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="123"/>
-      <c r="P7" s="123"/>
+      <c r="O7" s="134"/>
+      <c r="P7" s="134"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="112"/>
-      <c r="S7" s="112"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="123"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4492,24 +4512,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="122"/>
-      <c r="M8" s="122"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="133"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="134"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112"/>
+      <c r="R8" s="123"/>
+      <c r="S8" s="123"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4543,24 +4563,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="121"/>
-      <c r="J9" s="121"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="122"/>
-      <c r="M9" s="122"/>
+      <c r="L9" s="133"/>
+      <c r="M9" s="133"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="123"/>
-      <c r="P9" s="123"/>
+      <c r="O9" s="134"/>
+      <c r="P9" s="134"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="112"/>
-      <c r="S9" s="112"/>
+      <c r="R9" s="123"/>
+      <c r="S9" s="123"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4594,24 +4614,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="118"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="131"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="121"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="122"/>
-      <c r="M10" s="122"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="133"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="123"/>
-      <c r="P10" s="123"/>
+      <c r="O10" s="134"/>
+      <c r="P10" s="134"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="112"/>
-      <c r="S10" s="112"/>
+      <c r="R10" s="123"/>
+      <c r="S10" s="123"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4700,23 +4720,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="113" t="s">
+      <c r="F12" s="124" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="113"/>
+      <c r="G12" s="124"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="114" t="s">
+      <c r="I12" s="125" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="114"/>
+      <c r="J12" s="125"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="115" t="s">
+      <c r="L12" s="126" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="115"/>
+      <c r="M12" s="126"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="119"/>
-      <c r="P12" s="119"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4757,17 +4777,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="114"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="119"/>
-      <c r="P13" s="119"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4808,17 +4828,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="114"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="115"/>
+      <c r="L14" s="126"/>
+      <c r="M14" s="126"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="119"/>
-      <c r="P14" s="119"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4859,17 +4879,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="114"/>
-      <c r="J15" s="114"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="125"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="115"/>
-      <c r="M15" s="115"/>
+      <c r="L15" s="126"/>
+      <c r="M15" s="126"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="119"/>
-      <c r="P15" s="119"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -4910,17 +4930,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="113"/>
-      <c r="G16" s="113"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="114"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="125"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="115"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="126"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="119"/>
-      <c r="P16" s="119"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="130"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -4961,17 +4981,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="113"/>
-      <c r="G17" s="113"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="114"/>
-      <c r="J17" s="114"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="125"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
+      <c r="L17" s="126"/>
+      <c r="M17" s="126"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="119"/>
-      <c r="P17" s="119"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -5012,17 +5032,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="113"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="114"/>
+      <c r="I18" s="125"/>
+      <c r="J18" s="125"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="115"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="126"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="119"/>
-      <c r="P18" s="119"/>
+      <c r="O18" s="130"/>
+      <c r="P18" s="130"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -5063,17 +5083,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="113"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="114"/>
-      <c r="J19" s="114"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="115"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="119"/>
-      <c r="P19" s="119"/>
+      <c r="O19" s="130"/>
+      <c r="P19" s="130"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5114,17 +5134,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="113"/>
-      <c r="G20" s="113"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="114"/>
-      <c r="J20" s="114"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="125"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="126"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="119"/>
-      <c r="P20" s="119"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="130"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17697,7 +17717,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -18037,7 +18057,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="126"/>
+      <c r="A2" s="137"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18363,15 +18383,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="127"/>
-      <c r="DH2" s="127"/>
-      <c r="DI2" s="127"/>
-      <c r="DJ2" s="127"/>
+      <c r="DG2" s="138"/>
+      <c r="DH2" s="138"/>
+      <c r="DI2" s="138"/>
+      <c r="DJ2" s="138"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="126"/>
+      <c r="A3" s="137"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18708,7 +18728,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="139" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18850,7 +18870,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="128"/>
+      <c r="B5" s="139"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -18990,7 +19010,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="128"/>
+      <c r="B6" s="139"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19130,7 +19150,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="128"/>
+      <c r="B7" s="139"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19268,7 +19288,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="128"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19408,7 +19428,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="140" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19550,7 +19570,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="129"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19690,7 +19710,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="141" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19820,7 +19840,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="130"/>
+      <c r="B12" s="141"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -19958,7 +19978,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="130"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20098,7 +20118,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="130"/>
+      <c r="B14" s="141"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20234,7 +20254,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="130"/>
+      <c r="B15" s="141"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20370,7 +20390,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="130"/>
+      <c r="B16" s="141"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20506,7 +20526,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="130"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20642,7 +20662,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="130"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20782,7 +20802,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="130"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -20918,7 +20938,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="130"/>
+      <c r="B20" s="141"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -21054,7 +21074,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="124" t="s">
+      <c r="B21" s="135" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21188,7 +21208,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="124"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21324,7 +21344,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="124"/>
+      <c r="B23" s="135"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21456,7 +21476,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="124"/>
+      <c r="B24" s="135"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21590,7 +21610,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="124"/>
+      <c r="B25" s="135"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21734,7 +21754,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="125" t="s">
+      <c r="B26" s="136" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -21868,7 +21888,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="125"/>
+      <c r="B27" s="136"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -22008,7 +22028,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="125"/>
+      <c r="B28" s="136"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22140,7 +22160,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="125"/>
+      <c r="B29" s="136"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22268,7 +22288,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="125"/>
+      <c r="B30" s="136"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22394,7 +22414,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="125"/>
+      <c r="B31" s="136"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 11-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389B1183-E2DF-4CEB-90B9-3398DDFAA0B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B672131-F3C3-4B69-8A40-3F7485962200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="339">
   <si>
     <t>REDES</t>
   </si>
@@ -1117,6 +1117,18 @@
   </si>
   <si>
     <t>Organização dos repositórios e merges com a master e divisão de tarefas</t>
+  </si>
+  <si>
+    <t>Validação dos campos de cadastro de usuário, filtro nas listagens, teste unitário de usuário, loadings nas listagens WEB, refatoração do código front-end</t>
+  </si>
+  <si>
+    <t>Exportação de relatórios para PDF e migração de database fisrt para code first</t>
+  </si>
+  <si>
+    <t>Configuração de ambiente para projeto Mobile, página de listagem geral e exportação para .csv, testes de requisições API e implementação de métodos update API</t>
+  </si>
+  <si>
+    <t>Estilização da listagem de Levels, menu dropdown editar e excluir genérico, alteração nas funcionmalidades da tela de listagem de Levels</t>
   </si>
 </sst>
 </file>
@@ -1999,6 +2011,18 @@
     <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2007,18 +2031,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2514,7 +2526,8 @@
     <col min="61" max="61" width="20.77734375" customWidth="1"/>
     <col min="62" max="64" width="15.77734375" customWidth="1"/>
     <col min="65" max="66" width="20.77734375" customWidth="1"/>
-    <col min="67" max="71" width="5.77734375" customWidth="1"/>
+    <col min="67" max="67" width="25.77734375" customWidth="1"/>
+    <col min="68" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2524,7 +2537,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="120" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2804,7 +2817,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="117"/>
+      <c r="A2" s="121"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2914,7 +2927,7 @@
       <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="118"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3202,10 +3215,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3341,10 +3354,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="118" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="118" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3398,17 +3411,19 @@
       <c r="BN4" s="104" t="s">
         <v>331</v>
       </c>
-      <c r="BO4" s="104"/>
+      <c r="BO4" s="104" t="s">
+        <v>335</v>
+      </c>
       <c r="BP4" s="104"/>
       <c r="BQ4" s="104"/>
       <c r="BR4" s="104"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="120" t="s">
+      <c r="BT4" s="118" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="107"/>
       <c r="BV4" s="108"/>
-      <c r="BW4" s="120" t="s">
+      <c r="BW4" s="118" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="111"/>
@@ -3428,15 +3443,15 @@
       <c r="CL4" s="114"/>
       <c r="CM4" s="114"/>
       <c r="CN4" s="115"/>
-      <c r="CO4" s="120" t="s">
+      <c r="CO4" s="118" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3570,8 +3585,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3623,15 +3638,17 @@
       <c r="BN5" s="104" t="s">
         <v>332</v>
       </c>
-      <c r="BO5" s="104"/>
+      <c r="BO5" s="104" t="s">
+        <v>336</v>
+      </c>
       <c r="BP5" s="104"/>
       <c r="BQ5" s="104"/>
       <c r="BR5" s="104"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="120"/>
+      <c r="BT5" s="118"/>
       <c r="BU5" s="109"/>
       <c r="BV5" s="110"/>
-      <c r="BW5" s="120"/>
+      <c r="BW5" s="118"/>
       <c r="BX5" s="113"/>
       <c r="BY5" s="112"/>
       <c r="BZ5" s="112"/>
@@ -3649,13 +3666,13 @@
       <c r="CL5" s="114"/>
       <c r="CM5" s="114"/>
       <c r="CN5" s="115"/>
-      <c r="CO5" s="120"/>
+      <c r="CO5" s="118"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3791,8 +3808,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
+      <c r="AV6" s="118"/>
+      <c r="AW6" s="118"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3844,15 +3861,17 @@
       <c r="BN6" s="104" t="s">
         <v>333</v>
       </c>
-      <c r="BO6" s="104"/>
+      <c r="BO6" s="104" t="s">
+        <v>337</v>
+      </c>
       <c r="BP6" s="104"/>
       <c r="BQ6" s="104"/>
       <c r="BR6" s="104"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="120"/>
+      <c r="BT6" s="118"/>
       <c r="BU6" s="109"/>
       <c r="BV6" s="110"/>
-      <c r="BW6" s="120"/>
+      <c r="BW6" s="118"/>
       <c r="BX6" s="113"/>
       <c r="BY6" s="112"/>
       <c r="BZ6" s="112"/>
@@ -3870,13 +3889,13 @@
       <c r="CL6" s="114"/>
       <c r="CM6" s="114"/>
       <c r="CN6" s="115"/>
-      <c r="CO6" s="120"/>
+      <c r="CO6" s="118"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4012,8 +4031,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
+      <c r="AV7" s="118"/>
+      <c r="AW7" s="118"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4065,15 +4084,17 @@
       <c r="BN7" s="104" t="s">
         <v>334</v>
       </c>
-      <c r="BO7" s="104"/>
+      <c r="BO7" s="104" t="s">
+        <v>338</v>
+      </c>
       <c r="BP7" s="104"/>
       <c r="BQ7" s="104"/>
       <c r="BR7" s="104"/>
       <c r="BS7" s="106"/>
-      <c r="BT7" s="120"/>
+      <c r="BT7" s="118"/>
       <c r="BU7" s="109"/>
       <c r="BV7" s="110"/>
-      <c r="BW7" s="120"/>
+      <c r="BW7" s="118"/>
       <c r="BX7" s="113"/>
       <c r="BY7" s="112"/>
       <c r="BZ7" s="112"/>
@@ -4091,25 +4112,25 @@
       <c r="CL7" s="114"/>
       <c r="CM7" s="114"/>
       <c r="CN7" s="115"/>
-      <c r="CO7" s="120"/>
+      <c r="CO7" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 12 e 13-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B672131-F3C3-4B69-8A40-3F7485962200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFF98E9-65F7-40D5-913E-03F9873FCF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="347">
   <si>
     <t>REDES</t>
   </si>
@@ -1129,6 +1129,30 @@
   </si>
   <si>
     <t>Estilização da listagem de Levels, menu dropdown editar e excluir genérico, alteração nas funcionmalidades da tela de listagem de Levels</t>
+  </si>
+  <si>
+    <t>Validação dos campos de cadastro de usuário e filtro na listagem de usuários WEB</t>
+  </si>
+  <si>
+    <t>Integração da obtenção das informações e geração de gráficos, endpoints editar usuário API</t>
+  </si>
+  <si>
+    <t>Dashboard, editar e deletar na lista, permissão de endpoints, exportar e importar</t>
+  </si>
+  <si>
+    <t>Estudo busca de imagem pelo Blobs, estilização da listagem de Levels e cadastro de Achievements</t>
+  </si>
+  <si>
+    <t>Método de listagem de FAQs API, alteração na tela de editar usuário Mobile, editar usuário WEB, teste unitário de cadastro de usuário API</t>
+  </si>
+  <si>
+    <t>Integração gerar gráficos com o front-end, alteração para que a url de login do zabbix seja dinâmica no front e deploy da API</t>
+  </si>
+  <si>
+    <t>Dashboard separação na renderização de componentes, tela de listgem geral, cadastro de usuário, permissão de endpoints e atualização da lista quando fecha o modal no passo a passo</t>
+  </si>
+  <si>
+    <t>Dropdown de Achievements, tela de achievements, estudo e context Blobs e tela de listagem de Leves</t>
   </si>
 </sst>
 </file>
@@ -2011,18 +2035,6 @@
     <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2031,6 +2043,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2489,7 +2513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="BN4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BP5" sqref="BP5"/>
+      <selection pane="bottomRight" activeCell="BO7" sqref="BO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2527,7 +2551,9 @@
     <col min="62" max="64" width="15.77734375" customWidth="1"/>
     <col min="65" max="66" width="20.77734375" customWidth="1"/>
     <col min="67" max="67" width="25.77734375" customWidth="1"/>
-    <col min="68" max="71" width="5.77734375" customWidth="1"/>
+    <col min="68" max="68" width="20.77734375" customWidth="1"/>
+    <col min="69" max="69" width="30.77734375" customWidth="1"/>
+    <col min="70" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2537,7 +2563,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="116" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2817,7 +2843,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121"/>
+      <c r="A2" s="117"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2927,7 +2953,7 @@
       <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="122"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3215,10 +3241,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3354,10 +3380,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="118" t="s">
+      <c r="AV4" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="118" t="s">
+      <c r="AW4" s="120" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3414,16 +3440,20 @@
       <c r="BO4" s="104" t="s">
         <v>335</v>
       </c>
-      <c r="BP4" s="104"/>
-      <c r="BQ4" s="104"/>
+      <c r="BP4" s="104" t="s">
+        <v>339</v>
+      </c>
+      <c r="BQ4" s="104" t="s">
+        <v>343</v>
+      </c>
       <c r="BR4" s="104"/>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="118" t="s">
+      <c r="BT4" s="120" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="107"/>
       <c r="BV4" s="108"/>
-      <c r="BW4" s="118" t="s">
+      <c r="BW4" s="120" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="111"/>
@@ -3443,15 +3473,15 @@
       <c r="CL4" s="114"/>
       <c r="CM4" s="114"/>
       <c r="CN4" s="115"/>
-      <c r="CO4" s="118" t="s">
+      <c r="CO4" s="120" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="117"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3585,8 +3615,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3641,14 +3671,18 @@
       <c r="BO5" s="104" t="s">
         <v>336</v>
       </c>
-      <c r="BP5" s="104"/>
-      <c r="BQ5" s="104"/>
+      <c r="BP5" s="104" t="s">
+        <v>340</v>
+      </c>
+      <c r="BQ5" s="104" t="s">
+        <v>344</v>
+      </c>
       <c r="BR5" s="104"/>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="118"/>
+      <c r="BT5" s="120"/>
       <c r="BU5" s="109"/>
       <c r="BV5" s="110"/>
-      <c r="BW5" s="118"/>
+      <c r="BW5" s="120"/>
       <c r="BX5" s="113"/>
       <c r="BY5" s="112"/>
       <c r="BZ5" s="112"/>
@@ -3666,13 +3700,13 @@
       <c r="CL5" s="114"/>
       <c r="CM5" s="114"/>
       <c r="CN5" s="115"/>
-      <c r="CO5" s="118"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="117"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3808,8 +3842,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="118"/>
-      <c r="AW6" s="118"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3864,14 +3898,18 @@
       <c r="BO6" s="104" t="s">
         <v>337</v>
       </c>
-      <c r="BP6" s="104"/>
-      <c r="BQ6" s="104"/>
+      <c r="BP6" s="104" t="s">
+        <v>341</v>
+      </c>
+      <c r="BQ6" s="104" t="s">
+        <v>345</v>
+      </c>
       <c r="BR6" s="104"/>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="118"/>
+      <c r="BT6" s="120"/>
       <c r="BU6" s="109"/>
       <c r="BV6" s="110"/>
-      <c r="BW6" s="118"/>
+      <c r="BW6" s="120"/>
       <c r="BX6" s="113"/>
       <c r="BY6" s="112"/>
       <c r="BZ6" s="112"/>
@@ -3889,13 +3927,13 @@
       <c r="CL6" s="114"/>
       <c r="CM6" s="114"/>
       <c r="CN6" s="115"/>
-      <c r="CO6" s="118"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4031,8 +4069,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="118"/>
-      <c r="AW7" s="118"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4087,14 +4125,18 @@
       <c r="BO7" s="104" t="s">
         <v>338</v>
       </c>
-      <c r="BP7" s="104"/>
-      <c r="BQ7" s="104"/>
+      <c r="BP7" s="104" t="s">
+        <v>342</v>
+      </c>
+      <c r="BQ7" s="104" t="s">
+        <v>346</v>
+      </c>
       <c r="BR7" s="104"/>
       <c r="BS7" s="106"/>
-      <c r="BT7" s="118"/>
+      <c r="BT7" s="120"/>
       <c r="BU7" s="109"/>
       <c r="BV7" s="110"/>
-      <c r="BW7" s="118"/>
+      <c r="BW7" s="120"/>
       <c r="BX7" s="113"/>
       <c r="BY7" s="112"/>
       <c r="BZ7" s="112"/>
@@ -4112,25 +4154,25 @@
       <c r="CL7" s="114"/>
       <c r="CM7" s="114"/>
       <c r="CN7" s="115"/>
-      <c r="CO7" s="118"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 14-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFF98E9-65F7-40D5-913E-03F9873FCF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2E42AF-C0AB-4E93-80AE-47E038F2457E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="350">
   <si>
     <t>REDES</t>
   </si>
@@ -1153,6 +1153,15 @@
   </si>
   <si>
     <t>Dropdown de Achievements, tela de achievements, estudo e context Blobs e tela de listagem de Leves</t>
+  </si>
+  <si>
+    <t>Ajustes no gerenciamento de solicitação de cadastro de usuário API, teste unitário de cadastro de usuário API, editar usuário WEB</t>
+  </si>
+  <si>
+    <t>Editar usuário WEB, integração da obtenção das informações da API com os gráficos, revisão geral do projeto para buscar falhas</t>
+  </si>
+  <si>
+    <t>Alinhamento e ajustes para apresentação para o cliente</t>
   </si>
 </sst>
 </file>
@@ -2035,6 +2044,18 @@
     <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2043,18 +2064,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2513,7 +2522,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="BN4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BO7" sqref="BO7"/>
+      <selection pane="bottomRight" activeCell="BQ7" sqref="BQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2562,8 @@
     <col min="67" max="67" width="25.77734375" customWidth="1"/>
     <col min="68" max="68" width="20.77734375" customWidth="1"/>
     <col min="69" max="69" width="30.77734375" customWidth="1"/>
-    <col min="70" max="71" width="5.77734375" customWidth="1"/>
+    <col min="70" max="70" width="20.77734375" customWidth="1"/>
+    <col min="71" max="71" width="5.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2563,7 +2573,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="120" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2843,7 +2853,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="117"/>
+      <c r="A2" s="121"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2953,7 +2963,7 @@
       <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="118"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3241,10 +3251,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3380,10 +3390,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="118" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="118" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3446,14 +3456,16 @@
       <c r="BQ4" s="104" t="s">
         <v>343</v>
       </c>
-      <c r="BR4" s="104"/>
+      <c r="BR4" s="104" t="s">
+        <v>347</v>
+      </c>
       <c r="BS4" s="105"/>
-      <c r="BT4" s="120" t="s">
+      <c r="BT4" s="118" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="107"/>
       <c r="BV4" s="108"/>
-      <c r="BW4" s="120" t="s">
+      <c r="BW4" s="118" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="111"/>
@@ -3473,15 +3485,15 @@
       <c r="CL4" s="114"/>
       <c r="CM4" s="114"/>
       <c r="CN4" s="115"/>
-      <c r="CO4" s="120" t="s">
+      <c r="CO4" s="118" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3615,8 +3627,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3677,12 +3689,14 @@
       <c r="BQ5" s="104" t="s">
         <v>344</v>
       </c>
-      <c r="BR5" s="104"/>
+      <c r="BR5" s="104" t="s">
+        <v>348</v>
+      </c>
       <c r="BS5" s="105"/>
-      <c r="BT5" s="120"/>
+      <c r="BT5" s="118"/>
       <c r="BU5" s="109"/>
       <c r="BV5" s="110"/>
-      <c r="BW5" s="120"/>
+      <c r="BW5" s="118"/>
       <c r="BX5" s="113"/>
       <c r="BY5" s="112"/>
       <c r="BZ5" s="112"/>
@@ -3700,13 +3714,13 @@
       <c r="CL5" s="114"/>
       <c r="CM5" s="114"/>
       <c r="CN5" s="115"/>
-      <c r="CO5" s="120"/>
+      <c r="CO5" s="118"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3842,8 +3856,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
+      <c r="AV6" s="118"/>
+      <c r="AW6" s="118"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3904,12 +3918,14 @@
       <c r="BQ6" s="104" t="s">
         <v>345</v>
       </c>
-      <c r="BR6" s="104"/>
+      <c r="BR6" s="104" t="s">
+        <v>349</v>
+      </c>
       <c r="BS6" s="105"/>
-      <c r="BT6" s="120"/>
+      <c r="BT6" s="118"/>
       <c r="BU6" s="109"/>
       <c r="BV6" s="110"/>
-      <c r="BW6" s="120"/>
+      <c r="BW6" s="118"/>
       <c r="BX6" s="113"/>
       <c r="BY6" s="112"/>
       <c r="BZ6" s="112"/>
@@ -3927,13 +3943,13 @@
       <c r="CL6" s="114"/>
       <c r="CM6" s="114"/>
       <c r="CN6" s="115"/>
-      <c r="CO6" s="120"/>
+      <c r="CO6" s="118"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4069,8 +4085,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
+      <c r="AV7" s="118"/>
+      <c r="AW7" s="118"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4131,12 +4147,14 @@
       <c r="BQ7" s="104" t="s">
         <v>346</v>
       </c>
-      <c r="BR7" s="104"/>
+      <c r="BR7" s="104" t="s">
+        <v>349</v>
+      </c>
       <c r="BS7" s="106"/>
-      <c r="BT7" s="120"/>
+      <c r="BT7" s="118"/>
       <c r="BU7" s="109"/>
       <c r="BV7" s="110"/>
-      <c r="BW7" s="120"/>
+      <c r="BW7" s="118"/>
       <c r="BX7" s="113"/>
       <c r="BY7" s="112"/>
       <c r="BZ7" s="112"/>
@@ -4154,25 +4172,25 @@
       <c r="CL7" s="114"/>
       <c r="CM7" s="114"/>
       <c r="CN7" s="115"/>
-      <c r="CO7" s="120"/>
+      <c r="CO7" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 18-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2E42AF-C0AB-4E93-80AE-47E038F2457E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4212E3-9C1E-4711-9553-6C98B7592416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="354">
   <si>
     <t>REDES</t>
   </si>
@@ -1162,6 +1162,18 @@
   </si>
   <si>
     <t>Alinhamento e ajustes para apresentação para o cliente</t>
+  </si>
+  <si>
+    <t>Finalização de gerenciamento de solicitação de cadastro de usuário WEB, detalhes de UX mobile, filtros e abertura de chamado mobile, estilização listas WEB</t>
+  </si>
+  <si>
+    <t>Ajustes e correções para reunião com o cliente</t>
+  </si>
+  <si>
+    <t>Reunião com cliente skype, estilização dashboard, listagem de jornada e agenda mobile, fluxo de navegação mobile, finalização de exportação de clientes, autenticação API</t>
+  </si>
+  <si>
+    <t>Registro de imagem em Achievement API, estudo de biblioteca para unificação de estilos</t>
   </si>
 </sst>
 </file>
@@ -2044,18 +2056,6 @@
     <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2064,6 +2064,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2519,10 +2531,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BN4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BP4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BQ7" sqref="BQ7"/>
+      <selection pane="bottomRight" activeCell="BS8" sqref="BS8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2563,7 +2575,7 @@
     <col min="68" max="68" width="20.77734375" customWidth="1"/>
     <col min="69" max="69" width="30.77734375" customWidth="1"/>
     <col min="70" max="70" width="20.77734375" customWidth="1"/>
-    <col min="71" max="71" width="5.77734375" customWidth="1"/>
+    <col min="71" max="71" width="30.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
@@ -2573,7 +2585,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="116" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2853,7 +2865,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121"/>
+      <c r="A2" s="117"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -2963,7 +2975,7 @@
       <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="122"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3251,10 +3263,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3390,10 +3402,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="118" t="s">
+      <c r="AV4" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="118" t="s">
+      <c r="AW4" s="120" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3459,13 +3471,15 @@
       <c r="BR4" s="104" t="s">
         <v>347</v>
       </c>
-      <c r="BS4" s="105"/>
-      <c r="BT4" s="118" t="s">
+      <c r="BS4" s="105" t="s">
+        <v>350</v>
+      </c>
+      <c r="BT4" s="120" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="107"/>
       <c r="BV4" s="108"/>
-      <c r="BW4" s="118" t="s">
+      <c r="BW4" s="120" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="111"/>
@@ -3485,15 +3499,15 @@
       <c r="CL4" s="114"/>
       <c r="CM4" s="114"/>
       <c r="CN4" s="115"/>
-      <c r="CO4" s="118" t="s">
+      <c r="CO4" s="120" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="117"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3627,8 +3641,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3692,11 +3706,13 @@
       <c r="BR5" s="104" t="s">
         <v>348</v>
       </c>
-      <c r="BS5" s="105"/>
-      <c r="BT5" s="118"/>
+      <c r="BS5" s="105" t="s">
+        <v>351</v>
+      </c>
+      <c r="BT5" s="120"/>
       <c r="BU5" s="109"/>
       <c r="BV5" s="110"/>
-      <c r="BW5" s="118"/>
+      <c r="BW5" s="120"/>
       <c r="BX5" s="113"/>
       <c r="BY5" s="112"/>
       <c r="BZ5" s="112"/>
@@ -3714,13 +3730,13 @@
       <c r="CL5" s="114"/>
       <c r="CM5" s="114"/>
       <c r="CN5" s="115"/>
-      <c r="CO5" s="118"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="117"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3856,8 +3872,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="118"/>
-      <c r="AW6" s="118"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3921,11 +3937,13 @@
       <c r="BR6" s="104" t="s">
         <v>349</v>
       </c>
-      <c r="BS6" s="105"/>
-      <c r="BT6" s="118"/>
+      <c r="BS6" s="105" t="s">
+        <v>352</v>
+      </c>
+      <c r="BT6" s="120"/>
       <c r="BU6" s="109"/>
       <c r="BV6" s="110"/>
-      <c r="BW6" s="118"/>
+      <c r="BW6" s="120"/>
       <c r="BX6" s="113"/>
       <c r="BY6" s="112"/>
       <c r="BZ6" s="112"/>
@@ -3943,13 +3961,13 @@
       <c r="CL6" s="114"/>
       <c r="CM6" s="114"/>
       <c r="CN6" s="115"/>
-      <c r="CO6" s="118"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4085,8 +4103,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="118"/>
-      <c r="AW7" s="118"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4150,11 +4168,13 @@
       <c r="BR7" s="104" t="s">
         <v>349</v>
       </c>
-      <c r="BS7" s="106"/>
-      <c r="BT7" s="118"/>
+      <c r="BS7" s="106" t="s">
+        <v>353</v>
+      </c>
+      <c r="BT7" s="120"/>
       <c r="BU7" s="109"/>
       <c r="BV7" s="110"/>
-      <c r="BW7" s="118"/>
+      <c r="BW7" s="120"/>
       <c r="BX7" s="113"/>
       <c r="BY7" s="112"/>
       <c r="BZ7" s="112"/>
@@ -4172,25 +4192,25 @@
       <c r="CL7" s="114"/>
       <c r="CM7" s="114"/>
       <c r="CN7" s="115"/>
-      <c r="CO7" s="118"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 19-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4212E3-9C1E-4711-9553-6C98B7592416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF74F761-FE26-42A5-AE23-4B3C6C67BBBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="357">
   <si>
     <t>REDES</t>
   </si>
@@ -1174,6 +1174,15 @@
   </si>
   <si>
     <t>Registro de imagem em Achievement API, estudo de biblioteca para unificação de estilos</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente alocado na Blocktime</t>
+  </si>
+  <si>
+    <t>Planning, configuração ambiente Mobile, deploy para o servidor da escola</t>
+  </si>
+  <si>
+    <t>Planning (jornada e achievement)</t>
   </si>
 </sst>
 </file>
@@ -2029,18 +2038,6 @@
     <xf numFmtId="0" fontId="12" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2056,6 +2053,18 @@
     <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2064,18 +2073,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2132,6 +2129,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2531,10 +2540,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BP4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BR4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BS8" sqref="BS8"/>
+      <selection pane="bottomRight" activeCell="BV4" sqref="BV4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2577,7 +2586,7 @@
     <col min="70" max="70" width="20.77734375" customWidth="1"/>
     <col min="71" max="71" width="30.77734375" customWidth="1"/>
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
-    <col min="73" max="74" width="5.77734375" customWidth="1"/>
+    <col min="73" max="74" width="20.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
     <col min="76" max="92" width="5.77734375" customWidth="1"/>
     <col min="93" max="93" width="3.77734375" style="81" customWidth="1"/>
@@ -2869,110 +2878,110 @@
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="115" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="119" t="s">
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="115"/>
+      <c r="P2" s="115"/>
+      <c r="Q2" s="115"/>
+      <c r="R2" s="115" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="119"/>
-      <c r="T2" s="119"/>
-      <c r="U2" s="119"/>
-      <c r="V2" s="119"/>
-      <c r="W2" s="119"/>
-      <c r="X2" s="119"/>
-      <c r="Y2" s="119"/>
-      <c r="Z2" s="119"/>
-      <c r="AA2" s="119"/>
-      <c r="AB2" s="119"/>
-      <c r="AC2" s="119"/>
-      <c r="AD2" s="119"/>
-      <c r="AE2" s="119"/>
-      <c r="AF2" s="119"/>
-      <c r="AG2" s="119"/>
-      <c r="AH2" s="119"/>
-      <c r="AI2" s="119"/>
-      <c r="AJ2" s="119"/>
-      <c r="AK2" s="119"/>
-      <c r="AL2" s="119"/>
-      <c r="AM2" s="119" t="s">
+      <c r="S2" s="115"/>
+      <c r="T2" s="115"/>
+      <c r="U2" s="115"/>
+      <c r="V2" s="115"/>
+      <c r="W2" s="115"/>
+      <c r="X2" s="115"/>
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
+      <c r="AA2" s="115"/>
+      <c r="AB2" s="115"/>
+      <c r="AC2" s="115"/>
+      <c r="AD2" s="115"/>
+      <c r="AE2" s="115"/>
+      <c r="AF2" s="115"/>
+      <c r="AG2" s="115"/>
+      <c r="AH2" s="115"/>
+      <c r="AI2" s="115"/>
+      <c r="AJ2" s="115"/>
+      <c r="AK2" s="115"/>
+      <c r="AL2" s="115"/>
+      <c r="AM2" s="115" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="119"/>
-      <c r="AO2" s="119"/>
-      <c r="AP2" s="119"/>
-      <c r="AQ2" s="119"/>
-      <c r="AR2" s="119"/>
-      <c r="AS2" s="119"/>
-      <c r="AT2" s="119"/>
-      <c r="AU2" s="119"/>
-      <c r="AV2" s="119"/>
-      <c r="AW2" s="119"/>
-      <c r="AX2" s="119"/>
-      <c r="AY2" s="119"/>
-      <c r="AZ2" s="119"/>
-      <c r="BA2" s="119"/>
-      <c r="BB2" s="119"/>
-      <c r="BC2" s="119"/>
-      <c r="BD2" s="119"/>
-      <c r="BE2" s="119"/>
-      <c r="BF2" s="119"/>
-      <c r="BG2" s="119"/>
-      <c r="BH2" s="119"/>
-      <c r="BI2" s="119"/>
-      <c r="BJ2" s="119" t="s">
+      <c r="AN2" s="115"/>
+      <c r="AO2" s="115"/>
+      <c r="AP2" s="115"/>
+      <c r="AQ2" s="115"/>
+      <c r="AR2" s="115"/>
+      <c r="AS2" s="115"/>
+      <c r="AT2" s="115"/>
+      <c r="AU2" s="115"/>
+      <c r="AV2" s="115"/>
+      <c r="AW2" s="115"/>
+      <c r="AX2" s="115"/>
+      <c r="AY2" s="115"/>
+      <c r="AZ2" s="115"/>
+      <c r="BA2" s="115"/>
+      <c r="BB2" s="115"/>
+      <c r="BC2" s="115"/>
+      <c r="BD2" s="115"/>
+      <c r="BE2" s="115"/>
+      <c r="BF2" s="115"/>
+      <c r="BG2" s="115"/>
+      <c r="BH2" s="115"/>
+      <c r="BI2" s="115"/>
+      <c r="BJ2" s="115" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="119"/>
-      <c r="BL2" s="119"/>
-      <c r="BM2" s="119"/>
-      <c r="BN2" s="119"/>
-      <c r="BO2" s="119"/>
-      <c r="BP2" s="119"/>
-      <c r="BQ2" s="119"/>
-      <c r="BR2" s="119"/>
-      <c r="BS2" s="119"/>
-      <c r="BT2" s="119"/>
-      <c r="BU2" s="119"/>
-      <c r="BV2" s="119"/>
-      <c r="BW2" s="119"/>
-      <c r="BX2" s="119"/>
-      <c r="BY2" s="119"/>
-      <c r="BZ2" s="119"/>
-      <c r="CA2" s="119"/>
-      <c r="CB2" s="119"/>
-      <c r="CC2" s="119"/>
-      <c r="CD2" s="119"/>
-      <c r="CE2" s="119" t="s">
+      <c r="BK2" s="115"/>
+      <c r="BL2" s="115"/>
+      <c r="BM2" s="115"/>
+      <c r="BN2" s="115"/>
+      <c r="BO2" s="115"/>
+      <c r="BP2" s="115"/>
+      <c r="BQ2" s="115"/>
+      <c r="BR2" s="115"/>
+      <c r="BS2" s="115"/>
+      <c r="BT2" s="115"/>
+      <c r="BU2" s="115"/>
+      <c r="BV2" s="115"/>
+      <c r="BW2" s="115"/>
+      <c r="BX2" s="115"/>
+      <c r="BY2" s="115"/>
+      <c r="BZ2" s="115"/>
+      <c r="CA2" s="115"/>
+      <c r="CB2" s="115"/>
+      <c r="CC2" s="115"/>
+      <c r="CD2" s="115"/>
+      <c r="CE2" s="115" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="119"/>
-      <c r="CG2" s="119"/>
-      <c r="CH2" s="119"/>
-      <c r="CI2" s="119"/>
-      <c r="CJ2" s="119"/>
-      <c r="CK2" s="119"/>
-      <c r="CL2" s="119"/>
-      <c r="CM2" s="119"/>
-      <c r="CN2" s="119"/>
-      <c r="CO2" s="119"/>
-      <c r="CP2" s="119"/>
-      <c r="CQ2" s="119"/>
-      <c r="CR2" s="119"/>
+      <c r="CF2" s="115"/>
+      <c r="CG2" s="115"/>
+      <c r="CH2" s="115"/>
+      <c r="CI2" s="115"/>
+      <c r="CJ2" s="115"/>
+      <c r="CK2" s="115"/>
+      <c r="CL2" s="115"/>
+      <c r="CM2" s="115"/>
+      <c r="CN2" s="115"/>
+      <c r="CO2" s="115"/>
+      <c r="CP2" s="115"/>
+      <c r="CQ2" s="115"/>
+      <c r="CR2" s="115"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A3" s="118"/>
@@ -3263,10 +3272,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="112" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="113"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3402,10 +3411,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="114" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="114" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3474,40 +3483,42 @@
       <c r="BS4" s="105" t="s">
         <v>350</v>
       </c>
-      <c r="BT4" s="120" t="s">
+      <c r="BT4" s="114" t="s">
         <v>112</v>
       </c>
-      <c r="BU4" s="107"/>
-      <c r="BV4" s="108"/>
-      <c r="BW4" s="120" t="s">
+      <c r="BU4" s="138" t="s">
+        <v>310</v>
+      </c>
+      <c r="BV4" s="139"/>
+      <c r="BW4" s="114" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="111"/>
-      <c r="BY4" s="112"/>
-      <c r="BZ4" s="112"/>
-      <c r="CA4" s="112"/>
-      <c r="CB4" s="112"/>
-      <c r="CC4" s="112"/>
-      <c r="CD4" s="112"/>
-      <c r="CE4" s="114"/>
-      <c r="CF4" s="114"/>
-      <c r="CG4" s="114"/>
-      <c r="CH4" s="114"/>
-      <c r="CI4" s="114"/>
-      <c r="CJ4" s="114"/>
-      <c r="CK4" s="114"/>
-      <c r="CL4" s="114"/>
-      <c r="CM4" s="114"/>
-      <c r="CN4" s="115"/>
-      <c r="CO4" s="120" t="s">
+      <c r="BX4" s="107"/>
+      <c r="BY4" s="108"/>
+      <c r="BZ4" s="108"/>
+      <c r="CA4" s="108"/>
+      <c r="CB4" s="108"/>
+      <c r="CC4" s="108"/>
+      <c r="CD4" s="108"/>
+      <c r="CE4" s="110"/>
+      <c r="CF4" s="110"/>
+      <c r="CG4" s="110"/>
+      <c r="CH4" s="110"/>
+      <c r="CI4" s="110"/>
+      <c r="CJ4" s="110"/>
+      <c r="CK4" s="110"/>
+      <c r="CL4" s="110"/>
+      <c r="CM4" s="110"/>
+      <c r="CN4" s="111"/>
+      <c r="CO4" s="114" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="112" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="113"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3641,8 +3652,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
+      <c r="AV5" s="114"/>
+      <c r="AW5" s="114"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3709,34 +3720,36 @@
       <c r="BS5" s="105" t="s">
         <v>351</v>
       </c>
-      <c r="BT5" s="120"/>
-      <c r="BU5" s="109"/>
-      <c r="BV5" s="110"/>
-      <c r="BW5" s="120"/>
-      <c r="BX5" s="113"/>
-      <c r="BY5" s="112"/>
-      <c r="BZ5" s="112"/>
-      <c r="CA5" s="112"/>
-      <c r="CB5" s="112"/>
-      <c r="CC5" s="112"/>
-      <c r="CD5" s="112"/>
-      <c r="CE5" s="114"/>
-      <c r="CF5" s="114"/>
-      <c r="CG5" s="114"/>
-      <c r="CH5" s="114"/>
-      <c r="CI5" s="114"/>
-      <c r="CJ5" s="114"/>
-      <c r="CK5" s="114"/>
-      <c r="CL5" s="114"/>
-      <c r="CM5" s="114"/>
-      <c r="CN5" s="115"/>
-      <c r="CO5" s="120"/>
+      <c r="BT5" s="114"/>
+      <c r="BU5" s="140" t="s">
+        <v>354</v>
+      </c>
+      <c r="BV5" s="141"/>
+      <c r="BW5" s="114"/>
+      <c r="BX5" s="109"/>
+      <c r="BY5" s="108"/>
+      <c r="BZ5" s="108"/>
+      <c r="CA5" s="108"/>
+      <c r="CB5" s="108"/>
+      <c r="CC5" s="108"/>
+      <c r="CD5" s="108"/>
+      <c r="CE5" s="110"/>
+      <c r="CF5" s="110"/>
+      <c r="CG5" s="110"/>
+      <c r="CH5" s="110"/>
+      <c r="CI5" s="110"/>
+      <c r="CJ5" s="110"/>
+      <c r="CK5" s="110"/>
+      <c r="CL5" s="110"/>
+      <c r="CM5" s="110"/>
+      <c r="CN5" s="111"/>
+      <c r="CO5" s="114"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="112" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3872,8 +3885,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
+      <c r="AV6" s="114"/>
+      <c r="AW6" s="114"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3940,34 +3953,36 @@
       <c r="BS6" s="105" t="s">
         <v>352</v>
       </c>
-      <c r="BT6" s="120"/>
-      <c r="BU6" s="109"/>
-      <c r="BV6" s="110"/>
-      <c r="BW6" s="120"/>
-      <c r="BX6" s="113"/>
-      <c r="BY6" s="112"/>
-      <c r="BZ6" s="112"/>
-      <c r="CA6" s="112"/>
-      <c r="CB6" s="112"/>
-      <c r="CC6" s="112"/>
-      <c r="CD6" s="112"/>
-      <c r="CE6" s="114"/>
-      <c r="CF6" s="114"/>
-      <c r="CG6" s="114"/>
-      <c r="CH6" s="114"/>
-      <c r="CI6" s="114"/>
-      <c r="CJ6" s="114"/>
-      <c r="CK6" s="114"/>
-      <c r="CL6" s="114"/>
-      <c r="CM6" s="114"/>
-      <c r="CN6" s="115"/>
-      <c r="CO6" s="120"/>
+      <c r="BT6" s="114"/>
+      <c r="BU6" s="140" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV6" s="141"/>
+      <c r="BW6" s="114"/>
+      <c r="BX6" s="109"/>
+      <c r="BY6" s="108"/>
+      <c r="BZ6" s="108"/>
+      <c r="CA6" s="108"/>
+      <c r="CB6" s="108"/>
+      <c r="CC6" s="108"/>
+      <c r="CD6" s="108"/>
+      <c r="CE6" s="110"/>
+      <c r="CF6" s="110"/>
+      <c r="CG6" s="110"/>
+      <c r="CH6" s="110"/>
+      <c r="CI6" s="110"/>
+      <c r="CJ6" s="110"/>
+      <c r="CK6" s="110"/>
+      <c r="CL6" s="110"/>
+      <c r="CM6" s="110"/>
+      <c r="CN6" s="111"/>
+      <c r="CO6" s="114"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="112" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4103,8 +4118,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
+      <c r="AV7" s="114"/>
+      <c r="AW7" s="114"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4171,46 +4186,48 @@
       <c r="BS7" s="106" t="s">
         <v>353</v>
       </c>
-      <c r="BT7" s="120"/>
-      <c r="BU7" s="109"/>
-      <c r="BV7" s="110"/>
-      <c r="BW7" s="120"/>
-      <c r="BX7" s="113"/>
-      <c r="BY7" s="112"/>
-      <c r="BZ7" s="112"/>
-      <c r="CA7" s="112"/>
-      <c r="CB7" s="112"/>
-      <c r="CC7" s="112"/>
-      <c r="CD7" s="112"/>
-      <c r="CE7" s="114"/>
-      <c r="CF7" s="114"/>
-      <c r="CG7" s="114"/>
-      <c r="CH7" s="114"/>
-      <c r="CI7" s="114"/>
-      <c r="CJ7" s="114"/>
-      <c r="CK7" s="114"/>
-      <c r="CL7" s="114"/>
-      <c r="CM7" s="114"/>
-      <c r="CN7" s="115"/>
-      <c r="CO7" s="120"/>
+      <c r="BT7" s="114"/>
+      <c r="BU7" s="140" t="s">
+        <v>356</v>
+      </c>
+      <c r="BV7" s="141"/>
+      <c r="BW7" s="114"/>
+      <c r="BX7" s="109"/>
+      <c r="BY7" s="108"/>
+      <c r="BZ7" s="108"/>
+      <c r="CA7" s="108"/>
+      <c r="CB7" s="108"/>
+      <c r="CC7" s="108"/>
+      <c r="CD7" s="108"/>
+      <c r="CE7" s="110"/>
+      <c r="CF7" s="110"/>
+      <c r="CG7" s="110"/>
+      <c r="CH7" s="110"/>
+      <c r="CI7" s="110"/>
+      <c r="CJ7" s="110"/>
+      <c r="CK7" s="110"/>
+      <c r="CL7" s="110"/>
+      <c r="CM7" s="110"/>
+      <c r="CN7" s="111"/>
+      <c r="CO7" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4293,36 +4310,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="131" t="s">
+      <c r="F2" s="127" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="131"/>
+      <c r="G2" s="127"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="132" t="s">
+      <c r="I2" s="128" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="132"/>
+      <c r="J2" s="128"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="133" t="s">
+      <c r="L2" s="129" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="133"/>
+      <c r="M2" s="129"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="134" t="s">
+      <c r="O2" s="130" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="134"/>
+      <c r="P2" s="130"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="123" t="s">
+      <c r="R2" s="119" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="123"/>
+      <c r="S2" s="119"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4356,24 +4373,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="130"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="123"/>
-      <c r="S3" s="123"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="119"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4407,24 +4424,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="134"/>
-      <c r="P4" s="134"/>
+      <c r="O4" s="130"/>
+      <c r="P4" s="130"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4462,20 +4479,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="127"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="132"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="133"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="129"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="134"/>
-      <c r="P5" s="134"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="130"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="123"/>
-      <c r="S5" s="123"/>
+      <c r="R5" s="119"/>
+      <c r="S5" s="119"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4509,26 +4526,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="124" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="133"/>
-      <c r="M6" s="133"/>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
+      <c r="O6" s="130"/>
+      <c r="P6" s="130"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
+      <c r="R6" s="119"/>
+      <c r="S6" s="119"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4562,24 +4579,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="131"/>
-      <c r="G7" s="131"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="132"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
+      <c r="L7" s="129"/>
+      <c r="M7" s="129"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="134"/>
-      <c r="P7" s="134"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="123"/>
-      <c r="S7" s="123"/>
+      <c r="R7" s="119"/>
+      <c r="S7" s="119"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4613,24 +4630,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="127"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="133"/>
+      <c r="L8" s="129"/>
+      <c r="M8" s="129"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="134"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="123"/>
-      <c r="S8" s="123"/>
+      <c r="R8" s="119"/>
+      <c r="S8" s="119"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4664,24 +4681,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
+      <c r="B9" s="125"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="131"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="127"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="132"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="128"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="133"/>
-      <c r="M9" s="133"/>
+      <c r="L9" s="129"/>
+      <c r="M9" s="129"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="134"/>
-      <c r="P9" s="134"/>
+      <c r="O9" s="130"/>
+      <c r="P9" s="130"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="123"/>
-      <c r="S9" s="123"/>
+      <c r="R9" s="119"/>
+      <c r="S9" s="119"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4715,24 +4732,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="127"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="133"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="129"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="134"/>
-      <c r="P10" s="134"/>
+      <c r="O10" s="130"/>
+      <c r="P10" s="130"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="123"/>
-      <c r="S10" s="123"/>
+      <c r="R10" s="119"/>
+      <c r="S10" s="119"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4821,23 +4838,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="124" t="s">
+      <c r="F12" s="120" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="124"/>
+      <c r="G12" s="120"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="125" t="s">
+      <c r="I12" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="125"/>
+      <c r="J12" s="121"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="126" t="s">
+      <c r="L12" s="122" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="126"/>
+      <c r="M12" s="122"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="130"/>
-      <c r="P12" s="130"/>
+      <c r="O12" s="126"/>
+      <c r="P12" s="126"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4878,17 +4895,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="120"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="125"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="126"/>
-      <c r="M13" s="126"/>
+      <c r="L13" s="122"/>
+      <c r="M13" s="122"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="130"/>
-      <c r="P13" s="130"/>
+      <c r="O13" s="126"/>
+      <c r="P13" s="126"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4929,17 +4946,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="124"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="125"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="126"/>
+      <c r="L14" s="122"/>
+      <c r="M14" s="122"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="130"/>
-      <c r="P14" s="130"/>
+      <c r="O14" s="126"/>
+      <c r="P14" s="126"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4980,17 +4997,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="125"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="126"/>
-      <c r="M15" s="126"/>
+      <c r="L15" s="122"/>
+      <c r="M15" s="122"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="130"/>
-      <c r="P15" s="130"/>
+      <c r="O15" s="126"/>
+      <c r="P15" s="126"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -5031,17 +5048,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="124"/>
-      <c r="G16" s="124"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="125"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="126"/>
-      <c r="M16" s="126"/>
+      <c r="L16" s="122"/>
+      <c r="M16" s="122"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="130"/>
-      <c r="P16" s="130"/>
+      <c r="O16" s="126"/>
+      <c r="P16" s="126"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -5082,17 +5099,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="124"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="120"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="125"/>
-      <c r="J17" s="125"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="126"/>
-      <c r="M17" s="126"/>
+      <c r="L17" s="122"/>
+      <c r="M17" s="122"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="130"/>
-      <c r="P17" s="130"/>
+      <c r="O17" s="126"/>
+      <c r="P17" s="126"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -5133,17 +5150,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="124"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="125"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="126"/>
-      <c r="M18" s="126"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="122"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="130"/>
-      <c r="P18" s="130"/>
+      <c r="O18" s="126"/>
+      <c r="P18" s="126"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -5184,17 +5201,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="124"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="125"/>
-      <c r="J19" s="125"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="121"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="126"/>
+      <c r="L19" s="122"/>
+      <c r="M19" s="122"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="130"/>
-      <c r="P19" s="130"/>
+      <c r="O19" s="126"/>
+      <c r="P19" s="126"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5235,17 +5252,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="124"/>
+      <c r="F20" s="120"/>
+      <c r="G20" s="120"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="125"/>
-      <c r="J20" s="125"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="121"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="126"/>
-      <c r="M20" s="126"/>
+      <c r="L20" s="122"/>
+      <c r="M20" s="122"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="130"/>
+      <c r="O20" s="126"/>
+      <c r="P20" s="126"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17818,7 +17835,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="133" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -18158,7 +18175,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="137"/>
+      <c r="A2" s="133"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18484,15 +18501,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="138"/>
-      <c r="DH2" s="138"/>
-      <c r="DI2" s="138"/>
-      <c r="DJ2" s="138"/>
+      <c r="DG2" s="134"/>
+      <c r="DH2" s="134"/>
+      <c r="DI2" s="134"/>
+      <c r="DJ2" s="134"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="137"/>
+      <c r="A3" s="133"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18829,7 +18846,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="135" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18971,7 +18988,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="139"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -19111,7 +19128,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="139"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19251,7 +19268,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="139"/>
+      <c r="B7" s="135"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19389,7 +19406,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="139"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19529,7 +19546,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="136" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19671,7 +19688,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="140"/>
+      <c r="B10" s="136"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19811,7 +19828,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="137" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19941,7 +19958,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="141"/>
+      <c r="B12" s="137"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -20079,7 +20096,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="141"/>
+      <c r="B13" s="137"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20219,7 +20236,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="141"/>
+      <c r="B14" s="137"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20355,7 +20372,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="141"/>
+      <c r="B15" s="137"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20491,7 +20508,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="137"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20627,7 +20644,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="137"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20763,7 +20780,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="141"/>
+      <c r="B18" s="137"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20903,7 +20920,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="141"/>
+      <c r="B19" s="137"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -21039,7 +21056,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="141"/>
+      <c r="B20" s="137"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -21175,7 +21192,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="131" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21309,7 +21326,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="135"/>
+      <c r="B22" s="131"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21445,7 +21462,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="135"/>
+      <c r="B23" s="131"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21577,7 +21594,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="135"/>
+      <c r="B24" s="131"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21711,7 +21728,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="135"/>
+      <c r="B25" s="131"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21855,7 +21872,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="136" t="s">
+      <c r="B26" s="132" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -21989,7 +22006,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="136"/>
+      <c r="B27" s="132"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -22129,7 +22146,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="136"/>
+      <c r="B28" s="132"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22261,7 +22278,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="136"/>
+      <c r="B29" s="132"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22389,7 +22406,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="136"/>
+      <c r="B30" s="132"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22515,7 +22532,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="136"/>
+      <c r="B31" s="132"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 21-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF74F761-FE26-42A5-AE23-4B3C6C67BBBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD920A8-1638-4577-857F-231649B82142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="361">
   <si>
     <t>REDES</t>
   </si>
@@ -1183,6 +1183,18 @@
   </si>
   <si>
     <t>Planning (jornada e achievement)</t>
+  </si>
+  <si>
+    <t>Sprint Review e Planning</t>
+  </si>
+  <si>
+    <t>Sprint Review organização dos dados para exibição no gráfico</t>
+  </si>
+  <si>
+    <t>Correção de erros ao acessar métodos que contém permissão, autenticação API, estrutura da aplicação Mobile</t>
+  </si>
+  <si>
+    <t>Fluxo de navegação e layouts da jornadas</t>
   </si>
 </sst>
 </file>
@@ -2053,17 +2065,17 @@
     <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2073,6 +2085,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2129,18 +2153,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2543,7 +2555,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="BR4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BV4" sqref="BV4"/>
+      <selection pane="bottomRight" activeCell="BZ7" sqref="BZ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2878,110 +2890,110 @@
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="119" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="119"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="115"/>
-      <c r="AC2" s="115"/>
-      <c r="AD2" s="115"/>
-      <c r="AE2" s="115"/>
-      <c r="AF2" s="115"/>
-      <c r="AG2" s="115"/>
-      <c r="AH2" s="115"/>
-      <c r="AI2" s="115"/>
-      <c r="AJ2" s="115"/>
-      <c r="AK2" s="115"/>
-      <c r="AL2" s="115"/>
-      <c r="AM2" s="115" t="s">
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
+      <c r="AA2" s="119"/>
+      <c r="AB2" s="119"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="119"/>
+      <c r="AE2" s="119"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="119"/>
+      <c r="AH2" s="119"/>
+      <c r="AI2" s="119"/>
+      <c r="AJ2" s="119"/>
+      <c r="AK2" s="119"/>
+      <c r="AL2" s="119"/>
+      <c r="AM2" s="119" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="115"/>
-      <c r="AO2" s="115"/>
-      <c r="AP2" s="115"/>
-      <c r="AQ2" s="115"/>
-      <c r="AR2" s="115"/>
-      <c r="AS2" s="115"/>
-      <c r="AT2" s="115"/>
-      <c r="AU2" s="115"/>
-      <c r="AV2" s="115"/>
-      <c r="AW2" s="115"/>
-      <c r="AX2" s="115"/>
-      <c r="AY2" s="115"/>
-      <c r="AZ2" s="115"/>
-      <c r="BA2" s="115"/>
-      <c r="BB2" s="115"/>
-      <c r="BC2" s="115"/>
-      <c r="BD2" s="115"/>
-      <c r="BE2" s="115"/>
-      <c r="BF2" s="115"/>
-      <c r="BG2" s="115"/>
-      <c r="BH2" s="115"/>
-      <c r="BI2" s="115"/>
-      <c r="BJ2" s="115" t="s">
+      <c r="AN2" s="119"/>
+      <c r="AO2" s="119"/>
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="119"/>
+      <c r="AR2" s="119"/>
+      <c r="AS2" s="119"/>
+      <c r="AT2" s="119"/>
+      <c r="AU2" s="119"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="119"/>
+      <c r="AX2" s="119"/>
+      <c r="AY2" s="119"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="119"/>
+      <c r="BB2" s="119"/>
+      <c r="BC2" s="119"/>
+      <c r="BD2" s="119"/>
+      <c r="BE2" s="119"/>
+      <c r="BF2" s="119"/>
+      <c r="BG2" s="119"/>
+      <c r="BH2" s="119"/>
+      <c r="BI2" s="119"/>
+      <c r="BJ2" s="119" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="115"/>
-      <c r="BL2" s="115"/>
-      <c r="BM2" s="115"/>
-      <c r="BN2" s="115"/>
-      <c r="BO2" s="115"/>
-      <c r="BP2" s="115"/>
-      <c r="BQ2" s="115"/>
-      <c r="BR2" s="115"/>
-      <c r="BS2" s="115"/>
-      <c r="BT2" s="115"/>
-      <c r="BU2" s="115"/>
-      <c r="BV2" s="115"/>
-      <c r="BW2" s="115"/>
-      <c r="BX2" s="115"/>
-      <c r="BY2" s="115"/>
-      <c r="BZ2" s="115"/>
-      <c r="CA2" s="115"/>
-      <c r="CB2" s="115"/>
-      <c r="CC2" s="115"/>
-      <c r="CD2" s="115"/>
-      <c r="CE2" s="115" t="s">
+      <c r="BK2" s="119"/>
+      <c r="BL2" s="119"/>
+      <c r="BM2" s="119"/>
+      <c r="BN2" s="119"/>
+      <c r="BO2" s="119"/>
+      <c r="BP2" s="119"/>
+      <c r="BQ2" s="119"/>
+      <c r="BR2" s="119"/>
+      <c r="BS2" s="119"/>
+      <c r="BT2" s="119"/>
+      <c r="BU2" s="119"/>
+      <c r="BV2" s="119"/>
+      <c r="BW2" s="119"/>
+      <c r="BX2" s="119"/>
+      <c r="BY2" s="119"/>
+      <c r="BZ2" s="119"/>
+      <c r="CA2" s="119"/>
+      <c r="CB2" s="119"/>
+      <c r="CC2" s="119"/>
+      <c r="CD2" s="119"/>
+      <c r="CE2" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="115"/>
-      <c r="CG2" s="115"/>
-      <c r="CH2" s="115"/>
-      <c r="CI2" s="115"/>
-      <c r="CJ2" s="115"/>
-      <c r="CK2" s="115"/>
-      <c r="CL2" s="115"/>
-      <c r="CM2" s="115"/>
-      <c r="CN2" s="115"/>
-      <c r="CO2" s="115"/>
-      <c r="CP2" s="115"/>
-      <c r="CQ2" s="115"/>
-      <c r="CR2" s="115"/>
+      <c r="CF2" s="119"/>
+      <c r="CG2" s="119"/>
+      <c r="CH2" s="119"/>
+      <c r="CI2" s="119"/>
+      <c r="CJ2" s="119"/>
+      <c r="CK2" s="119"/>
+      <c r="CL2" s="119"/>
+      <c r="CM2" s="119"/>
+      <c r="CN2" s="119"/>
+      <c r="CO2" s="119"/>
+      <c r="CP2" s="119"/>
+      <c r="CQ2" s="119"/>
+      <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A3" s="118"/>
@@ -3272,10 +3284,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="113"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3411,10 +3423,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="114" t="s">
+      <c r="AV4" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="114" t="s">
+      <c r="AW4" s="120" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3483,14 +3495,16 @@
       <c r="BS4" s="105" t="s">
         <v>350</v>
       </c>
-      <c r="BT4" s="114" t="s">
+      <c r="BT4" s="120" t="s">
         <v>112</v>
       </c>
-      <c r="BU4" s="138" t="s">
+      <c r="BU4" s="112" t="s">
         <v>310</v>
       </c>
-      <c r="BV4" s="139"/>
-      <c r="BW4" s="114" t="s">
+      <c r="BV4" s="113" t="s">
+        <v>357</v>
+      </c>
+      <c r="BW4" s="120" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="107"/>
@@ -3510,15 +3524,15 @@
       <c r="CL4" s="110"/>
       <c r="CM4" s="110"/>
       <c r="CN4" s="111"/>
-      <c r="CO4" s="114" t="s">
+      <c r="CO4" s="120" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="113"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3652,8 +3666,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="114"/>
-      <c r="AW5" s="114"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3720,12 +3734,14 @@
       <c r="BS5" s="105" t="s">
         <v>351</v>
       </c>
-      <c r="BT5" s="114"/>
-      <c r="BU5" s="140" t="s">
+      <c r="BT5" s="120"/>
+      <c r="BU5" s="114" t="s">
         <v>354</v>
       </c>
-      <c r="BV5" s="141"/>
-      <c r="BW5" s="114"/>
+      <c r="BV5" s="115" t="s">
+        <v>358</v>
+      </c>
+      <c r="BW5" s="120"/>
       <c r="BX5" s="109"/>
       <c r="BY5" s="108"/>
       <c r="BZ5" s="108"/>
@@ -3743,13 +3759,13 @@
       <c r="CL5" s="110"/>
       <c r="CM5" s="110"/>
       <c r="CN5" s="111"/>
-      <c r="CO5" s="114"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="113"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3885,8 +3901,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="114"/>
-      <c r="AW6" s="114"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3953,12 +3969,14 @@
       <c r="BS6" s="105" t="s">
         <v>352</v>
       </c>
-      <c r="BT6" s="114"/>
-      <c r="BU6" s="140" t="s">
+      <c r="BT6" s="120"/>
+      <c r="BU6" s="114" t="s">
         <v>355</v>
       </c>
-      <c r="BV6" s="141"/>
-      <c r="BW6" s="114"/>
+      <c r="BV6" s="115" t="s">
+        <v>359</v>
+      </c>
+      <c r="BW6" s="120"/>
       <c r="BX6" s="109"/>
       <c r="BY6" s="108"/>
       <c r="BZ6" s="108"/>
@@ -3976,13 +3994,13 @@
       <c r="CL6" s="110"/>
       <c r="CM6" s="110"/>
       <c r="CN6" s="111"/>
-      <c r="CO6" s="114"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="113"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4118,8 +4136,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="114"/>
-      <c r="AW7" s="114"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4186,12 +4204,14 @@
       <c r="BS7" s="106" t="s">
         <v>353</v>
       </c>
-      <c r="BT7" s="114"/>
-      <c r="BU7" s="140" t="s">
+      <c r="BT7" s="120"/>
+      <c r="BU7" s="114" t="s">
         <v>356</v>
       </c>
-      <c r="BV7" s="141"/>
-      <c r="BW7" s="114"/>
+      <c r="BV7" s="115" t="s">
+        <v>360</v>
+      </c>
+      <c r="BW7" s="120"/>
       <c r="BX7" s="109"/>
       <c r="BY7" s="108"/>
       <c r="BZ7" s="108"/>
@@ -4209,25 +4229,25 @@
       <c r="CL7" s="110"/>
       <c r="CM7" s="110"/>
       <c r="CN7" s="111"/>
-      <c r="CO7" s="114"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4310,36 +4330,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="127" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="127" t="s">
+      <c r="F2" s="131" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="127"/>
+      <c r="G2" s="131"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="128" t="s">
+      <c r="I2" s="132" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="128"/>
+      <c r="J2" s="132"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="129" t="s">
+      <c r="L2" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="129"/>
+      <c r="M2" s="133"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="130" t="s">
+      <c r="O2" s="134" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="130"/>
+      <c r="P2" s="134"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="119" t="s">
+      <c r="R2" s="123" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="119"/>
+      <c r="S2" s="123"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4373,24 +4393,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="130"/>
-      <c r="P3" s="130"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="119"/>
-      <c r="S3" s="119"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4424,24 +4444,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="130"/>
-      <c r="P4" s="130"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="119"/>
-      <c r="S4" s="119"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4479,20 +4499,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="129"/>
-      <c r="M5" s="129"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="130"/>
-      <c r="P5" s="130"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4526,26 +4546,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="130"/>
-      <c r="P6" s="130"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="119"/>
-      <c r="S6" s="119"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4579,24 +4599,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="128"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="129"/>
-      <c r="M7" s="129"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="133"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="130"/>
-      <c r="P7" s="130"/>
+      <c r="O7" s="134"/>
+      <c r="P7" s="134"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="119"/>
-      <c r="S7" s="119"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="123"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4630,24 +4650,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="128"/>
-      <c r="J8" s="128"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="129"/>
-      <c r="M8" s="129"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="133"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="130"/>
-      <c r="P8" s="130"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="134"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="119"/>
-      <c r="S8" s="119"/>
+      <c r="R8" s="123"/>
+      <c r="S8" s="123"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4681,24 +4701,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="125"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="127"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="128"/>
-      <c r="J9" s="128"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="129"/>
-      <c r="M9" s="129"/>
+      <c r="L9" s="133"/>
+      <c r="M9" s="133"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="130"/>
-      <c r="P9" s="130"/>
+      <c r="O9" s="134"/>
+      <c r="P9" s="134"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="119"/>
-      <c r="S9" s="119"/>
+      <c r="R9" s="123"/>
+      <c r="S9" s="123"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4732,24 +4752,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="127"/>
-      <c r="G10" s="127"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="131"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="129"/>
-      <c r="M10" s="129"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="133"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="130"/>
-      <c r="P10" s="130"/>
+      <c r="O10" s="134"/>
+      <c r="P10" s="134"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="119"/>
-      <c r="S10" s="119"/>
+      <c r="R10" s="123"/>
+      <c r="S10" s="123"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4838,23 +4858,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="120" t="s">
+      <c r="F12" s="124" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="120"/>
+      <c r="G12" s="124"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="121" t="s">
+      <c r="I12" s="125" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="121"/>
+      <c r="J12" s="125"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="122" t="s">
+      <c r="L12" s="126" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="122"/>
+      <c r="M12" s="126"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="126"/>
-      <c r="P12" s="126"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4895,17 +4915,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="121"/>
-      <c r="J13" s="121"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="122"/>
-      <c r="M13" s="122"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="126"/>
-      <c r="P13" s="126"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4946,17 +4966,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="121"/>
-      <c r="J14" s="121"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="122"/>
-      <c r="M14" s="122"/>
+      <c r="L14" s="126"/>
+      <c r="M14" s="126"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="126"/>
-      <c r="P14" s="126"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -4997,17 +5017,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="121"/>
-      <c r="J15" s="121"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="125"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="122"/>
-      <c r="M15" s="122"/>
+      <c r="L15" s="126"/>
+      <c r="M15" s="126"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="126"/>
-      <c r="P15" s="126"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -5048,17 +5068,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="121"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="125"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="122"/>
-      <c r="M16" s="122"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="126"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="126"/>
-      <c r="P16" s="126"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="130"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -5099,17 +5119,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="125"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="122"/>
-      <c r="M17" s="122"/>
+      <c r="L17" s="126"/>
+      <c r="M17" s="126"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="126"/>
-      <c r="P17" s="126"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -5150,17 +5170,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="121"/>
-      <c r="J18" s="121"/>
+      <c r="I18" s="125"/>
+      <c r="J18" s="125"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="122"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="126"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="126"/>
-      <c r="P18" s="126"/>
+      <c r="O18" s="130"/>
+      <c r="P18" s="130"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -5201,17 +5221,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="120"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="121"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="122"/>
-      <c r="M19" s="122"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="126"/>
-      <c r="P19" s="126"/>
+      <c r="O19" s="130"/>
+      <c r="P19" s="130"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5252,17 +5272,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="121"/>
-      <c r="J20" s="121"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="125"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="122"/>
-      <c r="M20" s="122"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="126"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="126"/>
-      <c r="P20" s="126"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="130"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17835,7 +17855,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -18175,7 +18195,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="133"/>
+      <c r="A2" s="137"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18501,15 +18521,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="134"/>
-      <c r="DH2" s="134"/>
-      <c r="DI2" s="134"/>
-      <c r="DJ2" s="134"/>
+      <c r="DG2" s="138"/>
+      <c r="DH2" s="138"/>
+      <c r="DI2" s="138"/>
+      <c r="DJ2" s="138"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="133"/>
+      <c r="A3" s="137"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18846,7 +18866,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="139" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -18988,7 +19008,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="135"/>
+      <c r="B5" s="139"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -19128,7 +19148,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="135"/>
+      <c r="B6" s="139"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19268,7 +19288,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="135"/>
+      <c r="B7" s="139"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19406,7 +19426,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="135"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19546,7 +19566,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="140" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19688,7 +19708,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="136"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19828,7 +19848,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="137" t="s">
+      <c r="B11" s="141" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19958,7 +19978,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="137"/>
+      <c r="B12" s="141"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -20096,7 +20116,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="137"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20236,7 +20256,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="137"/>
+      <c r="B14" s="141"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20372,7 +20392,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="137"/>
+      <c r="B15" s="141"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20508,7 +20528,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="137"/>
+      <c r="B16" s="141"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20644,7 +20664,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="137"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20780,7 +20800,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="137"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20920,7 +20940,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="137"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -21056,7 +21076,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="137"/>
+      <c r="B20" s="141"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -21192,7 +21212,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="131" t="s">
+      <c r="B21" s="135" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21326,7 +21346,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="131"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21462,7 +21482,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="131"/>
+      <c r="B23" s="135"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21594,7 +21614,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="131"/>
+      <c r="B24" s="135"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21728,7 +21748,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="131"/>
+      <c r="B25" s="135"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21872,7 +21892,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="132" t="s">
+      <c r="B26" s="136" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -22006,7 +22026,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="132"/>
+      <c r="B27" s="136"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -22146,7 +22166,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="132"/>
+      <c r="B28" s="136"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22278,7 +22298,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="132"/>
+      <c r="B29" s="136"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22406,7 +22426,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="132"/>
+      <c r="B30" s="136"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22532,7 +22552,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="132"/>
+      <c r="B31" s="136"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona daily realizada em 22-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD920A8-1638-4577-857F-231649B82142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6B4DA4-33BD-4336-9F22-5E1C49346CC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="365">
   <si>
     <t>REDES</t>
   </si>
@@ -1195,6 +1195,18 @@
   </si>
   <si>
     <t>Fluxo de navegação e layouts da jornadas</t>
+  </si>
+  <si>
+    <t>Planning, abrir um chamado ao cadastrar usuário API, FAQ Mobile, editar usuário WEB, teste unitário de chamado</t>
+  </si>
+  <si>
+    <t>Organização dos dados para exibição no gráfico, editar usuário e histórico de relatórios</t>
+  </si>
+  <si>
+    <t>Login Mobile, resolução de erros da API, exibição do nome do usuário logado na tela e remoção do token ao fazer Logoff</t>
+  </si>
+  <si>
+    <t>Fluxo de navegação e wireframe jornada, alteração da API para métodos assíncronos, modelagem do banco de dados com a jornada e correção do endpoint da imagem na API</t>
   </si>
 </sst>
 </file>
@@ -2050,13 +2062,7 @@
     <xf numFmtId="0" fontId="12" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2077,6 +2083,18 @@
     <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2085,18 +2103,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2153,6 +2159,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2555,7 +2567,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="BR4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BZ7" sqref="BZ7"/>
+      <selection pane="bottomRight" activeCell="BX7" sqref="BX7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2600,13 +2612,14 @@
     <col min="72" max="72" width="3.77734375" style="80" customWidth="1"/>
     <col min="73" max="74" width="20.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
-    <col min="76" max="92" width="5.77734375" customWidth="1"/>
+    <col min="76" max="76" width="25.77734375" customWidth="1"/>
+    <col min="77" max="92" width="5.77734375" customWidth="1"/>
     <col min="93" max="93" width="3.77734375" style="81" customWidth="1"/>
     <col min="94" max="96" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2886,117 +2899,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="117"/>
+      <c r="A2" s="119"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="117" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="119" t="s">
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="119"/>
-      <c r="T2" s="119"/>
-      <c r="U2" s="119"/>
-      <c r="V2" s="119"/>
-      <c r="W2" s="119"/>
-      <c r="X2" s="119"/>
-      <c r="Y2" s="119"/>
-      <c r="Z2" s="119"/>
-      <c r="AA2" s="119"/>
-      <c r="AB2" s="119"/>
-      <c r="AC2" s="119"/>
-      <c r="AD2" s="119"/>
-      <c r="AE2" s="119"/>
-      <c r="AF2" s="119"/>
-      <c r="AG2" s="119"/>
-      <c r="AH2" s="119"/>
-      <c r="AI2" s="119"/>
-      <c r="AJ2" s="119"/>
-      <c r="AK2" s="119"/>
-      <c r="AL2" s="119"/>
-      <c r="AM2" s="119" t="s">
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
+      <c r="AA2" s="117"/>
+      <c r="AB2" s="117"/>
+      <c r="AC2" s="117"/>
+      <c r="AD2" s="117"/>
+      <c r="AE2" s="117"/>
+      <c r="AF2" s="117"/>
+      <c r="AG2" s="117"/>
+      <c r="AH2" s="117"/>
+      <c r="AI2" s="117"/>
+      <c r="AJ2" s="117"/>
+      <c r="AK2" s="117"/>
+      <c r="AL2" s="117"/>
+      <c r="AM2" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="119"/>
-      <c r="AO2" s="119"/>
-      <c r="AP2" s="119"/>
-      <c r="AQ2" s="119"/>
-      <c r="AR2" s="119"/>
-      <c r="AS2" s="119"/>
-      <c r="AT2" s="119"/>
-      <c r="AU2" s="119"/>
-      <c r="AV2" s="119"/>
-      <c r="AW2" s="119"/>
-      <c r="AX2" s="119"/>
-      <c r="AY2" s="119"/>
-      <c r="AZ2" s="119"/>
-      <c r="BA2" s="119"/>
-      <c r="BB2" s="119"/>
-      <c r="BC2" s="119"/>
-      <c r="BD2" s="119"/>
-      <c r="BE2" s="119"/>
-      <c r="BF2" s="119"/>
-      <c r="BG2" s="119"/>
-      <c r="BH2" s="119"/>
-      <c r="BI2" s="119"/>
-      <c r="BJ2" s="119" t="s">
+      <c r="AN2" s="117"/>
+      <c r="AO2" s="117"/>
+      <c r="AP2" s="117"/>
+      <c r="AQ2" s="117"/>
+      <c r="AR2" s="117"/>
+      <c r="AS2" s="117"/>
+      <c r="AT2" s="117"/>
+      <c r="AU2" s="117"/>
+      <c r="AV2" s="117"/>
+      <c r="AW2" s="117"/>
+      <c r="AX2" s="117"/>
+      <c r="AY2" s="117"/>
+      <c r="AZ2" s="117"/>
+      <c r="BA2" s="117"/>
+      <c r="BB2" s="117"/>
+      <c r="BC2" s="117"/>
+      <c r="BD2" s="117"/>
+      <c r="BE2" s="117"/>
+      <c r="BF2" s="117"/>
+      <c r="BG2" s="117"/>
+      <c r="BH2" s="117"/>
+      <c r="BI2" s="117"/>
+      <c r="BJ2" s="117" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="119"/>
-      <c r="BL2" s="119"/>
-      <c r="BM2" s="119"/>
-      <c r="BN2" s="119"/>
-      <c r="BO2" s="119"/>
-      <c r="BP2" s="119"/>
-      <c r="BQ2" s="119"/>
-      <c r="BR2" s="119"/>
-      <c r="BS2" s="119"/>
-      <c r="BT2" s="119"/>
-      <c r="BU2" s="119"/>
-      <c r="BV2" s="119"/>
-      <c r="BW2" s="119"/>
-      <c r="BX2" s="119"/>
-      <c r="BY2" s="119"/>
-      <c r="BZ2" s="119"/>
-      <c r="CA2" s="119"/>
-      <c r="CB2" s="119"/>
-      <c r="CC2" s="119"/>
-      <c r="CD2" s="119"/>
-      <c r="CE2" s="119" t="s">
+      <c r="BK2" s="117"/>
+      <c r="BL2" s="117"/>
+      <c r="BM2" s="117"/>
+      <c r="BN2" s="117"/>
+      <c r="BO2" s="117"/>
+      <c r="BP2" s="117"/>
+      <c r="BQ2" s="117"/>
+      <c r="BR2" s="117"/>
+      <c r="BS2" s="117"/>
+      <c r="BT2" s="117"/>
+      <c r="BU2" s="117"/>
+      <c r="BV2" s="117"/>
+      <c r="BW2" s="117"/>
+      <c r="BX2" s="117"/>
+      <c r="BY2" s="117"/>
+      <c r="BZ2" s="117"/>
+      <c r="CA2" s="117"/>
+      <c r="CB2" s="117"/>
+      <c r="CC2" s="117"/>
+      <c r="CD2" s="117"/>
+      <c r="CE2" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="119"/>
-      <c r="CG2" s="119"/>
-      <c r="CH2" s="119"/>
-      <c r="CI2" s="119"/>
-      <c r="CJ2" s="119"/>
-      <c r="CK2" s="119"/>
-      <c r="CL2" s="119"/>
-      <c r="CM2" s="119"/>
-      <c r="CN2" s="119"/>
-      <c r="CO2" s="119"/>
-      <c r="CP2" s="119"/>
-      <c r="CQ2" s="119"/>
-      <c r="CR2" s="119"/>
+      <c r="CF2" s="117"/>
+      <c r="CG2" s="117"/>
+      <c r="CH2" s="117"/>
+      <c r="CI2" s="117"/>
+      <c r="CJ2" s="117"/>
+      <c r="CK2" s="117"/>
+      <c r="CL2" s="117"/>
+      <c r="CM2" s="117"/>
+      <c r="CN2" s="117"/>
+      <c r="CO2" s="117"/>
+      <c r="CP2" s="117"/>
+      <c r="CQ2" s="117"/>
+      <c r="CR2" s="117"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="118"/>
+      <c r="A3" s="120"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3284,10 +3297,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="114" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3423,10 +3436,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="120" t="s">
+      <c r="AV4" s="116" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="120" t="s">
+      <c r="AW4" s="116" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3495,44 +3508,46 @@
       <c r="BS4" s="105" t="s">
         <v>350</v>
       </c>
-      <c r="BT4" s="120" t="s">
+      <c r="BT4" s="116" t="s">
         <v>112</v>
       </c>
-      <c r="BU4" s="112" t="s">
+      <c r="BU4" s="110" t="s">
         <v>310</v>
       </c>
-      <c r="BV4" s="113" t="s">
+      <c r="BV4" s="111" t="s">
         <v>357</v>
       </c>
-      <c r="BW4" s="120" t="s">
+      <c r="BW4" s="116" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="107"/>
-      <c r="BY4" s="108"/>
-      <c r="BZ4" s="108"/>
-      <c r="CA4" s="108"/>
-      <c r="CB4" s="108"/>
-      <c r="CC4" s="108"/>
-      <c r="CD4" s="108"/>
-      <c r="CE4" s="110"/>
-      <c r="CF4" s="110"/>
-      <c r="CG4" s="110"/>
-      <c r="CH4" s="110"/>
-      <c r="CI4" s="110"/>
-      <c r="CJ4" s="110"/>
-      <c r="CK4" s="110"/>
-      <c r="CL4" s="110"/>
-      <c r="CM4" s="110"/>
-      <c r="CN4" s="111"/>
-      <c r="CO4" s="120" t="s">
+      <c r="BX4" s="140" t="s">
+        <v>361</v>
+      </c>
+      <c r="BY4" s="107"/>
+      <c r="BZ4" s="107"/>
+      <c r="CA4" s="107"/>
+      <c r="CB4" s="107"/>
+      <c r="CC4" s="107"/>
+      <c r="CD4" s="107"/>
+      <c r="CE4" s="108"/>
+      <c r="CF4" s="108"/>
+      <c r="CG4" s="108"/>
+      <c r="CH4" s="108"/>
+      <c r="CI4" s="108"/>
+      <c r="CJ4" s="108"/>
+      <c r="CK4" s="108"/>
+      <c r="CL4" s="108"/>
+      <c r="CM4" s="108"/>
+      <c r="CN4" s="109"/>
+      <c r="CO4" s="116" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="114" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3666,8 +3681,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
+      <c r="AV5" s="116"/>
+      <c r="AW5" s="116"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3734,38 +3749,40 @@
       <c r="BS5" s="105" t="s">
         <v>351</v>
       </c>
-      <c r="BT5" s="120"/>
-      <c r="BU5" s="114" t="s">
+      <c r="BT5" s="116"/>
+      <c r="BU5" s="112" t="s">
         <v>354</v>
       </c>
-      <c r="BV5" s="115" t="s">
+      <c r="BV5" s="113" t="s">
         <v>358</v>
       </c>
-      <c r="BW5" s="120"/>
-      <c r="BX5" s="109"/>
-      <c r="BY5" s="108"/>
-      <c r="BZ5" s="108"/>
-      <c r="CA5" s="108"/>
-      <c r="CB5" s="108"/>
-      <c r="CC5" s="108"/>
-      <c r="CD5" s="108"/>
-      <c r="CE5" s="110"/>
-      <c r="CF5" s="110"/>
-      <c r="CG5" s="110"/>
-      <c r="CH5" s="110"/>
-      <c r="CI5" s="110"/>
-      <c r="CJ5" s="110"/>
-      <c r="CK5" s="110"/>
-      <c r="CL5" s="110"/>
-      <c r="CM5" s="110"/>
-      <c r="CN5" s="111"/>
-      <c r="CO5" s="120"/>
+      <c r="BW5" s="116"/>
+      <c r="BX5" s="141" t="s">
+        <v>362</v>
+      </c>
+      <c r="BY5" s="107"/>
+      <c r="BZ5" s="107"/>
+      <c r="CA5" s="107"/>
+      <c r="CB5" s="107"/>
+      <c r="CC5" s="107"/>
+      <c r="CD5" s="107"/>
+      <c r="CE5" s="108"/>
+      <c r="CF5" s="108"/>
+      <c r="CG5" s="108"/>
+      <c r="CH5" s="108"/>
+      <c r="CI5" s="108"/>
+      <c r="CJ5" s="108"/>
+      <c r="CK5" s="108"/>
+      <c r="CL5" s="108"/>
+      <c r="CM5" s="108"/>
+      <c r="CN5" s="109"/>
+      <c r="CO5" s="116"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="114" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="122"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3901,8 +3918,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
+      <c r="AV6" s="116"/>
+      <c r="AW6" s="116"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3969,38 +3986,40 @@
       <c r="BS6" s="105" t="s">
         <v>352</v>
       </c>
-      <c r="BT6" s="120"/>
-      <c r="BU6" s="114" t="s">
+      <c r="BT6" s="116"/>
+      <c r="BU6" s="112" t="s">
         <v>355</v>
       </c>
-      <c r="BV6" s="115" t="s">
+      <c r="BV6" s="113" t="s">
         <v>359</v>
       </c>
-      <c r="BW6" s="120"/>
-      <c r="BX6" s="109"/>
-      <c r="BY6" s="108"/>
-      <c r="BZ6" s="108"/>
-      <c r="CA6" s="108"/>
-      <c r="CB6" s="108"/>
-      <c r="CC6" s="108"/>
-      <c r="CD6" s="108"/>
-      <c r="CE6" s="110"/>
-      <c r="CF6" s="110"/>
-      <c r="CG6" s="110"/>
-      <c r="CH6" s="110"/>
-      <c r="CI6" s="110"/>
-      <c r="CJ6" s="110"/>
-      <c r="CK6" s="110"/>
-      <c r="CL6" s="110"/>
-      <c r="CM6" s="110"/>
-      <c r="CN6" s="111"/>
-      <c r="CO6" s="120"/>
+      <c r="BW6" s="116"/>
+      <c r="BX6" s="141" t="s">
+        <v>363</v>
+      </c>
+      <c r="BY6" s="107"/>
+      <c r="BZ6" s="107"/>
+      <c r="CA6" s="107"/>
+      <c r="CB6" s="107"/>
+      <c r="CC6" s="107"/>
+      <c r="CD6" s="107"/>
+      <c r="CE6" s="108"/>
+      <c r="CF6" s="108"/>
+      <c r="CG6" s="108"/>
+      <c r="CH6" s="108"/>
+      <c r="CI6" s="108"/>
+      <c r="CJ6" s="108"/>
+      <c r="CK6" s="108"/>
+      <c r="CL6" s="108"/>
+      <c r="CM6" s="108"/>
+      <c r="CN6" s="109"/>
+      <c r="CO6" s="116"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="114" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="122"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4136,8 +4155,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="120"/>
-      <c r="AW7" s="120"/>
+      <c r="AV7" s="116"/>
+      <c r="AW7" s="116"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4204,50 +4223,52 @@
       <c r="BS7" s="106" t="s">
         <v>353</v>
       </c>
-      <c r="BT7" s="120"/>
-      <c r="BU7" s="114" t="s">
+      <c r="BT7" s="116"/>
+      <c r="BU7" s="112" t="s">
         <v>356</v>
       </c>
-      <c r="BV7" s="115" t="s">
+      <c r="BV7" s="113" t="s">
         <v>360</v>
       </c>
-      <c r="BW7" s="120"/>
-      <c r="BX7" s="109"/>
-      <c r="BY7" s="108"/>
-      <c r="BZ7" s="108"/>
-      <c r="CA7" s="108"/>
-      <c r="CB7" s="108"/>
-      <c r="CC7" s="108"/>
-      <c r="CD7" s="108"/>
-      <c r="CE7" s="110"/>
-      <c r="CF7" s="110"/>
-      <c r="CG7" s="110"/>
-      <c r="CH7" s="110"/>
-      <c r="CI7" s="110"/>
-      <c r="CJ7" s="110"/>
-      <c r="CK7" s="110"/>
-      <c r="CL7" s="110"/>
-      <c r="CM7" s="110"/>
-      <c r="CN7" s="111"/>
-      <c r="CO7" s="120"/>
+      <c r="BW7" s="116"/>
+      <c r="BX7" s="141" t="s">
+        <v>364</v>
+      </c>
+      <c r="BY7" s="107"/>
+      <c r="BZ7" s="107"/>
+      <c r="CA7" s="107"/>
+      <c r="CB7" s="107"/>
+      <c r="CC7" s="107"/>
+      <c r="CD7" s="107"/>
+      <c r="CE7" s="108"/>
+      <c r="CF7" s="108"/>
+      <c r="CG7" s="108"/>
+      <c r="CH7" s="108"/>
+      <c r="CI7" s="108"/>
+      <c r="CJ7" s="108"/>
+      <c r="CK7" s="108"/>
+      <c r="CL7" s="108"/>
+      <c r="CM7" s="108"/>
+      <c r="CN7" s="109"/>
+      <c r="CO7" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4330,36 +4351,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="125" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="131" t="s">
+      <c r="F2" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="131"/>
+      <c r="G2" s="129"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="132" t="s">
+      <c r="I2" s="130" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="132"/>
+      <c r="J2" s="130"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="133" t="s">
+      <c r="L2" s="131" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="133"/>
+      <c r="M2" s="131"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="134" t="s">
+      <c r="O2" s="132" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="134"/>
+      <c r="P2" s="132"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="123" t="s">
+      <c r="R2" s="121" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="123"/>
+      <c r="S2" s="121"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4393,24 +4414,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="131"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="132"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="123"/>
-      <c r="S3" s="123"/>
+      <c r="R3" s="121"/>
+      <c r="S3" s="121"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4444,24 +4465,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="131"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="134"/>
-      <c r="P4" s="134"/>
+      <c r="O4" s="132"/>
+      <c r="P4" s="132"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
+      <c r="R4" s="121"/>
+      <c r="S4" s="121"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4499,20 +4520,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="132"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="130"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="133"/>
+      <c r="L5" s="131"/>
+      <c r="M5" s="131"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="134"/>
-      <c r="P5" s="134"/>
+      <c r="O5" s="132"/>
+      <c r="P5" s="132"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="123"/>
-      <c r="S5" s="123"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="121"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4546,26 +4567,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="126" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="133"/>
-      <c r="M6" s="133"/>
+      <c r="L6" s="131"/>
+      <c r="M6" s="131"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="121"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4599,24 +4620,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="131"/>
-      <c r="G7" s="131"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="132"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="131"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="134"/>
-      <c r="P7" s="134"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="123"/>
-      <c r="S7" s="123"/>
+      <c r="R7" s="121"/>
+      <c r="S7" s="121"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4650,24 +4671,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="127"/>
+      <c r="D8" s="127"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="133"/>
+      <c r="L8" s="131"/>
+      <c r="M8" s="131"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="134"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="123"/>
-      <c r="S8" s="123"/>
+      <c r="R8" s="121"/>
+      <c r="S8" s="121"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4701,24 +4722,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="127"/>
+      <c r="D9" s="127"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="131"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="132"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="133"/>
-      <c r="M9" s="133"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="131"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="134"/>
-      <c r="P9" s="134"/>
+      <c r="O9" s="132"/>
+      <c r="P9" s="132"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="123"/>
-      <c r="S9" s="123"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="121"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4752,24 +4773,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
+      <c r="B10" s="127"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="127"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="133"/>
+      <c r="L10" s="131"/>
+      <c r="M10" s="131"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="134"/>
-      <c r="P10" s="134"/>
+      <c r="O10" s="132"/>
+      <c r="P10" s="132"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="123"/>
-      <c r="S10" s="123"/>
+      <c r="R10" s="121"/>
+      <c r="S10" s="121"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4858,23 +4879,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="124" t="s">
+      <c r="F12" s="122" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="124"/>
+      <c r="G12" s="122"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="125" t="s">
+      <c r="I12" s="123" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="125"/>
+      <c r="J12" s="123"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="126" t="s">
+      <c r="L12" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="126"/>
+      <c r="M12" s="124"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="130"/>
-      <c r="P12" s="130"/>
+      <c r="O12" s="128"/>
+      <c r="P12" s="128"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4915,17 +4936,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="125"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="123"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="126"/>
-      <c r="M13" s="126"/>
+      <c r="L13" s="124"/>
+      <c r="M13" s="124"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="130"/>
-      <c r="P13" s="130"/>
+      <c r="O13" s="128"/>
+      <c r="P13" s="128"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4966,17 +4987,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="124"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="125"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="123"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="126"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="130"/>
-      <c r="P14" s="130"/>
+      <c r="O14" s="128"/>
+      <c r="P14" s="128"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -5017,17 +5038,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="122"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="125"/>
+      <c r="I15" s="123"/>
+      <c r="J15" s="123"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="126"/>
-      <c r="M15" s="126"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="130"/>
-      <c r="P15" s="130"/>
+      <c r="O15" s="128"/>
+      <c r="P15" s="128"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -5068,17 +5089,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="124"/>
-      <c r="G16" s="124"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="122"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="125"/>
+      <c r="I16" s="123"/>
+      <c r="J16" s="123"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="126"/>
-      <c r="M16" s="126"/>
+      <c r="L16" s="124"/>
+      <c r="M16" s="124"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="130"/>
-      <c r="P16" s="130"/>
+      <c r="O16" s="128"/>
+      <c r="P16" s="128"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -5119,17 +5140,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="124"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="125"/>
-      <c r="J17" s="125"/>
+      <c r="I17" s="123"/>
+      <c r="J17" s="123"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="126"/>
-      <c r="M17" s="126"/>
+      <c r="L17" s="124"/>
+      <c r="M17" s="124"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="130"/>
-      <c r="P17" s="130"/>
+      <c r="O17" s="128"/>
+      <c r="P17" s="128"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -5170,17 +5191,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="124"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="125"/>
+      <c r="I18" s="123"/>
+      <c r="J18" s="123"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="126"/>
-      <c r="M18" s="126"/>
+      <c r="L18" s="124"/>
+      <c r="M18" s="124"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="130"/>
-      <c r="P18" s="130"/>
+      <c r="O18" s="128"/>
+      <c r="P18" s="128"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -5221,17 +5242,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="124"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="125"/>
-      <c r="J19" s="125"/>
+      <c r="I19" s="123"/>
+      <c r="J19" s="123"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="126"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="130"/>
-      <c r="P19" s="130"/>
+      <c r="O19" s="128"/>
+      <c r="P19" s="128"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5272,17 +5293,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="124"/>
+      <c r="F20" s="122"/>
+      <c r="G20" s="122"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="125"/>
-      <c r="J20" s="125"/>
+      <c r="I20" s="123"/>
+      <c r="J20" s="123"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="126"/>
-      <c r="M20" s="126"/>
+      <c r="L20" s="124"/>
+      <c r="M20" s="124"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="130"/>
+      <c r="O20" s="128"/>
+      <c r="P20" s="128"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17855,7 +17876,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="135" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -18195,7 +18216,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="137"/>
+      <c r="A2" s="135"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18521,15 +18542,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="138"/>
-      <c r="DH2" s="138"/>
-      <c r="DI2" s="138"/>
-      <c r="DJ2" s="138"/>
+      <c r="DG2" s="136"/>
+      <c r="DH2" s="136"/>
+      <c r="DI2" s="136"/>
+      <c r="DJ2" s="136"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="137"/>
+      <c r="A3" s="135"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18866,7 +18887,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="137" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -19008,7 +19029,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="139"/>
+      <c r="B5" s="137"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -19148,7 +19169,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="139"/>
+      <c r="B6" s="137"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19288,7 +19309,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="139"/>
+      <c r="B7" s="137"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19426,7 +19447,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="139"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19566,7 +19587,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="138" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19708,7 +19729,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="140"/>
+      <c r="B10" s="138"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19848,7 +19869,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="139" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19978,7 +19999,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="141"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -20116,7 +20137,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="141"/>
+      <c r="B13" s="139"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20256,7 +20277,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="141"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20392,7 +20413,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="141"/>
+      <c r="B15" s="139"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20528,7 +20549,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="139"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20664,7 +20685,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="139"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20800,7 +20821,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="141"/>
+      <c r="B18" s="139"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20940,7 +20961,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="141"/>
+      <c r="B19" s="139"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -21076,7 +21097,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="141"/>
+      <c r="B20" s="139"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -21212,7 +21233,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="133" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21346,7 +21367,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="135"/>
+      <c r="B22" s="133"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21482,7 +21503,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="135"/>
+      <c r="B23" s="133"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21614,7 +21635,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="135"/>
+      <c r="B24" s="133"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21748,7 +21769,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="135"/>
+      <c r="B25" s="133"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21892,7 +21913,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="136" t="s">
+      <c r="B26" s="134" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -22026,7 +22047,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="136"/>
+      <c r="B27" s="134"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -22166,7 +22187,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="136"/>
+      <c r="B28" s="134"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22298,7 +22319,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="136"/>
+      <c r="B29" s="134"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22426,7 +22447,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="136"/>
+      <c r="B30" s="134"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22552,7 +22573,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="136"/>
+      <c r="B31" s="134"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 25 e 26-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6B4DA4-33BD-4336-9F22-5E1C49346CC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D1734-11FA-4EA0-A9E4-148F42A31F0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="373">
   <si>
     <t>REDES</t>
   </si>
@@ -1207,6 +1207,30 @@
   </si>
   <si>
     <t>Fluxo de navegação e wireframe jornada, alteração da API para métodos assíncronos, modelagem do banco de dados com a jornada e correção do endpoint da imagem na API</t>
+  </si>
+  <si>
+    <t>Buscar última tarefa e o responsável pelo chamado API, cadastro de usuário Mobile, reabrir chamado WEB, continuação teste unitário</t>
+  </si>
+  <si>
+    <t>Histórico de relatórios API, organização dos dados para exibição no gráfico e editar usuário</t>
+  </si>
+  <si>
+    <t>Alteração na cor da barra de status no card, métodos update no passo a passo inicial WEB, correção de erros nos loopings das requisições para a API, logout e permissão de rotas WEB e login Mobile</t>
+  </si>
+  <si>
+    <t>Upload de imagens no Blobs, CRUD jornada na API, layout alta fidelidade jornada</t>
+  </si>
+  <si>
+    <t>Validação de cadastro de usuário na API, reabrir chamado WEB, teste unitário</t>
+  </si>
+  <si>
+    <t>Organização dos dados para exibição no gráfico, editar usuário e filtro por data na API</t>
+  </si>
+  <si>
+    <t>Alteração na cor da barra de status no card, atualizar e deletar no passo a passo inicial, correção de erros nos loopings das requisições para a API, estilização na página de listagem geral</t>
+  </si>
+  <si>
+    <t>Layout de alta fidelidade do mapa da jornada, configuração de rotas da aplicação e editar e deletar imagem no Blobs</t>
   </si>
 </sst>
 </file>
@@ -2062,15 +2086,6 @@
     <xf numFmtId="0" fontId="12" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2083,17 +2098,11 @@
     <xf numFmtId="0" fontId="12" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2103,6 +2112,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2161,10 +2182,13 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2564,10 +2588,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BR4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BX4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BX7" sqref="BX7"/>
+      <selection pane="bottomRight" activeCell="BZ11" sqref="BZ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2613,13 +2637,15 @@
     <col min="73" max="74" width="20.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
     <col min="76" max="76" width="25.77734375" customWidth="1"/>
-    <col min="77" max="92" width="5.77734375" customWidth="1"/>
+    <col min="77" max="77" width="30.77734375" customWidth="1"/>
+    <col min="78" max="78" width="25.77734375" customWidth="1"/>
+    <col min="79" max="92" width="5.77734375" customWidth="1"/>
     <col min="93" max="93" width="3.77734375" style="81" customWidth="1"/>
     <col min="94" max="96" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="113" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2899,117 +2925,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="119"/>
+      <c r="A2" s="114"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="117" t="s">
+      <c r="C2" s="116" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="117"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117" t="s">
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="117"/>
-      <c r="Y2" s="117"/>
-      <c r="Z2" s="117"/>
-      <c r="AA2" s="117"/>
-      <c r="AB2" s="117"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="117"/>
-      <c r="AE2" s="117"/>
-      <c r="AF2" s="117"/>
-      <c r="AG2" s="117"/>
-      <c r="AH2" s="117"/>
-      <c r="AI2" s="117"/>
-      <c r="AJ2" s="117"/>
-      <c r="AK2" s="117"/>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="117" t="s">
+      <c r="S2" s="116"/>
+      <c r="T2" s="116"/>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="116"/>
+      <c r="X2" s="116"/>
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="116"/>
+      <c r="AH2" s="116"/>
+      <c r="AI2" s="116"/>
+      <c r="AJ2" s="116"/>
+      <c r="AK2" s="116"/>
+      <c r="AL2" s="116"/>
+      <c r="AM2" s="116" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="117"/>
-      <c r="AO2" s="117"/>
-      <c r="AP2" s="117"/>
-      <c r="AQ2" s="117"/>
-      <c r="AR2" s="117"/>
-      <c r="AS2" s="117"/>
-      <c r="AT2" s="117"/>
-      <c r="AU2" s="117"/>
-      <c r="AV2" s="117"/>
-      <c r="AW2" s="117"/>
-      <c r="AX2" s="117"/>
-      <c r="AY2" s="117"/>
-      <c r="AZ2" s="117"/>
-      <c r="BA2" s="117"/>
-      <c r="BB2" s="117"/>
-      <c r="BC2" s="117"/>
-      <c r="BD2" s="117"/>
-      <c r="BE2" s="117"/>
-      <c r="BF2" s="117"/>
-      <c r="BG2" s="117"/>
-      <c r="BH2" s="117"/>
-      <c r="BI2" s="117"/>
-      <c r="BJ2" s="117" t="s">
+      <c r="AN2" s="116"/>
+      <c r="AO2" s="116"/>
+      <c r="AP2" s="116"/>
+      <c r="AQ2" s="116"/>
+      <c r="AR2" s="116"/>
+      <c r="AS2" s="116"/>
+      <c r="AT2" s="116"/>
+      <c r="AU2" s="116"/>
+      <c r="AV2" s="116"/>
+      <c r="AW2" s="116"/>
+      <c r="AX2" s="116"/>
+      <c r="AY2" s="116"/>
+      <c r="AZ2" s="116"/>
+      <c r="BA2" s="116"/>
+      <c r="BB2" s="116"/>
+      <c r="BC2" s="116"/>
+      <c r="BD2" s="116"/>
+      <c r="BE2" s="116"/>
+      <c r="BF2" s="116"/>
+      <c r="BG2" s="116"/>
+      <c r="BH2" s="116"/>
+      <c r="BI2" s="116"/>
+      <c r="BJ2" s="116" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="117"/>
-      <c r="BL2" s="117"/>
-      <c r="BM2" s="117"/>
-      <c r="BN2" s="117"/>
-      <c r="BO2" s="117"/>
-      <c r="BP2" s="117"/>
-      <c r="BQ2" s="117"/>
-      <c r="BR2" s="117"/>
-      <c r="BS2" s="117"/>
-      <c r="BT2" s="117"/>
-      <c r="BU2" s="117"/>
-      <c r="BV2" s="117"/>
-      <c r="BW2" s="117"/>
-      <c r="BX2" s="117"/>
-      <c r="BY2" s="117"/>
-      <c r="BZ2" s="117"/>
-      <c r="CA2" s="117"/>
-      <c r="CB2" s="117"/>
-      <c r="CC2" s="117"/>
-      <c r="CD2" s="117"/>
-      <c r="CE2" s="117" t="s">
+      <c r="BK2" s="116"/>
+      <c r="BL2" s="116"/>
+      <c r="BM2" s="116"/>
+      <c r="BN2" s="116"/>
+      <c r="BO2" s="116"/>
+      <c r="BP2" s="116"/>
+      <c r="BQ2" s="116"/>
+      <c r="BR2" s="116"/>
+      <c r="BS2" s="116"/>
+      <c r="BT2" s="116"/>
+      <c r="BU2" s="116"/>
+      <c r="BV2" s="116"/>
+      <c r="BW2" s="116"/>
+      <c r="BX2" s="116"/>
+      <c r="BY2" s="116"/>
+      <c r="BZ2" s="116"/>
+      <c r="CA2" s="116"/>
+      <c r="CB2" s="116"/>
+      <c r="CC2" s="116"/>
+      <c r="CD2" s="116"/>
+      <c r="CE2" s="116" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="117"/>
-      <c r="CG2" s="117"/>
-      <c r="CH2" s="117"/>
-      <c r="CI2" s="117"/>
-      <c r="CJ2" s="117"/>
-      <c r="CK2" s="117"/>
-      <c r="CL2" s="117"/>
-      <c r="CM2" s="117"/>
-      <c r="CN2" s="117"/>
-      <c r="CO2" s="117"/>
-      <c r="CP2" s="117"/>
-      <c r="CQ2" s="117"/>
-      <c r="CR2" s="117"/>
+      <c r="CF2" s="116"/>
+      <c r="CG2" s="116"/>
+      <c r="CH2" s="116"/>
+      <c r="CI2" s="116"/>
+      <c r="CJ2" s="116"/>
+      <c r="CK2" s="116"/>
+      <c r="CL2" s="116"/>
+      <c r="CM2" s="116"/>
+      <c r="CN2" s="116"/>
+      <c r="CO2" s="116"/>
+      <c r="CP2" s="116"/>
+      <c r="CQ2" s="116"/>
+      <c r="CR2" s="116"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="120"/>
+      <c r="A3" s="115"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3297,10 +3323,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="118" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3436,10 +3462,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="116" t="s">
+      <c r="AV4" s="117" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="116" t="s">
+      <c r="AW4" s="117" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3508,46 +3534,50 @@
       <c r="BS4" s="105" t="s">
         <v>350</v>
       </c>
-      <c r="BT4" s="116" t="s">
+      <c r="BT4" s="117" t="s">
         <v>112</v>
       </c>
-      <c r="BU4" s="110" t="s">
+      <c r="BU4" s="107" t="s">
         <v>310</v>
       </c>
-      <c r="BV4" s="111" t="s">
+      <c r="BV4" s="108" t="s">
         <v>357</v>
       </c>
-      <c r="BW4" s="116" t="s">
+      <c r="BW4" s="117" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="140" t="s">
+      <c r="BX4" s="111" t="s">
         <v>361</v>
       </c>
-      <c r="BY4" s="107"/>
-      <c r="BZ4" s="107"/>
-      <c r="CA4" s="107"/>
-      <c r="CB4" s="107"/>
-      <c r="CC4" s="107"/>
-      <c r="CD4" s="107"/>
-      <c r="CE4" s="108"/>
-      <c r="CF4" s="108"/>
-      <c r="CG4" s="108"/>
-      <c r="CH4" s="108"/>
-      <c r="CI4" s="108"/>
-      <c r="CJ4" s="108"/>
-      <c r="CK4" s="108"/>
-      <c r="CL4" s="108"/>
-      <c r="CM4" s="108"/>
-      <c r="CN4" s="109"/>
-      <c r="CO4" s="116" t="s">
+      <c r="BY4" s="139" t="s">
+        <v>365</v>
+      </c>
+      <c r="BZ4" s="139" t="s">
+        <v>369</v>
+      </c>
+      <c r="CA4" s="139"/>
+      <c r="CB4" s="139"/>
+      <c r="CC4" s="139"/>
+      <c r="CD4" s="139"/>
+      <c r="CE4" s="140"/>
+      <c r="CF4" s="140"/>
+      <c r="CG4" s="140"/>
+      <c r="CH4" s="140"/>
+      <c r="CI4" s="140"/>
+      <c r="CJ4" s="140"/>
+      <c r="CK4" s="140"/>
+      <c r="CL4" s="140"/>
+      <c r="CM4" s="140"/>
+      <c r="CN4" s="141"/>
+      <c r="CO4" s="117" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3681,8 +3711,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="116"/>
-      <c r="AW5" s="116"/>
+      <c r="AV5" s="117"/>
+      <c r="AW5" s="117"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3749,40 +3779,44 @@
       <c r="BS5" s="105" t="s">
         <v>351</v>
       </c>
-      <c r="BT5" s="116"/>
-      <c r="BU5" s="112" t="s">
+      <c r="BT5" s="117"/>
+      <c r="BU5" s="109" t="s">
         <v>354</v>
       </c>
-      <c r="BV5" s="113" t="s">
+      <c r="BV5" s="110" t="s">
         <v>358</v>
       </c>
-      <c r="BW5" s="116"/>
-      <c r="BX5" s="141" t="s">
+      <c r="BW5" s="117"/>
+      <c r="BX5" s="112" t="s">
         <v>362</v>
       </c>
-      <c r="BY5" s="107"/>
-      <c r="BZ5" s="107"/>
-      <c r="CA5" s="107"/>
-      <c r="CB5" s="107"/>
-      <c r="CC5" s="107"/>
-      <c r="CD5" s="107"/>
-      <c r="CE5" s="108"/>
-      <c r="CF5" s="108"/>
-      <c r="CG5" s="108"/>
-      <c r="CH5" s="108"/>
-      <c r="CI5" s="108"/>
-      <c r="CJ5" s="108"/>
-      <c r="CK5" s="108"/>
-      <c r="CL5" s="108"/>
-      <c r="CM5" s="108"/>
-      <c r="CN5" s="109"/>
-      <c r="CO5" s="116"/>
+      <c r="BY5" s="139" t="s">
+        <v>366</v>
+      </c>
+      <c r="BZ5" s="139" t="s">
+        <v>370</v>
+      </c>
+      <c r="CA5" s="139"/>
+      <c r="CB5" s="139"/>
+      <c r="CC5" s="139"/>
+      <c r="CD5" s="139"/>
+      <c r="CE5" s="140"/>
+      <c r="CF5" s="140"/>
+      <c r="CG5" s="140"/>
+      <c r="CH5" s="140"/>
+      <c r="CI5" s="140"/>
+      <c r="CJ5" s="140"/>
+      <c r="CK5" s="140"/>
+      <c r="CL5" s="140"/>
+      <c r="CM5" s="140"/>
+      <c r="CN5" s="141"/>
+      <c r="CO5" s="117"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="118" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="115"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3918,8 +3952,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="116"/>
-      <c r="AW6" s="116"/>
+      <c r="AV6" s="117"/>
+      <c r="AW6" s="117"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -3986,40 +4020,44 @@
       <c r="BS6" s="105" t="s">
         <v>352</v>
       </c>
-      <c r="BT6" s="116"/>
-      <c r="BU6" s="112" t="s">
+      <c r="BT6" s="117"/>
+      <c r="BU6" s="109" t="s">
         <v>355</v>
       </c>
-      <c r="BV6" s="113" t="s">
+      <c r="BV6" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="BW6" s="116"/>
-      <c r="BX6" s="141" t="s">
+      <c r="BW6" s="117"/>
+      <c r="BX6" s="112" t="s">
         <v>363</v>
       </c>
-      <c r="BY6" s="107"/>
-      <c r="BZ6" s="107"/>
-      <c r="CA6" s="107"/>
-      <c r="CB6" s="107"/>
-      <c r="CC6" s="107"/>
-      <c r="CD6" s="107"/>
-      <c r="CE6" s="108"/>
-      <c r="CF6" s="108"/>
-      <c r="CG6" s="108"/>
-      <c r="CH6" s="108"/>
-      <c r="CI6" s="108"/>
-      <c r="CJ6" s="108"/>
-      <c r="CK6" s="108"/>
-      <c r="CL6" s="108"/>
-      <c r="CM6" s="108"/>
-      <c r="CN6" s="109"/>
-      <c r="CO6" s="116"/>
+      <c r="BY6" s="139" t="s">
+        <v>367</v>
+      </c>
+      <c r="BZ6" s="139" t="s">
+        <v>371</v>
+      </c>
+      <c r="CA6" s="139"/>
+      <c r="CB6" s="139"/>
+      <c r="CC6" s="139"/>
+      <c r="CD6" s="139"/>
+      <c r="CE6" s="140"/>
+      <c r="CF6" s="140"/>
+      <c r="CG6" s="140"/>
+      <c r="CH6" s="140"/>
+      <c r="CI6" s="140"/>
+      <c r="CJ6" s="140"/>
+      <c r="CK6" s="140"/>
+      <c r="CL6" s="140"/>
+      <c r="CM6" s="140"/>
+      <c r="CN6" s="141"/>
+      <c r="CO6" s="117"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="114" t="s">
+      <c r="A7" s="118" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4155,8 +4193,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="116"/>
-      <c r="AW7" s="116"/>
+      <c r="AV7" s="117"/>
+      <c r="AW7" s="117"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4223,52 +4261,56 @@
       <c r="BS7" s="106" t="s">
         <v>353</v>
       </c>
-      <c r="BT7" s="116"/>
-      <c r="BU7" s="112" t="s">
+      <c r="BT7" s="117"/>
+      <c r="BU7" s="109" t="s">
         <v>356</v>
       </c>
-      <c r="BV7" s="113" t="s">
+      <c r="BV7" s="110" t="s">
         <v>360</v>
       </c>
-      <c r="BW7" s="116"/>
-      <c r="BX7" s="141" t="s">
+      <c r="BW7" s="117"/>
+      <c r="BX7" s="112" t="s">
         <v>364</v>
       </c>
-      <c r="BY7" s="107"/>
-      <c r="BZ7" s="107"/>
-      <c r="CA7" s="107"/>
-      <c r="CB7" s="107"/>
-      <c r="CC7" s="107"/>
-      <c r="CD7" s="107"/>
-      <c r="CE7" s="108"/>
-      <c r="CF7" s="108"/>
-      <c r="CG7" s="108"/>
-      <c r="CH7" s="108"/>
-      <c r="CI7" s="108"/>
-      <c r="CJ7" s="108"/>
-      <c r="CK7" s="108"/>
-      <c r="CL7" s="108"/>
-      <c r="CM7" s="108"/>
-      <c r="CN7" s="109"/>
-      <c r="CO7" s="116"/>
+      <c r="BY7" s="139" t="s">
+        <v>368</v>
+      </c>
+      <c r="BZ7" s="139" t="s">
+        <v>372</v>
+      </c>
+      <c r="CA7" s="139"/>
+      <c r="CB7" s="139"/>
+      <c r="CC7" s="139"/>
+      <c r="CD7" s="139"/>
+      <c r="CE7" s="140"/>
+      <c r="CF7" s="140"/>
+      <c r="CG7" s="140"/>
+      <c r="CH7" s="140"/>
+      <c r="CI7" s="140"/>
+      <c r="CJ7" s="140"/>
+      <c r="CK7" s="140"/>
+      <c r="CL7" s="140"/>
+      <c r="CM7" s="140"/>
+      <c r="CN7" s="141"/>
+      <c r="CO7" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4351,36 +4393,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="124" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="129" t="s">
+      <c r="F2" s="128" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="129"/>
+      <c r="G2" s="128"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="129" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="130"/>
+      <c r="J2" s="129"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="131" t="s">
+      <c r="L2" s="130" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="131"/>
+      <c r="M2" s="130"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="132" t="s">
+      <c r="O2" s="131" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="132"/>
+      <c r="P2" s="131"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="121" t="s">
+      <c r="R2" s="120" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="121"/>
+      <c r="S2" s="120"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4414,24 +4456,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="131"/>
-      <c r="M3" s="131"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="132"/>
-      <c r="P3" s="132"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="121"/>
-      <c r="S3" s="121"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4465,24 +4507,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="130"/>
-      <c r="J4" s="130"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="132"/>
-      <c r="P4" s="132"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="121"/>
-      <c r="S4" s="121"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="120"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4520,20 +4562,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="130"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
+      <c r="L5" s="130"/>
+      <c r="M5" s="130"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="132"/>
-      <c r="P5" s="132"/>
+      <c r="O5" s="131"/>
+      <c r="P5" s="131"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="121"/>
-      <c r="S5" s="121"/>
+      <c r="R5" s="120"/>
+      <c r="S5" s="120"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4567,26 +4609,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="125" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="130"/>
-      <c r="J6" s="130"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="131"/>
-      <c r="M6" s="131"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="130"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="132"/>
-      <c r="P6" s="132"/>
+      <c r="O6" s="131"/>
+      <c r="P6" s="131"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="121"/>
-      <c r="S6" s="121"/>
+      <c r="R6" s="120"/>
+      <c r="S6" s="120"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4620,24 +4662,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="127"/>
-      <c r="C7" s="127"/>
-      <c r="D7" s="127"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="131"/>
-      <c r="M7" s="131"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="132"/>
-      <c r="P7" s="132"/>
+      <c r="O7" s="131"/>
+      <c r="P7" s="131"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="121"/>
-      <c r="S7" s="121"/>
+      <c r="R7" s="120"/>
+      <c r="S7" s="120"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4671,24 +4713,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="127"/>
-      <c r="C8" s="127"/>
-      <c r="D8" s="127"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="130"/>
-      <c r="J8" s="130"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="131"/>
-      <c r="M8" s="131"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="132"/>
-      <c r="P8" s="132"/>
+      <c r="O8" s="131"/>
+      <c r="P8" s="131"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="121"/>
-      <c r="S8" s="121"/>
+      <c r="R8" s="120"/>
+      <c r="S8" s="120"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4722,24 +4764,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="127"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="127"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="129"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="131"/>
-      <c r="M9" s="131"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="130"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="132"/>
-      <c r="P9" s="132"/>
+      <c r="O9" s="131"/>
+      <c r="P9" s="131"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="121"/>
-      <c r="S9" s="121"/>
+      <c r="R9" s="120"/>
+      <c r="S9" s="120"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4773,24 +4815,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="127"/>
-      <c r="C10" s="127"/>
-      <c r="D10" s="127"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="126"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="131"/>
-      <c r="M10" s="131"/>
+      <c r="L10" s="130"/>
+      <c r="M10" s="130"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="132"/>
-      <c r="P10" s="132"/>
+      <c r="O10" s="131"/>
+      <c r="P10" s="131"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="121"/>
-      <c r="S10" s="121"/>
+      <c r="R10" s="120"/>
+      <c r="S10" s="120"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4879,23 +4921,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="122" t="s">
+      <c r="F12" s="121" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="122"/>
+      <c r="G12" s="121"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="123" t="s">
+      <c r="I12" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="123"/>
+      <c r="J12" s="122"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="124" t="s">
+      <c r="L12" s="123" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="124"/>
+      <c r="M12" s="123"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="128"/>
-      <c r="P12" s="128"/>
+      <c r="O12" s="127"/>
+      <c r="P12" s="127"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4936,17 +4978,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="122"/>
-      <c r="G13" s="122"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="123"/>
-      <c r="J13" s="123"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="124"/>
+      <c r="L13" s="123"/>
+      <c r="M13" s="123"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="128"/>
-      <c r="P13" s="128"/>
+      <c r="O13" s="127"/>
+      <c r="P13" s="127"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -4987,17 +5029,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="122"/>
-      <c r="G14" s="122"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="123"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="122"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="124"/>
+      <c r="L14" s="123"/>
+      <c r="M14" s="123"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="128"/>
-      <c r="P14" s="128"/>
+      <c r="O14" s="127"/>
+      <c r="P14" s="127"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -5038,17 +5080,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="122"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="123"/>
-      <c r="J15" s="123"/>
+      <c r="I15" s="122"/>
+      <c r="J15" s="122"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="124"/>
+      <c r="L15" s="123"/>
+      <c r="M15" s="123"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="128"/>
-      <c r="P15" s="128"/>
+      <c r="O15" s="127"/>
+      <c r="P15" s="127"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -5089,17 +5131,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="122"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="123"/>
-      <c r="J16" s="123"/>
+      <c r="I16" s="122"/>
+      <c r="J16" s="122"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="124"/>
-      <c r="M16" s="124"/>
+      <c r="L16" s="123"/>
+      <c r="M16" s="123"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="128"/>
-      <c r="P16" s="128"/>
+      <c r="O16" s="127"/>
+      <c r="P16" s="127"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -5140,17 +5182,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="122"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="123"/>
-      <c r="J17" s="123"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="122"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="124"/>
-      <c r="M17" s="124"/>
+      <c r="L17" s="123"/>
+      <c r="M17" s="123"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="128"/>
-      <c r="P17" s="128"/>
+      <c r="O17" s="127"/>
+      <c r="P17" s="127"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -5191,17 +5233,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="122"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="121"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="123"/>
+      <c r="I18" s="122"/>
+      <c r="J18" s="122"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="124"/>
-      <c r="M18" s="124"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="123"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="128"/>
-      <c r="P18" s="128"/>
+      <c r="O18" s="127"/>
+      <c r="P18" s="127"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -5242,17 +5284,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="122"/>
-      <c r="G19" s="122"/>
+      <c r="F19" s="121"/>
+      <c r="G19" s="121"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="123"/>
-      <c r="J19" s="123"/>
+      <c r="I19" s="122"/>
+      <c r="J19" s="122"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="124"/>
+      <c r="L19" s="123"/>
+      <c r="M19" s="123"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="128"/>
-      <c r="P19" s="128"/>
+      <c r="O19" s="127"/>
+      <c r="P19" s="127"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5293,17 +5335,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="122"/>
-      <c r="G20" s="122"/>
+      <c r="F20" s="121"/>
+      <c r="G20" s="121"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="123"/>
-      <c r="J20" s="123"/>
+      <c r="I20" s="122"/>
+      <c r="J20" s="122"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="124"/>
-      <c r="M20" s="124"/>
+      <c r="L20" s="123"/>
+      <c r="M20" s="123"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="128"/>
-      <c r="P20" s="128"/>
+      <c r="O20" s="127"/>
+      <c r="P20" s="127"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17876,7 +17918,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -18216,7 +18258,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="135"/>
+      <c r="A2" s="134"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18542,15 +18584,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="136"/>
-      <c r="DH2" s="136"/>
-      <c r="DI2" s="136"/>
-      <c r="DJ2" s="136"/>
+      <c r="DG2" s="135"/>
+      <c r="DH2" s="135"/>
+      <c r="DI2" s="135"/>
+      <c r="DJ2" s="135"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="135"/>
+      <c r="A3" s="134"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18887,7 +18929,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="136" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -19029,7 +19071,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="137"/>
+      <c r="B5" s="136"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -19169,7 +19211,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="137"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19309,7 +19351,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="137"/>
+      <c r="B7" s="136"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19447,7 +19489,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="137"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19587,7 +19629,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="138" t="s">
+      <c r="B9" s="137" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19729,7 +19771,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="138"/>
+      <c r="B10" s="137"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19869,7 +19911,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="139" t="s">
+      <c r="B11" s="138" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -19999,7 +20041,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="139"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -20137,7 +20179,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="139"/>
+      <c r="B13" s="138"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20277,7 +20319,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="139"/>
+      <c r="B14" s="138"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20413,7 +20455,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="139"/>
+      <c r="B15" s="138"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20549,7 +20591,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="139"/>
+      <c r="B16" s="138"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20685,7 +20727,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="139"/>
+      <c r="B17" s="138"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20821,7 +20863,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="139"/>
+      <c r="B18" s="138"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -20961,7 +21003,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="139"/>
+      <c r="B19" s="138"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -21097,7 +21139,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="139"/>
+      <c r="B20" s="138"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -21233,7 +21275,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="133" t="s">
+      <c r="B21" s="132" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21367,7 +21409,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="133"/>
+      <c r="B22" s="132"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21503,7 +21545,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="133"/>
+      <c r="B23" s="132"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21635,7 +21677,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="133"/>
+      <c r="B24" s="132"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21769,7 +21811,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="133"/>
+      <c r="B25" s="132"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21913,7 +21955,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="134" t="s">
+      <c r="B26" s="133" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -22047,7 +22089,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="134"/>
+      <c r="B27" s="133"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -22187,7 +22229,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="134"/>
+      <c r="B28" s="133"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22319,7 +22361,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="134"/>
+      <c r="B29" s="133"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22447,7 +22489,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="134"/>
+      <c r="B30" s="133"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22573,7 +22615,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="134"/>
+      <c r="B31" s="133"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 27 e 28-11
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D1734-11FA-4EA0-A9E4-148F42A31F0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9358EB4-C446-474B-B597-29685F28A1B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="381">
   <si>
     <t>REDES</t>
   </si>
@@ -1231,6 +1231,31 @@
   </si>
   <si>
     <t>Layout de alta fidelidade do mapa da jornada, configuração de rotas da aplicação e editar e deletar imagem no Blobs</t>
+  </si>
+  <si>
+    <t>Testes API com versão Glpi virtual machine, estilização chamados WEB, refatoração código Mobile, teste unitário</t>
+  </si>
+  <si>
+    <t>Organização dos dados para exibição no gráfico e editar usuário WEB</t>
+  </si>
+  <si>
+    <t>Buscar todas as jornadas de um usuário logado WEB, atualizar e deletar no passo a passo inicial, feedback login Mobile, logout Mobile, correção de erros nos loopings das requisições para a API e deletar na página de listagem geral</t>
+  </si>
+  <si>
+    <t>Requisição genérica que associa Levels, Blocos e Achievements, query para busca de Levels com suas associações, correção da exibição de categorias nos cards, layout de alta fidelidade do mapa da jornada</t>
+  </si>
+  <si>
+    <t>Estudo requisição Zabbix, FAQ Mobile, Login Zabbix API, exibição de gráficos na tela através do Zabbix</t>
+  </si>
+  <si>
+    <t>Organização dos dados para exibição no gráfico, 
+criação de novo servidor para hospedar API e editar usuário</t>
+  </si>
+  <si>
+    <t>Filtros nas listas do dashboard, correção das listas na página de exportação, validações nos campos de login Mobile e na listagem de agendas e jornadas Mobile</t>
+  </si>
+  <si>
+    <t>Requisição genérica que associa Levels, Blobs, e Achievements, diagramas para documentação e layout de alta fidelidade do mapa da jornada</t>
   </si>
 </sst>
 </file>
@@ -2104,6 +2129,27 @@
     <xf numFmtId="0" fontId="12" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2112,18 +2158,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2180,15 +2214,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2588,10 +2613,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BX4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="BZ4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BZ11" sqref="BZ11"/>
+      <selection pane="bottomRight" activeCell="CD7" sqref="CD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2639,13 +2664,15 @@
     <col min="76" max="76" width="25.77734375" customWidth="1"/>
     <col min="77" max="77" width="30.77734375" customWidth="1"/>
     <col min="78" max="78" width="25.77734375" customWidth="1"/>
-    <col min="79" max="92" width="5.77734375" customWidth="1"/>
+    <col min="79" max="79" width="35.77734375" customWidth="1"/>
+    <col min="80" max="80" width="25.77734375" customWidth="1"/>
+    <col min="81" max="92" width="5.77734375" customWidth="1"/>
     <col min="93" max="93" width="3.77734375" style="81" customWidth="1"/>
     <col min="94" max="96" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="120" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2925,117 +2952,117 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="114"/>
+      <c r="A2" s="121"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="119" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="116" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="119"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="116"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="116"/>
-      <c r="V2" s="116"/>
-      <c r="W2" s="116"/>
-      <c r="X2" s="116"/>
-      <c r="Y2" s="116"/>
-      <c r="Z2" s="116"/>
-      <c r="AA2" s="116"/>
-      <c r="AB2" s="116"/>
-      <c r="AC2" s="116"/>
-      <c r="AD2" s="116"/>
-      <c r="AE2" s="116"/>
-      <c r="AF2" s="116"/>
-      <c r="AG2" s="116"/>
-      <c r="AH2" s="116"/>
-      <c r="AI2" s="116"/>
-      <c r="AJ2" s="116"/>
-      <c r="AK2" s="116"/>
-      <c r="AL2" s="116"/>
-      <c r="AM2" s="116" t="s">
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
+      <c r="AA2" s="119"/>
+      <c r="AB2" s="119"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="119"/>
+      <c r="AE2" s="119"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="119"/>
+      <c r="AH2" s="119"/>
+      <c r="AI2" s="119"/>
+      <c r="AJ2" s="119"/>
+      <c r="AK2" s="119"/>
+      <c r="AL2" s="119"/>
+      <c r="AM2" s="119" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="116"/>
-      <c r="AO2" s="116"/>
-      <c r="AP2" s="116"/>
-      <c r="AQ2" s="116"/>
-      <c r="AR2" s="116"/>
-      <c r="AS2" s="116"/>
-      <c r="AT2" s="116"/>
-      <c r="AU2" s="116"/>
-      <c r="AV2" s="116"/>
-      <c r="AW2" s="116"/>
-      <c r="AX2" s="116"/>
-      <c r="AY2" s="116"/>
-      <c r="AZ2" s="116"/>
-      <c r="BA2" s="116"/>
-      <c r="BB2" s="116"/>
-      <c r="BC2" s="116"/>
-      <c r="BD2" s="116"/>
-      <c r="BE2" s="116"/>
-      <c r="BF2" s="116"/>
-      <c r="BG2" s="116"/>
-      <c r="BH2" s="116"/>
-      <c r="BI2" s="116"/>
-      <c r="BJ2" s="116" t="s">
+      <c r="AN2" s="119"/>
+      <c r="AO2" s="119"/>
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="119"/>
+      <c r="AR2" s="119"/>
+      <c r="AS2" s="119"/>
+      <c r="AT2" s="119"/>
+      <c r="AU2" s="119"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="119"/>
+      <c r="AX2" s="119"/>
+      <c r="AY2" s="119"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="119"/>
+      <c r="BB2" s="119"/>
+      <c r="BC2" s="119"/>
+      <c r="BD2" s="119"/>
+      <c r="BE2" s="119"/>
+      <c r="BF2" s="119"/>
+      <c r="BG2" s="119"/>
+      <c r="BH2" s="119"/>
+      <c r="BI2" s="119"/>
+      <c r="BJ2" s="119" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="116"/>
-      <c r="BL2" s="116"/>
-      <c r="BM2" s="116"/>
-      <c r="BN2" s="116"/>
-      <c r="BO2" s="116"/>
-      <c r="BP2" s="116"/>
-      <c r="BQ2" s="116"/>
-      <c r="BR2" s="116"/>
-      <c r="BS2" s="116"/>
-      <c r="BT2" s="116"/>
-      <c r="BU2" s="116"/>
-      <c r="BV2" s="116"/>
-      <c r="BW2" s="116"/>
-      <c r="BX2" s="116"/>
-      <c r="BY2" s="116"/>
-      <c r="BZ2" s="116"/>
-      <c r="CA2" s="116"/>
-      <c r="CB2" s="116"/>
-      <c r="CC2" s="116"/>
-      <c r="CD2" s="116"/>
-      <c r="CE2" s="116" t="s">
+      <c r="BK2" s="119"/>
+      <c r="BL2" s="119"/>
+      <c r="BM2" s="119"/>
+      <c r="BN2" s="119"/>
+      <c r="BO2" s="119"/>
+      <c r="BP2" s="119"/>
+      <c r="BQ2" s="119"/>
+      <c r="BR2" s="119"/>
+      <c r="BS2" s="119"/>
+      <c r="BT2" s="119"/>
+      <c r="BU2" s="119"/>
+      <c r="BV2" s="119"/>
+      <c r="BW2" s="119"/>
+      <c r="BX2" s="119"/>
+      <c r="BY2" s="119"/>
+      <c r="BZ2" s="119"/>
+      <c r="CA2" s="119"/>
+      <c r="CB2" s="119"/>
+      <c r="CC2" s="119"/>
+      <c r="CD2" s="119"/>
+      <c r="CE2" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="116"/>
-      <c r="CG2" s="116"/>
-      <c r="CH2" s="116"/>
-      <c r="CI2" s="116"/>
-      <c r="CJ2" s="116"/>
-      <c r="CK2" s="116"/>
-      <c r="CL2" s="116"/>
-      <c r="CM2" s="116"/>
-      <c r="CN2" s="116"/>
-      <c r="CO2" s="116"/>
-      <c r="CP2" s="116"/>
-      <c r="CQ2" s="116"/>
-      <c r="CR2" s="116"/>
+      <c r="CF2" s="119"/>
+      <c r="CG2" s="119"/>
+      <c r="CH2" s="119"/>
+      <c r="CI2" s="119"/>
+      <c r="CJ2" s="119"/>
+      <c r="CK2" s="119"/>
+      <c r="CL2" s="119"/>
+      <c r="CM2" s="119"/>
+      <c r="CN2" s="119"/>
+      <c r="CO2" s="119"/>
+      <c r="CP2" s="119"/>
+      <c r="CQ2" s="119"/>
+      <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="115"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3323,10 +3350,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="119"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3462,10 +3489,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="117" t="s">
+      <c r="AV4" s="118" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="117" t="s">
+      <c r="AW4" s="118" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3534,7 +3561,7 @@
       <c r="BS4" s="105" t="s">
         <v>350</v>
       </c>
-      <c r="BT4" s="117" t="s">
+      <c r="BT4" s="118" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="107" t="s">
@@ -3543,41 +3570,45 @@
       <c r="BV4" s="108" t="s">
         <v>357</v>
       </c>
-      <c r="BW4" s="117" t="s">
+      <c r="BW4" s="118" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="111" t="s">
         <v>361</v>
       </c>
-      <c r="BY4" s="139" t="s">
+      <c r="BY4" s="113" t="s">
         <v>365</v>
       </c>
-      <c r="BZ4" s="139" t="s">
+      <c r="BZ4" s="113" t="s">
         <v>369</v>
       </c>
-      <c r="CA4" s="139"/>
-      <c r="CB4" s="139"/>
-      <c r="CC4" s="139"/>
-      <c r="CD4" s="139"/>
-      <c r="CE4" s="140"/>
-      <c r="CF4" s="140"/>
-      <c r="CG4" s="140"/>
-      <c r="CH4" s="140"/>
-      <c r="CI4" s="140"/>
-      <c r="CJ4" s="140"/>
-      <c r="CK4" s="140"/>
-      <c r="CL4" s="140"/>
-      <c r="CM4" s="140"/>
-      <c r="CN4" s="141"/>
-      <c r="CO4" s="117" t="s">
+      <c r="CA4" s="113" t="s">
+        <v>373</v>
+      </c>
+      <c r="CB4" s="113" t="s">
+        <v>377</v>
+      </c>
+      <c r="CC4" s="113"/>
+      <c r="CD4" s="113"/>
+      <c r="CE4" s="114"/>
+      <c r="CF4" s="114"/>
+      <c r="CG4" s="114"/>
+      <c r="CH4" s="114"/>
+      <c r="CI4" s="114"/>
+      <c r="CJ4" s="114"/>
+      <c r="CK4" s="114"/>
+      <c r="CL4" s="114"/>
+      <c r="CM4" s="114"/>
+      <c r="CN4" s="115"/>
+      <c r="CO4" s="118" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="119"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3711,8 +3742,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="117"/>
-      <c r="AW5" s="117"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3779,44 +3810,48 @@
       <c r="BS5" s="105" t="s">
         <v>351</v>
       </c>
-      <c r="BT5" s="117"/>
+      <c r="BT5" s="118"/>
       <c r="BU5" s="109" t="s">
         <v>354</v>
       </c>
       <c r="BV5" s="110" t="s">
         <v>358</v>
       </c>
-      <c r="BW5" s="117"/>
+      <c r="BW5" s="118"/>
       <c r="BX5" s="112" t="s">
         <v>362</v>
       </c>
-      <c r="BY5" s="139" t="s">
+      <c r="BY5" s="113" t="s">
         <v>366</v>
       </c>
-      <c r="BZ5" s="139" t="s">
+      <c r="BZ5" s="113" t="s">
         <v>370</v>
       </c>
-      <c r="CA5" s="139"/>
-      <c r="CB5" s="139"/>
-      <c r="CC5" s="139"/>
-      <c r="CD5" s="139"/>
-      <c r="CE5" s="140"/>
-      <c r="CF5" s="140"/>
-      <c r="CG5" s="140"/>
-      <c r="CH5" s="140"/>
-      <c r="CI5" s="140"/>
-      <c r="CJ5" s="140"/>
-      <c r="CK5" s="140"/>
-      <c r="CL5" s="140"/>
-      <c r="CM5" s="140"/>
-      <c r="CN5" s="141"/>
-      <c r="CO5" s="117"/>
+      <c r="CA5" s="113" t="s">
+        <v>374</v>
+      </c>
+      <c r="CB5" s="113" t="s">
+        <v>378</v>
+      </c>
+      <c r="CC5" s="113"/>
+      <c r="CD5" s="113"/>
+      <c r="CE5" s="114"/>
+      <c r="CF5" s="114"/>
+      <c r="CG5" s="114"/>
+      <c r="CH5" s="114"/>
+      <c r="CI5" s="114"/>
+      <c r="CJ5" s="114"/>
+      <c r="CK5" s="114"/>
+      <c r="CL5" s="114"/>
+      <c r="CM5" s="114"/>
+      <c r="CN5" s="115"/>
+      <c r="CO5" s="118"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="119"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3952,8 +3987,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="117"/>
-      <c r="AW6" s="117"/>
+      <c r="AV6" s="118"/>
+      <c r="AW6" s="118"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -4020,44 +4055,48 @@
       <c r="BS6" s="105" t="s">
         <v>352</v>
       </c>
-      <c r="BT6" s="117"/>
+      <c r="BT6" s="118"/>
       <c r="BU6" s="109" t="s">
         <v>355</v>
       </c>
       <c r="BV6" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="BW6" s="117"/>
+      <c r="BW6" s="118"/>
       <c r="BX6" s="112" t="s">
         <v>363</v>
       </c>
-      <c r="BY6" s="139" t="s">
+      <c r="BY6" s="113" t="s">
         <v>367</v>
       </c>
-      <c r="BZ6" s="139" t="s">
+      <c r="BZ6" s="113" t="s">
         <v>371</v>
       </c>
-      <c r="CA6" s="139"/>
-      <c r="CB6" s="139"/>
-      <c r="CC6" s="139"/>
-      <c r="CD6" s="139"/>
-      <c r="CE6" s="140"/>
-      <c r="CF6" s="140"/>
-      <c r="CG6" s="140"/>
-      <c r="CH6" s="140"/>
-      <c r="CI6" s="140"/>
-      <c r="CJ6" s="140"/>
-      <c r="CK6" s="140"/>
-      <c r="CL6" s="140"/>
-      <c r="CM6" s="140"/>
-      <c r="CN6" s="141"/>
-      <c r="CO6" s="117"/>
+      <c r="CA6" s="113" t="s">
+        <v>375</v>
+      </c>
+      <c r="CB6" s="113" t="s">
+        <v>379</v>
+      </c>
+      <c r="CC6" s="113"/>
+      <c r="CD6" s="113"/>
+      <c r="CE6" s="114"/>
+      <c r="CF6" s="114"/>
+      <c r="CG6" s="114"/>
+      <c r="CH6" s="114"/>
+      <c r="CI6" s="114"/>
+      <c r="CJ6" s="114"/>
+      <c r="CK6" s="114"/>
+      <c r="CL6" s="114"/>
+      <c r="CM6" s="114"/>
+      <c r="CN6" s="115"/>
+      <c r="CO6" s="118"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="119"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4193,8 +4232,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="117"/>
-      <c r="AW7" s="117"/>
+      <c r="AV7" s="118"/>
+      <c r="AW7" s="118"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4261,56 +4300,60 @@
       <c r="BS7" s="106" t="s">
         <v>353</v>
       </c>
-      <c r="BT7" s="117"/>
+      <c r="BT7" s="118"/>
       <c r="BU7" s="109" t="s">
         <v>356</v>
       </c>
       <c r="BV7" s="110" t="s">
         <v>360</v>
       </c>
-      <c r="BW7" s="117"/>
+      <c r="BW7" s="118"/>
       <c r="BX7" s="112" t="s">
         <v>364</v>
       </c>
-      <c r="BY7" s="139" t="s">
+      <c r="BY7" s="113" t="s">
         <v>368</v>
       </c>
-      <c r="BZ7" s="139" t="s">
+      <c r="BZ7" s="113" t="s">
         <v>372</v>
       </c>
-      <c r="CA7" s="139"/>
-      <c r="CB7" s="139"/>
-      <c r="CC7" s="139"/>
-      <c r="CD7" s="139"/>
-      <c r="CE7" s="140"/>
-      <c r="CF7" s="140"/>
-      <c r="CG7" s="140"/>
-      <c r="CH7" s="140"/>
-      <c r="CI7" s="140"/>
-      <c r="CJ7" s="140"/>
-      <c r="CK7" s="140"/>
-      <c r="CL7" s="140"/>
-      <c r="CM7" s="140"/>
-      <c r="CN7" s="141"/>
-      <c r="CO7" s="117"/>
+      <c r="CA7" s="113" t="s">
+        <v>376</v>
+      </c>
+      <c r="CB7" s="113" t="s">
+        <v>380</v>
+      </c>
+      <c r="CC7" s="113"/>
+      <c r="CD7" s="113"/>
+      <c r="CE7" s="114"/>
+      <c r="CF7" s="114"/>
+      <c r="CG7" s="114"/>
+      <c r="CH7" s="114"/>
+      <c r="CI7" s="114"/>
+      <c r="CJ7" s="114"/>
+      <c r="CK7" s="114"/>
+      <c r="CL7" s="114"/>
+      <c r="CM7" s="114"/>
+      <c r="CN7" s="115"/>
+      <c r="CO7" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4393,36 +4436,36 @@
     </row>
     <row r="2" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="127" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
       <c r="E2" s="89"/>
-      <c r="F2" s="128" t="s">
+      <c r="F2" s="131" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="128"/>
+      <c r="G2" s="131"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="129" t="s">
+      <c r="I2" s="132" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="129"/>
+      <c r="J2" s="132"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="130" t="s">
+      <c r="L2" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="130"/>
+      <c r="M2" s="133"/>
       <c r="N2" s="90"/>
-      <c r="O2" s="131" t="s">
+      <c r="O2" s="134" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="131"/>
+      <c r="P2" s="134"/>
       <c r="Q2" s="89"/>
-      <c r="R2" s="120" t="s">
+      <c r="R2" s="123" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="120"/>
+      <c r="S2" s="123"/>
       <c r="T2" s="89"/>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -4456,24 +4499,24 @@
     </row>
     <row r="3" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
       <c r="E3" s="89"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="89"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
       <c r="K3" s="89"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
       <c r="N3" s="90"/>
-      <c r="O3" s="131"/>
-      <c r="P3" s="131"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="89"/>
-      <c r="R3" s="120"/>
-      <c r="S3" s="120"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
       <c r="T3" s="89"/>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
@@ -4507,24 +4550,24 @@
     </row>
     <row r="4" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
       <c r="E4" s="89"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="89"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
       <c r="K4" s="89"/>
-      <c r="L4" s="130"/>
-      <c r="M4" s="130"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
       <c r="N4" s="90"/>
-      <c r="O4" s="131"/>
-      <c r="P4" s="131"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
       <c r="Q4" s="89"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="120"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
       <c r="T4" s="89"/>
       <c r="U4" s="89"/>
       <c r="V4" s="89"/>
@@ -4562,20 +4605,20 @@
       <c r="C5" s="89"/>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="89"/>
-      <c r="I5" s="129"/>
-      <c r="J5" s="129"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="89"/>
-      <c r="L5" s="130"/>
-      <c r="M5" s="130"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
       <c r="N5" s="89"/>
-      <c r="O5" s="131"/>
-      <c r="P5" s="131"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
       <c r="Q5" s="89"/>
-      <c r="R5" s="120"/>
-      <c r="S5" s="120"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
       <c r="V5" s="89"/>
@@ -4609,26 +4652,26 @@
     </row>
     <row r="6" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
       <c r="E6" s="89"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
       <c r="H6" s="89"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
       <c r="K6" s="89"/>
-      <c r="L6" s="130"/>
-      <c r="M6" s="130"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
       <c r="N6" s="89"/>
-      <c r="O6" s="131"/>
-      <c r="P6" s="131"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
       <c r="Q6" s="89"/>
-      <c r="R6" s="120"/>
-      <c r="S6" s="120"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
       <c r="T6" s="89"/>
       <c r="U6" s="89"/>
       <c r="V6" s="89"/>
@@ -4662,24 +4705,24 @@
     </row>
     <row r="7" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
       <c r="E7" s="89"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="129"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
       <c r="K7" s="89"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="130"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="133"/>
       <c r="N7" s="89"/>
-      <c r="O7" s="131"/>
-      <c r="P7" s="131"/>
+      <c r="O7" s="134"/>
+      <c r="P7" s="134"/>
       <c r="Q7" s="89"/>
-      <c r="R7" s="120"/>
-      <c r="S7" s="120"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="123"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
       <c r="V7" s="89"/>
@@ -4713,24 +4756,24 @@
     </row>
     <row r="8" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
       <c r="E8" s="89"/>
-      <c r="F8" s="128"/>
-      <c r="G8" s="128"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
       <c r="H8" s="89"/>
-      <c r="I8" s="129"/>
-      <c r="J8" s="129"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="130"/>
-      <c r="M8" s="130"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="133"/>
       <c r="N8" s="89"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="134"/>
       <c r="Q8" s="89"/>
-      <c r="R8" s="120"/>
-      <c r="S8" s="120"/>
+      <c r="R8" s="123"/>
+      <c r="S8" s="123"/>
       <c r="T8" s="89"/>
       <c r="U8" s="89"/>
       <c r="V8" s="89"/>
@@ -4764,24 +4807,24 @@
     </row>
     <row r="9" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
       <c r="E9" s="89"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="128"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
       <c r="H9" s="89"/>
-      <c r="I9" s="129"/>
-      <c r="J9" s="129"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
       <c r="K9" s="89"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="130"/>
+      <c r="L9" s="133"/>
+      <c r="M9" s="133"/>
       <c r="N9" s="89"/>
-      <c r="O9" s="131"/>
-      <c r="P9" s="131"/>
+      <c r="O9" s="134"/>
+      <c r="P9" s="134"/>
       <c r="Q9" s="89"/>
-      <c r="R9" s="120"/>
-      <c r="S9" s="120"/>
+      <c r="R9" s="123"/>
+      <c r="S9" s="123"/>
       <c r="T9" s="89"/>
       <c r="U9" s="89"/>
       <c r="V9" s="89"/>
@@ -4815,24 +4858,24 @@
     </row>
     <row r="10" spans="1:49" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="126"/>
-      <c r="C10" s="126"/>
-      <c r="D10" s="126"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
       <c r="E10" s="89"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="131"/>
       <c r="H10" s="89"/>
-      <c r="I10" s="129"/>
-      <c r="J10" s="129"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
       <c r="K10" s="89"/>
-      <c r="L10" s="130"/>
-      <c r="M10" s="130"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="133"/>
       <c r="N10" s="89"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
+      <c r="O10" s="134"/>
+      <c r="P10" s="134"/>
       <c r="Q10" s="89"/>
-      <c r="R10" s="120"/>
-      <c r="S10" s="120"/>
+      <c r="R10" s="123"/>
+      <c r="S10" s="123"/>
       <c r="T10" s="89"/>
       <c r="U10" s="89"/>
       <c r="V10" s="89"/>
@@ -4921,23 +4964,23 @@
       <c r="C12" s="89"/>
       <c r="D12" s="89"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="121" t="s">
+      <c r="F12" s="124" t="s">
         <v>171</v>
       </c>
-      <c r="G12" s="121"/>
+      <c r="G12" s="124"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="122" t="s">
+      <c r="I12" s="125" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="122"/>
+      <c r="J12" s="125"/>
       <c r="K12" s="89"/>
-      <c r="L12" s="123" t="s">
+      <c r="L12" s="126" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="123"/>
+      <c r="M12" s="126"/>
       <c r="N12" s="89"/>
-      <c r="O12" s="127"/>
-      <c r="P12" s="127"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
       <c r="Q12" s="89"/>
       <c r="R12" s="89"/>
       <c r="S12" s="89"/>
@@ -4978,17 +5021,17 @@
       <c r="C13" s="89"/>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="89"/>
-      <c r="I13" s="122"/>
-      <c r="J13" s="122"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
       <c r="K13" s="89"/>
-      <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
       <c r="N13" s="89"/>
-      <c r="O13" s="127"/>
-      <c r="P13" s="127"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
       <c r="Q13" s="89"/>
       <c r="R13" s="89"/>
       <c r="S13" s="89"/>
@@ -5029,17 +5072,17 @@
       <c r="C14" s="89"/>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="121"/>
-      <c r="G14" s="121"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
       <c r="H14" s="89"/>
-      <c r="I14" s="122"/>
-      <c r="J14" s="122"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125"/>
       <c r="K14" s="89"/>
-      <c r="L14" s="123"/>
-      <c r="M14" s="123"/>
+      <c r="L14" s="126"/>
+      <c r="M14" s="126"/>
       <c r="N14" s="89"/>
-      <c r="O14" s="127"/>
-      <c r="P14" s="127"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
       <c r="Q14" s="89"/>
       <c r="R14" s="89"/>
       <c r="S14" s="89"/>
@@ -5080,17 +5123,17 @@
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="121"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
       <c r="H15" s="89"/>
-      <c r="I15" s="122"/>
-      <c r="J15" s="122"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="125"/>
       <c r="K15" s="89"/>
-      <c r="L15" s="123"/>
-      <c r="M15" s="123"/>
+      <c r="L15" s="126"/>
+      <c r="M15" s="126"/>
       <c r="N15" s="89"/>
-      <c r="O15" s="127"/>
-      <c r="P15" s="127"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
       <c r="Q15" s="89"/>
       <c r="R15" s="89"/>
       <c r="S15" s="89"/>
@@ -5131,17 +5174,17 @@
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="89"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="121"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
       <c r="H16" s="89"/>
-      <c r="I16" s="122"/>
-      <c r="J16" s="122"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="125"/>
       <c r="K16" s="89"/>
-      <c r="L16" s="123"/>
-      <c r="M16" s="123"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="126"/>
       <c r="N16" s="89"/>
-      <c r="O16" s="127"/>
-      <c r="P16" s="127"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="130"/>
       <c r="Q16" s="89"/>
       <c r="R16" s="89"/>
       <c r="S16" s="89"/>
@@ -5182,17 +5225,17 @@
       <c r="C17" s="89"/>
       <c r="D17" s="89"/>
       <c r="E17" s="89"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
       <c r="H17" s="89"/>
-      <c r="I17" s="122"/>
-      <c r="J17" s="122"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="125"/>
       <c r="K17" s="89"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
+      <c r="L17" s="126"/>
+      <c r="M17" s="126"/>
       <c r="N17" s="89"/>
-      <c r="O17" s="127"/>
-      <c r="P17" s="127"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
       <c r="S17" s="89"/>
@@ -5233,17 +5276,17 @@
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="121"/>
-      <c r="G18" s="121"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="122"/>
-      <c r="J18" s="122"/>
+      <c r="I18" s="125"/>
+      <c r="J18" s="125"/>
       <c r="K18" s="89"/>
-      <c r="L18" s="123"/>
-      <c r="M18" s="123"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="126"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="127"/>
-      <c r="P18" s="127"/>
+      <c r="O18" s="130"/>
+      <c r="P18" s="130"/>
       <c r="Q18" s="89"/>
       <c r="R18" s="89"/>
       <c r="S18" s="89"/>
@@ -5284,17 +5327,17 @@
       <c r="C19" s="89"/>
       <c r="D19" s="89"/>
       <c r="E19" s="89"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
       <c r="H19" s="89"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="122"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
       <c r="K19" s="89"/>
-      <c r="L19" s="123"/>
-      <c r="M19" s="123"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
       <c r="N19" s="89"/>
-      <c r="O19" s="127"/>
-      <c r="P19" s="127"/>
+      <c r="O19" s="130"/>
+      <c r="P19" s="130"/>
       <c r="Q19" s="89"/>
       <c r="R19" s="89"/>
       <c r="S19" s="89"/>
@@ -5335,17 +5378,17 @@
       <c r="C20" s="89"/>
       <c r="D20" s="89"/>
       <c r="E20" s="89"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="122"/>
-      <c r="J20" s="122"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="125"/>
       <c r="K20" s="89"/>
-      <c r="L20" s="123"/>
-      <c r="M20" s="123"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="126"/>
       <c r="N20" s="89"/>
-      <c r="O20" s="127"/>
-      <c r="P20" s="127"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="130"/>
       <c r="Q20" s="89"/>
       <c r="R20" s="89"/>
       <c r="S20" s="89"/>
@@ -17918,7 +17961,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -18258,7 +18301,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="134"/>
+      <c r="A2" s="137"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -18584,15 +18627,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="135"/>
-      <c r="DH2" s="135"/>
-      <c r="DI2" s="135"/>
-      <c r="DJ2" s="135"/>
+      <c r="DG2" s="138"/>
+      <c r="DH2" s="138"/>
+      <c r="DI2" s="138"/>
+      <c r="DJ2" s="138"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="134"/>
+      <c r="A3" s="137"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -18929,7 +18972,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="139" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -19071,7 +19114,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="136"/>
+      <c r="B5" s="139"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -19211,7 +19254,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="136"/>
+      <c r="B6" s="139"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -19351,7 +19394,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="136"/>
+      <c r="B7" s="139"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -19489,7 +19532,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="136"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -19629,7 +19672,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="137" t="s">
+      <c r="B9" s="140" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -19771,7 +19814,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="137"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -19911,7 +19954,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="141" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -20041,7 +20084,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="138"/>
+      <c r="B12" s="141"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -20179,7 +20222,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="138"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -20319,7 +20362,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="138"/>
+      <c r="B14" s="141"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -20455,7 +20498,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="138"/>
+      <c r="B15" s="141"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -20591,7 +20634,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="138"/>
+      <c r="B16" s="141"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -20727,7 +20770,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="138"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -20863,7 +20906,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="138"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -21003,7 +21046,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="138"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -21139,7 +21182,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="138"/>
+      <c r="B20" s="141"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -21275,7 +21318,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="132" t="s">
+      <c r="B21" s="135" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -21409,7 +21452,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="132"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -21545,7 +21588,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="132"/>
+      <c r="B23" s="135"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -21677,7 +21720,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="132"/>
+      <c r="B24" s="135"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -21811,7 +21854,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="132"/>
+      <c r="B25" s="135"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -21955,7 +21998,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="133" t="s">
+      <c r="B26" s="136" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -22089,7 +22132,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="133"/>
+      <c r="B27" s="136"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -22229,7 +22272,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="133"/>
+      <c r="B28" s="136"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -22361,7 +22404,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="133"/>
+      <c r="B29" s="136"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -22489,7 +22532,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="133"/>
+      <c r="B30" s="136"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -22615,7 +22658,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="133"/>
+      <c r="B31" s="136"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>

</xml_diff>

<commit_message>
Adiciona dailies realizadas em 29-11, 02 e 03-12
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
+++ b/Cronograma/Projeto_Cronograma_acompanhamento_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9358EB4-C446-474B-B597-29685F28A1B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FDE28B-F209-4937-8D6C-761B9135D2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="393">
   <si>
     <t>REDES</t>
   </si>
@@ -1256,6 +1256,43 @@
   </si>
   <si>
     <t>Requisição genérica que associa Levels, Blobs, e Achievements, diagramas para documentação e layout de alta fidelidade do mapa da jornada</t>
+  </si>
+  <si>
+    <t>Estudo da biblioteca chart.Js, estilização lista de usuários e editar usuário WEB, FAQ Mobile e estudo requisição Zabbix</t>
+  </si>
+  <si>
+    <t>Organização dos dados para exibição no gráfico, criação de novo servidor para hospedar API e editar usuário</t>
+  </si>
+  <si>
+    <t>Filtro nas listas do dashboard, ajustes no cadastro de agendas na dashboard, listagem de jornadas Mobile e 
+método editar na página de listagem de geral</t>
+  </si>
+  <si>
+    <t>Fluxo de navegação de telas e correção de bugs gerais</t>
+  </si>
+  <si>
+    <t>Estilização lista de chamadas adicionando grupo responsável e última tarefa e estudo da biblioteca chart Js</t>
+  </si>
+  <si>
+    <t>Estilização dos relatórios gerados com os gráficos e hospedagem da API</t>
+  </si>
+  <si>
+    <t>Merge de arquivos nas branches, ajustes e responsividade gerais e listagem de agendas Mobile</t>
+  </si>
+  <si>
+    <t>Documentação e preparação da apresentação para o cliente</t>
+  </si>
+  <si>
+    <t>Estilização e funcionalidade reabrir chamado WEB, ajustes na lista de chamados Mobile, estudo das requests para o Zabbix e requisições da API para o Zabbix para trazer os Hosts</t>
+  </si>
+  <si>
+    <t>Busca e solução de bugs no front-end e integração das funcionalidades front-end para mesma branch</t>
+  </si>
+  <si>
+    <t>Resolução de problemas com requisições e renderizações na dashboard, ajustes em estilizações gerais de todas as páginas, permissão de requisições, ordenação de agendas Mobile e seleção de clientes para exportação</t>
+  </si>
+  <si>
+    <t>Cadastro de Jornadas, finalização redirecionamentos, documentação e componentes relacionados à jornada</t>
   </si>
 </sst>
 </file>
@@ -2138,18 +2175,6 @@
     <xf numFmtId="0" fontId="12" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2158,6 +2183,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2613,10 +2650,10 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BZ4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="CA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CD7" sqref="CD7"/>
+      <selection pane="bottomRight" activeCell="CE4" sqref="CE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2666,13 +2703,15 @@
     <col min="78" max="78" width="25.77734375" customWidth="1"/>
     <col min="79" max="79" width="35.77734375" customWidth="1"/>
     <col min="80" max="80" width="25.77734375" customWidth="1"/>
-    <col min="81" max="92" width="5.77734375" customWidth="1"/>
+    <col min="81" max="82" width="20.77734375" customWidth="1"/>
+    <col min="83" max="83" width="30.77734375" customWidth="1"/>
+    <col min="84" max="92" width="5.77734375" customWidth="1"/>
     <col min="93" max="93" width="3.77734375" style="81" customWidth="1"/>
     <col min="94" max="96" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="116" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -2952,7 +2991,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121"/>
+      <c r="A2" s="117"/>
       <c r="B2" s="86" t="s">
         <v>104</v>
       </c>
@@ -3062,7 +3101,7 @@
       <c r="CR2" s="119"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="122"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="86" t="s">
         <v>110</v>
       </c>
@@ -3350,10 +3389,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="91" t="s">
         <v>117</v>
       </c>
@@ -3489,10 +3528,10 @@
       <c r="AU4" s="97" t="s">
         <v>277</v>
       </c>
-      <c r="AV4" s="118" t="s">
+      <c r="AV4" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="AW4" s="118" t="s">
+      <c r="AW4" s="120" t="s">
         <v>281</v>
       </c>
       <c r="AX4" s="98" t="s">
@@ -3561,7 +3600,7 @@
       <c r="BS4" s="105" t="s">
         <v>350</v>
       </c>
-      <c r="BT4" s="118" t="s">
+      <c r="BT4" s="120" t="s">
         <v>112</v>
       </c>
       <c r="BU4" s="107" t="s">
@@ -3570,7 +3609,7 @@
       <c r="BV4" s="108" t="s">
         <v>357</v>
       </c>
-      <c r="BW4" s="118" t="s">
+      <c r="BW4" s="120" t="s">
         <v>113</v>
       </c>
       <c r="BX4" s="111" t="s">
@@ -3588,9 +3627,15 @@
       <c r="CB4" s="113" t="s">
         <v>377</v>
       </c>
-      <c r="CC4" s="113"/>
-      <c r="CD4" s="113"/>
-      <c r="CE4" s="114"/>
+      <c r="CC4" s="113" t="s">
+        <v>381</v>
+      </c>
+      <c r="CD4" s="113" t="s">
+        <v>385</v>
+      </c>
+      <c r="CE4" s="114" t="s">
+        <v>389</v>
+      </c>
       <c r="CF4" s="114"/>
       <c r="CG4" s="114"/>
       <c r="CH4" s="114"/>
@@ -3600,15 +3645,15 @@
       <c r="CL4" s="114"/>
       <c r="CM4" s="114"/>
       <c r="CN4" s="115"/>
-      <c r="CO4" s="118" t="s">
+      <c r="CO4" s="120" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="117"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="91" t="s">
         <v>117</v>
       </c>
@@ -3742,8 +3787,8 @@
       <c r="AU5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
+      <c r="AV5" s="120"/>
+      <c r="AW5" s="120"/>
       <c r="AX5" s="102" t="s">
         <v>283</v>
       </c>
@@ -3810,14 +3855,14 @@
       <c r="BS5" s="105" t="s">
         <v>351</v>
       </c>
-      <c r="BT5" s="118"/>
+      <c r="BT5" s="120"/>
       <c r="BU5" s="109" t="s">
         <v>354</v>
       </c>
       <c r="BV5" s="110" t="s">
         <v>358</v>
       </c>
-      <c r="BW5" s="118"/>
+      <c r="BW5" s="120"/>
       <c r="BX5" s="112" t="s">
         <v>362</v>
       </c>
@@ -3833,9 +3878,15 @@
       <c r="CB5" s="113" t="s">
         <v>378</v>
       </c>
-      <c r="CC5" s="113"/>
-      <c r="CD5" s="113"/>
-      <c r="CE5" s="114"/>
+      <c r="CC5" s="113" t="s">
+        <v>382</v>
+      </c>
+      <c r="CD5" s="113" t="s">
+        <v>386</v>
+      </c>
+      <c r="CE5" s="114" t="s">
+        <v>390</v>
+      </c>
       <c r="CF5" s="114"/>
       <c r="CG5" s="114"/>
       <c r="CH5" s="114"/>
@@ -3845,13 +3896,13 @@
       <c r="CL5" s="114"/>
       <c r="CM5" s="114"/>
       <c r="CN5" s="115"/>
-      <c r="CO5" s="118"/>
+      <c r="CO5" s="120"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="117"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="91" t="s">
         <v>117</v>
       </c>
@@ -3987,8 +4038,8 @@
       <c r="AU6" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="AV6" s="118"/>
-      <c r="AW6" s="118"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
       <c r="AX6" s="102" t="s">
         <v>284</v>
       </c>
@@ -4055,14 +4106,14 @@
       <c r="BS6" s="105" t="s">
         <v>352</v>
       </c>
-      <c r="BT6" s="118"/>
+      <c r="BT6" s="120"/>
       <c r="BU6" s="109" t="s">
         <v>355</v>
       </c>
       <c r="BV6" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="BW6" s="118"/>
+      <c r="BW6" s="120"/>
       <c r="BX6" s="112" t="s">
         <v>363</v>
       </c>
@@ -4078,9 +4129,15 @@
       <c r="CB6" s="113" t="s">
         <v>379</v>
       </c>
-      <c r="CC6" s="113"/>
-      <c r="CD6" s="113"/>
-      <c r="CE6" s="114"/>
+      <c r="CC6" s="113" t="s">
+        <v>383</v>
+      </c>
+      <c r="CD6" s="113" t="s">
+        <v>387</v>
+      </c>
+      <c r="CE6" s="114" t="s">
+        <v>391</v>
+      </c>
       <c r="CF6" s="114"/>
       <c r="CG6" s="114"/>
       <c r="CH6" s="114"/>
@@ -4090,13 +4147,13 @@
       <c r="CL6" s="114"/>
       <c r="CM6" s="114"/>
       <c r="CN6" s="115"/>
-      <c r="CO6" s="118"/>
+      <c r="CO6" s="120"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="91" t="s">
         <v>117</v>
       </c>
@@ -4232,8 +4289,8 @@
       <c r="AU7" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="AV7" s="118"/>
-      <c r="AW7" s="118"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
       <c r="AX7" s="102" t="s">
         <v>285</v>
       </c>
@@ -4300,14 +4357,14 @@
       <c r="BS7" s="106" t="s">
         <v>353</v>
       </c>
-      <c r="BT7" s="118"/>
+      <c r="BT7" s="120"/>
       <c r="BU7" s="109" t="s">
         <v>356</v>
       </c>
       <c r="BV7" s="110" t="s">
         <v>360</v>
       </c>
-      <c r="BW7" s="118"/>
+      <c r="BW7" s="120"/>
       <c r="BX7" s="112" t="s">
         <v>364</v>
       </c>
@@ -4323,9 +4380,15 @@
       <c r="CB7" s="113" t="s">
         <v>380</v>
       </c>
-      <c r="CC7" s="113"/>
-      <c r="CD7" s="113"/>
-      <c r="CE7" s="114"/>
+      <c r="CC7" s="113" t="s">
+        <v>384</v>
+      </c>
+      <c r="CD7" s="113" t="s">
+        <v>388</v>
+      </c>
+      <c r="CE7" s="114" t="s">
+        <v>392</v>
+      </c>
       <c r="CF7" s="114"/>
       <c r="CG7" s="114"/>
       <c r="CH7" s="114"/>
@@ -4335,25 +4398,25 @@
       <c r="CL7" s="114"/>
       <c r="CM7" s="114"/>
       <c r="CN7" s="115"/>
-      <c r="CO7" s="118"/>
+      <c r="CO7" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>